<commit_message>
Fixed bug in memory map Fixed bug in FORTH word J
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Map" sheetId="1" r:id="rId1"/>
@@ -1004,8 +1004,8 @@
   </sheetPr>
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -2454,7 +2454,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Updated paramater and return stacks to operate with 32 bit SRAM bus
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545"/>
@@ -11,7 +11,7 @@
     <sheet name="Hardware registers" sheetId="2" r:id="rId2"/>
     <sheet name="Copyright and license" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -510,8 +510,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -789,6 +789,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -823,6 +824,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -998,17 +1000,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="5" width="12.42578125" style="1" customWidth="1"/>
@@ -1021,12 +1023,12 @@
     <col min="14" max="14" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1">
+    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -1041,7 +1043,7 @@
       <c r="M3"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -1071,7 +1073,7 @@
       <c r="M4"/>
       <c r="N4"/>
     </row>
-    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13" t="s">
         <v>8</v>
@@ -1094,7 +1096,7 @@
       <c r="M5"/>
       <c r="N5"/>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1110,7 +1112,7 @@
       <c r="M6"/>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>45056</v>
       </c>
@@ -1140,7 +1142,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>12288</v>
       </c>
@@ -1165,7 +1167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <f>2048</f>
         <v>2048</v>
@@ -1197,7 +1199,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <f>2048</f>
         <v>2048</v>
@@ -1229,7 +1231,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>2048</v>
       </c>
@@ -1260,10 +1262,10 @@
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1">
+    <row r="13" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>59</v>
       </c>
@@ -1278,7 +1280,7 @@
       <c r="M13"/>
       <c r="N13"/>
     </row>
-    <row r="14" spans="1:14" s="10" customFormat="1">
+    <row r="14" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>6</v>
       </c>
@@ -1306,7 +1308,7 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" s="11" customFormat="1">
+    <row r="15" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="13" t="s">
         <v>8</v>
@@ -1329,7 +1331,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" s="2" customFormat="1">
+    <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1345,7 +1347,7 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>4</v>
       </c>
@@ -1376,7 +1378,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>4</v>
       </c>
@@ -1407,7 +1409,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>1</v>
       </c>
@@ -1438,7 +1440,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>1</v>
       </c>
@@ -1469,7 +1471,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>1</v>
       </c>
@@ -1500,7 +1502,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>1</v>
       </c>
@@ -1531,7 +1533,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>2</v>
       </c>
@@ -1562,7 +1564,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>1</v>
       </c>
@@ -1593,7 +1595,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>1</v>
       </c>
@@ -1624,7 +1626,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>2</v>
       </c>
@@ -1655,7 +1657,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>1</v>
       </c>
@@ -1686,7 +1688,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>1</v>
       </c>
@@ -1717,7 +1719,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>4</v>
       </c>
@@ -1748,7 +1750,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>4</v>
       </c>
@@ -1779,7 +1781,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>2</v>
       </c>
@@ -1810,7 +1812,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>2</v>
       </c>
@@ -1841,7 +1843,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>1</v>
       </c>
@@ -1872,7 +1874,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>1</v>
       </c>
@@ -1903,7 +1905,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>1</v>
       </c>
@@ -1934,7 +1936,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>1</v>
       </c>
@@ -1965,7 +1967,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>1</v>
       </c>
@@ -1996,7 +1998,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <f>C38-B38</f>
         <v>2010</v>
@@ -2022,7 +2024,7 @@
       </c>
       <c r="H38" s="34"/>
     </row>
-    <row r="40" spans="1:14" s="9" customFormat="1">
+    <row r="40" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>33</v>
       </c>
@@ -2037,7 +2039,7 @@
       <c r="M40"/>
       <c r="N40"/>
     </row>
-    <row r="41" spans="1:14" s="10" customFormat="1">
+    <row r="41" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>6</v>
       </c>
@@ -2065,7 +2067,7 @@
       <c r="M41"/>
       <c r="N41"/>
     </row>
-    <row r="42" spans="1:14" s="10" customFormat="1">
+    <row r="42" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13" t="s">
         <v>8</v>
@@ -2088,7 +2090,7 @@
       <c r="M42"/>
       <c r="N42"/>
     </row>
-    <row r="43" spans="1:14" s="5" customFormat="1">
+    <row r="43" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -2104,7 +2106,7 @@
       <c r="M43"/>
       <c r="N43"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>65536</v>
       </c>
@@ -2129,7 +2131,7 @@
       </c>
       <c r="H44" s="34"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>256</v>
       </c>
@@ -2157,7 +2159,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>256</v>
       </c>
@@ -2185,7 +2187,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>256</v>
       </c>
@@ -2213,7 +2215,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>256</v>
       </c>
@@ -2241,7 +2243,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>256</v>
       </c>
@@ -2269,7 +2271,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>256</v>
       </c>
@@ -2297,7 +2299,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>256</v>
       </c>
@@ -2325,7 +2327,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <f>2*(100*75*2)</f>
         <v>30000</v>
@@ -2354,7 +2356,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <f>(640*480*1)</f>
         <v>307200</v>
@@ -2383,7 +2385,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="54" spans="1:9">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <f>64*1024</f>
         <v>65536</v>
@@ -2412,7 +2414,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="55" spans="1:9">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <f>C55-B55</f>
         <v>16307151</v>
@@ -2451,14 +2453,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="6" width="1.5703125" customWidth="1"/>
@@ -2471,7 +2473,7 @@
     <col min="15" max="15" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>82</v>
       </c>
@@ -2480,13 +2482,13 @@
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -2517,7 +2519,7 @@
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="13" t="s">
         <v>8</v>
@@ -2558,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -2575,7 +2577,7 @@
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" s="21" customFormat="1" ht="30">
+    <row r="6" spans="1:15" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <f>'Memory Map'!A20</f>
         <v>1</v>
@@ -2626,7 +2628,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="21" customFormat="1">
+    <row r="7" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -2643,7 +2645,7 @@
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -2660,7 +2662,7 @@
       <c r="N8" s="26"/>
       <c r="O8" s="26"/>
     </row>
-    <row r="9" spans="1:15" s="21" customFormat="1" ht="30">
+    <row r="9" spans="1:15" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <f>'Memory Map'!A27</f>
         <v>1</v>
@@ -2711,7 +2713,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="21" customFormat="1">
+    <row r="10" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -2728,7 +2730,7 @@
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
     </row>
-    <row r="11" spans="1:15" s="21" customFormat="1">
+    <row r="11" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -2745,7 +2747,7 @@
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>'Memory Map'!A31-1</f>
         <v>1</v>
@@ -2799,7 +2801,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G13" s="2"/>
       <c r="H13" s="24"/>
       <c r="I13" s="27">
@@ -2824,20 +2826,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G14" s="2"/>
       <c r="H14" s="24" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G15" s="2"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:15" ht="30">
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <f>'Memory Map'!A35</f>
         <v>1</v>
@@ -2887,7 +2889,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
@@ -2897,7 +2899,7 @@
       <c r="N18" s="27"/>
       <c r="O18" s="27"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -2905,7 +2907,7 @@
       <c r="E19" s="22"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <f>'Memory Map'!A36</f>
         <v>1</v>
@@ -2955,7 +2957,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>86</v>
       </c>
@@ -2967,60 +2969,60 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="109.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30">
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="45">
+    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
     </row>
-    <row r="10" spans="1:1" ht="60">
+    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>101</v>
       </c>

</xml_diff>

<commit_message>
Various small bug fixes to make the wide SRAM compatible with the revised hardware registers and interrupts, including fixed initialization of TBE interrupt line in interrupt controller.
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545"/>
@@ -11,7 +11,7 @@
     <sheet name="Hardware registers" sheetId="2" r:id="rId2"/>
     <sheet name="Copyright and license" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -478,8 +478,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -757,6 +757,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -791,6 +792,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -966,17 +968,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="5" width="12.42578125" style="1" customWidth="1"/>
@@ -989,12 +991,12 @@
     <col min="14" max="14" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1">
+    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -1009,7 +1011,7 @@
       <c r="M3"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -1039,7 +1041,7 @@
       <c r="M4"/>
       <c r="N4"/>
     </row>
-    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13" t="s">
         <v>8</v>
@@ -1062,7 +1064,7 @@
       <c r="M5"/>
       <c r="N5"/>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1078,7 +1080,7 @@
       <c r="M6"/>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>45056</v>
       </c>
@@ -1108,7 +1110,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>12288</v>
       </c>
@@ -1133,7 +1135,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <f>2048</f>
         <v>2048</v>
@@ -1165,7 +1167,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <f>2048</f>
         <v>2048</v>
@@ -1197,7 +1199,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>2048</v>
       </c>
@@ -1228,10 +1230,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1">
+    <row r="13" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>52</v>
       </c>
@@ -1246,7 +1248,7 @@
       <c r="M13"/>
       <c r="N13"/>
     </row>
-    <row r="14" spans="1:14" s="10" customFormat="1">
+    <row r="14" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>6</v>
       </c>
@@ -1274,7 +1276,7 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" s="11" customFormat="1">
+    <row r="15" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="13" t="s">
         <v>8</v>
@@ -1297,7 +1299,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" s="2" customFormat="1">
+    <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1313,7 +1315,7 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>4</v>
       </c>
@@ -1344,12 +1346,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>4</v>
       </c>
       <c r="B18" s="7">
-        <f>C17+1</f>
+        <f>B17+4</f>
         <v>63492</v>
       </c>
       <c r="C18" s="7">
@@ -1375,12 +1377,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>1</v>
       </c>
       <c r="B19" s="7">
-        <f t="shared" ref="B19:B22" si="9">C18+1</f>
+        <f t="shared" ref="B19:B35" si="9">B18+4</f>
         <v>63496</v>
       </c>
       <c r="C19" s="7">
@@ -1406,25 +1408,25 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>1</v>
       </c>
       <c r="B20" s="7">
         <f t="shared" si="9"/>
-        <v>63497</v>
+        <v>63500</v>
       </c>
       <c r="C20" s="7">
         <f t="shared" si="10"/>
-        <v>63497</v>
+        <v>63500</v>
       </c>
       <c r="D20" s="7" t="str">
         <f t="shared" si="11"/>
-        <v>F809</v>
+        <v>F80C</v>
       </c>
       <c r="E20" s="7" t="str">
         <f t="shared" si="12"/>
-        <v>F809</v>
+        <v>F80C</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="8" t="s">
@@ -1437,25 +1439,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>1</v>
       </c>
       <c r="B21" s="7">
         <f t="shared" si="9"/>
-        <v>63498</v>
+        <v>63504</v>
       </c>
       <c r="C21" s="7">
         <f t="shared" si="10"/>
-        <v>63498</v>
+        <v>63504</v>
       </c>
       <c r="D21" s="7" t="str">
         <f t="shared" si="11"/>
-        <v>F80A</v>
+        <v>F810</v>
       </c>
       <c r="E21" s="7" t="str">
         <f t="shared" si="12"/>
-        <v>F80A</v>
+        <v>F810</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="8" t="s">
@@ -1468,25 +1470,25 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>1</v>
       </c>
       <c r="B22" s="7">
         <f t="shared" si="9"/>
-        <v>63499</v>
+        <v>63508</v>
       </c>
       <c r="C22" s="7">
         <f t="shared" si="10"/>
-        <v>63499</v>
+        <v>63508</v>
       </c>
       <c r="D22" s="7" t="str">
         <f t="shared" si="11"/>
-        <v>F80B</v>
+        <v>F814</v>
       </c>
       <c r="E22" s="7" t="str">
         <f t="shared" si="12"/>
-        <v>F80B</v>
+        <v>F814</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8" t="s">
@@ -1499,25 +1501,25 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>2</v>
       </c>
       <c r="B23" s="7">
-        <f>C22+1</f>
-        <v>63500</v>
+        <f t="shared" si="9"/>
+        <v>63512</v>
       </c>
       <c r="C23" s="7">
         <f t="shared" ref="C23:C25" si="13">B23+A23-1</f>
-        <v>63501</v>
+        <v>63513</v>
       </c>
       <c r="D23" s="7" t="str">
         <f t="shared" ref="D23:D25" si="14">DEC2HEX(B23,4)</f>
-        <v>F80C</v>
+        <v>F818</v>
       </c>
       <c r="E23" s="7" t="str">
         <f t="shared" ref="E23:E25" si="15">DEC2HEX(C23,4)</f>
-        <v>F80D</v>
+        <v>F819</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8" t="s">
@@ -1530,25 +1532,25 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>1</v>
       </c>
       <c r="B24" s="7">
-        <f>C23+1</f>
-        <v>63502</v>
+        <f t="shared" si="9"/>
+        <v>63516</v>
       </c>
       <c r="C24" s="7">
         <f>B24+A24-1</f>
-        <v>63502</v>
+        <v>63516</v>
       </c>
       <c r="D24" s="7" t="str">
         <f>DEC2HEX(B24,4)</f>
-        <v>F80E</v>
+        <v>F81C</v>
       </c>
       <c r="E24" s="7" t="str">
         <f>DEC2HEX(C24,4)</f>
-        <v>F80E</v>
+        <v>F81C</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8" t="s">
@@ -1561,25 +1563,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>1</v>
       </c>
       <c r="B25" s="7">
-        <f t="shared" ref="B25:B33" si="16">C24+1</f>
-        <v>63503</v>
+        <f t="shared" si="9"/>
+        <v>63520</v>
       </c>
       <c r="C25" s="7">
         <f t="shared" si="13"/>
-        <v>63503</v>
+        <v>63520</v>
       </c>
       <c r="D25" s="7" t="str">
         <f t="shared" si="14"/>
-        <v>F80F</v>
+        <v>F820</v>
       </c>
       <c r="E25" s="7" t="str">
         <f t="shared" si="15"/>
-        <v>F80F</v>
+        <v>F820</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8" t="s">
@@ -1592,25 +1594,25 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>4</v>
       </c>
       <c r="B26" s="7">
-        <f t="shared" si="16"/>
-        <v>63504</v>
+        <f t="shared" si="9"/>
+        <v>63524</v>
       </c>
       <c r="C26" s="7">
-        <f t="shared" ref="C26" si="17">B26+A26-1</f>
-        <v>63507</v>
+        <f t="shared" ref="C26" si="16">B26+A26-1</f>
+        <v>63527</v>
       </c>
       <c r="D26" s="7" t="str">
-        <f t="shared" ref="D26" si="18">DEC2HEX(B26,4)</f>
-        <v>F810</v>
+        <f t="shared" ref="D26" si="17">DEC2HEX(B26,4)</f>
+        <v>F824</v>
       </c>
       <c r="E26" s="7" t="str">
-        <f t="shared" ref="E26" si="19">DEC2HEX(C26,4)</f>
-        <v>F813</v>
+        <f t="shared" ref="E26" si="18">DEC2HEX(C26,4)</f>
+        <v>F827</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
@@ -1623,25 +1625,25 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>4</v>
       </c>
       <c r="B27" s="7">
-        <f t="shared" si="16"/>
-        <v>63508</v>
+        <f t="shared" si="9"/>
+        <v>63528</v>
       </c>
       <c r="C27" s="7">
-        <f t="shared" ref="C27" si="20">B27+A27-1</f>
-        <v>63511</v>
+        <f t="shared" ref="C27" si="19">B27+A27-1</f>
+        <v>63531</v>
       </c>
       <c r="D27" s="7" t="str">
-        <f t="shared" ref="D27" si="21">DEC2HEX(B27,4)</f>
-        <v>F814</v>
+        <f t="shared" ref="D27" si="20">DEC2HEX(B27,4)</f>
+        <v>F828</v>
       </c>
       <c r="E27" s="7" t="str">
-        <f t="shared" ref="E27" si="22">DEC2HEX(C27,4)</f>
-        <v>F817</v>
+        <f t="shared" ref="E27" si="21">DEC2HEX(C27,4)</f>
+        <v>F82B</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8" t="s">
@@ -1654,25 +1656,25 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>2</v>
       </c>
       <c r="B28" s="7">
-        <f>C27+1</f>
-        <v>63512</v>
+        <f t="shared" si="9"/>
+        <v>63532</v>
       </c>
       <c r="C28" s="7">
-        <f t="shared" ref="C28" si="23">B28+A28-1</f>
-        <v>63513</v>
+        <f t="shared" ref="C28" si="22">B28+A28-1</f>
+        <v>63533</v>
       </c>
       <c r="D28" s="7" t="str">
-        <f t="shared" ref="D28" si="24">DEC2HEX(B28,4)</f>
-        <v>F818</v>
+        <f t="shared" ref="D28" si="23">DEC2HEX(B28,4)</f>
+        <v>F82C</v>
       </c>
       <c r="E28" s="7" t="str">
-        <f t="shared" ref="E28" si="25">DEC2HEX(C28,4)</f>
-        <v>F819</v>
+        <f t="shared" ref="E28" si="24">DEC2HEX(C28,4)</f>
+        <v>F82D</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8" t="s">
@@ -1685,25 +1687,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>2</v>
       </c>
       <c r="B29" s="7">
-        <f>C28+1</f>
-        <v>63514</v>
+        <f t="shared" si="9"/>
+        <v>63536</v>
       </c>
       <c r="C29" s="7">
-        <f t="shared" ref="C29:C30" si="26">B29+A29-1</f>
-        <v>63515</v>
+        <f t="shared" ref="C29:C30" si="25">B29+A29-1</f>
+        <v>63537</v>
       </c>
       <c r="D29" s="7" t="str">
-        <f t="shared" ref="D29:D30" si="27">DEC2HEX(B29,4)</f>
-        <v>F81A</v>
+        <f t="shared" ref="D29:D30" si="26">DEC2HEX(B29,4)</f>
+        <v>F830</v>
       </c>
       <c r="E29" s="7" t="str">
-        <f t="shared" ref="E29:E30" si="28">DEC2HEX(C29,4)</f>
-        <v>F81B</v>
+        <f t="shared" ref="E29:E30" si="27">DEC2HEX(C29,4)</f>
+        <v>F831</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8" t="s">
@@ -1716,25 +1718,25 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>1</v>
       </c>
       <c r="B30" s="7">
-        <f>C29+1</f>
-        <v>63516</v>
+        <f t="shared" si="9"/>
+        <v>63540</v>
       </c>
       <c r="C30" s="7">
+        <f t="shared" si="25"/>
+        <v>63540</v>
+      </c>
+      <c r="D30" s="7" t="str">
         <f t="shared" si="26"/>
-        <v>63516</v>
-      </c>
-      <c r="D30" s="7" t="str">
+        <v>F834</v>
+      </c>
+      <c r="E30" s="7" t="str">
         <f t="shared" si="27"/>
-        <v>F81C</v>
-      </c>
-      <c r="E30" s="7" t="str">
-        <f t="shared" si="28"/>
-        <v>F81C</v>
+        <v>F834</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8" t="s">
@@ -1747,25 +1749,25 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>1</v>
       </c>
       <c r="B31" s="7">
-        <f>C30+1</f>
-        <v>63517</v>
+        <f t="shared" si="9"/>
+        <v>63544</v>
       </c>
       <c r="C31" s="7">
-        <f t="shared" ref="C31:C33" si="29">B31+A31-1</f>
-        <v>63517</v>
+        <f t="shared" ref="C31:C33" si="28">B31+A31-1</f>
+        <v>63544</v>
       </c>
       <c r="D31" s="7" t="str">
-        <f t="shared" ref="D31:D33" si="30">DEC2HEX(B31,4)</f>
-        <v>F81D</v>
+        <f t="shared" ref="D31:D33" si="29">DEC2HEX(B31,4)</f>
+        <v>F838</v>
       </c>
       <c r="E31" s="7" t="str">
-        <f t="shared" ref="E31:E33" si="31">DEC2HEX(C31,4)</f>
-        <v>F81D</v>
+        <f t="shared" ref="E31:E33" si="30">DEC2HEX(C31,4)</f>
+        <v>F838</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8" t="s">
@@ -1778,25 +1780,25 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>1</v>
       </c>
       <c r="B32" s="7">
-        <f t="shared" si="16"/>
-        <v>63518</v>
+        <f t="shared" si="9"/>
+        <v>63548</v>
       </c>
       <c r="C32" s="7">
+        <f t="shared" si="28"/>
+        <v>63548</v>
+      </c>
+      <c r="D32" s="7" t="str">
         <f t="shared" si="29"/>
-        <v>63518</v>
-      </c>
-      <c r="D32" s="7" t="str">
+        <v>F83C</v>
+      </c>
+      <c r="E32" s="7" t="str">
         <f t="shared" si="30"/>
-        <v>F81E</v>
-      </c>
-      <c r="E32" s="7" t="str">
-        <f t="shared" si="31"/>
-        <v>F81E</v>
+        <v>F83C</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="8" t="s">
@@ -1809,25 +1811,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>1</v>
       </c>
       <c r="B33" s="7">
-        <f t="shared" si="16"/>
-        <v>63519</v>
+        <f t="shared" si="9"/>
+        <v>63552</v>
       </c>
       <c r="C33" s="7">
+        <f t="shared" si="28"/>
+        <v>63552</v>
+      </c>
+      <c r="D33" s="7" t="str">
         <f t="shared" si="29"/>
-        <v>63519</v>
-      </c>
-      <c r="D33" s="7" t="str">
+        <v>F840</v>
+      </c>
+      <c r="E33" s="7" t="str">
         <f t="shared" si="30"/>
-        <v>F81F</v>
-      </c>
-      <c r="E33" s="7" t="str">
-        <f t="shared" si="31"/>
-        <v>F81F</v>
+        <v>F840</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="8" t="s">
@@ -1840,25 +1842,25 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>1</v>
       </c>
       <c r="B34" s="7">
-        <f t="shared" ref="B34" si="32">C33+1</f>
-        <v>63520</v>
+        <f t="shared" si="9"/>
+        <v>63556</v>
       </c>
       <c r="C34" s="7">
-        <f t="shared" ref="C34" si="33">B34+A34-1</f>
-        <v>63520</v>
+        <f t="shared" ref="C34" si="31">B34+A34-1</f>
+        <v>63556</v>
       </c>
       <c r="D34" s="7" t="str">
-        <f t="shared" ref="D34" si="34">DEC2HEX(B34,4)</f>
-        <v>F820</v>
+        <f t="shared" ref="D34" si="32">DEC2HEX(B34,4)</f>
+        <v>F844</v>
       </c>
       <c r="E34" s="7" t="str">
-        <f t="shared" ref="E34" si="35">DEC2HEX(C34,4)</f>
-        <v>F820</v>
+        <f t="shared" ref="E34" si="33">DEC2HEX(C34,4)</f>
+        <v>F844</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8" t="s">
@@ -1871,24 +1873,24 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <f>C35-B35</f>
-        <v>2014</v>
+        <v>1975</v>
       </c>
       <c r="B35" s="7">
-        <f>C34+1</f>
-        <v>63521</v>
+        <f t="shared" si="9"/>
+        <v>63560</v>
       </c>
       <c r="C35" s="7">
         <v>65535</v>
       </c>
       <c r="D35" s="7" t="str">
-        <f t="shared" ref="D35" si="36">DEC2HEX(B35,4)</f>
-        <v>F821</v>
+        <f t="shared" ref="D35" si="34">DEC2HEX(B35,4)</f>
+        <v>F848</v>
       </c>
       <c r="E35" s="7" t="str">
-        <f t="shared" ref="E35" si="37">DEC2HEX(C35,4)</f>
+        <f t="shared" ref="E35" si="35">DEC2HEX(C35,4)</f>
         <v>FFFF</v>
       </c>
       <c r="F35" s="7"/>
@@ -1897,7 +1899,7 @@
       </c>
       <c r="H35" s="34"/>
     </row>
-    <row r="37" spans="1:14" s="9" customFormat="1">
+    <row r="37" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="10" t="s">
         <v>28</v>
       </c>
@@ -1912,7 +1914,7 @@
       <c r="M37"/>
       <c r="N37"/>
     </row>
-    <row r="38" spans="1:14" s="10" customFormat="1">
+    <row r="38" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="13" t="s">
         <v>6</v>
       </c>
@@ -1940,7 +1942,7 @@
       <c r="M38"/>
       <c r="N38"/>
     </row>
-    <row r="39" spans="1:14" s="10" customFormat="1">
+    <row r="39" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="13"/>
       <c r="B39" s="13" t="s">
         <v>8</v>
@@ -1963,7 +1965,7 @@
       <c r="M39"/>
       <c r="N39"/>
     </row>
-    <row r="40" spans="1:14" s="5" customFormat="1">
+    <row r="40" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="6"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
@@ -1979,7 +1981,7 @@
       <c r="M40"/>
       <c r="N40"/>
     </row>
-    <row r="41" spans="1:14">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>65536</v>
       </c>
@@ -2004,7 +2006,7 @@
       </c>
       <c r="H41" s="34"/>
     </row>
-    <row r="42" spans="1:14">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>256</v>
       </c>
@@ -2013,15 +2015,15 @@
         <v>65536</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" ref="C42" si="38">B42+A42-1</f>
+        <f t="shared" ref="C42" si="36">B42+A42-1</f>
         <v>65791</v>
       </c>
       <c r="D42" s="7" t="str">
-        <f t="shared" ref="D42:D43" si="39">DEC2HEX(B42,6)</f>
+        <f t="shared" ref="D42:D43" si="37">DEC2HEX(B42,6)</f>
         <v>010000</v>
       </c>
       <c r="E42" s="7" t="str">
-        <f t="shared" ref="E42:E43" si="40">DEC2HEX(C42,6)</f>
+        <f t="shared" ref="E42:E43" si="38">DEC2HEX(C42,6)</f>
         <v>0100FF</v>
       </c>
       <c r="F42" s="7"/>
@@ -2032,7 +2034,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="43" spans="1:14">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>256</v>
       </c>
@@ -2041,15 +2043,15 @@
         <v>65792</v>
       </c>
       <c r="C43" s="7">
-        <f t="shared" ref="C43" si="41">B43+A43-1</f>
+        <f t="shared" ref="C43" si="39">B43+A43-1</f>
         <v>66047</v>
       </c>
       <c r="D43" s="7" t="str">
-        <f t="shared" si="39"/>
+        <f t="shared" si="37"/>
         <v>010100</v>
       </c>
       <c r="E43" s="7" t="str">
-        <f t="shared" si="40"/>
+        <f t="shared" si="38"/>
         <v>0101FF</v>
       </c>
       <c r="F43" s="7"/>
@@ -2060,7 +2062,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>256</v>
       </c>
@@ -2069,15 +2071,15 @@
         <v>66048</v>
       </c>
       <c r="C44" s="7">
-        <f t="shared" ref="C44:C48" si="42">B44+A44-1</f>
+        <f t="shared" ref="C44:C48" si="40">B44+A44-1</f>
         <v>66303</v>
       </c>
       <c r="D44" s="7" t="str">
-        <f t="shared" ref="D44:D50" si="43">DEC2HEX(B44,6)</f>
+        <f t="shared" ref="D44:D50" si="41">DEC2HEX(B44,6)</f>
         <v>010200</v>
       </c>
       <c r="E44" s="7" t="str">
-        <f t="shared" ref="E44:E50" si="44">DEC2HEX(C44,6)</f>
+        <f t="shared" ref="E44:E50" si="42">DEC2HEX(C44,6)</f>
         <v>0102FF</v>
       </c>
       <c r="F44" s="7"/>
@@ -2088,7 +2090,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>256</v>
       </c>
@@ -2097,15 +2099,15 @@
         <v>66304</v>
       </c>
       <c r="C45" s="7">
+        <f t="shared" si="40"/>
+        <v>66559</v>
+      </c>
+      <c r="D45" s="7" t="str">
+        <f t="shared" si="41"/>
+        <v>010300</v>
+      </c>
+      <c r="E45" s="7" t="str">
         <f t="shared" si="42"/>
-        <v>66559</v>
-      </c>
-      <c r="D45" s="7" t="str">
-        <f t="shared" si="43"/>
-        <v>010300</v>
-      </c>
-      <c r="E45" s="7" t="str">
-        <f t="shared" si="44"/>
         <v>0103FF</v>
       </c>
       <c r="F45" s="7"/>
@@ -2116,24 +2118,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>256</v>
       </c>
       <c r="B46" s="7">
-        <f t="shared" ref="B46" si="45">C45+1</f>
+        <f t="shared" ref="B46" si="43">C45+1</f>
         <v>66560</v>
       </c>
       <c r="C46" s="7">
+        <f t="shared" si="40"/>
+        <v>66815</v>
+      </c>
+      <c r="D46" s="7" t="str">
+        <f t="shared" si="41"/>
+        <v>010400</v>
+      </c>
+      <c r="E46" s="7" t="str">
         <f t="shared" si="42"/>
-        <v>66815</v>
-      </c>
-      <c r="D46" s="7" t="str">
-        <f t="shared" si="43"/>
-        <v>010400</v>
-      </c>
-      <c r="E46" s="7" t="str">
-        <f t="shared" si="44"/>
         <v>0104FF</v>
       </c>
       <c r="F46" s="7"/>
@@ -2144,24 +2146,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>256</v>
       </c>
       <c r="B47" s="7">
-        <f t="shared" ref="B47" si="46">C46+1</f>
+        <f t="shared" ref="B47" si="44">C46+1</f>
         <v>66816</v>
       </c>
       <c r="C47" s="7">
-        <f t="shared" ref="C47" si="47">B47+A47-1</f>
+        <f t="shared" ref="C47" si="45">B47+A47-1</f>
         <v>67071</v>
       </c>
       <c r="D47" s="7" t="str">
-        <f t="shared" ref="D47" si="48">DEC2HEX(B47,6)</f>
+        <f t="shared" ref="D47" si="46">DEC2HEX(B47,6)</f>
         <v>010500</v>
       </c>
       <c r="E47" s="7" t="str">
-        <f t="shared" ref="E47" si="49">DEC2HEX(C47,6)</f>
+        <f t="shared" ref="E47" si="47">DEC2HEX(C47,6)</f>
         <v>0105FF</v>
       </c>
       <c r="F47" s="7"/>
@@ -2172,7 +2174,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <f>2*(100*75*2)</f>
         <v>30000</v>
@@ -2182,15 +2184,15 @@
         <v>67072</v>
       </c>
       <c r="C48" s="7">
+        <f t="shared" si="40"/>
+        <v>97071</v>
+      </c>
+      <c r="D48" s="7" t="str">
+        <f t="shared" si="41"/>
+        <v>010600</v>
+      </c>
+      <c r="E48" s="7" t="str">
         <f t="shared" si="42"/>
-        <v>97071</v>
-      </c>
-      <c r="D48" s="7" t="str">
-        <f t="shared" si="43"/>
-        <v>010600</v>
-      </c>
-      <c r="E48" s="7" t="str">
-        <f t="shared" si="44"/>
         <v>017B2F</v>
       </c>
       <c r="F48" s="7"/>
@@ -2201,7 +2203,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>1024</v>
       </c>
@@ -2210,15 +2212,15 @@
         <v>97072</v>
       </c>
       <c r="C49" s="7">
-        <f t="shared" ref="C49" si="50">B49+A49-1</f>
+        <f t="shared" ref="C49" si="48">B49+A49-1</f>
         <v>98095</v>
       </c>
       <c r="D49" s="7" t="str">
-        <f t="shared" ref="D49" si="51">DEC2HEX(B49,6)</f>
+        <f t="shared" ref="D49" si="49">DEC2HEX(B49,6)</f>
         <v>017B30</v>
       </c>
       <c r="E49" s="7" t="str">
-        <f t="shared" ref="E49" si="52">DEC2HEX(C49,6)</f>
+        <f t="shared" ref="E49" si="50">DEC2HEX(C49,6)</f>
         <v>017F2F</v>
       </c>
       <c r="F49" s="7"/>
@@ -2229,7 +2231,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <f>C50-B50</f>
         <v>16679119</v>
@@ -2243,11 +2245,11 @@
         <v>16777215</v>
       </c>
       <c r="D50" s="7" t="str">
-        <f t="shared" si="43"/>
+        <f t="shared" si="41"/>
         <v>017F30</v>
       </c>
       <c r="E50" s="7" t="str">
-        <f t="shared" si="44"/>
+        <f t="shared" si="42"/>
         <v>FFFFFF</v>
       </c>
       <c r="F50" s="7"/>
@@ -2262,20 +2264,20 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
   <pageSetup paperSize="9" scale="63" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="6" width="1.5703125" customWidth="1"/>
@@ -2288,7 +2290,7 @@
     <col min="15" max="15" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>70</v>
       </c>
@@ -2297,13 +2299,13 @@
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="8"/>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -2334,7 +2336,7 @@
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="13" t="s">
         <v>8</v>
@@ -2375,7 +2377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -2392,26 +2394,26 @@
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" s="21" customFormat="1" ht="30">
+    <row r="6" spans="1:15" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <f>'Memory Map'!A20</f>
         <v>1</v>
       </c>
       <c r="B6" s="22">
         <f>'Memory Map'!B20</f>
-        <v>63497</v>
+        <v>63500</v>
       </c>
       <c r="C6" s="22">
         <f>'Memory Map'!C20</f>
-        <v>63497</v>
+        <v>63500</v>
       </c>
       <c r="D6" s="22" t="str">
         <f>'Memory Map'!D20</f>
-        <v>F809</v>
+        <v>F80C</v>
       </c>
       <c r="E6" s="22" t="str">
         <f>'Memory Map'!E20</f>
-        <v>F809</v>
+        <v>F80C</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="28" t="str">
@@ -2443,7 +2445,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="21" customFormat="1">
+    <row r="7" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -2460,7 +2462,7 @@
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -2477,26 +2479,26 @@
       <c r="N8" s="26"/>
       <c r="O8" s="26"/>
     </row>
-    <row r="9" spans="1:15" s="21" customFormat="1" ht="30">
+    <row r="9" spans="1:15" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <f>'Memory Map'!A24</f>
         <v>1</v>
       </c>
       <c r="B9" s="22">
         <f>'Memory Map'!B24</f>
-        <v>63502</v>
+        <v>63516</v>
       </c>
       <c r="C9" s="22">
         <f>'Memory Map'!C24</f>
-        <v>63502</v>
+        <v>63516</v>
       </c>
       <c r="D9" s="22" t="str">
         <f>'Memory Map'!D24</f>
-        <v>F80E</v>
+        <v>F81C</v>
       </c>
       <c r="E9" s="22" t="str">
         <f>'Memory Map'!E24</f>
-        <v>F80E</v>
+        <v>F81C</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="28" t="str">
@@ -2528,7 +2530,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="21" customFormat="1">
+    <row r="10" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -2545,7 +2547,7 @@
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
     </row>
-    <row r="11" spans="1:15" s="21" customFormat="1">
+    <row r="11" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -2562,26 +2564,26 @@
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>'Memory Map'!A28-1</f>
         <v>1</v>
       </c>
       <c r="B12" s="1">
         <f>'Memory Map'!B28</f>
-        <v>63512</v>
+        <v>63532</v>
       </c>
       <c r="C12" s="1">
         <f>'Memory Map'!C28</f>
-        <v>63513</v>
+        <v>63533</v>
       </c>
       <c r="D12" s="1" t="str">
         <f>'Memory Map'!D28</f>
-        <v>F818</v>
+        <v>F82C</v>
       </c>
       <c r="E12" s="1" t="str">
         <f>'Memory Map'!E28</f>
-        <v>F819</v>
+        <v>F82D</v>
       </c>
       <c r="F12">
         <f>'Memory Map'!F28</f>
@@ -2616,7 +2618,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G13" s="2"/>
       <c r="H13" s="27">
         <v>0</v>
@@ -2643,39 +2645,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G14" s="2"/>
       <c r="H14" s="24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G15" s="2"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:15" ht="30">
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <f>'Memory Map'!A32</f>
         <v>1</v>
       </c>
       <c r="B17" s="22">
         <f>'Memory Map'!B32</f>
-        <v>63518</v>
+        <v>63548</v>
       </c>
       <c r="C17" s="22">
         <f>'Memory Map'!C32</f>
-        <v>63518</v>
+        <v>63548</v>
       </c>
       <c r="D17" s="22" t="str">
         <f>'Memory Map'!D32</f>
-        <v>F81E</v>
+        <v>F83C</v>
       </c>
       <c r="E17" s="22" t="str">
         <f>'Memory Map'!E32</f>
-        <v>F81E</v>
+        <v>F83C</v>
       </c>
       <c r="G17" s="29" t="str">
         <f>'Memory Map'!G32</f>
@@ -2706,7 +2708,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
@@ -2716,7 +2718,7 @@
       <c r="N18" s="27"/>
       <c r="O18" s="27"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -2724,26 +2726,26 @@
       <c r="E19" s="22"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <f>'Memory Map'!A33</f>
         <v>1</v>
       </c>
       <c r="B20" s="22">
         <f>'Memory Map'!B33</f>
-        <v>63519</v>
+        <v>63552</v>
       </c>
       <c r="C20" s="22">
         <f>'Memory Map'!C33</f>
-        <v>63519</v>
+        <v>63552</v>
       </c>
       <c r="D20" s="22" t="str">
         <f>'Memory Map'!D33</f>
-        <v>F81F</v>
+        <v>F840</v>
       </c>
       <c r="E20" s="22" t="str">
         <f>'Memory Map'!E33</f>
-        <v>F81F</v>
+        <v>F840</v>
       </c>
       <c r="G20" s="2" t="str">
         <f>'Memory Map'!G33</f>
@@ -2774,7 +2776,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -2786,60 +2788,60 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="109.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30">
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="45">
+    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
     </row>
-    <row r="10" spans="1:1" ht="60">
+    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
Testing synthesis and place and route on the wide SRAM design. Preparing benchmark tests based on MPE resource
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Map" sheetId="1" r:id="rId1"/>
@@ -974,8 +974,8 @@
   </sheetPr>
   <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2273,8 +2273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N14" sqref="N14"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N15" sqref="N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2642,7 +2642,7 @@
         <v>1</v>
       </c>
       <c r="O13" s="27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Included a new hardware register for VGA Vertical Blank (VBLANK)
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Map" sheetId="1" r:id="rId1"/>
     <sheet name="Hardware registers" sheetId="2" r:id="rId2"/>
     <sheet name="Copyright and license" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -474,12 +474,18 @@
   <si>
     <t>FAT buffers</t>
   </si>
+  <si>
+    <t>VBLANK</t>
+  </si>
+  <si>
+    <t>VGA vertical blank</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -757,6 +763,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -791,6 +798,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -966,17 +974,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="5" width="12.42578125" style="1" customWidth="1"/>
@@ -989,12 +997,12 @@
     <col min="14" max="14" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1">
+    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -1009,7 +1017,7 @@
       <c r="M3"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -1039,7 +1047,7 @@
       <c r="M4"/>
       <c r="N4"/>
     </row>
-    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13" t="s">
         <v>8</v>
@@ -1062,7 +1070,7 @@
       <c r="M5"/>
       <c r="N5"/>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1078,7 +1086,7 @@
       <c r="M6"/>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <v>45056</v>
       </c>
@@ -1108,7 +1116,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <v>12288</v>
       </c>
@@ -1133,7 +1141,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <f>2048</f>
         <v>2048</v>
@@ -1165,7 +1173,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <f>2048</f>
         <v>2048</v>
@@ -1197,7 +1205,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>2048</v>
       </c>
@@ -1228,10 +1236,10 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:14" s="9" customFormat="1">
+    <row r="13" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>52</v>
       </c>
@@ -1246,7 +1254,7 @@
       <c r="M13"/>
       <c r="N13"/>
     </row>
-    <row r="14" spans="1:14" s="10" customFormat="1">
+    <row r="14" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>6</v>
       </c>
@@ -1274,7 +1282,7 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" s="11" customFormat="1">
+    <row r="15" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15"/>
       <c r="B15" s="13" t="s">
         <v>8</v>
@@ -1297,7 +1305,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" s="2" customFormat="1">
+    <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1313,7 +1321,7 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>4</v>
       </c>
@@ -1344,7 +1352,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:9">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>4</v>
       </c>
@@ -1375,7 +1383,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>1</v>
       </c>
@@ -1406,7 +1414,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>1</v>
       </c>
@@ -1437,7 +1445,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:9">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>1</v>
       </c>
@@ -1468,7 +1476,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>1</v>
       </c>
@@ -1499,7 +1507,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:9">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>2</v>
       </c>
@@ -1530,7 +1538,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="24" spans="1:9">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>1</v>
       </c>
@@ -1561,7 +1569,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:9">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>1</v>
       </c>
@@ -1592,7 +1600,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:9">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>4</v>
       </c>
@@ -1623,7 +1631,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:9">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>4</v>
       </c>
@@ -1654,7 +1662,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="28" spans="1:9">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>2</v>
       </c>
@@ -1685,7 +1693,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>2</v>
       </c>
@@ -1716,7 +1724,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:9">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>1</v>
       </c>
@@ -1747,7 +1755,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>1</v>
       </c>
@@ -1778,7 +1786,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="32" spans="1:9">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>1</v>
       </c>
@@ -1809,7 +1817,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>1</v>
       </c>
@@ -1840,7 +1848,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>1</v>
       </c>
@@ -1871,68 +1879,71 @@
         <v>55</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
-        <f>C35-B35</f>
-        <v>1975</v>
+        <v>1</v>
       </c>
       <c r="B35" s="7">
         <f t="shared" si="9"/>
         <v>63560</v>
       </c>
       <c r="C35" s="7">
+        <f t="shared" ref="C35" si="34">B35+A35-1</f>
+        <v>63560</v>
+      </c>
+      <c r="D35" s="7" t="str">
+        <f t="shared" ref="D35" si="35">DEC2HEX(B35,4)</f>
+        <v>F848</v>
+      </c>
+      <c r="E35" s="7" t="str">
+        <f t="shared" ref="E35" si="36">DEC2HEX(C35,4)</f>
+        <v>F848</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H35" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="I35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <f>C36-B36</f>
+        <v>1971</v>
+      </c>
+      <c r="B36" s="7">
+        <f>B35+4</f>
+        <v>63564</v>
+      </c>
+      <c r="C36" s="7">
         <v>65535</v>
       </c>
-      <c r="D35" s="7" t="str">
-        <f t="shared" ref="D35" si="34">DEC2HEX(B35,4)</f>
-        <v>F848</v>
-      </c>
-      <c r="E35" s="7" t="str">
-        <f t="shared" ref="E35" si="35">DEC2HEX(C35,4)</f>
+      <c r="D36" s="7" t="str">
+        <f t="shared" ref="D36" si="37">DEC2HEX(B36,4)</f>
+        <v>F84C</v>
+      </c>
+      <c r="E36" s="7" t="str">
+        <f t="shared" ref="E36" si="38">DEC2HEX(C36,4)</f>
         <v>FFFF</v>
       </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="12" t="s">
+      <c r="F36" s="7"/>
+      <c r="G36" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H35" s="34"/>
-    </row>
-    <row r="37" spans="1:14" s="9" customFormat="1">
-      <c r="A37" s="10" t="s">
+      <c r="H36" s="34"/>
+    </row>
+    <row r="38" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
-      <c r="F37" s="16"/>
-      <c r="H37" s="31"/>
-      <c r="I37"/>
-      <c r="J37"/>
-      <c r="K37"/>
-      <c r="L37"/>
-      <c r="M37"/>
-      <c r="N37"/>
-    </row>
-    <row r="38" spans="1:14" s="10" customFormat="1">
-      <c r="A38" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B38" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C38" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D38" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H38" s="32"/>
+      <c r="D38" s="16"/>
+      <c r="E38" s="16"/>
+      <c r="F38" s="16"/>
+      <c r="H38" s="31"/>
       <c r="I38"/>
       <c r="J38"/>
       <c r="K38"/>
@@ -1940,21 +1951,26 @@
       <c r="M38"/>
       <c r="N38"/>
     </row>
-    <row r="39" spans="1:14" s="10" customFormat="1">
-      <c r="A39" s="13"/>
+    <row r="39" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="13" t="s">
+        <v>6</v>
+      </c>
       <c r="B39" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C39" s="13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E39" s="13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F39" s="13"/>
+      <c r="G39" s="10" t="s">
+        <v>0</v>
+      </c>
       <c r="H39" s="32"/>
       <c r="I39"/>
       <c r="J39"/>
@@ -1963,14 +1979,21 @@
       <c r="M39"/>
       <c r="N39"/>
     </row>
-    <row r="40" spans="1:14" s="5" customFormat="1">
-      <c r="A40" s="6"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="10"/>
+    <row r="40" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="13"/>
+      <c r="B40" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F40" s="13"/>
       <c r="H40" s="32"/>
       <c r="I40"/>
       <c r="J40"/>
@@ -1979,285 +2002,301 @@
       <c r="M40"/>
       <c r="N40"/>
     </row>
-    <row r="41" spans="1:14">
-      <c r="A41" s="7">
+    <row r="41" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="10"/>
+      <c r="H41" s="32"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
         <v>65536</v>
       </c>
-      <c r="B41" s="7">
+      <c r="B42" s="7">
         <v>0</v>
       </c>
-      <c r="C41" s="7">
-        <f>A41-1</f>
+      <c r="C42" s="7">
+        <f>A42-1</f>
         <v>65535</v>
       </c>
-      <c r="D41" s="7" t="str">
-        <f>DEC2HEX(B41,6)</f>
+      <c r="D42" s="7" t="str">
+        <f>DEC2HEX(B42,6)</f>
         <v>000000</v>
       </c>
-      <c r="E41" s="7" t="str">
-        <f>DEC2HEX(C41,6)</f>
+      <c r="E42" s="7" t="str">
+        <f>DEC2HEX(C42,6)</f>
         <v>00FFFF</v>
       </c>
-      <c r="F41" s="7"/>
-      <c r="G41" s="12" t="s">
+      <c r="F42" s="7"/>
+      <c r="G42" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H41" s="34"/>
-    </row>
-    <row r="42" spans="1:14">
-      <c r="A42" s="7">
-        <v>256</v>
-      </c>
-      <c r="B42" s="7">
-        <f>C41+1</f>
-        <v>65536</v>
-      </c>
-      <c r="C42" s="7">
-        <f t="shared" ref="C42" si="36">B42+A42-1</f>
-        <v>65791</v>
-      </c>
-      <c r="D42" s="7" t="str">
-        <f t="shared" ref="D42:D43" si="37">DEC2HEX(B42,6)</f>
-        <v>010000</v>
-      </c>
-      <c r="E42" s="7" t="str">
-        <f t="shared" ref="E42:E43" si="38">DEC2HEX(C42,6)</f>
-        <v>0100FF</v>
-      </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H42" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14">
+      <c r="H42" s="34"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>256</v>
       </c>
       <c r="B43" s="7">
         <f>C42+1</f>
-        <v>65792</v>
+        <v>65536</v>
       </c>
       <c r="C43" s="7">
         <f t="shared" ref="C43" si="39">B43+A43-1</f>
-        <v>66047</v>
+        <v>65791</v>
       </c>
       <c r="D43" s="7" t="str">
-        <f t="shared" si="37"/>
-        <v>010100</v>
+        <f t="shared" ref="D43:D44" si="40">DEC2HEX(B43,6)</f>
+        <v>010000</v>
       </c>
       <c r="E43" s="7" t="str">
-        <f t="shared" si="38"/>
-        <v>0101FF</v>
+        <f t="shared" ref="E43:E44" si="41">DEC2HEX(C43,6)</f>
+        <v>0100FF</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H43" s="30" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>256</v>
       </c>
       <c r="B44" s="7">
         <f>C43+1</f>
-        <v>66048</v>
+        <v>65792</v>
       </c>
       <c r="C44" s="7">
-        <f t="shared" ref="C44:C48" si="40">B44+A44-1</f>
-        <v>66303</v>
+        <f t="shared" ref="C44" si="42">B44+A44-1</f>
+        <v>66047</v>
       </c>
       <c r="D44" s="7" t="str">
-        <f t="shared" ref="D44:D50" si="41">DEC2HEX(B44,6)</f>
-        <v>010200</v>
+        <f t="shared" si="40"/>
+        <v>010100</v>
       </c>
       <c r="E44" s="7" t="str">
-        <f t="shared" ref="E44:E50" si="42">DEC2HEX(C44,6)</f>
-        <v>0102FF</v>
+        <f t="shared" si="41"/>
+        <v>0101FF</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H44" s="30" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>256</v>
       </c>
       <c r="B45" s="7">
         <f>C44+1</f>
-        <v>66304</v>
+        <v>66048</v>
       </c>
       <c r="C45" s="7">
-        <f t="shared" si="40"/>
-        <v>66559</v>
+        <f t="shared" ref="C45:C49" si="43">B45+A45-1</f>
+        <v>66303</v>
       </c>
       <c r="D45" s="7" t="str">
-        <f t="shared" si="41"/>
-        <v>010300</v>
+        <f t="shared" ref="D45:D51" si="44">DEC2HEX(B45,6)</f>
+        <v>010200</v>
       </c>
       <c r="E45" s="7" t="str">
-        <f t="shared" si="42"/>
-        <v>0103FF</v>
+        <f t="shared" ref="E45:E51" si="45">DEC2HEX(C45,6)</f>
+        <v>0102FF</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H45" s="30" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>256</v>
       </c>
       <c r="B46" s="7">
-        <f t="shared" ref="B46" si="43">C45+1</f>
-        <v>66560</v>
+        <f>C45+1</f>
+        <v>66304</v>
       </c>
       <c r="C46" s="7">
-        <f t="shared" si="40"/>
-        <v>66815</v>
+        <f t="shared" si="43"/>
+        <v>66559</v>
       </c>
       <c r="D46" s="7" t="str">
-        <f t="shared" si="41"/>
-        <v>010400</v>
+        <f t="shared" si="44"/>
+        <v>010300</v>
       </c>
       <c r="E46" s="7" t="str">
-        <f t="shared" si="42"/>
-        <v>0104FF</v>
+        <f t="shared" si="45"/>
+        <v>0103FF</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H46" s="30" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>256</v>
       </c>
       <c r="B47" s="7">
-        <f t="shared" ref="B47" si="44">C46+1</f>
-        <v>66816</v>
+        <f t="shared" ref="B47" si="46">C46+1</f>
+        <v>66560</v>
       </c>
       <c r="C47" s="7">
-        <f t="shared" ref="C47" si="45">B47+A47-1</f>
-        <v>67071</v>
+        <f t="shared" si="43"/>
+        <v>66815</v>
       </c>
       <c r="D47" s="7" t="str">
-        <f t="shared" ref="D47" si="46">DEC2HEX(B47,6)</f>
-        <v>010500</v>
+        <f t="shared" si="44"/>
+        <v>010400</v>
       </c>
       <c r="E47" s="7" t="str">
-        <f t="shared" ref="E47" si="47">DEC2HEX(C47,6)</f>
-        <v>0105FF</v>
+        <f t="shared" si="45"/>
+        <v>0104FF</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="8" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="H47" s="30" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
+        <v>256</v>
+      </c>
+      <c r="B48" s="7">
+        <f t="shared" ref="B48" si="47">C47+1</f>
+        <v>66816</v>
+      </c>
+      <c r="C48" s="7">
+        <f t="shared" ref="C48" si="48">B48+A48-1</f>
+        <v>67071</v>
+      </c>
+      <c r="D48" s="7" t="str">
+        <f t="shared" ref="D48" si="49">DEC2HEX(B48,6)</f>
+        <v>010500</v>
+      </c>
+      <c r="E48" s="7" t="str">
+        <f t="shared" ref="E48" si="50">DEC2HEX(C48,6)</f>
+        <v>0105FF</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="H48" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
         <f>2*(100*75*2)</f>
         <v>30000</v>
       </c>
-      <c r="B48" s="7">
-        <f>C47+1</f>
-        <v>67072</v>
-      </c>
-      <c r="C48" s="7">
-        <f t="shared" si="40"/>
-        <v>97071</v>
-      </c>
-      <c r="D48" s="7" t="str">
-        <f t="shared" si="41"/>
-        <v>010600</v>
-      </c>
-      <c r="E48" s="7" t="str">
-        <f t="shared" si="42"/>
-        <v>017B2F</v>
-      </c>
-      <c r="F48" s="7"/>
-      <c r="G48" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H48" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9">
-      <c r="A49" s="7">
-        <v>1024</v>
-      </c>
       <c r="B49" s="7">
         <f>C48+1</f>
-        <v>97072</v>
+        <v>67072</v>
       </c>
       <c r="C49" s="7">
-        <f t="shared" ref="C49" si="48">B49+A49-1</f>
-        <v>98095</v>
+        <f t="shared" si="43"/>
+        <v>97071</v>
       </c>
       <c r="D49" s="7" t="str">
-        <f t="shared" ref="D49" si="49">DEC2HEX(B49,6)</f>
-        <v>017B30</v>
+        <f t="shared" si="44"/>
+        <v>010600</v>
       </c>
       <c r="E49" s="7" t="str">
-        <f t="shared" ref="E49" si="50">DEC2HEX(C49,6)</f>
-        <v>017F2F</v>
+        <f t="shared" si="45"/>
+        <v>017B2F</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="8" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="H49" s="30" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
-        <f>C50-B50</f>
-        <v>16679119</v>
+        <v>1024</v>
       </c>
       <c r="B50" s="7">
         <f>C49+1</f>
+        <v>97072</v>
+      </c>
+      <c r="C50" s="7">
+        <f t="shared" ref="C50" si="51">B50+A50-1</f>
+        <v>98095</v>
+      </c>
+      <c r="D50" s="7" t="str">
+        <f t="shared" ref="D50" si="52">DEC2HEX(B50,6)</f>
+        <v>017B30</v>
+      </c>
+      <c r="E50" s="7" t="str">
+        <f t="shared" ref="E50" si="53">DEC2HEX(C50,6)</f>
+        <v>017F2F</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="H50" s="30" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <f>C51-B51</f>
+        <v>16679119</v>
+      </c>
+      <c r="B51" s="7">
+        <f>C50+1</f>
         <v>98096</v>
       </c>
-      <c r="C50" s="7">
+      <c r="C51" s="7">
         <f>16*1024*1024-1</f>
         <v>16777215</v>
       </c>
-      <c r="D50" s="7" t="str">
-        <f t="shared" si="41"/>
+      <c r="D51" s="7" t="str">
+        <f t="shared" si="44"/>
         <v>017F30</v>
       </c>
-      <c r="E50" s="7" t="str">
-        <f t="shared" si="42"/>
+      <c r="E51" s="7" t="str">
+        <f t="shared" si="45"/>
         <v>FFFFFF</v>
       </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="8" t="s">
+      <c r="F51" s="7"/>
+      <c r="G51" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H50" s="30" t="s">
+      <c r="H51" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I51" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2268,14 +2307,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="6" width="1.5703125" customWidth="1"/>
@@ -2288,7 +2327,7 @@
     <col min="15" max="15" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>70</v>
       </c>
@@ -2297,7 +2336,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2318,7 +2357,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -2349,7 +2388,7 @@
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="13" t="s">
         <v>8</v>
@@ -2390,7 +2429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -2407,7 +2446,7 @@
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" s="21" customFormat="1" ht="30">
+    <row r="6" spans="1:15" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <f>'Memory Map'!A20</f>
         <v>1</v>
@@ -2458,7 +2497,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:15" s="21" customFormat="1">
+    <row r="7" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -2475,7 +2514,7 @@
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -2492,7 +2531,7 @@
       <c r="N8" s="26"/>
       <c r="O8" s="26"/>
     </row>
-    <row r="9" spans="1:15" s="21" customFormat="1" ht="30">
+    <row r="9" spans="1:15" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <f>'Memory Map'!A24</f>
         <v>1</v>
@@ -2543,7 +2582,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="21" customFormat="1">
+    <row r="10" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -2560,7 +2599,7 @@
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
     </row>
-    <row r="11" spans="1:15" s="21" customFormat="1">
+    <row r="11" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -2577,7 +2616,7 @@
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>'Memory Map'!A28-1</f>
         <v>1</v>
@@ -2631,7 +2670,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G13" s="2"/>
       <c r="H13" s="27">
         <v>0</v>
@@ -2658,20 +2697,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G14" s="2"/>
       <c r="H14" s="24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G15" s="2"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:15" ht="30">
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <f>'Memory Map'!A32</f>
         <v>1</v>
@@ -2721,7 +2760,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
@@ -2731,7 +2770,7 @@
       <c r="N18" s="27"/>
       <c r="O18" s="27"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -2739,7 +2778,7 @@
       <c r="E19" s="22"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <f>'Memory Map'!A33</f>
         <v>1</v>
@@ -2789,7 +2828,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>74</v>
       </c>
@@ -2801,60 +2840,60 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="109.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30">
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="45">
+    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
     </row>
-    <row r="10" spans="1:1" ht="60">
+    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>89</v>
       </c>

</xml_diff>

<commit_message>
Functional and tested VGA controller on Nexys4, including new color RAM palette and XGA (1024x768) screen mode Known issues  - in XGA mode the last character of the row is duplicated  - evidence of duplicate/missing character at a PSDRAM row boundary  - need to implement software VGA clock switching
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Map" sheetId="1" r:id="rId1"/>
     <sheet name="Hardware registers" sheetId="2" r:id="rId2"/>
     <sheet name="Copyright and license" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="100">
   <si>
     <t>Name</t>
   </si>
@@ -195,23 +195,6 @@
   <si>
     <t>Port 0
 Read Data Available</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">0 = VGA mode
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 = SVGA mode</t>
-    </r>
   </si>
   <si>
     <r>
@@ -232,30 +215,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>0 = pixel graphics off</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-1 = pixel graphics on</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">0 = 16&amp;16 color mode
 </t>
     </r>
@@ -269,23 +228,6 @@
         <scheme val="minor"/>
       </rPr>
       <t>1 = 0&amp;256 color mode</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">0 = text graphics off
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1 = text graphics on</t>
     </r>
   </si>
   <si>
@@ -480,12 +422,21 @@
   <si>
     <t>VGA vertical blank</t>
   </si>
+  <si>
+    <t>Color RAM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Access to the color RAM in the CPU address space </t>
+  </si>
+  <si>
+    <t>000 = off, 001 = 640*480, 010 = 800*600, 011 = 1024*768</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,7 +542,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -673,6 +624,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -763,7 +717,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -798,7 +751,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -974,17 +926,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7:J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="5" width="12.42578125" style="1" customWidth="1"/>
@@ -997,12 +949,12 @@
     <col min="14" max="14" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="21">
       <c r="A1" s="17" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="9" customFormat="1">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -1017,7 +969,7 @@
       <c r="M3"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -1038,7 +990,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -1047,7 +999,7 @@
       <c r="M4"/>
       <c r="N4"/>
     </row>
-    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" s="13" t="s">
         <v>8</v>
@@ -1070,7 +1022,7 @@
       <c r="M5"/>
       <c r="N5"/>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1086,7 +1038,7 @@
       <c r="M6"/>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="7">
         <v>45056</v>
       </c>
@@ -1110,23 +1062,24 @@
         <v>1</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I7" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="7">
-        <v>12288</v>
+        <f>12288-2048</f>
+        <v>10240</v>
       </c>
       <c r="B8" s="7">
         <f>C7+1</f>
         <v>45056</v>
       </c>
       <c r="C8" s="7">
-        <f t="shared" ref="C8:C11" si="0">B8+A8-1</f>
-        <v>57343</v>
+        <f t="shared" ref="C8:C12" si="0">B8+A8-1</f>
+        <v>55295</v>
       </c>
       <c r="D8" s="7" t="str">
         <f t="shared" ref="D8" si="1">DEC2HEX(B8,4)</f>
@@ -1134,147 +1087,150 @@
       </c>
       <c r="E8" s="7" t="str">
         <f t="shared" ref="E8" si="2">DEC2HEX(C8,4)</f>
-        <v>DFFF</v>
+        <v>D7FF</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="12" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="7">
-        <f>2048</f>
         <v>2048</v>
       </c>
       <c r="B9" s="7">
-        <f t="shared" ref="B9" si="3">C8+1</f>
-        <v>57344</v>
+        <f>C8+1</f>
+        <v>55296</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" si="0"/>
-        <v>59391</v>
+        <f>B9+A9-1</f>
+        <v>57343</v>
       </c>
       <c r="D9" s="7" t="str">
-        <f t="shared" ref="D9:D11" si="4">DEC2HEX(B9,4)</f>
-        <v>E000</v>
+        <f t="shared" ref="D9" si="3">DEC2HEX(B9,4)</f>
+        <v>D800</v>
       </c>
       <c r="E9" s="7" t="str">
-        <f t="shared" ref="E9:E11" si="5">DEC2HEX(C9,4)</f>
-        <v>E7FF</v>
+        <f t="shared" ref="E9" si="4">DEC2HEX(C9,4)</f>
+        <v>DFFF</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8" t="s">
-        <v>2</v>
+        <v>97</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="7">
         <f>2048</f>
         <v>2048</v>
       </c>
       <c r="B10" s="7">
         <f>C9+1</f>
-        <v>59392</v>
+        <v>57344</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" si="0"/>
-        <v>61439</v>
+        <v>59391</v>
       </c>
       <c r="D10" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>E800</v>
+        <f t="shared" ref="D10:D12" si="5">DEC2HEX(B10,4)</f>
+        <v>E000</v>
       </c>
       <c r="E10" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>EFFF</v>
+        <f t="shared" ref="E10:E12" si="6">DEC2HEX(C10,4)</f>
+        <v>E7FF</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I10" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
       <c r="A11" s="7">
+        <f>2048</f>
         <v>2048</v>
       </c>
       <c r="B11" s="7">
         <f>C10+1</f>
-        <v>61440</v>
+        <v>59392</v>
       </c>
       <c r="C11" s="7">
         <f t="shared" si="0"/>
-        <v>63487</v>
+        <v>61439</v>
       </c>
       <c r="D11" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>F000</v>
+        <f t="shared" si="5"/>
+        <v>E800</v>
       </c>
       <c r="E11" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>F7FF</v>
+        <f t="shared" si="6"/>
+        <v>EFFF</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I11" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="7">
+        <v>2048</v>
+      </c>
+      <c r="B12" s="7">
+        <f>C11+1</f>
+        <v>61440</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="0"/>
+        <v>63487</v>
+      </c>
+      <c r="D12" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>F000</v>
+      </c>
+      <c r="E12" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>F7FF</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="H12" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I12" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-    </row>
-    <row r="13" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="14" t="s">
+    <row r="13" spans="1:14">
+      <c r="A13" s="3"/>
+    </row>
+    <row r="14" spans="1:14" s="9" customFormat="1">
+      <c r="A14" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="H13" s="31"/>
-      <c r="I13"/>
-      <c r="J13"/>
-      <c r="K13"/>
-      <c r="L13"/>
-      <c r="M13"/>
-      <c r="N13"/>
-    </row>
-    <row r="14" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F14" s="13"/>
-      <c r="G14" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="32"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="16"/>
+      <c r="F14" s="16"/>
+      <c r="H14" s="31"/>
       <c r="I14"/>
       <c r="J14"/>
       <c r="K14"/>
@@ -1282,22 +1238,27 @@
       <c r="M14"/>
       <c r="N14"/>
     </row>
-    <row r="15" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="15"/>
+    <row r="15" spans="1:14" s="10" customFormat="1">
+      <c r="A15" s="13" t="s">
+        <v>6</v>
+      </c>
       <c r="B15" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F15" s="13"/>
-      <c r="H15" s="33"/>
+      <c r="G15" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="32"/>
       <c r="I15"/>
       <c r="J15"/>
       <c r="K15"/>
@@ -1305,14 +1266,21 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="11"/>
+    <row r="16" spans="1:14" s="11" customFormat="1">
+      <c r="A16" s="15"/>
+      <c r="B16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" s="13"/>
       <c r="H16" s="33"/>
       <c r="I16"/>
       <c r="J16"/>
@@ -1321,657 +1289,645 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="7">
-        <v>4</v>
-      </c>
-      <c r="B17" s="7">
-        <f>C11+1</f>
-        <v>63488</v>
-      </c>
-      <c r="C17" s="7">
-        <f>B17+A17-1</f>
-        <v>63491</v>
-      </c>
-      <c r="D17" s="7" t="str">
-        <f>DEC2HEX(B17,4)</f>
-        <v>F800</v>
-      </c>
-      <c r="E17" s="7" t="str">
-        <f>DEC2HEX(C17,4)</f>
-        <v>F803</v>
-      </c>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H17" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I17" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="2" customFormat="1">
+      <c r="A17" s="4"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="33"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+    </row>
+    <row r="18" spans="1:14">
       <c r="A18" s="7">
         <v>4</v>
       </c>
       <c r="B18" s="7">
-        <f>B17+4</f>
-        <v>63492</v>
+        <f>C12+1</f>
+        <v>63488</v>
       </c>
       <c r="C18" s="7">
-        <f t="shared" ref="C18" si="6">B18+A18-1</f>
-        <v>63495</v>
+        <f>B18+A18-1</f>
+        <v>63491</v>
       </c>
       <c r="D18" s="7" t="str">
-        <f t="shared" ref="D18" si="7">DEC2HEX(B18,4)</f>
-        <v>F804</v>
+        <f>DEC2HEX(B18,4)</f>
+        <v>F800</v>
       </c>
       <c r="E18" s="7" t="str">
-        <f t="shared" ref="E18" si="8">DEC2HEX(C18,4)</f>
-        <v>F807</v>
+        <f>DEC2HEX(C18,4)</f>
+        <v>F803</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="I18" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
       <c r="A19" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B19" s="7">
-        <f t="shared" ref="B19:B35" si="9">B18+4</f>
-        <v>63496</v>
+        <f>B18+4</f>
+        <v>63492</v>
       </c>
       <c r="C19" s="7">
-        <f t="shared" ref="C19:C22" si="10">B19+A19-1</f>
-        <v>63496</v>
+        <f t="shared" ref="C19" si="7">B19+A19-1</f>
+        <v>63495</v>
       </c>
       <c r="D19" s="7" t="str">
-        <f t="shared" ref="D19:D22" si="11">DEC2HEX(B19,4)</f>
-        <v>F808</v>
+        <f t="shared" ref="D19" si="8">DEC2HEX(B19,4)</f>
+        <v>F804</v>
       </c>
       <c r="E19" s="7" t="str">
-        <f t="shared" ref="E19:E22" si="12">DEC2HEX(C19,4)</f>
-        <v>F808</v>
+        <f t="shared" ref="E19" si="9">DEC2HEX(C19,4)</f>
+        <v>F807</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="H19" s="30" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
       <c r="A20" s="7">
         <v>1</v>
       </c>
       <c r="B20" s="7">
-        <f t="shared" si="9"/>
-        <v>63500</v>
+        <f t="shared" ref="B20:B36" si="10">B19+4</f>
+        <v>63496</v>
       </c>
       <c r="C20" s="7">
+        <f t="shared" ref="C20:C23" si="11">B20+A20-1</f>
+        <v>63496</v>
+      </c>
+      <c r="D20" s="7" t="str">
+        <f t="shared" ref="D20:D23" si="12">DEC2HEX(B20,4)</f>
+        <v>F808</v>
+      </c>
+      <c r="E20" s="7" t="str">
+        <f t="shared" ref="E20:E23" si="13">DEC2HEX(C20,4)</f>
+        <v>F808</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="7">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7">
         <f t="shared" si="10"/>
         <v>63500</v>
       </c>
-      <c r="D20" s="7" t="str">
+      <c r="C21" s="7">
         <f t="shared" si="11"/>
-        <v>F80C</v>
-      </c>
-      <c r="E20" s="7" t="str">
+        <v>63500</v>
+      </c>
+      <c r="D21" s="7" t="str">
         <f t="shared" si="12"/>
         <v>F80C</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8" t="s">
+      <c r="E21" s="7" t="str">
+        <f t="shared" si="13"/>
+        <v>F80C</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="H20" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="H21" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I21" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="7">
+    <row r="22" spans="1:14">
+      <c r="A22" s="7">
         <v>1</v>
       </c>
-      <c r="B21" s="7">
-        <f t="shared" si="9"/>
-        <v>63504</v>
-      </c>
-      <c r="C21" s="7">
+      <c r="B22" s="7">
         <f t="shared" si="10"/>
         <v>63504</v>
       </c>
-      <c r="D21" s="7" t="str">
+      <c r="C22" s="7">
         <f t="shared" si="11"/>
-        <v>F810</v>
-      </c>
-      <c r="E21" s="7" t="str">
+        <v>63504</v>
+      </c>
+      <c r="D22" s="7" t="str">
         <f t="shared" si="12"/>
         <v>F810</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8" t="s">
+      <c r="E22" s="7" t="str">
+        <f t="shared" si="13"/>
+        <v>F810</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H21" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="I21" t="s">
+      <c r="H22" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I22" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="7">
+    <row r="23" spans="1:14">
+      <c r="A23" s="7">
         <v>1</v>
       </c>
-      <c r="B22" s="7">
-        <f t="shared" si="9"/>
-        <v>63508</v>
-      </c>
-      <c r="C22" s="7">
+      <c r="B23" s="7">
         <f t="shared" si="10"/>
         <v>63508</v>
       </c>
-      <c r="D22" s="7" t="str">
+      <c r="C23" s="7">
         <f t="shared" si="11"/>
-        <v>F814</v>
-      </c>
-      <c r="E22" s="7" t="str">
+        <v>63508</v>
+      </c>
+      <c r="D23" s="7" t="str">
         <f t="shared" si="12"/>
         <v>F814</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="H22" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="I22" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="7">
-        <v>2</v>
-      </c>
-      <c r="B23" s="7">
-        <f t="shared" si="9"/>
-        <v>63512</v>
-      </c>
-      <c r="C23" s="7">
-        <f t="shared" ref="C23:C25" si="13">B23+A23-1</f>
-        <v>63513</v>
-      </c>
-      <c r="D23" s="7" t="str">
-        <f t="shared" ref="D23:D25" si="14">DEC2HEX(B23,4)</f>
-        <v>F818</v>
-      </c>
       <c r="E23" s="7" t="str">
-        <f t="shared" ref="E23:E25" si="15">DEC2HEX(C23,4)</f>
-        <v>F819</v>
+        <f t="shared" si="13"/>
+        <v>F814</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H23" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" t="s">
         <v>78</v>
       </c>
-      <c r="I23" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:14">
       <c r="A24" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B24" s="7">
-        <f t="shared" si="9"/>
-        <v>63516</v>
+        <f t="shared" si="10"/>
+        <v>63512</v>
       </c>
       <c r="C24" s="7">
-        <f>B24+A24-1</f>
-        <v>63516</v>
+        <f t="shared" ref="C24:C26" si="14">B24+A24-1</f>
+        <v>63513</v>
       </c>
       <c r="D24" s="7" t="str">
-        <f>DEC2HEX(B24,4)</f>
-        <v>F81C</v>
+        <f t="shared" ref="D24:D26" si="15">DEC2HEX(B24,4)</f>
+        <v>F818</v>
       </c>
       <c r="E24" s="7" t="str">
-        <f>DEC2HEX(C24,4)</f>
-        <v>F81C</v>
+        <f t="shared" ref="E24:E26" si="16">DEC2HEX(C24,4)</f>
+        <v>F819</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I24" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
       <c r="A25" s="7">
         <v>1</v>
       </c>
       <c r="B25" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
+        <v>63516</v>
+      </c>
+      <c r="C25" s="7">
+        <f>B25+A25-1</f>
+        <v>63516</v>
+      </c>
+      <c r="D25" s="7" t="str">
+        <f>DEC2HEX(B25,4)</f>
+        <v>F81C</v>
+      </c>
+      <c r="E25" s="7" t="str">
+        <f>DEC2HEX(C25,4)</f>
+        <v>F81C</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H25" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="7">
+        <v>1</v>
+      </c>
+      <c r="B26" s="7">
+        <f t="shared" si="10"/>
         <v>63520</v>
       </c>
-      <c r="C25" s="7">
-        <f t="shared" si="13"/>
+      <c r="C26" s="7">
+        <f t="shared" si="14"/>
         <v>63520</v>
       </c>
-      <c r="D25" s="7" t="str">
-        <f t="shared" si="14"/>
-        <v>F820</v>
-      </c>
-      <c r="E25" s="7" t="str">
+      <c r="D26" s="7" t="str">
         <f t="shared" si="15"/>
         <v>F820</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="H25" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="I25" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
-        <v>4</v>
-      </c>
-      <c r="B26" s="7">
-        <f t="shared" si="9"/>
-        <v>63524</v>
-      </c>
-      <c r="C26" s="7">
-        <f t="shared" ref="C26" si="16">B26+A26-1</f>
-        <v>63527</v>
-      </c>
-      <c r="D26" s="7" t="str">
-        <f t="shared" ref="D26" si="17">DEC2HEX(B26,4)</f>
-        <v>F824</v>
-      </c>
       <c r="E26" s="7" t="str">
-        <f t="shared" ref="E26" si="18">DEC2HEX(C26,4)</f>
-        <v>F827</v>
+        <f t="shared" si="16"/>
+        <v>F820</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I26" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
       <c r="A27" s="7">
         <v>4</v>
       </c>
       <c r="B27" s="7">
-        <f t="shared" si="9"/>
-        <v>63528</v>
+        <f t="shared" si="10"/>
+        <v>63524</v>
       </c>
       <c r="C27" s="7">
-        <f t="shared" ref="C27" si="19">B27+A27-1</f>
-        <v>63531</v>
+        <f t="shared" ref="C27" si="17">B27+A27-1</f>
+        <v>63527</v>
       </c>
       <c r="D27" s="7" t="str">
-        <f t="shared" ref="D27" si="20">DEC2HEX(B27,4)</f>
-        <v>F828</v>
+        <f t="shared" ref="D27" si="18">DEC2HEX(B27,4)</f>
+        <v>F824</v>
       </c>
       <c r="E27" s="7" t="str">
-        <f t="shared" ref="E27" si="21">DEC2HEX(C27,4)</f>
-        <v>F82B</v>
+        <f t="shared" ref="E27" si="19">DEC2HEX(C27,4)</f>
+        <v>F827</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
       <c r="A28" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B28" s="7">
-        <f t="shared" si="9"/>
-        <v>63532</v>
+        <f t="shared" si="10"/>
+        <v>63528</v>
       </c>
       <c r="C28" s="7">
-        <f t="shared" ref="C28" si="22">B28+A28-1</f>
-        <v>63533</v>
+        <f t="shared" ref="C28" si="20">B28+A28-1</f>
+        <v>63531</v>
       </c>
       <c r="D28" s="7" t="str">
-        <f t="shared" ref="D28" si="23">DEC2HEX(B28,4)</f>
-        <v>F82C</v>
+        <f t="shared" ref="D28" si="21">DEC2HEX(B28,4)</f>
+        <v>F828</v>
       </c>
       <c r="E28" s="7" t="str">
-        <f t="shared" ref="E28" si="24">DEC2HEX(C28,4)</f>
-        <v>F82D</v>
+        <f t="shared" ref="E28" si="22">DEC2HEX(C28,4)</f>
+        <v>F82B</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
       <c r="A29" s="7">
         <v>2</v>
       </c>
       <c r="B29" s="7">
-        <f t="shared" si="9"/>
-        <v>63536</v>
+        <f t="shared" si="10"/>
+        <v>63532</v>
       </c>
       <c r="C29" s="7">
-        <f t="shared" ref="C29:C30" si="25">B29+A29-1</f>
-        <v>63537</v>
+        <f t="shared" ref="C29" si="23">B29+A29-1</f>
+        <v>63533</v>
       </c>
       <c r="D29" s="7" t="str">
-        <f t="shared" ref="D29:D30" si="26">DEC2HEX(B29,4)</f>
-        <v>F830</v>
+        <f t="shared" ref="D29" si="24">DEC2HEX(B29,4)</f>
+        <v>F82C</v>
       </c>
       <c r="E29" s="7" t="str">
-        <f t="shared" ref="E29:E30" si="27">DEC2HEX(C29,4)</f>
-        <v>F831</v>
+        <f t="shared" ref="E29" si="25">DEC2HEX(C29,4)</f>
+        <v>F82D</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I29" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="7">
+        <v>2</v>
+      </c>
+      <c r="B30" s="7">
+        <f t="shared" si="10"/>
+        <v>63536</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" ref="C30:C31" si="26">B30+A30-1</f>
+        <v>63537</v>
+      </c>
+      <c r="D30" s="7" t="str">
+        <f t="shared" ref="D30:D31" si="27">DEC2HEX(B30,4)</f>
+        <v>F830</v>
+      </c>
+      <c r="E30" s="7" t="str">
+        <f t="shared" ref="E30:E31" si="28">DEC2HEX(C30,4)</f>
+        <v>F831</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H29" s="30" t="s">
-        <v>78</v>
-      </c>
-      <c r="I29" t="s">
+      <c r="H30" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="I30" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="7">
+    <row r="31" spans="1:14">
+      <c r="A31" s="7">
         <v>1</v>
       </c>
-      <c r="B30" s="7">
-        <f t="shared" si="9"/>
+      <c r="B31" s="7">
+        <f t="shared" si="10"/>
         <v>63540</v>
       </c>
-      <c r="C30" s="7">
-        <f t="shared" si="25"/>
+      <c r="C31" s="7">
+        <f t="shared" si="26"/>
         <v>63540</v>
       </c>
-      <c r="D30" s="7" t="str">
-        <f t="shared" si="26"/>
-        <v>F834</v>
-      </c>
-      <c r="E30" s="7" t="str">
+      <c r="D31" s="7" t="str">
         <f t="shared" si="27"/>
         <v>F834</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="H30" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="I30" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="7">
-        <v>1</v>
-      </c>
-      <c r="B31" s="7">
-        <f t="shared" si="9"/>
-        <v>63544</v>
-      </c>
-      <c r="C31" s="7">
-        <f t="shared" ref="C31:C33" si="28">B31+A31-1</f>
-        <v>63544</v>
-      </c>
-      <c r="D31" s="7" t="str">
-        <f t="shared" ref="D31:D33" si="29">DEC2HEX(B31,4)</f>
-        <v>F838</v>
-      </c>
       <c r="E31" s="7" t="str">
-        <f t="shared" ref="E31:E33" si="30">DEC2HEX(C31,4)</f>
-        <v>F838</v>
+        <f t="shared" si="28"/>
+        <v>F834</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I31" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
       <c r="A32" s="7">
         <v>1</v>
       </c>
       <c r="B32" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
+        <v>63544</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" ref="C32:C34" si="29">B32+A32-1</f>
+        <v>63544</v>
+      </c>
+      <c r="D32" s="7" t="str">
+        <f t="shared" ref="D32:D34" si="30">DEC2HEX(B32,4)</f>
+        <v>F838</v>
+      </c>
+      <c r="E32" s="7" t="str">
+        <f t="shared" ref="E32:E34" si="31">DEC2HEX(C32,4)</f>
+        <v>F838</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H32" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14">
+      <c r="A33" s="7">
+        <v>1</v>
+      </c>
+      <c r="B33" s="7">
+        <f t="shared" si="10"/>
         <v>63548</v>
       </c>
-      <c r="C32" s="7">
-        <f t="shared" si="28"/>
+      <c r="C33" s="7">
+        <f t="shared" si="29"/>
         <v>63548</v>
       </c>
-      <c r="D32" s="7" t="str">
-        <f t="shared" si="29"/>
-        <v>F83C</v>
-      </c>
-      <c r="E32" s="7" t="str">
+      <c r="D33" s="7" t="str">
         <f t="shared" si="30"/>
         <v>F83C</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8" t="s">
+      <c r="E33" s="7" t="str">
+        <f t="shared" si="31"/>
+        <v>F83C</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="H32" s="30" t="s">
-        <v>77</v>
-      </c>
-      <c r="I32" t="s">
+      <c r="H33" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I33" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="7">
+    <row r="34" spans="1:14">
+      <c r="A34" s="7">
         <v>1</v>
       </c>
-      <c r="B33" s="7">
-        <f t="shared" si="9"/>
+      <c r="B34" s="7">
+        <f t="shared" si="10"/>
         <v>63552</v>
       </c>
-      <c r="C33" s="7">
-        <f t="shared" si="28"/>
+      <c r="C34" s="7">
+        <f t="shared" si="29"/>
         <v>63552</v>
       </c>
-      <c r="D33" s="7" t="str">
-        <f t="shared" si="29"/>
-        <v>F840</v>
-      </c>
-      <c r="E33" s="7" t="str">
+      <c r="D34" s="7" t="str">
         <f t="shared" si="30"/>
         <v>F840</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H33" s="30" t="s">
-        <v>79</v>
-      </c>
-      <c r="I33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="7">
-        <v>1</v>
-      </c>
-      <c r="B34" s="7">
-        <f t="shared" si="9"/>
-        <v>63556</v>
-      </c>
-      <c r="C34" s="7">
-        <f t="shared" ref="C34" si="31">B34+A34-1</f>
-        <v>63556</v>
-      </c>
-      <c r="D34" s="7" t="str">
-        <f t="shared" ref="D34" si="32">DEC2HEX(B34,4)</f>
-        <v>F844</v>
-      </c>
       <c r="E34" s="7" t="str">
-        <f t="shared" ref="E34" si="33">DEC2HEX(C34,4)</f>
-        <v>F844</v>
+        <f t="shared" si="31"/>
+        <v>F840</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="I34" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14">
       <c r="A35" s="7">
         <v>1</v>
       </c>
       <c r="B35" s="7">
-        <f t="shared" si="9"/>
-        <v>63560</v>
+        <f t="shared" si="10"/>
+        <v>63556</v>
       </c>
       <c r="C35" s="7">
-        <f t="shared" ref="C35" si="34">B35+A35-1</f>
-        <v>63560</v>
+        <f t="shared" ref="C35" si="32">B35+A35-1</f>
+        <v>63556</v>
       </c>
       <c r="D35" s="7" t="str">
-        <f t="shared" ref="D35" si="35">DEC2HEX(B35,4)</f>
-        <v>F848</v>
+        <f t="shared" ref="D35" si="33">DEC2HEX(B35,4)</f>
+        <v>F844</v>
       </c>
       <c r="E35" s="7" t="str">
-        <f t="shared" ref="E35" si="36">DEC2HEX(C35,4)</f>
-        <v>F848</v>
+        <f t="shared" ref="E35" si="34">DEC2HEX(C35,4)</f>
+        <v>F844</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8" t="s">
-        <v>98</v>
+        <v>27</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="I35" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14">
       <c r="A36" s="7">
-        <f>C36-B36</f>
+        <v>1</v>
+      </c>
+      <c r="B36" s="7">
+        <f t="shared" si="10"/>
+        <v>63560</v>
+      </c>
+      <c r="C36" s="7">
+        <f t="shared" ref="C36" si="35">B36+A36-1</f>
+        <v>63560</v>
+      </c>
+      <c r="D36" s="7" t="str">
+        <f t="shared" ref="D36" si="36">DEC2HEX(B36,4)</f>
+        <v>F848</v>
+      </c>
+      <c r="E36" s="7" t="str">
+        <f t="shared" ref="E36" si="37">DEC2HEX(C36,4)</f>
+        <v>F848</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="I36" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14">
+      <c r="A37" s="7">
+        <f>C37-B37</f>
         <v>1971</v>
       </c>
-      <c r="B36" s="7">
-        <f>B35+4</f>
+      <c r="B37" s="7">
+        <f>B36+4</f>
         <v>63564</v>
       </c>
-      <c r="C36" s="7">
+      <c r="C37" s="7">
         <v>65535</v>
       </c>
-      <c r="D36" s="7" t="str">
-        <f t="shared" ref="D36" si="37">DEC2HEX(B36,4)</f>
+      <c r="D37" s="7" t="str">
+        <f t="shared" ref="D37" si="38">DEC2HEX(B37,4)</f>
         <v>F84C</v>
       </c>
-      <c r="E36" s="7" t="str">
-        <f t="shared" ref="E36" si="38">DEC2HEX(C36,4)</f>
+      <c r="E37" s="7" t="str">
+        <f t="shared" ref="E37" si="39">DEC2HEX(C37,4)</f>
         <v>FFFF</v>
       </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="12" t="s">
+      <c r="F37" s="7"/>
+      <c r="G37" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="H36" s="34"/>
-    </row>
-    <row r="38" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
+      <c r="H37" s="34"/>
+    </row>
+    <row r="39" spans="1:14" s="9" customFormat="1">
+      <c r="A39" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
-      <c r="F38" s="16"/>
-      <c r="H38" s="31"/>
-      <c r="I38"/>
-      <c r="J38"/>
-      <c r="K38"/>
-      <c r="L38"/>
-      <c r="M38"/>
-      <c r="N38"/>
-    </row>
-    <row r="39" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B39" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F39" s="13"/>
-      <c r="G39" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H39" s="32"/>
+      <c r="D39" s="16"/>
+      <c r="E39" s="16"/>
+      <c r="F39" s="16"/>
+      <c r="H39" s="31"/>
       <c r="I39"/>
       <c r="J39"/>
       <c r="K39"/>
@@ -1979,21 +1935,26 @@
       <c r="M39"/>
       <c r="N39"/>
     </row>
-    <row r="40" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="13"/>
+    <row r="40" spans="1:14" s="10" customFormat="1">
+      <c r="A40" s="13" t="s">
+        <v>6</v>
+      </c>
       <c r="B40" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C40" s="13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F40" s="13"/>
+      <c r="G40" s="10" t="s">
+        <v>0</v>
+      </c>
       <c r="H40" s="32"/>
       <c r="I40"/>
       <c r="J40"/>
@@ -2002,14 +1963,21 @@
       <c r="M40"/>
       <c r="N40"/>
     </row>
-    <row r="41" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="10"/>
+    <row r="41" spans="1:14" s="10" customFormat="1">
+      <c r="A41" s="13"/>
+      <c r="B41" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F41" s="13"/>
       <c r="H41" s="32"/>
       <c r="I41"/>
       <c r="J41"/>
@@ -2018,286 +1986,302 @@
       <c r="M41"/>
       <c r="N41"/>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
+    <row r="42" spans="1:14" s="5" customFormat="1">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="10"/>
+      <c r="H42" s="32"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+    </row>
+    <row r="43" spans="1:14">
+      <c r="A43" s="7">
         <v>65536</v>
       </c>
-      <c r="B42" s="7">
+      <c r="B43" s="7">
         <v>0</v>
       </c>
-      <c r="C42" s="7">
-        <f>A42-1</f>
+      <c r="C43" s="7">
+        <f>A43-1</f>
         <v>65535</v>
       </c>
-      <c r="D42" s="7" t="str">
-        <f>DEC2HEX(B42,6)</f>
+      <c r="D43" s="7" t="str">
+        <f>DEC2HEX(B43,6)</f>
         <v>000000</v>
       </c>
-      <c r="E42" s="7" t="str">
-        <f>DEC2HEX(C42,6)</f>
+      <c r="E43" s="7" t="str">
+        <f>DEC2HEX(C43,6)</f>
         <v>00FFFF</v>
       </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="12" t="s">
+      <c r="F43" s="7"/>
+      <c r="G43" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H42" s="34"/>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
-        <v>256</v>
-      </c>
-      <c r="B43" s="7">
-        <f>C42+1</f>
-        <v>65536</v>
-      </c>
-      <c r="C43" s="7">
-        <f t="shared" ref="C43" si="39">B43+A43-1</f>
-        <v>65791</v>
-      </c>
-      <c r="D43" s="7" t="str">
-        <f t="shared" ref="D43:D44" si="40">DEC2HEX(B43,6)</f>
-        <v>010000</v>
-      </c>
-      <c r="E43" s="7" t="str">
-        <f t="shared" ref="E43:E44" si="41">DEC2HEX(C43,6)</f>
-        <v>0100FF</v>
-      </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H43" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H43" s="34"/>
+    </row>
+    <row r="44" spans="1:14">
       <c r="A44" s="7">
         <v>256</v>
       </c>
       <c r="B44" s="7">
         <f>C43+1</f>
-        <v>65792</v>
+        <v>65536</v>
       </c>
       <c r="C44" s="7">
-        <f t="shared" ref="C44" si="42">B44+A44-1</f>
-        <v>66047</v>
+        <f t="shared" ref="C44" si="40">B44+A44-1</f>
+        <v>65791</v>
       </c>
       <c r="D44" s="7" t="str">
-        <f t="shared" si="40"/>
-        <v>010100</v>
+        <f t="shared" ref="D44:D45" si="41">DEC2HEX(B44,6)</f>
+        <v>010000</v>
       </c>
       <c r="E44" s="7" t="str">
-        <f t="shared" si="41"/>
-        <v>0101FF</v>
+        <f t="shared" ref="E44:E45" si="42">DEC2HEX(C44,6)</f>
+        <v>0100FF</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14">
       <c r="A45" s="7">
         <v>256</v>
       </c>
       <c r="B45" s="7">
         <f>C44+1</f>
-        <v>66048</v>
+        <v>65792</v>
       </c>
       <c r="C45" s="7">
-        <f t="shared" ref="C45:C49" si="43">B45+A45-1</f>
-        <v>66303</v>
+        <f t="shared" ref="C45" si="43">B45+A45-1</f>
+        <v>66047</v>
       </c>
       <c r="D45" s="7" t="str">
-        <f t="shared" ref="D45:D51" si="44">DEC2HEX(B45,6)</f>
-        <v>010200</v>
+        <f t="shared" si="41"/>
+        <v>010100</v>
       </c>
       <c r="E45" s="7" t="str">
-        <f t="shared" ref="E45:E51" si="45">DEC2HEX(C45,6)</f>
-        <v>0102FF</v>
+        <f t="shared" si="42"/>
+        <v>0101FF</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="8" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="H45" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14">
       <c r="A46" s="7">
         <v>256</v>
       </c>
       <c r="B46" s="7">
         <f>C45+1</f>
-        <v>66304</v>
+        <v>66048</v>
       </c>
       <c r="C46" s="7">
-        <f t="shared" si="43"/>
-        <v>66559</v>
+        <f t="shared" ref="C46:C50" si="44">B46+A46-1</f>
+        <v>66303</v>
       </c>
       <c r="D46" s="7" t="str">
-        <f t="shared" si="44"/>
-        <v>010300</v>
+        <f t="shared" ref="D46:D52" si="45">DEC2HEX(B46,6)</f>
+        <v>010200</v>
       </c>
       <c r="E46" s="7" t="str">
-        <f t="shared" si="45"/>
-        <v>0103FF</v>
+        <f t="shared" ref="E46:E52" si="46">DEC2HEX(C46,6)</f>
+        <v>0102FF</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14">
       <c r="A47" s="7">
         <v>256</v>
       </c>
       <c r="B47" s="7">
-        <f t="shared" ref="B47" si="46">C46+1</f>
-        <v>66560</v>
+        <f>C46+1</f>
+        <v>66304</v>
       </c>
       <c r="C47" s="7">
-        <f t="shared" si="43"/>
-        <v>66815</v>
+        <f t="shared" si="44"/>
+        <v>66559</v>
       </c>
       <c r="D47" s="7" t="str">
-        <f t="shared" si="44"/>
-        <v>010400</v>
+        <f t="shared" si="45"/>
+        <v>010300</v>
       </c>
       <c r="E47" s="7" t="str">
-        <f t="shared" si="45"/>
-        <v>0104FF</v>
+        <f t="shared" si="46"/>
+        <v>0103FF</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14">
       <c r="A48" s="7">
         <v>256</v>
       </c>
       <c r="B48" s="7">
         <f t="shared" ref="B48" si="47">C47+1</f>
-        <v>66816</v>
+        <v>66560</v>
       </c>
       <c r="C48" s="7">
-        <f t="shared" ref="C48" si="48">B48+A48-1</f>
-        <v>67071</v>
+        <f t="shared" si="44"/>
+        <v>66815</v>
       </c>
       <c r="D48" s="7" t="str">
-        <f t="shared" ref="D48" si="49">DEC2HEX(B48,6)</f>
-        <v>010500</v>
+        <f t="shared" si="45"/>
+        <v>010400</v>
       </c>
       <c r="E48" s="7" t="str">
-        <f t="shared" ref="E48" si="50">DEC2HEX(C48,6)</f>
-        <v>0105FF</v>
+        <f t="shared" si="46"/>
+        <v>0104FF</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="8" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49" s="7">
+        <v>256</v>
+      </c>
+      <c r="B49" s="7">
+        <f t="shared" ref="B49" si="48">C48+1</f>
+        <v>66816</v>
+      </c>
+      <c r="C49" s="7">
+        <f t="shared" ref="C49" si="49">B49+A49-1</f>
+        <v>67071</v>
+      </c>
+      <c r="D49" s="7" t="str">
+        <f t="shared" ref="D49" si="50">DEC2HEX(B49,6)</f>
+        <v>010500</v>
+      </c>
+      <c r="E49" s="7" t="str">
+        <f t="shared" ref="E49" si="51">DEC2HEX(C49,6)</f>
+        <v>0105FF</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="7">
         <f>2*(100*75*2)</f>
         <v>30000</v>
       </c>
-      <c r="B49" s="7">
-        <f>C48+1</f>
-        <v>67072</v>
-      </c>
-      <c r="C49" s="7">
-        <f t="shared" si="43"/>
-        <v>97071</v>
-      </c>
-      <c r="D49" s="7" t="str">
-        <f t="shared" si="44"/>
-        <v>010600</v>
-      </c>
-      <c r="E49" s="7" t="str">
-        <f t="shared" si="45"/>
-        <v>017B2F</v>
-      </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="H49" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
-        <v>1024</v>
-      </c>
       <c r="B50" s="7">
         <f>C49+1</f>
-        <v>97072</v>
+        <v>67072</v>
       </c>
       <c r="C50" s="7">
-        <f t="shared" ref="C50" si="51">B50+A50-1</f>
-        <v>98095</v>
+        <f t="shared" si="44"/>
+        <v>97071</v>
       </c>
       <c r="D50" s="7" t="str">
-        <f t="shared" ref="D50" si="52">DEC2HEX(B50,6)</f>
-        <v>017B30</v>
+        <f t="shared" si="45"/>
+        <v>010600</v>
       </c>
       <c r="E50" s="7" t="str">
-        <f t="shared" ref="E50" si="53">DEC2HEX(C50,6)</f>
-        <v>017F2F</v>
+        <f t="shared" si="46"/>
+        <v>017B2F</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="8" t="s">
-        <v>97</v>
+        <v>24</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51" s="7">
-        <f>C51-B51</f>
-        <v>16679119</v>
+        <v>1024</v>
       </c>
       <c r="B51" s="7">
         <f>C50+1</f>
+        <v>97072</v>
+      </c>
+      <c r="C51" s="7">
+        <f t="shared" ref="C51" si="52">B51+A51-1</f>
+        <v>98095</v>
+      </c>
+      <c r="D51" s="7" t="str">
+        <f t="shared" ref="D51" si="53">DEC2HEX(B51,6)</f>
+        <v>017B30</v>
+      </c>
+      <c r="E51" s="7" t="str">
+        <f t="shared" ref="E51" si="54">DEC2HEX(C51,6)</f>
+        <v>017F2F</v>
+      </c>
+      <c r="F51" s="7"/>
+      <c r="G51" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="H51" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="7">
+        <f>C52-B52</f>
+        <v>16679119</v>
+      </c>
+      <c r="B52" s="7">
+        <f>C51+1</f>
         <v>98096</v>
       </c>
-      <c r="C51" s="7">
+      <c r="C52" s="7">
         <f>16*1024*1024-1</f>
         <v>16777215</v>
       </c>
-      <c r="D51" s="7" t="str">
-        <f t="shared" si="44"/>
+      <c r="D52" s="7" t="str">
+        <f t="shared" si="45"/>
         <v>017F30</v>
       </c>
-      <c r="E51" s="7" t="str">
-        <f t="shared" si="45"/>
+      <c r="E52" s="7" t="str">
+        <f t="shared" si="46"/>
         <v>FFFFFF</v>
       </c>
-      <c r="F51" s="7"/>
-      <c r="G51" s="8" t="s">
+      <c r="F52" s="7"/>
+      <c r="G52" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H51" s="30" t="s">
+      <c r="H52" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I52" t="s">
         <v>77</v>
-      </c>
-      <c r="I51" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2307,14 +2291,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="6" width="1.5703125" customWidth="1"/>
@@ -2327,16 +2311,16 @@
     <col min="15" max="15" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="21">
       <c r="A1" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2357,7 +2341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -2378,7 +2362,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
@@ -2388,7 +2372,7 @@
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75">
       <c r="A4" s="15"/>
       <c r="B4" s="13" t="s">
         <v>8</v>
@@ -2429,7 +2413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75">
       <c r="A5" s="15"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -2446,30 +2430,30 @@
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="21" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="22">
-        <f>'Memory Map'!A20</f>
+        <f>'Memory Map'!A21</f>
         <v>1</v>
       </c>
       <c r="B6" s="22">
-        <f>'Memory Map'!B20</f>
+        <f>'Memory Map'!B21</f>
         <v>63500</v>
       </c>
       <c r="C6" s="22">
-        <f>'Memory Map'!C20</f>
+        <f>'Memory Map'!C21</f>
         <v>63500</v>
       </c>
       <c r="D6" s="22" t="str">
-        <f>'Memory Map'!D20</f>
+        <f>'Memory Map'!D21</f>
         <v>F80C</v>
       </c>
       <c r="E6" s="22" t="str">
-        <f>'Memory Map'!E20</f>
+        <f>'Memory Map'!E21</f>
         <v>F80C</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="28" t="str">
-        <f>'Memory Map'!G20</f>
+        <f>'Memory Map'!G21</f>
         <v>Graphics mode</v>
       </c>
       <c r="H6" s="24" t="s">
@@ -2487,17 +2471,13 @@
       <c r="L6" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="M6" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="N6" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="O6" s="25" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M6" s="36" t="s">
+        <v>99</v>
+      </c>
+      <c r="N6" s="36"/>
+      <c r="O6" s="36"/>
+    </row>
+    <row r="7" spans="1:15" s="21" customFormat="1">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -2514,7 +2494,7 @@
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -2531,30 +2511,30 @@
       <c r="N8" s="26"/>
       <c r="O8" s="26"/>
     </row>
-    <row r="9" spans="1:15" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="21" customFormat="1" ht="30">
       <c r="A9" s="22">
-        <f>'Memory Map'!A24</f>
+        <f>'Memory Map'!A25</f>
         <v>1</v>
       </c>
       <c r="B9" s="22">
-        <f>'Memory Map'!B24</f>
+        <f>'Memory Map'!B25</f>
         <v>63516</v>
       </c>
       <c r="C9" s="22">
-        <f>'Memory Map'!C24</f>
+        <f>'Memory Map'!C25</f>
         <v>63516</v>
       </c>
       <c r="D9" s="22" t="str">
-        <f>'Memory Map'!D24</f>
+        <f>'Memory Map'!D25</f>
         <v>F81C</v>
       </c>
       <c r="E9" s="22" t="str">
-        <f>'Memory Map'!E24</f>
+        <f>'Memory Map'!E25</f>
         <v>F81C</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="28" t="str">
-        <f>'Memory Map'!G24</f>
+        <f>'Memory Map'!G25</f>
         <v>RS232 status signals</v>
       </c>
       <c r="H9" s="24" t="s">
@@ -2582,7 +2562,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="21" customFormat="1">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -2599,7 +2579,7 @@
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
     </row>
-    <row r="11" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="21" customFormat="1">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -2616,33 +2596,33 @@
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
-        <f>'Memory Map'!A28-1</f>
+        <f>'Memory Map'!A29-1</f>
         <v>1</v>
       </c>
       <c r="B12" s="1">
-        <f>'Memory Map'!B28</f>
+        <f>'Memory Map'!B29</f>
         <v>63532</v>
       </c>
       <c r="C12" s="1">
-        <f>'Memory Map'!C28</f>
+        <f>'Memory Map'!C29</f>
         <v>63533</v>
       </c>
       <c r="D12" s="1" t="str">
-        <f>'Memory Map'!D28</f>
+        <f>'Memory Map'!D29</f>
         <v>F82C</v>
       </c>
       <c r="E12" s="1" t="str">
-        <f>'Memory Map'!E28</f>
+        <f>'Memory Map'!E29</f>
         <v>F82D</v>
       </c>
       <c r="F12">
-        <f>'Memory Map'!F28</f>
+        <f>'Memory Map'!F29</f>
         <v>0</v>
       </c>
       <c r="G12" s="2" t="str">
-        <f>'Memory Map'!G28</f>
+        <f>'Memory Map'!G29</f>
         <v>IRQ mask</v>
       </c>
       <c r="H12" s="24" t="s">
@@ -2655,22 +2635,22 @@
         <v>56</v>
       </c>
       <c r="K12" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="L12" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="M12" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="N12" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="O12" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="G13" s="2"/>
       <c r="H13" s="27">
         <v>0</v>
@@ -2697,42 +2677,42 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="G14" s="2"/>
       <c r="H14" s="24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="G15" s="2"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="30">
       <c r="A17" s="22">
-        <f>'Memory Map'!A32</f>
+        <f>'Memory Map'!A33</f>
         <v>1</v>
       </c>
       <c r="B17" s="22">
-        <f>'Memory Map'!B32</f>
+        <f>'Memory Map'!B33</f>
         <v>63548</v>
       </c>
       <c r="C17" s="22">
-        <f>'Memory Map'!C32</f>
+        <f>'Memory Map'!C33</f>
         <v>63548</v>
       </c>
       <c r="D17" s="22" t="str">
-        <f>'Memory Map'!D32</f>
+        <f>'Memory Map'!D33</f>
         <v>F83C</v>
       </c>
       <c r="E17" s="22" t="str">
-        <f>'Memory Map'!E32</f>
+        <f>'Memory Map'!E33</f>
         <v>F83C</v>
       </c>
       <c r="G17" s="29" t="str">
-        <f>'Memory Map'!G32</f>
+        <f>'Memory Map'!G33</f>
         <v>SPI control</v>
       </c>
       <c r="H17" s="24" t="s">
@@ -2748,19 +2728,19 @@
         <v>56</v>
       </c>
       <c r="L17" s="21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="M17" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="N17" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="O17" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="N17" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="O17" s="21" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
@@ -2770,7 +2750,7 @@
       <c r="N18" s="27"/>
       <c r="O18" s="27"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -2778,29 +2758,29 @@
       <c r="E19" s="22"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="22">
-        <f>'Memory Map'!A33</f>
+        <f>'Memory Map'!A34</f>
         <v>1</v>
       </c>
       <c r="B20" s="22">
-        <f>'Memory Map'!B33</f>
+        <f>'Memory Map'!B34</f>
         <v>63552</v>
       </c>
       <c r="C20" s="22">
-        <f>'Memory Map'!C33</f>
+        <f>'Memory Map'!C34</f>
         <v>63552</v>
       </c>
       <c r="D20" s="22" t="str">
-        <f>'Memory Map'!D33</f>
+        <f>'Memory Map'!D34</f>
         <v>F840</v>
       </c>
       <c r="E20" s="22" t="str">
-        <f>'Memory Map'!E33</f>
+        <f>'Memory Map'!E34</f>
         <v>F840</v>
       </c>
       <c r="G20" s="2" t="str">
-        <f>'Memory Map'!G33</f>
+        <f>'Memory Map'!G34</f>
         <v>SPI status</v>
       </c>
       <c r="H20" s="24" t="s">
@@ -2816,86 +2796,89 @@
         <v>56</v>
       </c>
       <c r="L20" s="24" t="s">
+        <v>89</v>
+      </c>
+      <c r="M20" s="24" t="s">
+        <v>90</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="O20" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="M20" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="N20" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="O20" s="21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M6:O6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="109.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="21" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="21" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="21"/>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="21" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="21" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+    <row r="6" spans="1:1" ht="30">
+      <c r="A6" s="21" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
+    <row r="7" spans="1:1">
+      <c r="A7" s="21" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="45">
+      <c r="A8" s="35" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="21"/>
+    </row>
+    <row r="10" spans="1:1" ht="60">
+      <c r="A10" s="35" t="s">
         <v>86</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="21"/>
-    </row>
-    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="35" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Supporting project files updated
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -429,7 +429,30 @@
     <t xml:space="preserve">Access to the color RAM in the CPU address space </t>
   </si>
   <si>
-    <t>000 = off, 001 = 640*480, 010 = 800*600, 011 = 1024*768</t>
+    <r>
+      <t xml:space="preserve">000 = off, 001 = 640*480, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>010 = 800*600</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, 011 = 1024*768</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2295,7 +2318,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Improved timing issues with v3.0 - moved PSDRAM buffers above 256KB in preparation for expanded memory - fixed BAUD calculation fro 100MHz - extended SWITCHES to all 16 external switches
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Map" sheetId="1" r:id="rId1"/>
@@ -69,9 +69,6 @@
     <t>TEXT zero (31 downto 0)</t>
   </si>
   <si>
-    <t>not used</t>
-  </si>
-  <si>
     <t>Board switches</t>
   </si>
   <si>
@@ -88,9 +85,6 @@
   </si>
   <si>
     <t>PS2 buffer</t>
-  </si>
-  <si>
-    <t>Text RAM 2 * 100 * 75 * 8+8bit</t>
   </si>
   <si>
     <t>SPI data</t>
@@ -453,6 +447,12 @@
       </rPr>
       <t>, 011 = 1024*768</t>
     </r>
+  </si>
+  <si>
+    <t>Text RAM 2 * 128 * 96 * 8+8bit</t>
+  </si>
+  <si>
+    <t>Reserved for expansion</t>
   </si>
 </sst>
 </file>
@@ -955,8 +955,8 @@
   </sheetPr>
   <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7:J12"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -974,7 +974,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="21">
       <c r="A1" s="17" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:14" s="9" customFormat="1">
@@ -1013,7 +1013,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="32" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I4"/>
       <c r="J4"/>
@@ -1063,58 +1063,58 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="7">
-        <v>45056</v>
+        <f>(64-10)*1024</f>
+        <v>55296</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
       </c>
       <c r="C7" s="7">
         <f>B7+A7-1</f>
-        <v>45055</v>
+        <v>55295</v>
       </c>
       <c r="D7" s="7" t="str">
-        <f>DEC2HEX(B7,4)</f>
-        <v>0000</v>
+        <f>DEC2HEX(B7,6)</f>
+        <v>000000</v>
       </c>
       <c r="E7" s="7" t="str">
-        <f>DEC2HEX(C7,4)</f>
-        <v>AFFF</v>
+        <f>DEC2HEX(C7,6)</f>
+        <v>00D7FF</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8" t="s">
         <v>1</v>
       </c>
       <c r="H7" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I7" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="7">
-        <f>12288-2048</f>
-        <v>10240</v>
+        <v>0</v>
       </c>
       <c r="B8" s="7">
         <f>C7+1</f>
-        <v>45056</v>
+        <v>55296</v>
       </c>
       <c r="C8" s="7">
-        <f t="shared" ref="C8:C12" si="0">B8+A8-1</f>
+        <f>B8+A8-1</f>
         <v>55295</v>
       </c>
       <c r="D8" s="7" t="str">
-        <f t="shared" ref="D8" si="1">DEC2HEX(B8,4)</f>
-        <v>B000</v>
+        <f t="shared" ref="D8" si="0">DEC2HEX(B8,6)</f>
+        <v>00D800</v>
       </c>
       <c r="E8" s="7" t="str">
-        <f t="shared" ref="E8" si="2">DEC2HEX(C8,4)</f>
-        <v>D7FF</v>
+        <f t="shared" ref="E8" si="1">DEC2HEX(C8,6)</f>
+        <v>00D7FF</v>
       </c>
       <c r="F8" s="7"/>
-      <c r="G8" s="12" t="s">
-        <v>17</v>
+      <c r="G8" s="8" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1130,22 +1130,22 @@
         <v>57343</v>
       </c>
       <c r="D9" s="7" t="str">
-        <f t="shared" ref="D9" si="3">DEC2HEX(B9,4)</f>
-        <v>D800</v>
+        <f t="shared" ref="D9:D12" si="2">DEC2HEX(B9,6)</f>
+        <v>00D800</v>
       </c>
       <c r="E9" s="7" t="str">
-        <f t="shared" ref="E9" si="4">DEC2HEX(C9,4)</f>
-        <v>DFFF</v>
+        <f t="shared" ref="E9:E12" si="3">DEC2HEX(C9,6)</f>
+        <v>00DFFF</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H9" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -1158,26 +1158,26 @@
         <v>57344</v>
       </c>
       <c r="C10" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="C10:C12" si="4">B10+A10-1</f>
         <v>59391</v>
       </c>
       <c r="D10" s="7" t="str">
-        <f t="shared" ref="D10:D12" si="5">DEC2HEX(B10,4)</f>
-        <v>E000</v>
+        <f t="shared" si="2"/>
+        <v>00E000</v>
       </c>
       <c r="E10" s="7" t="str">
-        <f t="shared" ref="E10:E12" si="6">DEC2HEX(C10,4)</f>
-        <v>E7FF</v>
+        <f t="shared" si="3"/>
+        <v>00E7FF</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8" t="s">
         <v>2</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -1190,26 +1190,26 @@
         <v>59392</v>
       </c>
       <c r="C11" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>61439</v>
       </c>
       <c r="D11" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>E800</v>
+        <f t="shared" si="2"/>
+        <v>00E800</v>
       </c>
       <c r="E11" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>EFFF</v>
+        <f t="shared" si="3"/>
+        <v>00EFFF</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -1221,26 +1221,26 @@
         <v>61440</v>
       </c>
       <c r="C12" s="7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="4"/>
         <v>63487</v>
       </c>
       <c r="D12" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>F000</v>
+        <f t="shared" si="2"/>
+        <v>00F000</v>
       </c>
       <c r="E12" s="7" t="str">
-        <f t="shared" si="6"/>
-        <v>F7FF</v>
+        <f t="shared" si="3"/>
+        <v>00F7FF</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="8" t="s">
         <v>4</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -1248,7 +1248,7 @@
     </row>
     <row r="14" spans="1:14" s="9" customFormat="1">
       <c r="A14" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D14" s="16"/>
       <c r="E14" s="16"/>
@@ -1341,22 +1341,22 @@
         <v>63491</v>
       </c>
       <c r="D18" s="7" t="str">
-        <f>DEC2HEX(B18,4)</f>
-        <v>F800</v>
+        <f t="shared" ref="D18:D37" si="5">DEC2HEX(B18,6)</f>
+        <v>00F800</v>
       </c>
       <c r="E18" s="7" t="str">
-        <f>DEC2HEX(C18,4)</f>
-        <v>F803</v>
+        <f t="shared" ref="E18:E37" si="6">DEC2HEX(C18,6)</f>
+        <v>00F803</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8" t="s">
         <v>16</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -1372,22 +1372,22 @@
         <v>63495</v>
       </c>
       <c r="D19" s="7" t="str">
-        <f t="shared" ref="D19" si="8">DEC2HEX(B19,4)</f>
-        <v>F804</v>
+        <f t="shared" si="5"/>
+        <v>00F804</v>
       </c>
       <c r="E19" s="7" t="str">
-        <f t="shared" ref="E19" si="9">DEC2HEX(C19,4)</f>
-        <v>F807</v>
+        <f t="shared" si="6"/>
+        <v>00F807</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" t="s">
         <v>29</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="I19" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -1395,30 +1395,30 @@
         <v>1</v>
       </c>
       <c r="B20" s="7">
-        <f t="shared" ref="B20:B36" si="10">B19+4</f>
+        <f t="shared" ref="B20:B36" si="8">B19+4</f>
         <v>63496</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" ref="C20:C23" si="11">B20+A20-1</f>
+        <f t="shared" ref="C20:C23" si="9">B20+A20-1</f>
         <v>63496</v>
       </c>
       <c r="D20" s="7" t="str">
-        <f t="shared" ref="D20:D23" si="12">DEC2HEX(B20,4)</f>
-        <v>F808</v>
+        <f t="shared" si="5"/>
+        <v>00F808</v>
       </c>
       <c r="E20" s="7" t="str">
-        <f t="shared" ref="E20:E23" si="13">DEC2HEX(C20,4)</f>
-        <v>F808</v>
+        <f t="shared" si="6"/>
+        <v>00F808</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -1426,30 +1426,30 @@
         <v>1</v>
       </c>
       <c r="B21" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63500</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>63500</v>
       </c>
       <c r="D21" s="7" t="str">
-        <f t="shared" si="12"/>
-        <v>F80C</v>
+        <f t="shared" si="5"/>
+        <v>00F80C</v>
       </c>
       <c r="E21" s="7" t="str">
-        <f t="shared" si="13"/>
-        <v>F80C</v>
+        <f t="shared" si="6"/>
+        <v>00F80C</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I21" t="s">
         <v>33</v>
-      </c>
-      <c r="H21" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="I21" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -1457,30 +1457,30 @@
         <v>1</v>
       </c>
       <c r="B22" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63504</v>
       </c>
       <c r="C22" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>63504</v>
       </c>
       <c r="D22" s="7" t="str">
-        <f t="shared" si="12"/>
-        <v>F810</v>
+        <f t="shared" si="5"/>
+        <v>00F810</v>
       </c>
       <c r="E22" s="7" t="str">
-        <f t="shared" si="13"/>
-        <v>F810</v>
+        <f t="shared" si="6"/>
+        <v>00F810</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I22" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -1488,30 +1488,30 @@
         <v>1</v>
       </c>
       <c r="B23" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63508</v>
       </c>
       <c r="C23" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>63508</v>
       </c>
       <c r="D23" s="7" t="str">
-        <f t="shared" si="12"/>
-        <v>F814</v>
+        <f t="shared" si="5"/>
+        <v>00F814</v>
       </c>
       <c r="E23" s="7" t="str">
-        <f t="shared" si="13"/>
-        <v>F814</v>
+        <f t="shared" si="6"/>
+        <v>00F814</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I23" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="24" spans="1:14">
@@ -1519,30 +1519,30 @@
         <v>2</v>
       </c>
       <c r="B24" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63512</v>
       </c>
       <c r="C24" s="7">
-        <f t="shared" ref="C24:C26" si="14">B24+A24-1</f>
+        <f t="shared" ref="C24:C26" si="10">B24+A24-1</f>
         <v>63513</v>
       </c>
       <c r="D24" s="7" t="str">
-        <f t="shared" ref="D24:D26" si="15">DEC2HEX(B24,4)</f>
-        <v>F818</v>
+        <f t="shared" si="5"/>
+        <v>00F818</v>
       </c>
       <c r="E24" s="7" t="str">
-        <f t="shared" ref="E24:E26" si="16">DEC2HEX(C24,4)</f>
-        <v>F819</v>
+        <f t="shared" si="6"/>
+        <v>00F819</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:14">
@@ -1550,7 +1550,7 @@
         <v>1</v>
       </c>
       <c r="B25" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63516</v>
       </c>
       <c r="C25" s="7">
@@ -1558,22 +1558,22 @@
         <v>63516</v>
       </c>
       <c r="D25" s="7" t="str">
-        <f>DEC2HEX(B25,4)</f>
-        <v>F81C</v>
+        <f t="shared" si="5"/>
+        <v>00F81C</v>
       </c>
       <c r="E25" s="7" t="str">
-        <f>DEC2HEX(C25,4)</f>
-        <v>F81C</v>
+        <f t="shared" si="6"/>
+        <v>00F81C</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H25" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I25" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:14">
@@ -1581,30 +1581,30 @@
         <v>1</v>
       </c>
       <c r="B26" s="7">
+        <f t="shared" si="8"/>
+        <v>63520</v>
+      </c>
+      <c r="C26" s="7">
         <f t="shared" si="10"/>
         <v>63520</v>
       </c>
-      <c r="C26" s="7">
-        <f t="shared" si="14"/>
-        <v>63520</v>
-      </c>
       <c r="D26" s="7" t="str">
-        <f t="shared" si="15"/>
-        <v>F820</v>
+        <f t="shared" si="5"/>
+        <v>00F820</v>
       </c>
       <c r="E26" s="7" t="str">
-        <f t="shared" si="16"/>
-        <v>F820</v>
+        <f t="shared" si="6"/>
+        <v>00F820</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I26" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:14">
@@ -1612,30 +1612,30 @@
         <v>4</v>
       </c>
       <c r="B27" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63524</v>
       </c>
       <c r="C27" s="7">
-        <f t="shared" ref="C27" si="17">B27+A27-1</f>
+        <f t="shared" ref="C27" si="11">B27+A27-1</f>
         <v>63527</v>
       </c>
       <c r="D27" s="7" t="str">
-        <f t="shared" ref="D27" si="18">DEC2HEX(B27,4)</f>
-        <v>F824</v>
+        <f t="shared" si="5"/>
+        <v>00F824</v>
       </c>
       <c r="E27" s="7" t="str">
-        <f t="shared" ref="E27" si="19">DEC2HEX(C27,4)</f>
-        <v>F827</v>
+        <f t="shared" si="6"/>
+        <v>00F827</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H27" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I27" t="s">
         <v>40</v>
-      </c>
-      <c r="H27" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="I27" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="28" spans="1:14">
@@ -1643,30 +1643,30 @@
         <v>4</v>
       </c>
       <c r="B28" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63528</v>
       </c>
       <c r="C28" s="7">
-        <f t="shared" ref="C28" si="20">B28+A28-1</f>
+        <f t="shared" ref="C28" si="12">B28+A28-1</f>
         <v>63531</v>
       </c>
       <c r="D28" s="7" t="str">
-        <f t="shared" ref="D28" si="21">DEC2HEX(B28,4)</f>
-        <v>F828</v>
+        <f t="shared" si="5"/>
+        <v>00F828</v>
       </c>
       <c r="E28" s="7" t="str">
-        <f t="shared" ref="E28" si="22">DEC2HEX(C28,4)</f>
-        <v>F82B</v>
+        <f t="shared" si="6"/>
+        <v>00F82B</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" t="s">
         <v>41</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="I28" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="29" spans="1:14">
@@ -1674,30 +1674,30 @@
         <v>2</v>
       </c>
       <c r="B29" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63532</v>
       </c>
       <c r="C29" s="7">
-        <f t="shared" ref="C29" si="23">B29+A29-1</f>
+        <f t="shared" ref="C29" si="13">B29+A29-1</f>
         <v>63533</v>
       </c>
       <c r="D29" s="7" t="str">
-        <f t="shared" ref="D29" si="24">DEC2HEX(B29,4)</f>
-        <v>F82C</v>
+        <f t="shared" si="5"/>
+        <v>00F82C</v>
       </c>
       <c r="E29" s="7" t="str">
-        <f t="shared" ref="E29" si="25">DEC2HEX(C29,4)</f>
-        <v>F82D</v>
+        <f t="shared" si="6"/>
+        <v>00F82D</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H29" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:14">
@@ -1705,30 +1705,30 @@
         <v>2</v>
       </c>
       <c r="B30" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63536</v>
       </c>
       <c r="C30" s="7">
-        <f t="shared" ref="C30:C31" si="26">B30+A30-1</f>
+        <f t="shared" ref="C30:C31" si="14">B30+A30-1</f>
         <v>63537</v>
       </c>
       <c r="D30" s="7" t="str">
-        <f t="shared" ref="D30:D31" si="27">DEC2HEX(B30,4)</f>
-        <v>F830</v>
+        <f t="shared" si="5"/>
+        <v>00F830</v>
       </c>
       <c r="E30" s="7" t="str">
-        <f t="shared" ref="E30:E31" si="28">DEC2HEX(C30,4)</f>
-        <v>F831</v>
+        <f t="shared" si="6"/>
+        <v>00F831</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I30" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31" spans="1:14">
@@ -1736,30 +1736,30 @@
         <v>1</v>
       </c>
       <c r="B31" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63540</v>
       </c>
       <c r="C31" s="7">
-        <f t="shared" si="26"/>
+        <f t="shared" si="14"/>
         <v>63540</v>
       </c>
       <c r="D31" s="7" t="str">
-        <f t="shared" si="27"/>
-        <v>F834</v>
+        <f t="shared" si="5"/>
+        <v>00F834</v>
       </c>
       <c r="E31" s="7" t="str">
-        <f t="shared" si="28"/>
-        <v>F834</v>
+        <f t="shared" si="6"/>
+        <v>00F834</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I31" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="32" spans="1:14">
@@ -1767,30 +1767,30 @@
         <v>1</v>
       </c>
       <c r="B32" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63544</v>
       </c>
       <c r="C32" s="7">
-        <f t="shared" ref="C32:C34" si="29">B32+A32-1</f>
+        <f t="shared" ref="C32:C34" si="15">B32+A32-1</f>
         <v>63544</v>
       </c>
       <c r="D32" s="7" t="str">
-        <f t="shared" ref="D32:D34" si="30">DEC2HEX(B32,4)</f>
-        <v>F838</v>
+        <f t="shared" si="5"/>
+        <v>00F838</v>
       </c>
       <c r="E32" s="7" t="str">
-        <f t="shared" ref="E32:E34" si="31">DEC2HEX(C32,4)</f>
-        <v>F838</v>
+        <f t="shared" si="6"/>
+        <v>00F838</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I32" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:14">
@@ -1798,30 +1798,30 @@
         <v>1</v>
       </c>
       <c r="B33" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63548</v>
       </c>
       <c r="C33" s="7">
-        <f t="shared" si="29"/>
+        <f t="shared" si="15"/>
         <v>63548</v>
       </c>
       <c r="D33" s="7" t="str">
-        <f t="shared" si="30"/>
-        <v>F83C</v>
+        <f t="shared" si="5"/>
+        <v>00F83C</v>
       </c>
       <c r="E33" s="7" t="str">
-        <f t="shared" si="31"/>
-        <v>F83C</v>
+        <f t="shared" si="6"/>
+        <v>00F83C</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I33" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:14">
@@ -1829,30 +1829,30 @@
         <v>1</v>
       </c>
       <c r="B34" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63552</v>
       </c>
       <c r="C34" s="7">
-        <f t="shared" si="29"/>
+        <f t="shared" si="15"/>
         <v>63552</v>
       </c>
       <c r="D34" s="7" t="str">
-        <f t="shared" si="30"/>
-        <v>F840</v>
+        <f t="shared" si="5"/>
+        <v>00F840</v>
       </c>
       <c r="E34" s="7" t="str">
-        <f t="shared" si="31"/>
-        <v>F840</v>
+        <f t="shared" si="6"/>
+        <v>00F840</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I34" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -1860,30 +1860,30 @@
         <v>1</v>
       </c>
       <c r="B35" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63556</v>
       </c>
       <c r="C35" s="7">
-        <f t="shared" ref="C35" si="32">B35+A35-1</f>
+        <f t="shared" ref="C35" si="16">B35+A35-1</f>
         <v>63556</v>
       </c>
       <c r="D35" s="7" t="str">
-        <f t="shared" ref="D35" si="33">DEC2HEX(B35,4)</f>
-        <v>F844</v>
+        <f t="shared" si="5"/>
+        <v>00F844</v>
       </c>
       <c r="E35" s="7" t="str">
-        <f t="shared" ref="E35" si="34">DEC2HEX(C35,4)</f>
-        <v>F844</v>
+        <f t="shared" si="6"/>
+        <v>00F844</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I35" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -1891,61 +1891,62 @@
         <v>1</v>
       </c>
       <c r="B36" s="7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="8"/>
         <v>63560</v>
       </c>
       <c r="C36" s="7">
-        <f t="shared" ref="C36" si="35">B36+A36-1</f>
+        <f t="shared" ref="C36" si="17">B36+A36-1</f>
         <v>63560</v>
       </c>
       <c r="D36" s="7" t="str">
-        <f t="shared" ref="D36" si="36">DEC2HEX(B36,4)</f>
-        <v>F848</v>
+        <f t="shared" si="5"/>
+        <v>00F848</v>
       </c>
       <c r="E36" s="7" t="str">
-        <f t="shared" ref="E36" si="37">DEC2HEX(C36,4)</f>
-        <v>F848</v>
+        <f t="shared" si="6"/>
+        <v>00F848</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="8" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="37" spans="1:14">
       <c r="A37" s="7">
         <f>C37-B37</f>
-        <v>1971</v>
+        <v>198579</v>
       </c>
       <c r="B37" s="7">
         <f>B36+4</f>
         <v>63564</v>
       </c>
       <c r="C37" s="7">
-        <v>65535</v>
+        <f>A43-1</f>
+        <v>262143</v>
       </c>
       <c r="D37" s="7" t="str">
-        <f t="shared" ref="D37" si="38">DEC2HEX(B37,4)</f>
-        <v>F84C</v>
+        <f t="shared" si="5"/>
+        <v>00F84C</v>
       </c>
       <c r="E37" s="7" t="str">
-        <f t="shared" ref="E37" si="39">DEC2HEX(C37,4)</f>
-        <v>FFFF</v>
+        <f t="shared" si="6"/>
+        <v>03FFFF</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H37" s="34"/>
     </row>
     <row r="39" spans="1:14" s="9" customFormat="1">
       <c r="A39" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D39" s="16"/>
       <c r="E39" s="16"/>
@@ -2027,14 +2028,15 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43" s="7">
-        <v>65536</v>
+        <f>256*1024</f>
+        <v>262144</v>
       </c>
       <c r="B43" s="7">
         <v>0</v>
       </c>
       <c r="C43" s="7">
         <f>A43-1</f>
-        <v>65535</v>
+        <v>262143</v>
       </c>
       <c r="D43" s="7" t="str">
         <f>DEC2HEX(B43,6)</f>
@@ -2042,11 +2044,11 @@
       </c>
       <c r="E43" s="7" t="str">
         <f>DEC2HEX(C43,6)</f>
-        <v>00FFFF</v>
+        <v>03FFFF</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H43" s="34"/>
     </row>
@@ -2056,26 +2058,26 @@
       </c>
       <c r="B44" s="7">
         <f>C43+1</f>
-        <v>65536</v>
+        <v>262144</v>
       </c>
       <c r="C44" s="7">
-        <f t="shared" ref="C44" si="40">B44+A44-1</f>
-        <v>65791</v>
+        <f t="shared" ref="C44" si="18">B44+A44-1</f>
+        <v>262399</v>
       </c>
       <c r="D44" s="7" t="str">
-        <f t="shared" ref="D44:D45" si="41">DEC2HEX(B44,6)</f>
-        <v>010000</v>
+        <f t="shared" ref="D44:D45" si="19">DEC2HEX(B44,6)</f>
+        <v>040000</v>
       </c>
       <c r="E44" s="7" t="str">
-        <f t="shared" ref="E44:E45" si="42">DEC2HEX(C44,6)</f>
-        <v>0100FF</v>
+        <f t="shared" ref="E44:E45" si="20">DEC2HEX(C44,6)</f>
+        <v>0400FF</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -2084,26 +2086,26 @@
       </c>
       <c r="B45" s="7">
         <f>C44+1</f>
-        <v>65792</v>
+        <v>262400</v>
       </c>
       <c r="C45" s="7">
-        <f t="shared" ref="C45" si="43">B45+A45-1</f>
-        <v>66047</v>
+        <f t="shared" ref="C45" si="21">B45+A45-1</f>
+        <v>262655</v>
       </c>
       <c r="D45" s="7" t="str">
-        <f t="shared" si="41"/>
-        <v>010100</v>
+        <f t="shared" si="19"/>
+        <v>040100</v>
       </c>
       <c r="E45" s="7" t="str">
-        <f t="shared" si="42"/>
-        <v>0101FF</v>
+        <f t="shared" si="20"/>
+        <v>0401FF</v>
       </c>
       <c r="F45" s="7"/>
       <c r="G45" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H45" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -2112,26 +2114,26 @@
       </c>
       <c r="B46" s="7">
         <f>C45+1</f>
-        <v>66048</v>
+        <v>262656</v>
       </c>
       <c r="C46" s="7">
-        <f t="shared" ref="C46:C50" si="44">B46+A46-1</f>
-        <v>66303</v>
+        <f t="shared" ref="C46:C50" si="22">B46+A46-1</f>
+        <v>262911</v>
       </c>
       <c r="D46" s="7" t="str">
-        <f t="shared" ref="D46:D52" si="45">DEC2HEX(B46,6)</f>
-        <v>010200</v>
+        <f t="shared" ref="D46:D52" si="23">DEC2HEX(B46,6)</f>
+        <v>040200</v>
       </c>
       <c r="E46" s="7" t="str">
-        <f t="shared" ref="E46:E52" si="46">DEC2HEX(C46,6)</f>
-        <v>0102FF</v>
+        <f t="shared" ref="E46:E52" si="24">DEC2HEX(C46,6)</f>
+        <v>0402FF</v>
       </c>
       <c r="F46" s="7"/>
       <c r="G46" s="8" t="s">
         <v>15</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -2140,26 +2142,26 @@
       </c>
       <c r="B47" s="7">
         <f>C46+1</f>
-        <v>66304</v>
+        <v>262912</v>
       </c>
       <c r="C47" s="7">
-        <f t="shared" si="44"/>
-        <v>66559</v>
+        <f t="shared" si="22"/>
+        <v>263167</v>
       </c>
       <c r="D47" s="7" t="str">
-        <f t="shared" si="45"/>
-        <v>010300</v>
+        <f t="shared" si="23"/>
+        <v>040300</v>
       </c>
       <c r="E47" s="7" t="str">
-        <f t="shared" si="46"/>
-        <v>0103FF</v>
+        <f t="shared" si="24"/>
+        <v>0403FF</v>
       </c>
       <c r="F47" s="7"/>
       <c r="G47" s="8" t="s">
         <v>13</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -2167,27 +2169,27 @@
         <v>256</v>
       </c>
       <c r="B48" s="7">
-        <f t="shared" ref="B48" si="47">C47+1</f>
-        <v>66560</v>
+        <f t="shared" ref="B48" si="25">C47+1</f>
+        <v>263168</v>
       </c>
       <c r="C48" s="7">
-        <f t="shared" si="44"/>
-        <v>66815</v>
+        <f t="shared" si="22"/>
+        <v>263423</v>
       </c>
       <c r="D48" s="7" t="str">
-        <f t="shared" si="45"/>
-        <v>010400</v>
+        <f t="shared" si="23"/>
+        <v>040400</v>
       </c>
       <c r="E48" s="7" t="str">
-        <f t="shared" si="46"/>
-        <v>0104FF</v>
+        <f t="shared" si="24"/>
+        <v>0404FF</v>
       </c>
       <c r="F48" s="7"/>
       <c r="G48" s="8" t="s">
         <v>14</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2195,56 +2197,56 @@
         <v>256</v>
       </c>
       <c r="B49" s="7">
-        <f t="shared" ref="B49" si="48">C48+1</f>
-        <v>66816</v>
+        <f t="shared" ref="B49" si="26">C48+1</f>
+        <v>263424</v>
       </c>
       <c r="C49" s="7">
-        <f t="shared" ref="C49" si="49">B49+A49-1</f>
-        <v>67071</v>
+        <f t="shared" ref="C49" si="27">B49+A49-1</f>
+        <v>263679</v>
       </c>
       <c r="D49" s="7" t="str">
-        <f t="shared" ref="D49" si="50">DEC2HEX(B49,6)</f>
-        <v>010500</v>
+        <f t="shared" ref="D49" si="28">DEC2HEX(B49,6)</f>
+        <v>040500</v>
       </c>
       <c r="E49" s="7" t="str">
-        <f t="shared" ref="E49" si="51">DEC2HEX(C49,6)</f>
-        <v>0105FF</v>
+        <f t="shared" ref="E49" si="29">DEC2HEX(C49,6)</f>
+        <v>0405FF</v>
       </c>
       <c r="F49" s="7"/>
       <c r="G49" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H49" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="50" spans="1:9">
       <c r="A50" s="7">
-        <f>2*(100*75*2)</f>
-        <v>30000</v>
+        <f>2*(128*96*2)</f>
+        <v>49152</v>
       </c>
       <c r="B50" s="7">
         <f>C49+1</f>
-        <v>67072</v>
+        <v>263680</v>
       </c>
       <c r="C50" s="7">
-        <f t="shared" si="44"/>
-        <v>97071</v>
+        <f t="shared" si="22"/>
+        <v>312831</v>
       </c>
       <c r="D50" s="7" t="str">
-        <f t="shared" si="45"/>
-        <v>010600</v>
+        <f t="shared" si="23"/>
+        <v>040600</v>
       </c>
       <c r="E50" s="7" t="str">
-        <f t="shared" si="46"/>
-        <v>017B2F</v>
+        <f t="shared" si="24"/>
+        <v>04C5FF</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="8" t="s">
-        <v>24</v>
+        <v>98</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2253,47 +2255,47 @@
       </c>
       <c r="B51" s="7">
         <f>C50+1</f>
-        <v>97072</v>
+        <v>312832</v>
       </c>
       <c r="C51" s="7">
-        <f t="shared" ref="C51" si="52">B51+A51-1</f>
-        <v>98095</v>
+        <f t="shared" ref="C51" si="30">B51+A51-1</f>
+        <v>313855</v>
       </c>
       <c r="D51" s="7" t="str">
-        <f t="shared" ref="D51" si="53">DEC2HEX(B51,6)</f>
-        <v>017B30</v>
+        <f t="shared" ref="D51" si="31">DEC2HEX(B51,6)</f>
+        <v>04C600</v>
       </c>
       <c r="E51" s="7" t="str">
-        <f t="shared" ref="E51" si="54">DEC2HEX(C51,6)</f>
-        <v>017F2F</v>
+        <f t="shared" ref="E51" si="32">DEC2HEX(C51,6)</f>
+        <v>04C9FF</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H51" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" s="7">
         <f>C52-B52</f>
-        <v>16679119</v>
+        <v>16463359</v>
       </c>
       <c r="B52" s="7">
         <f>C51+1</f>
-        <v>98096</v>
+        <v>313856</v>
       </c>
       <c r="C52" s="7">
         <f>16*1024*1024-1</f>
         <v>16777215</v>
       </c>
       <c r="D52" s="7" t="str">
-        <f t="shared" si="45"/>
-        <v>017F30</v>
+        <f t="shared" si="23"/>
+        <v>04CA00</v>
       </c>
       <c r="E52" s="7" t="str">
-        <f t="shared" si="46"/>
+        <f t="shared" si="24"/>
         <v>FFFFFF</v>
       </c>
       <c r="F52" s="7"/>
@@ -2301,10 +2303,10 @@
         <v>7</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I52" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2317,7 +2319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
@@ -2336,7 +2338,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="21">
       <c r="A1" s="17" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
@@ -2385,7 +2387,7 @@
         <v>0</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I3" s="20"/>
       <c r="J3" s="20"/>
@@ -2468,11 +2470,11 @@
       </c>
       <c r="D6" s="22" t="str">
         <f>'Memory Map'!D21</f>
-        <v>F80C</v>
+        <v>00F80C</v>
       </c>
       <c r="E6" s="22" t="str">
         <f>'Memory Map'!E21</f>
-        <v>F80C</v>
+        <v>00F80C</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="28" t="str">
@@ -2480,22 +2482,22 @@
         <v>Graphics mode</v>
       </c>
       <c r="H6" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I6" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K6" s="25" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="M6" s="36" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N6" s="36"/>
       <c r="O6" s="36"/>
@@ -2549,11 +2551,11 @@
       </c>
       <c r="D9" s="22" t="str">
         <f>'Memory Map'!D25</f>
-        <v>F81C</v>
+        <v>00F81C</v>
       </c>
       <c r="E9" s="22" t="str">
         <f>'Memory Map'!E25</f>
-        <v>F81C</v>
+        <v>00F81C</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="28" t="str">
@@ -2561,28 +2563,28 @@
         <v>RS232 status signals</v>
       </c>
       <c r="H9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="I9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="K9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="L9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="M9" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="O9" s="23" t="s">
         <v>56</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="J9" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="K9" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="L9" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="M9" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="N9" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="O9" s="23" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:15" s="21" customFormat="1">
@@ -2634,11 +2636,11 @@
       </c>
       <c r="D12" s="1" t="str">
         <f>'Memory Map'!D29</f>
-        <v>F82C</v>
+        <v>00F82C</v>
       </c>
       <c r="E12" s="1" t="str">
         <f>'Memory Map'!E29</f>
-        <v>F82D</v>
+        <v>00F82D</v>
       </c>
       <c r="F12">
         <f>'Memory Map'!F29</f>
@@ -2649,28 +2651,28 @@
         <v>IRQ mask</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K12" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="L12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="M12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="N12" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="O12" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -2703,7 +2705,7 @@
     <row r="14" spans="1:15">
       <c r="G14" s="2"/>
       <c r="H14" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:15">
@@ -2728,39 +2730,39 @@
       </c>
       <c r="D17" s="22" t="str">
         <f>'Memory Map'!D33</f>
-        <v>F83C</v>
+        <v>00F83C</v>
       </c>
       <c r="E17" s="22" t="str">
         <f>'Memory Map'!E33</f>
-        <v>F83C</v>
+        <v>00F83C</v>
       </c>
       <c r="G17" s="29" t="str">
         <f>'Memory Map'!G33</f>
         <v>SPI control</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J17" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K17" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L17" s="21" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="M17" s="21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N17" s="21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:15">
@@ -2796,44 +2798,44 @@
       </c>
       <c r="D20" s="22" t="str">
         <f>'Memory Map'!D34</f>
-        <v>F840</v>
+        <v>00F840</v>
       </c>
       <c r="E20" s="22" t="str">
         <f>'Memory Map'!E34</f>
-        <v>F840</v>
+        <v>00F840</v>
       </c>
       <c r="G20" s="2" t="str">
         <f>'Memory Map'!G34</f>
         <v>SPI status</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="J20" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K20" s="24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L20" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="M20" s="24" t="s">
+        <v>88</v>
+      </c>
+      <c r="N20" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="M20" s="24" t="s">
+      <c r="O20" s="21" t="s">
         <v>90</v>
-      </c>
-      <c r="N20" s="21" t="s">
-        <v>91</v>
-      </c>
-      <c r="O20" s="21" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:15">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2860,12 +2862,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="21" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="21" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:1">
@@ -2873,27 +2875,27 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="30">
       <c r="A6" s="21" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:1">
       <c r="A7" s="21" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="45">
       <c r="A8" s="35" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:1">
@@ -2901,7 +2903,7 @@
     </row>
     <row r="10" spans="1:1" ht="60">
       <c r="A10" s="35" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added selectable VGA clock Expanded SRAM to 128KB Moved hardware registers and updated FORTH.asm Registered FPGA outputs to improve timing
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -956,7 +956,7 @@
   <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1063,15 +1063,15 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" s="7">
-        <f>(64-10)*1024</f>
-        <v>55296</v>
+        <f>(128)*1024</f>
+        <v>131072</v>
       </c>
       <c r="B7" s="7">
         <v>0</v>
       </c>
       <c r="C7" s="7">
         <f>B7+A7-1</f>
-        <v>55295</v>
+        <v>131071</v>
       </c>
       <c r="D7" s="7" t="str">
         <f>DEC2HEX(B7,6)</f>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="E7" s="7" t="str">
         <f>DEC2HEX(C7,6)</f>
-        <v>00D7FF</v>
+        <v>01FFFF</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8" t="s">
@@ -1094,23 +1094,24 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" s="7">
-        <v>0</v>
+        <f>(128-10)*1024</f>
+        <v>120832</v>
       </c>
       <c r="B8" s="7">
         <f>C7+1</f>
-        <v>55296</v>
+        <v>131072</v>
       </c>
       <c r="C8" s="7">
         <f>B8+A8-1</f>
-        <v>55295</v>
+        <v>251903</v>
       </c>
       <c r="D8" s="7" t="str">
         <f t="shared" ref="D8" si="0">DEC2HEX(B8,6)</f>
-        <v>00D800</v>
+        <v>020000</v>
       </c>
       <c r="E8" s="7" t="str">
         <f t="shared" ref="E8" si="1">DEC2HEX(C8,6)</f>
-        <v>00D7FF</v>
+        <v>03D7FF</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8" t="s">
@@ -1123,19 +1124,19 @@
       </c>
       <c r="B9" s="7">
         <f>C8+1</f>
-        <v>55296</v>
+        <v>251904</v>
       </c>
       <c r="C9" s="7">
         <f>B9+A9-1</f>
-        <v>57343</v>
+        <v>253951</v>
       </c>
       <c r="D9" s="7" t="str">
         <f t="shared" ref="D9:D12" si="2">DEC2HEX(B9,6)</f>
-        <v>00D800</v>
+        <v>03D800</v>
       </c>
       <c r="E9" s="7" t="str">
         <f t="shared" ref="E9:E12" si="3">DEC2HEX(C9,6)</f>
-        <v>00DFFF</v>
+        <v>03DFFF</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8" t="s">
@@ -1155,19 +1156,19 @@
       </c>
       <c r="B10" s="7">
         <f>C9+1</f>
-        <v>57344</v>
+        <v>253952</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10:C12" si="4">B10+A10-1</f>
-        <v>59391</v>
+        <v>255999</v>
       </c>
       <c r="D10" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>00E000</v>
+        <v>03E000</v>
       </c>
       <c r="E10" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00E7FF</v>
+        <v>03E7FF</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8" t="s">
@@ -1187,19 +1188,19 @@
       </c>
       <c r="B11" s="7">
         <f>C10+1</f>
-        <v>59392</v>
+        <v>256000</v>
       </c>
       <c r="C11" s="7">
         <f t="shared" si="4"/>
-        <v>61439</v>
+        <v>258047</v>
       </c>
       <c r="D11" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>00E800</v>
+        <v>03E800</v>
       </c>
       <c r="E11" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00EFFF</v>
+        <v>03EFFF</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8" t="s">
@@ -1218,19 +1219,19 @@
       </c>
       <c r="B12" s="7">
         <f>C11+1</f>
-        <v>61440</v>
+        <v>258048</v>
       </c>
       <c r="C12" s="7">
         <f t="shared" si="4"/>
-        <v>63487</v>
+        <v>260095</v>
       </c>
       <c r="D12" s="7" t="str">
         <f t="shared" si="2"/>
-        <v>00F000</v>
+        <v>03F000</v>
       </c>
       <c r="E12" s="7" t="str">
         <f t="shared" si="3"/>
-        <v>00F7FF</v>
+        <v>03F7FF</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="8" t="s">
@@ -1334,19 +1335,19 @@
       </c>
       <c r="B18" s="7">
         <f>C12+1</f>
-        <v>63488</v>
+        <v>260096</v>
       </c>
       <c r="C18" s="7">
         <f>B18+A18-1</f>
-        <v>63491</v>
+        <v>260099</v>
       </c>
       <c r="D18" s="7" t="str">
         <f t="shared" ref="D18:D37" si="5">DEC2HEX(B18,6)</f>
-        <v>00F800</v>
+        <v>03F800</v>
       </c>
       <c r="E18" s="7" t="str">
         <f t="shared" ref="E18:E37" si="6">DEC2HEX(C18,6)</f>
-        <v>00F803</v>
+        <v>03F803</v>
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8" t="s">
@@ -1365,19 +1366,19 @@
       </c>
       <c r="B19" s="7">
         <f>B18+4</f>
-        <v>63492</v>
+        <v>260100</v>
       </c>
       <c r="C19" s="7">
         <f t="shared" ref="C19" si="7">B19+A19-1</f>
-        <v>63495</v>
+        <v>260103</v>
       </c>
       <c r="D19" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F804</v>
+        <v>03F804</v>
       </c>
       <c r="E19" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F807</v>
+        <v>03F807</v>
       </c>
       <c r="F19" s="7"/>
       <c r="G19" s="8" t="s">
@@ -1396,19 +1397,19 @@
       </c>
       <c r="B20" s="7">
         <f t="shared" ref="B20:B36" si="8">B19+4</f>
-        <v>63496</v>
+        <v>260104</v>
       </c>
       <c r="C20" s="7">
         <f t="shared" ref="C20:C23" si="9">B20+A20-1</f>
-        <v>63496</v>
+        <v>260104</v>
       </c>
       <c r="D20" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F808</v>
+        <v>03F808</v>
       </c>
       <c r="E20" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F808</v>
+        <v>03F808</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="8" t="s">
@@ -1427,19 +1428,19 @@
       </c>
       <c r="B21" s="7">
         <f t="shared" si="8"/>
-        <v>63500</v>
+        <v>260108</v>
       </c>
       <c r="C21" s="7">
         <f t="shared" si="9"/>
-        <v>63500</v>
+        <v>260108</v>
       </c>
       <c r="D21" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F80C</v>
+        <v>03F80C</v>
       </c>
       <c r="E21" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F80C</v>
+        <v>03F80C</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="8" t="s">
@@ -1458,19 +1459,19 @@
       </c>
       <c r="B22" s="7">
         <f t="shared" si="8"/>
-        <v>63504</v>
+        <v>260112</v>
       </c>
       <c r="C22" s="7">
         <f t="shared" si="9"/>
-        <v>63504</v>
+        <v>260112</v>
       </c>
       <c r="D22" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F810</v>
+        <v>03F810</v>
       </c>
       <c r="E22" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F810</v>
+        <v>03F810</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8" t="s">
@@ -1489,19 +1490,19 @@
       </c>
       <c r="B23" s="7">
         <f t="shared" si="8"/>
-        <v>63508</v>
+        <v>260116</v>
       </c>
       <c r="C23" s="7">
         <f t="shared" si="9"/>
-        <v>63508</v>
+        <v>260116</v>
       </c>
       <c r="D23" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F814</v>
+        <v>03F814</v>
       </c>
       <c r="E23" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F814</v>
+        <v>03F814</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8" t="s">
@@ -1520,19 +1521,19 @@
       </c>
       <c r="B24" s="7">
         <f t="shared" si="8"/>
-        <v>63512</v>
+        <v>260120</v>
       </c>
       <c r="C24" s="7">
         <f t="shared" ref="C24:C26" si="10">B24+A24-1</f>
-        <v>63513</v>
+        <v>260121</v>
       </c>
       <c r="D24" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F818</v>
+        <v>03F818</v>
       </c>
       <c r="E24" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F819</v>
+        <v>03F819</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8" t="s">
@@ -1551,19 +1552,19 @@
       </c>
       <c r="B25" s="7">
         <f t="shared" si="8"/>
-        <v>63516</v>
+        <v>260124</v>
       </c>
       <c r="C25" s="7">
         <f>B25+A25-1</f>
-        <v>63516</v>
+        <v>260124</v>
       </c>
       <c r="D25" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F81C</v>
+        <v>03F81C</v>
       </c>
       <c r="E25" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F81C</v>
+        <v>03F81C</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8" t="s">
@@ -1582,19 +1583,19 @@
       </c>
       <c r="B26" s="7">
         <f t="shared" si="8"/>
-        <v>63520</v>
+        <v>260128</v>
       </c>
       <c r="C26" s="7">
         <f t="shared" si="10"/>
-        <v>63520</v>
+        <v>260128</v>
       </c>
       <c r="D26" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F820</v>
+        <v>03F820</v>
       </c>
       <c r="E26" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F820</v>
+        <v>03F820</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
@@ -1613,19 +1614,19 @@
       </c>
       <c r="B27" s="7">
         <f t="shared" si="8"/>
-        <v>63524</v>
+        <v>260132</v>
       </c>
       <c r="C27" s="7">
         <f t="shared" ref="C27" si="11">B27+A27-1</f>
-        <v>63527</v>
+        <v>260135</v>
       </c>
       <c r="D27" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F824</v>
+        <v>03F824</v>
       </c>
       <c r="E27" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F827</v>
+        <v>03F827</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8" t="s">
@@ -1644,19 +1645,19 @@
       </c>
       <c r="B28" s="7">
         <f t="shared" si="8"/>
-        <v>63528</v>
+        <v>260136</v>
       </c>
       <c r="C28" s="7">
         <f t="shared" ref="C28" si="12">B28+A28-1</f>
-        <v>63531</v>
+        <v>260139</v>
       </c>
       <c r="D28" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F828</v>
+        <v>03F828</v>
       </c>
       <c r="E28" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F82B</v>
+        <v>03F82B</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8" t="s">
@@ -1675,19 +1676,19 @@
       </c>
       <c r="B29" s="7">
         <f t="shared" si="8"/>
-        <v>63532</v>
+        <v>260140</v>
       </c>
       <c r="C29" s="7">
         <f t="shared" ref="C29" si="13">B29+A29-1</f>
-        <v>63533</v>
+        <v>260141</v>
       </c>
       <c r="D29" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F82C</v>
+        <v>03F82C</v>
       </c>
       <c r="E29" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F82D</v>
+        <v>03F82D</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8" t="s">
@@ -1706,19 +1707,19 @@
       </c>
       <c r="B30" s="7">
         <f t="shared" si="8"/>
-        <v>63536</v>
+        <v>260144</v>
       </c>
       <c r="C30" s="7">
         <f t="shared" ref="C30:C31" si="14">B30+A30-1</f>
-        <v>63537</v>
+        <v>260145</v>
       </c>
       <c r="D30" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F830</v>
+        <v>03F830</v>
       </c>
       <c r="E30" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F831</v>
+        <v>03F831</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8" t="s">
@@ -1737,19 +1738,19 @@
       </c>
       <c r="B31" s="7">
         <f t="shared" si="8"/>
-        <v>63540</v>
+        <v>260148</v>
       </c>
       <c r="C31" s="7">
         <f t="shared" si="14"/>
-        <v>63540</v>
+        <v>260148</v>
       </c>
       <c r="D31" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F834</v>
+        <v>03F834</v>
       </c>
       <c r="E31" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F834</v>
+        <v>03F834</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8" t="s">
@@ -1768,19 +1769,19 @@
       </c>
       <c r="B32" s="7">
         <f t="shared" si="8"/>
-        <v>63544</v>
+        <v>260152</v>
       </c>
       <c r="C32" s="7">
         <f t="shared" ref="C32:C34" si="15">B32+A32-1</f>
-        <v>63544</v>
+        <v>260152</v>
       </c>
       <c r="D32" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F838</v>
+        <v>03F838</v>
       </c>
       <c r="E32" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F838</v>
+        <v>03F838</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="8" t="s">
@@ -1799,19 +1800,19 @@
       </c>
       <c r="B33" s="7">
         <f t="shared" si="8"/>
-        <v>63548</v>
+        <v>260156</v>
       </c>
       <c r="C33" s="7">
         <f t="shared" si="15"/>
-        <v>63548</v>
+        <v>260156</v>
       </c>
       <c r="D33" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F83C</v>
+        <v>03F83C</v>
       </c>
       <c r="E33" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F83C</v>
+        <v>03F83C</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="8" t="s">
@@ -1830,19 +1831,19 @@
       </c>
       <c r="B34" s="7">
         <f t="shared" si="8"/>
-        <v>63552</v>
+        <v>260160</v>
       </c>
       <c r="C34" s="7">
         <f t="shared" si="15"/>
-        <v>63552</v>
+        <v>260160</v>
       </c>
       <c r="D34" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F840</v>
+        <v>03F840</v>
       </c>
       <c r="E34" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F840</v>
+        <v>03F840</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8" t="s">
@@ -1861,19 +1862,19 @@
       </c>
       <c r="B35" s="7">
         <f t="shared" si="8"/>
-        <v>63556</v>
+        <v>260164</v>
       </c>
       <c r="C35" s="7">
         <f t="shared" ref="C35" si="16">B35+A35-1</f>
-        <v>63556</v>
+        <v>260164</v>
       </c>
       <c r="D35" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F844</v>
+        <v>03F844</v>
       </c>
       <c r="E35" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F844</v>
+        <v>03F844</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8" t="s">
@@ -1892,19 +1893,19 @@
       </c>
       <c r="B36" s="7">
         <f t="shared" si="8"/>
-        <v>63560</v>
+        <v>260168</v>
       </c>
       <c r="C36" s="7">
         <f t="shared" ref="C36" si="17">B36+A36-1</f>
-        <v>63560</v>
+        <v>260168</v>
       </c>
       <c r="D36" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F848</v>
+        <v>03F848</v>
       </c>
       <c r="E36" s="7" t="str">
         <f t="shared" si="6"/>
-        <v>00F848</v>
+        <v>03F848</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="8" t="s">
@@ -1920,11 +1921,11 @@
     <row r="37" spans="1:14">
       <c r="A37" s="7">
         <f>C37-B37</f>
-        <v>198579</v>
+        <v>1971</v>
       </c>
       <c r="B37" s="7">
         <f>B36+4</f>
-        <v>63564</v>
+        <v>260172</v>
       </c>
       <c r="C37" s="7">
         <f>A43-1</f>
@@ -1932,7 +1933,7 @@
       </c>
       <c r="D37" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>00F84C</v>
+        <v>03F84C</v>
       </c>
       <c r="E37" s="7" t="str">
         <f t="shared" si="6"/>
@@ -2462,19 +2463,19 @@
       </c>
       <c r="B6" s="22">
         <f>'Memory Map'!B21</f>
-        <v>63500</v>
+        <v>260108</v>
       </c>
       <c r="C6" s="22">
         <f>'Memory Map'!C21</f>
-        <v>63500</v>
+        <v>260108</v>
       </c>
       <c r="D6" s="22" t="str">
         <f>'Memory Map'!D21</f>
-        <v>00F80C</v>
+        <v>03F80C</v>
       </c>
       <c r="E6" s="22" t="str">
         <f>'Memory Map'!E21</f>
-        <v>00F80C</v>
+        <v>03F80C</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="28" t="str">
@@ -2543,19 +2544,19 @@
       </c>
       <c r="B9" s="22">
         <f>'Memory Map'!B25</f>
-        <v>63516</v>
+        <v>260124</v>
       </c>
       <c r="C9" s="22">
         <f>'Memory Map'!C25</f>
-        <v>63516</v>
+        <v>260124</v>
       </c>
       <c r="D9" s="22" t="str">
         <f>'Memory Map'!D25</f>
-        <v>00F81C</v>
+        <v>03F81C</v>
       </c>
       <c r="E9" s="22" t="str">
         <f>'Memory Map'!E25</f>
-        <v>00F81C</v>
+        <v>03F81C</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="28" t="str">
@@ -2628,19 +2629,19 @@
       </c>
       <c r="B12" s="1">
         <f>'Memory Map'!B29</f>
-        <v>63532</v>
+        <v>260140</v>
       </c>
       <c r="C12" s="1">
         <f>'Memory Map'!C29</f>
-        <v>63533</v>
+        <v>260141</v>
       </c>
       <c r="D12" s="1" t="str">
         <f>'Memory Map'!D29</f>
-        <v>00F82C</v>
+        <v>03F82C</v>
       </c>
       <c r="E12" s="1" t="str">
         <f>'Memory Map'!E29</f>
-        <v>00F82D</v>
+        <v>03F82D</v>
       </c>
       <c r="F12">
         <f>'Memory Map'!F29</f>
@@ -2722,19 +2723,19 @@
       </c>
       <c r="B17" s="22">
         <f>'Memory Map'!B33</f>
-        <v>63548</v>
+        <v>260156</v>
       </c>
       <c r="C17" s="22">
         <f>'Memory Map'!C33</f>
-        <v>63548</v>
+        <v>260156</v>
       </c>
       <c r="D17" s="22" t="str">
         <f>'Memory Map'!D33</f>
-        <v>00F83C</v>
+        <v>03F83C</v>
       </c>
       <c r="E17" s="22" t="str">
         <f>'Memory Map'!E33</f>
-        <v>00F83C</v>
+        <v>03F83C</v>
       </c>
       <c r="G17" s="29" t="str">
         <f>'Memory Map'!G33</f>
@@ -2790,19 +2791,19 @@
       </c>
       <c r="B20" s="22">
         <f>'Memory Map'!B34</f>
-        <v>63552</v>
+        <v>260160</v>
       </c>
       <c r="C20" s="22">
         <f>'Memory Map'!C34</f>
-        <v>63552</v>
+        <v>260160</v>
       </c>
       <c r="D20" s="22" t="str">
         <f>'Memory Map'!D34</f>
-        <v>00F840</v>
+        <v>03F840</v>
       </c>
       <c r="E20" s="22" t="str">
         <f>'Memory Map'!E34</f>
-        <v>00F840</v>
+        <v>03F840</v>
       </c>
       <c r="G20" s="2" t="str">
         <f>'Memory Map'!G34</f>

</xml_diff>

<commit_message>
Working version of N.I.G.E. with new return stack model - THROW will cancel interrupt status if called within an interrup handler - Updated system software to use CATCH and THROW - Improved timing by including some path registers - Reordered memory regions to place access to subroutine and exception stacks in a more logical order
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545"/>
@@ -11,7 +11,7 @@
     <sheet name="Hardware registers" sheetId="2" r:id="rId2"/>
     <sheet name="Copyright and license" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -455,17 +455,17 @@
     <t>Reserved for expansion</t>
   </si>
   <si>
-    <t>Stack access</t>
-  </si>
-  <si>
     <t>Access to subroutine and exception stacks</t>
+  </si>
+  <si>
+    <t>Subroutine and exception stacks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,7 +746,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -781,7 +780,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -957,22 +955,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="5" width="12.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="31.28515625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" style="8" customWidth="1"/>
     <col min="8" max="8" width="10.140625" style="30" customWidth="1"/>
     <col min="9" max="9" width="79.140625" customWidth="1"/>
     <col min="10" max="12" width="19.140625" customWidth="1"/>
@@ -980,27 +978,25 @@
     <col min="14" max="14" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="21">
       <c r="A1" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" s="9" customFormat="1">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
-      <c r="H3" s="31"/>
-      <c r="I3"/>
       <c r="J3"/>
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -1030,7 +1026,7 @@
       <c r="M4"/>
       <c r="N4"/>
     </row>
-    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
       <c r="A5" s="13"/>
       <c r="B5" s="13" t="s">
         <v>8</v>
@@ -1053,7 +1049,7 @@
       <c r="M5"/>
       <c r="N5"/>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1069,7 +1065,7 @@
       <c r="M6"/>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14">
       <c r="A7" s="7">
         <f>(128)*1024</f>
         <v>131072</v>
@@ -1100,13 +1096,13 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14">
       <c r="A8" s="7">
         <f>(128-12)*1024</f>
         <v>118784</v>
       </c>
       <c r="B8" s="7">
-        <f>C7+1</f>
+        <f t="shared" ref="B8:B13" si="0">C7+1</f>
         <v>131072</v>
       </c>
       <c r="C8" s="7">
@@ -1114,11 +1110,11 @@
         <v>249855</v>
       </c>
       <c r="D8" s="7" t="str">
-        <f t="shared" ref="D8:D9" si="0">DEC2HEX(B8,6)</f>
+        <f t="shared" ref="D8:D9" si="1">DEC2HEX(B8,6)</f>
         <v>020000</v>
       </c>
       <c r="E8" s="7" t="str">
-        <f t="shared" ref="E8:E9" si="1">DEC2HEX(C8,6)</f>
+        <f t="shared" ref="E8:E9" si="2">DEC2HEX(C8,6)</f>
         <v>03CFFF</v>
       </c>
       <c r="F8" s="7"/>
@@ -1126,43 +1122,43 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14">
       <c r="A9" s="7">
         <v>2048</v>
       </c>
       <c r="B9" s="7">
-        <f>C8+1</f>
+        <f t="shared" si="0"/>
         <v>249856</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" ref="C9" si="2">B9+A9-1</f>
+        <f t="shared" ref="C9" si="3">B9+A9-1</f>
         <v>251903</v>
       </c>
       <c r="D9" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03D000</v>
       </c>
       <c r="E9" s="7" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>03D7FF</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8" t="s">
-        <v>100</v>
+        <v>4</v>
       </c>
       <c r="H9" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
       <c r="A10" s="7">
         <v>2048</v>
       </c>
       <c r="B10" s="7">
-        <f>C9+1</f>
+        <f t="shared" si="0"/>
         <v>251904</v>
       </c>
       <c r="C10" s="7">
@@ -1170,11 +1166,11 @@
         <v>253951</v>
       </c>
       <c r="D10" s="7" t="str">
-        <f t="shared" ref="D10:D13" si="3">DEC2HEX(B10,6)</f>
+        <f t="shared" ref="D10:D13" si="4">DEC2HEX(B10,6)</f>
         <v>03D800</v>
       </c>
       <c r="E10" s="7" t="str">
-        <f t="shared" ref="E10:E13" si="4">DEC2HEX(C10,6)</f>
+        <f t="shared" ref="E10:E13" si="5">DEC2HEX(C10,6)</f>
         <v>03DFFF</v>
       </c>
       <c r="F10" s="7"/>
@@ -1188,25 +1184,25 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14">
       <c r="A11" s="7">
         <f>2048</f>
         <v>2048</v>
       </c>
       <c r="B11" s="7">
-        <f>C10+1</f>
+        <f t="shared" si="0"/>
         <v>253952</v>
       </c>
       <c r="C11" s="7">
-        <f t="shared" ref="C11:C13" si="5">B11+A11-1</f>
+        <f t="shared" ref="C11:C13" si="6">B11+A11-1</f>
         <v>255999</v>
       </c>
       <c r="D11" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>03E000</v>
       </c>
       <c r="E11" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>03E7FF</v>
       </c>
       <c r="F11" s="7"/>
@@ -1220,25 +1216,25 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14">
       <c r="A12" s="7">
         <f>2048</f>
         <v>2048</v>
       </c>
       <c r="B12" s="7">
-        <f>C11+1</f>
+        <f t="shared" si="0"/>
         <v>256000</v>
       </c>
       <c r="C12" s="7">
+        <f t="shared" si="6"/>
+        <v>258047</v>
+      </c>
+      <c r="D12" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>03E800</v>
+      </c>
+      <c r="E12" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>258047</v>
-      </c>
-      <c r="D12" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>03E800</v>
-      </c>
-      <c r="E12" s="7" t="str">
-        <f t="shared" si="4"/>
         <v>03EFFF</v>
       </c>
       <c r="F12" s="7"/>
@@ -1252,41 +1248,41 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14">
       <c r="A13" s="7">
         <v>2048</v>
       </c>
       <c r="B13" s="7">
-        <f>C12+1</f>
+        <f t="shared" si="0"/>
         <v>258048</v>
       </c>
       <c r="C13" s="7">
+        <f t="shared" si="6"/>
+        <v>260095</v>
+      </c>
+      <c r="D13" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>03F000</v>
+      </c>
+      <c r="E13" s="7" t="str">
         <f t="shared" si="5"/>
-        <v>260095</v>
-      </c>
-      <c r="D13" s="7" t="str">
-        <f t="shared" si="3"/>
-        <v>03F000</v>
-      </c>
-      <c r="E13" s="7" t="str">
-        <f t="shared" si="4"/>
         <v>03F7FF</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="H13" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I13" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="9" customFormat="1">
       <c r="A15" s="14" t="s">
         <v>50</v>
       </c>
@@ -1301,7 +1297,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="10" customFormat="1">
       <c r="A16" s="13" t="s">
         <v>6</v>
       </c>
@@ -1329,7 +1325,7 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="11" customFormat="1">
       <c r="A17" s="15"/>
       <c r="B17" s="13" t="s">
         <v>8</v>
@@ -1352,7 +1348,7 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="2" customFormat="1">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1368,7 +1364,7 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14">
       <c r="A19" s="7">
         <v>4</v>
       </c>
@@ -1381,11 +1377,11 @@
         <v>260099</v>
       </c>
       <c r="D19" s="7" t="str">
-        <f t="shared" ref="D19:D38" si="6">DEC2HEX(B19,6)</f>
+        <f t="shared" ref="D19:D38" si="7">DEC2HEX(B19,6)</f>
         <v>03F800</v>
       </c>
       <c r="E19" s="7" t="str">
-        <f t="shared" ref="E19:E38" si="7">DEC2HEX(C19,6)</f>
+        <f t="shared" ref="E19:E38" si="8">DEC2HEX(C19,6)</f>
         <v>03F803</v>
       </c>
       <c r="F19" s="7"/>
@@ -1399,7 +1395,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14">
       <c r="A20" s="7">
         <v>4</v>
       </c>
@@ -1408,15 +1404,15 @@
         <v>260100</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" ref="C20" si="8">B20+A20-1</f>
+        <f t="shared" ref="C20" si="9">B20+A20-1</f>
         <v>260103</v>
       </c>
       <c r="D20" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F804</v>
       </c>
       <c r="E20" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F807</v>
       </c>
       <c r="F20" s="7"/>
@@ -1430,24 +1426,24 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14">
       <c r="A21" s="7">
         <v>1</v>
       </c>
       <c r="B21" s="7">
-        <f t="shared" ref="B21:B37" si="9">B20+4</f>
+        <f t="shared" ref="B21:B37" si="10">B20+4</f>
         <v>260104</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" ref="C21:C24" si="10">B21+A21-1</f>
+        <f t="shared" ref="C21:C24" si="11">B21+A21-1</f>
         <v>260104</v>
       </c>
       <c r="D21" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F808</v>
       </c>
       <c r="E21" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F808</v>
       </c>
       <c r="F21" s="7"/>
@@ -1461,24 +1457,24 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14">
       <c r="A22" s="7">
         <v>1</v>
       </c>
       <c r="B22" s="7">
-        <f t="shared" si="9"/>
-        <v>260108</v>
-      </c>
-      <c r="C22" s="7">
         <f t="shared" si="10"/>
         <v>260108</v>
       </c>
+      <c r="C22" s="7">
+        <f t="shared" si="11"/>
+        <v>260108</v>
+      </c>
       <c r="D22" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F80C</v>
       </c>
       <c r="E22" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F80C</v>
       </c>
       <c r="F22" s="7"/>
@@ -1492,24 +1488,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14">
       <c r="A23" s="7">
         <v>1</v>
       </c>
       <c r="B23" s="7">
-        <f t="shared" si="9"/>
-        <v>260112</v>
-      </c>
-      <c r="C23" s="7">
         <f t="shared" si="10"/>
         <v>260112</v>
       </c>
+      <c r="C23" s="7">
+        <f t="shared" si="11"/>
+        <v>260112</v>
+      </c>
       <c r="D23" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F810</v>
       </c>
       <c r="E23" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F810</v>
       </c>
       <c r="F23" s="7"/>
@@ -1523,24 +1519,24 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14">
       <c r="A24" s="7">
         <v>1</v>
       </c>
       <c r="B24" s="7">
-        <f t="shared" si="9"/>
-        <v>260116</v>
-      </c>
-      <c r="C24" s="7">
         <f t="shared" si="10"/>
         <v>260116</v>
       </c>
+      <c r="C24" s="7">
+        <f t="shared" si="11"/>
+        <v>260116</v>
+      </c>
       <c r="D24" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F814</v>
       </c>
       <c r="E24" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F814</v>
       </c>
       <c r="F24" s="7"/>
@@ -1554,24 +1550,24 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14">
       <c r="A25" s="7">
         <v>2</v>
       </c>
       <c r="B25" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260120</v>
       </c>
       <c r="C25" s="7">
-        <f t="shared" ref="C25:C27" si="11">B25+A25-1</f>
+        <f t="shared" ref="C25:C27" si="12">B25+A25-1</f>
         <v>260121</v>
       </c>
       <c r="D25" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F818</v>
       </c>
       <c r="E25" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F819</v>
       </c>
       <c r="F25" s="7"/>
@@ -1585,12 +1581,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14">
       <c r="A26" s="7">
         <v>1</v>
       </c>
       <c r="B26" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260124</v>
       </c>
       <c r="C26" s="7">
@@ -1598,11 +1594,11 @@
         <v>260124</v>
       </c>
       <c r="D26" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F81C</v>
       </c>
       <c r="E26" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F81C</v>
       </c>
       <c r="F26" s="7"/>
@@ -1616,24 +1612,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14">
       <c r="A27" s="7">
         <v>1</v>
       </c>
       <c r="B27" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260128</v>
       </c>
       <c r="C27" s="7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>260128</v>
       </c>
       <c r="D27" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F820</v>
       </c>
       <c r="E27" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F820</v>
       </c>
       <c r="F27" s="7"/>
@@ -1647,24 +1643,24 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14">
       <c r="A28" s="7">
         <v>4</v>
       </c>
       <c r="B28" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260132</v>
       </c>
       <c r="C28" s="7">
-        <f t="shared" ref="C28" si="12">B28+A28-1</f>
+        <f t="shared" ref="C28" si="13">B28+A28-1</f>
         <v>260135</v>
       </c>
       <c r="D28" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F824</v>
       </c>
       <c r="E28" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F827</v>
       </c>
       <c r="F28" s="7"/>
@@ -1678,24 +1674,24 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14">
       <c r="A29" s="7">
         <v>4</v>
       </c>
       <c r="B29" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260136</v>
       </c>
       <c r="C29" s="7">
-        <f t="shared" ref="C29" si="13">B29+A29-1</f>
+        <f t="shared" ref="C29" si="14">B29+A29-1</f>
         <v>260139</v>
       </c>
       <c r="D29" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F828</v>
       </c>
       <c r="E29" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F82B</v>
       </c>
       <c r="F29" s="7"/>
@@ -1709,24 +1705,24 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14">
       <c r="A30" s="7">
         <v>2</v>
       </c>
       <c r="B30" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260140</v>
       </c>
       <c r="C30" s="7">
-        <f t="shared" ref="C30" si="14">B30+A30-1</f>
+        <f t="shared" ref="C30" si="15">B30+A30-1</f>
         <v>260141</v>
       </c>
       <c r="D30" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F82C</v>
       </c>
       <c r="E30" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F82D</v>
       </c>
       <c r="F30" s="7"/>
@@ -1740,24 +1736,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14">
       <c r="A31" s="7">
         <v>2</v>
       </c>
       <c r="B31" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260144</v>
       </c>
       <c r="C31" s="7">
-        <f t="shared" ref="C31:C32" si="15">B31+A31-1</f>
+        <f t="shared" ref="C31:C32" si="16">B31+A31-1</f>
         <v>260145</v>
       </c>
       <c r="D31" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F830</v>
       </c>
       <c r="E31" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F831</v>
       </c>
       <c r="F31" s="7"/>
@@ -1771,24 +1767,24 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14">
       <c r="A32" s="7">
         <v>1</v>
       </c>
       <c r="B32" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260148</v>
       </c>
       <c r="C32" s="7">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>260148</v>
       </c>
       <c r="D32" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F834</v>
       </c>
       <c r="E32" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F834</v>
       </c>
       <c r="F32" s="7"/>
@@ -1802,24 +1798,24 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14">
       <c r="A33" s="7">
         <v>1</v>
       </c>
       <c r="B33" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260152</v>
       </c>
       <c r="C33" s="7">
-        <f t="shared" ref="C33:C35" si="16">B33+A33-1</f>
+        <f t="shared" ref="C33:C35" si="17">B33+A33-1</f>
         <v>260152</v>
       </c>
       <c r="D33" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F838</v>
       </c>
       <c r="E33" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F838</v>
       </c>
       <c r="F33" s="7"/>
@@ -1833,24 +1829,24 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14">
       <c r="A34" s="7">
         <v>1</v>
       </c>
       <c r="B34" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260156</v>
       </c>
       <c r="C34" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>260156</v>
       </c>
       <c r="D34" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F83C</v>
       </c>
       <c r="E34" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F83C</v>
       </c>
       <c r="F34" s="7"/>
@@ -1864,24 +1860,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14">
       <c r="A35" s="7">
         <v>1</v>
       </c>
       <c r="B35" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260160</v>
       </c>
       <c r="C35" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>260160</v>
       </c>
       <c r="D35" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F840</v>
       </c>
       <c r="E35" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F840</v>
       </c>
       <c r="F35" s="7"/>
@@ -1895,24 +1891,24 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14">
       <c r="A36" s="7">
         <v>1</v>
       </c>
       <c r="B36" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260164</v>
       </c>
       <c r="C36" s="7">
-        <f t="shared" ref="C36" si="17">B36+A36-1</f>
+        <f t="shared" ref="C36" si="18">B36+A36-1</f>
         <v>260164</v>
       </c>
       <c r="D36" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F844</v>
       </c>
       <c r="E36" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F844</v>
       </c>
       <c r="F36" s="7"/>
@@ -1926,24 +1922,24 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14">
       <c r="A37" s="7">
         <v>1</v>
       </c>
       <c r="B37" s="7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>260168</v>
       </c>
       <c r="C37" s="7">
-        <f t="shared" ref="C37" si="18">B37+A37-1</f>
+        <f t="shared" ref="C37" si="19">B37+A37-1</f>
         <v>260168</v>
       </c>
       <c r="D37" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F848</v>
       </c>
       <c r="E37" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03F848</v>
       </c>
       <c r="F37" s="7"/>
@@ -1957,7 +1953,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14">
       <c r="A38" s="7">
         <f>C38-B38</f>
         <v>1971</v>
@@ -1971,11 +1967,11 @@
         <v>262143</v>
       </c>
       <c r="D38" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>03F84C</v>
       </c>
       <c r="E38" s="7" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>03FFFF</v>
       </c>
       <c r="F38" s="7"/>
@@ -1984,7 +1980,7 @@
       </c>
       <c r="H38" s="34"/>
     </row>
-    <row r="40" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" s="9" customFormat="1">
       <c r="A40" s="10" t="s">
         <v>26</v>
       </c>
@@ -1999,7 +1995,7 @@
       <c r="M40"/>
       <c r="N40"/>
     </row>
-    <row r="41" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" s="10" customFormat="1">
       <c r="A41" s="13" t="s">
         <v>6</v>
       </c>
@@ -2027,7 +2023,7 @@
       <c r="M41"/>
       <c r="N41"/>
     </row>
-    <row r="42" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" s="10" customFormat="1">
       <c r="A42" s="13"/>
       <c r="B42" s="13" t="s">
         <v>8</v>
@@ -2050,7 +2046,7 @@
       <c r="M42"/>
       <c r="N42"/>
     </row>
-    <row r="43" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" s="5" customFormat="1">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -2066,7 +2062,7 @@
       <c r="M43"/>
       <c r="N43"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14">
       <c r="A44" s="7">
         <f>256*1024</f>
         <v>262144</v>
@@ -2092,7 +2088,7 @@
       </c>
       <c r="H44" s="34"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14">
       <c r="A45" s="7">
         <v>256</v>
       </c>
@@ -2101,15 +2097,15 @@
         <v>262144</v>
       </c>
       <c r="C45" s="7">
-        <f t="shared" ref="C45" si="19">B45+A45-1</f>
+        <f t="shared" ref="C45" si="20">B45+A45-1</f>
         <v>262399</v>
       </c>
       <c r="D45" s="7" t="str">
-        <f t="shared" ref="D45:D46" si="20">DEC2HEX(B45,6)</f>
+        <f t="shared" ref="D45:D46" si="21">DEC2HEX(B45,6)</f>
         <v>040000</v>
       </c>
       <c r="E45" s="7" t="str">
-        <f t="shared" ref="E45:E46" si="21">DEC2HEX(C45,6)</f>
+        <f t="shared" ref="E45:E46" si="22">DEC2HEX(C45,6)</f>
         <v>0400FF</v>
       </c>
       <c r="F45" s="7"/>
@@ -2120,7 +2116,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14">
       <c r="A46" s="7">
         <v>256</v>
       </c>
@@ -2129,15 +2125,15 @@
         <v>262400</v>
       </c>
       <c r="C46" s="7">
-        <f t="shared" ref="C46" si="22">B46+A46-1</f>
+        <f t="shared" ref="C46" si="23">B46+A46-1</f>
         <v>262655</v>
       </c>
       <c r="D46" s="7" t="str">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>040100</v>
       </c>
       <c r="E46" s="7" t="str">
-        <f t="shared" si="21"/>
+        <f t="shared" si="22"/>
         <v>0401FF</v>
       </c>
       <c r="F46" s="7"/>
@@ -2148,7 +2144,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14">
       <c r="A47" s="7">
         <v>256</v>
       </c>
@@ -2157,15 +2153,15 @@
         <v>262656</v>
       </c>
       <c r="C47" s="7">
-        <f t="shared" ref="C47:C51" si="23">B47+A47-1</f>
+        <f t="shared" ref="C47:C51" si="24">B47+A47-1</f>
         <v>262911</v>
       </c>
       <c r="D47" s="7" t="str">
-        <f t="shared" ref="D47:D53" si="24">DEC2HEX(B47,6)</f>
+        <f t="shared" ref="D47:D53" si="25">DEC2HEX(B47,6)</f>
         <v>040200</v>
       </c>
       <c r="E47" s="7" t="str">
-        <f t="shared" ref="E47:E53" si="25">DEC2HEX(C47,6)</f>
+        <f t="shared" ref="E47:E53" si="26">DEC2HEX(C47,6)</f>
         <v>0402FF</v>
       </c>
       <c r="F47" s="7"/>
@@ -2176,7 +2172,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14">
       <c r="A48" s="7">
         <v>256</v>
       </c>
@@ -2185,15 +2181,15 @@
         <v>262912</v>
       </c>
       <c r="C48" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>263167</v>
       </c>
       <c r="D48" s="7" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>040300</v>
       </c>
       <c r="E48" s="7" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0403FF</v>
       </c>
       <c r="F48" s="7"/>
@@ -2204,24 +2200,24 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49" s="7">
         <v>256</v>
       </c>
       <c r="B49" s="7">
-        <f t="shared" ref="B49" si="26">C48+1</f>
+        <f t="shared" ref="B49" si="27">C48+1</f>
         <v>263168</v>
       </c>
       <c r="C49" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>263423</v>
       </c>
       <c r="D49" s="7" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>040400</v>
       </c>
       <c r="E49" s="7" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>0404FF</v>
       </c>
       <c r="F49" s="7"/>
@@ -2232,24 +2228,24 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50" s="7">
         <v>256</v>
       </c>
       <c r="B50" s="7">
-        <f t="shared" ref="B50" si="27">C49+1</f>
+        <f t="shared" ref="B50" si="28">C49+1</f>
         <v>263424</v>
       </c>
       <c r="C50" s="7">
-        <f t="shared" ref="C50" si="28">B50+A50-1</f>
+        <f t="shared" ref="C50" si="29">B50+A50-1</f>
         <v>263679</v>
       </c>
       <c r="D50" s="7" t="str">
-        <f t="shared" ref="D50" si="29">DEC2HEX(B50,6)</f>
+        <f t="shared" ref="D50" si="30">DEC2HEX(B50,6)</f>
         <v>040500</v>
       </c>
       <c r="E50" s="7" t="str">
-        <f t="shared" ref="E50" si="30">DEC2HEX(C50,6)</f>
+        <f t="shared" ref="E50" si="31">DEC2HEX(C50,6)</f>
         <v>0405FF</v>
       </c>
       <c r="F50" s="7"/>
@@ -2260,7 +2256,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51" s="7">
         <f>2*(128*96*2)</f>
         <v>49152</v>
@@ -2270,15 +2266,15 @@
         <v>263680</v>
       </c>
       <c r="C51" s="7">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>312831</v>
       </c>
       <c r="D51" s="7" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>040600</v>
       </c>
       <c r="E51" s="7" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>04C5FF</v>
       </c>
       <c r="F51" s="7"/>
@@ -2289,7 +2285,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52" s="7">
         <v>1024</v>
       </c>
@@ -2298,15 +2294,15 @@
         <v>312832</v>
       </c>
       <c r="C52" s="7">
-        <f t="shared" ref="C52" si="31">B52+A52-1</f>
+        <f t="shared" ref="C52" si="32">B52+A52-1</f>
         <v>313855</v>
       </c>
       <c r="D52" s="7" t="str">
-        <f t="shared" ref="D52" si="32">DEC2HEX(B52,6)</f>
+        <f t="shared" ref="D52" si="33">DEC2HEX(B52,6)</f>
         <v>04C600</v>
       </c>
       <c r="E52" s="7" t="str">
-        <f t="shared" ref="E52" si="33">DEC2HEX(C52,6)</f>
+        <f t="shared" ref="E52" si="34">DEC2HEX(C52,6)</f>
         <v>04C9FF</v>
       </c>
       <c r="F52" s="7"/>
@@ -2317,7 +2313,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53" s="7">
         <f>C53-B53</f>
         <v>16463359</v>
@@ -2331,11 +2327,11 @@
         <v>16777215</v>
       </c>
       <c r="D53" s="7" t="str">
-        <f t="shared" si="24"/>
+        <f t="shared" si="25"/>
         <v>04CA00</v>
       </c>
       <c r="E53" s="7" t="str">
-        <f t="shared" si="25"/>
+        <f t="shared" si="26"/>
         <v>FFFFFF</v>
       </c>
       <c r="F53" s="7"/>
@@ -2356,14 +2352,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="6" width="1.5703125" customWidth="1"/>
@@ -2376,7 +2372,7 @@
     <col min="15" max="15" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="21">
       <c r="A1" s="17" t="s">
         <v>65</v>
       </c>
@@ -2385,7 +2381,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" ht="15.75">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2406,7 +2402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" ht="15.75">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -2437,7 +2433,7 @@
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="15.75">
       <c r="A4" s="15"/>
       <c r="B4" s="13" t="s">
         <v>8</v>
@@ -2478,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="15.75">
       <c r="A5" s="15"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -2495,7 +2491,7 @@
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" s="21" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="22">
         <f>'Memory Map'!A22</f>
         <v>1</v>
@@ -2542,7 +2538,7 @@
       <c r="N6" s="36"/>
       <c r="O6" s="36"/>
     </row>
-    <row r="7" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" s="21" customFormat="1">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -2559,7 +2555,7 @@
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -2576,7 +2572,7 @@
       <c r="N8" s="26"/>
       <c r="O8" s="26"/>
     </row>
-    <row r="9" spans="1:15" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" s="21" customFormat="1" ht="30">
       <c r="A9" s="22">
         <f>'Memory Map'!A26</f>
         <v>1</v>
@@ -2627,7 +2623,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" s="21" customFormat="1">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -2644,7 +2640,7 @@
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
     </row>
-    <row r="11" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" s="21" customFormat="1">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -2661,7 +2657,7 @@
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15">
       <c r="A12" s="1">
         <f>'Memory Map'!A30-1</f>
         <v>1</v>
@@ -2715,7 +2711,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15">
       <c r="G13" s="2"/>
       <c r="H13" s="27">
         <v>0</v>
@@ -2742,20 +2738,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15">
       <c r="G14" s="2"/>
       <c r="H14" s="24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15">
       <c r="G15" s="2"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15">
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="30">
       <c r="A17" s="22">
         <f>'Memory Map'!A34</f>
         <v>1</v>
@@ -2805,7 +2801,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
@@ -2815,7 +2811,7 @@
       <c r="N18" s="27"/>
       <c r="O18" s="27"/>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -2823,7 +2819,7 @@
       <c r="E19" s="22"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15">
       <c r="A20" s="22">
         <f>'Memory Map'!A35</f>
         <v>1</v>
@@ -2873,7 +2869,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -2888,60 +2884,60 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="109.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1">
       <c r="A1" s="21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1">
       <c r="A2" s="21" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1">
       <c r="A3" s="21"/>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1">
       <c r="A4" s="21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1">
       <c r="A5" s="21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="30">
       <c r="A6" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1">
       <c r="A7" s="21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="45">
       <c r="A8" s="35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1">
       <c r="A9" s="21"/>
     </row>
-    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="60">
       <c r="A10" s="35" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
Updated paramater stack RAM and datapath to operate in write first mode
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545"/>
@@ -11,7 +11,7 @@
     <sheet name="Hardware registers" sheetId="2" r:id="rId2"/>
     <sheet name="Copyright and license" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -464,8 +464,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -746,6 +746,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -780,6 +781,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -955,7 +957,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -965,7 +967,7 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="5" width="12.42578125" style="1" customWidth="1"/>
@@ -978,12 +980,12 @@
     <col min="14" max="14" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1">
+    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
@@ -996,7 +998,7 @@
       <c r="M3"/>
       <c r="N3"/>
     </row>
-    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -1026,7 +1028,7 @@
       <c r="M4"/>
       <c r="N4"/>
     </row>
-    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1">
+    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13" t="s">
         <v>8</v>
@@ -1049,7 +1051,7 @@
       <c r="M5"/>
       <c r="N5"/>
     </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1">
+    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1065,7 +1067,7 @@
       <c r="M6"/>
       <c r="N6"/>
     </row>
-    <row r="7" spans="1:14">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <f>(128)*1024</f>
         <v>131072</v>
@@ -1096,7 +1098,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <f>(128-12)*1024</f>
         <v>118784</v>
@@ -1122,7 +1124,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:14">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>2048</v>
       </c>
@@ -1153,7 +1155,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:14">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>2048</v>
       </c>
@@ -1184,7 +1186,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="11" spans="1:14">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <f>2048</f>
         <v>2048</v>
@@ -1216,7 +1218,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:14">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <f>2048</f>
         <v>2048</v>
@@ -1248,7 +1250,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:14">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>2048</v>
       </c>
@@ -1279,10 +1281,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:14">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:14" s="9" customFormat="1">
+    <row r="15" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>50</v>
       </c>
@@ -1297,7 +1299,7 @@
       <c r="M15"/>
       <c r="N15"/>
     </row>
-    <row r="16" spans="1:14" s="10" customFormat="1">
+    <row r="16" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>6</v>
       </c>
@@ -1325,7 +1327,7 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:14" s="11" customFormat="1">
+    <row r="17" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="13" t="s">
         <v>8</v>
@@ -1348,7 +1350,7 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1">
+    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1364,7 +1366,7 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>4</v>
       </c>
@@ -1395,7 +1397,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>4</v>
       </c>
@@ -1426,7 +1428,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>1</v>
       </c>
@@ -1457,7 +1459,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>1</v>
       </c>
@@ -1488,7 +1490,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>1</v>
       </c>
@@ -1519,7 +1521,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>1</v>
       </c>
@@ -1550,7 +1552,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>2</v>
       </c>
@@ -1581,7 +1583,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>1</v>
       </c>
@@ -1612,7 +1614,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>1</v>
       </c>
@@ -1643,7 +1645,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>4</v>
       </c>
@@ -1674,7 +1676,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>4</v>
       </c>
@@ -1705,7 +1707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>2</v>
       </c>
@@ -1736,7 +1738,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>2</v>
       </c>
@@ -1767,7 +1769,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>1</v>
       </c>
@@ -1798,7 +1800,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:14">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>1</v>
       </c>
@@ -1829,7 +1831,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:14">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>1</v>
       </c>
@@ -1860,7 +1862,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:14">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>1</v>
       </c>
@@ -1891,7 +1893,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:14">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>1</v>
       </c>
@@ -1922,7 +1924,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:14">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>1</v>
       </c>
@@ -1953,7 +1955,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:14">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <f>C38-B38</f>
         <v>1971</v>
@@ -1980,7 +1982,7 @@
       </c>
       <c r="H38" s="34"/>
     </row>
-    <row r="40" spans="1:14" s="9" customFormat="1">
+    <row r="40" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="10" t="s">
         <v>26</v>
       </c>
@@ -1995,7 +1997,7 @@
       <c r="M40"/>
       <c r="N40"/>
     </row>
-    <row r="41" spans="1:14" s="10" customFormat="1">
+    <row r="41" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="13" t="s">
         <v>6</v>
       </c>
@@ -2023,7 +2025,7 @@
       <c r="M41"/>
       <c r="N41"/>
     </row>
-    <row r="42" spans="1:14" s="10" customFormat="1">
+    <row r="42" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13"/>
       <c r="B42" s="13" t="s">
         <v>8</v>
@@ -2046,7 +2048,7 @@
       <c r="M42"/>
       <c r="N42"/>
     </row>
-    <row r="43" spans="1:14" s="5" customFormat="1">
+    <row r="43" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="6"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
@@ -2062,7 +2064,7 @@
       <c r="M43"/>
       <c r="N43"/>
     </row>
-    <row r="44" spans="1:14">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <f>256*1024</f>
         <v>262144</v>
@@ -2088,7 +2090,7 @@
       </c>
       <c r="H44" s="34"/>
     </row>
-    <row r="45" spans="1:14">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>256</v>
       </c>
@@ -2116,7 +2118,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:14">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>256</v>
       </c>
@@ -2144,7 +2146,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:14">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>256</v>
       </c>
@@ -2172,7 +2174,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="48" spans="1:14">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>256</v>
       </c>
@@ -2200,7 +2202,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="49" spans="1:9">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>256</v>
       </c>
@@ -2228,7 +2230,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>256</v>
       </c>
@@ -2256,7 +2258,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:9">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <f>2*(128*96*2)</f>
         <v>49152</v>
@@ -2285,7 +2287,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:9">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>1024</v>
       </c>
@@ -2313,7 +2315,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:9">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <f>C53-B53</f>
         <v>16463359</v>
@@ -2352,14 +2354,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="5" width="8.140625" customWidth="1"/>
     <col min="6" max="6" width="1.5703125" customWidth="1"/>
@@ -2372,7 +2374,7 @@
     <col min="15" max="15" width="23.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="21">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>65</v>
       </c>
@@ -2381,7 +2383,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="8"/>
     </row>
-    <row r="2" spans="1:15" ht="15.75">
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -2402,7 +2404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="15.75">
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>6</v>
       </c>
@@ -2433,7 +2435,7 @@
       <c r="N3" s="20"/>
       <c r="O3" s="20"/>
     </row>
-    <row r="4" spans="1:15" ht="15.75">
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
       <c r="B4" s="13" t="s">
         <v>8</v>
@@ -2474,7 +2476,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="15.75">
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="13"/>
       <c r="C5" s="13"/>
@@ -2491,7 +2493,7 @@
       <c r="N5" s="18"/>
       <c r="O5" s="18"/>
     </row>
-    <row r="6" spans="1:15" s="21" customFormat="1" ht="30" customHeight="1">
+    <row r="6" spans="1:15" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
         <f>'Memory Map'!A22</f>
         <v>1</v>
@@ -2538,7 +2540,7 @@
       <c r="N6" s="36"/>
       <c r="O6" s="36"/>
     </row>
-    <row r="7" spans="1:15" s="21" customFormat="1">
+    <row r="7" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="22"/>
       <c r="C7" s="22"/>
@@ -2555,7 +2557,7 @@
       <c r="N7" s="25"/>
       <c r="O7" s="25"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="26"/>
       <c r="B8" s="26"/>
       <c r="C8" s="26"/>
@@ -2572,7 +2574,7 @@
       <c r="N8" s="26"/>
       <c r="O8" s="26"/>
     </row>
-    <row r="9" spans="1:15" s="21" customFormat="1" ht="30">
+    <row r="9" spans="1:15" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
         <f>'Memory Map'!A26</f>
         <v>1</v>
@@ -2623,7 +2625,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:15" s="21" customFormat="1">
+    <row r="10" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="22"/>
       <c r="B10" s="22"/>
       <c r="C10" s="22"/>
@@ -2640,7 +2642,7 @@
       <c r="N10" s="23"/>
       <c r="O10" s="23"/>
     </row>
-    <row r="11" spans="1:15" s="21" customFormat="1">
+    <row r="11" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="22"/>
       <c r="C11" s="22"/>
@@ -2657,7 +2659,7 @@
       <c r="N11" s="23"/>
       <c r="O11" s="23"/>
     </row>
-    <row r="12" spans="1:15">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <f>'Memory Map'!A30-1</f>
         <v>1</v>
@@ -2711,7 +2713,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:15">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G13" s="2"/>
       <c r="H13" s="27">
         <v>0</v>
@@ -2738,20 +2740,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:15">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G14" s="2"/>
       <c r="H14" s="24" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:15">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G15" s="2"/>
       <c r="H15" s="24"/>
     </row>
-    <row r="16" spans="1:15">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:15" ht="30">
+    <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
         <f>'Memory Map'!A34</f>
         <v>1</v>
@@ -2801,7 +2803,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="22"/>
       <c r="B18" s="22"/>
       <c r="C18" s="22"/>
@@ -2811,7 +2813,7 @@
       <c r="N18" s="27"/>
       <c r="O18" s="27"/>
     </row>
-    <row r="19" spans="1:15">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="22"/>
       <c r="B19" s="22"/>
       <c r="C19" s="22"/>
@@ -2819,7 +2821,7 @@
       <c r="E19" s="22"/>
       <c r="G19" s="2"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
         <f>'Memory Map'!A35</f>
         <v>1</v>
@@ -2869,7 +2871,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="23" spans="1:15">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>69</v>
       </c>
@@ -2884,60 +2886,60 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="109.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="21" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="21"/>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="21" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="30">
+    <row r="6" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="21" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="45">
+    <row r="8" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="21"/>
     </row>
-    <row r="10" spans="1:1" ht="60">
+    <row r="10" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>84</v>
       </c>

</xml_diff>

<commit_message>
Reconfigured hardware to include USER data area
1. SRAM_Controller now uses byte enable and completes in 1 cycle less

2. timing enhancements to the control unit
2.1. use registered NOS for memory bus data output channel
2.2. avoid using equalzero on the unregistered value of TOS to select state_n
with ?dup and THROW, rather make the necessary decision on the second cycle with a registered value

3  included 32 VM * 2K USER RAM blocks
3.1. a temporary hardware register is used to select the VM no.

Tested in simulation and on the Nexys board
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="22995" windowHeight="10545"/>
+    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Memory Map" sheetId="1" r:id="rId1"/>
-    <sheet name="Hardware registers" sheetId="2" r:id="rId2"/>
-    <sheet name="Copyright and license" sheetId="3" r:id="rId3"/>
+    <sheet name="NEW Memory Map" sheetId="4" r:id="rId1"/>
+    <sheet name="USER" sheetId="5" r:id="rId2"/>
+    <sheet name="Hardware registers" sheetId="2" r:id="rId3"/>
+    <sheet name="OLD Memory Map" sheetId="1" r:id="rId4"/>
+    <sheet name="Copyright and license" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="133">
   <si>
     <t>Name</t>
   </si>
@@ -460,12 +462,105 @@
   <si>
     <t>Subroutine and exception stacks</t>
   </si>
+  <si>
+    <t>USER data area</t>
+  </si>
+  <si>
+    <t>Access to each VM's local user data</t>
+  </si>
+  <si>
+    <t>VM#</t>
+  </si>
+  <si>
+    <t>Pre-emptive interval</t>
+  </si>
+  <si>
+    <t>Unsigned 32-bit counter at 100MHz</t>
+  </si>
+  <si>
+    <t>Multi tasking on/off</t>
+  </si>
+  <si>
+    <t>When zero, PAUSE (pre-emptive or elective) becomes a NOP</t>
+  </si>
+  <si>
+    <t>VM schedule registers</t>
+  </si>
+  <si>
+    <t>32 registers, each of 16 bits.  Lowest 5 bits are interpreted as next task no.</t>
+  </si>
+  <si>
+    <t>Number of currently executing VM</t>
+  </si>
+  <si>
+    <t>PC of next-to-execute VM</t>
+  </si>
+  <si>
+    <t>Write through via next-task port of task table BLOCK RAM (need true dual port)</t>
+  </si>
+  <si>
+    <t>Access to the paramater stack in the CPU address space (current task)</t>
+  </si>
+  <si>
+    <t>Access to the return stack in the CPU address space (current task)</t>
+  </si>
+  <si>
+    <t>Access to subroutine and exception stacks (current task)</t>
+  </si>
+  <si>
+    <t>Interval for pre-emptive multi-tasking (units: clock cycles).  Zero = pre-emptive off</t>
+  </si>
+  <si>
+    <t>USER RAM</t>
+  </si>
+  <si>
+    <t>ACCEPT input buffer</t>
+  </si>
+  <si>
+    <t>PAD</t>
+  </si>
+  <si>
+    <t>Available for additional USER variables</t>
+  </si>
+  <si>
+    <t>STRINGP, next available location in the string buffer</t>
+  </si>
+  <si>
+    <t>STATE, compile/interpret flag</t>
+  </si>
+  <si>
+    <t>input_buff, address of the input buffer</t>
+  </si>
+  <si>
+    <t>input_size, size capacity of the input buffer</t>
+  </si>
+  <si>
+    <t>&gt;IN, offset to current parse area</t>
+  </si>
+  <si>
+    <t>IN_LEN, number of characters in the input buffer</t>
+  </si>
+  <si>
+    <t>Current compilation WID</t>
+  </si>
+  <si>
+    <t>Number of WID's in the search list</t>
+  </si>
+  <si>
+    <t>Search list of up to 14 WID's</t>
+  </si>
+  <si>
+    <t>HLD_, pointer used by picture numeric conversion</t>
+  </si>
+  <si>
+    <t>Absolute address</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -541,6 +636,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -571,7 +673,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -656,6 +758,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -961,10 +1069,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1100,24 +1208,24 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <f>(128-12)*1024</f>
-        <v>118784</v>
+        <f>(128-16)*1024</f>
+        <v>114688</v>
       </c>
       <c r="B8" s="7">
-        <f t="shared" ref="B8:B13" si="0">C7+1</f>
+        <f t="shared" ref="B8:B14" si="0">C7+1</f>
         <v>131072</v>
       </c>
       <c r="C8" s="7">
         <f>B8+A8-1</f>
-        <v>249855</v>
+        <v>245759</v>
       </c>
       <c r="D8" s="7" t="str">
-        <f t="shared" ref="D8:D9" si="1">DEC2HEX(B8,6)</f>
+        <f t="shared" ref="D8:E14" si="1">DEC2HEX(B8,6)</f>
         <v>020000</v>
       </c>
       <c r="E8" s="7" t="str">
-        <f t="shared" ref="E8:E9" si="2">DEC2HEX(C8,6)</f>
-        <v>03CFFF</v>
+        <f t="shared" si="1"/>
+        <v>03BFFF</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8" t="s">
@@ -1126,33 +1234,33 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="B9" s="7">
-        <f t="shared" si="0"/>
-        <v>249856</v>
+        <f>C8+1</f>
+        <v>245760</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" ref="C9" si="3">B9+A9-1</f>
-        <v>251903</v>
+        <f t="shared" ref="C9" si="2">B9+A9-1</f>
+        <v>249855</v>
       </c>
       <c r="D9" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>03D000</v>
+        <f t="shared" ref="D9" si="3">DEC2HEX(B9,6)</f>
+        <v>03C000</v>
       </c>
       <c r="E9" s="7" t="str">
-        <f t="shared" si="2"/>
-        <v>03D7FF</v>
+        <f t="shared" ref="E9" si="4">DEC2HEX(C9,6)</f>
+        <v>03CFFF</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
       <c r="H9" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -1160,62 +1268,61 @@
         <v>2048</v>
       </c>
       <c r="B10" s="7">
+        <f>C9+1</f>
+        <v>249856</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" ref="C10" si="5">B10+A10-1</f>
+        <v>251903</v>
+      </c>
+      <c r="D10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03D000</v>
+      </c>
+      <c r="E10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03D7FF</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>2048</v>
+      </c>
+      <c r="B11" s="7">
         <f t="shared" si="0"/>
         <v>251904</v>
       </c>
-      <c r="C10" s="7">
-        <f>B10+A10-1</f>
+      <c r="C11" s="7">
+        <f>B11+A11-1</f>
         <v>253951</v>
       </c>
-      <c r="D10" s="7" t="str">
-        <f t="shared" ref="D10:D13" si="4">DEC2HEX(B10,6)</f>
+      <c r="D11" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>03D800</v>
       </c>
-      <c r="E10" s="7" t="str">
-        <f t="shared" ref="E10:E13" si="5">DEC2HEX(C10,6)</f>
+      <c r="E11" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>03DFFF</v>
-      </c>
-      <c r="F10" s="7"/>
-      <c r="G10" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="H10" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" s="7">
-        <f>2048</f>
-        <v>2048</v>
-      </c>
-      <c r="B11" s="7">
-        <f t="shared" si="0"/>
-        <v>253952</v>
-      </c>
-      <c r="C11" s="7">
-        <f t="shared" ref="C11:C13" si="6">B11+A11-1</f>
-        <v>255999</v>
-      </c>
-      <c r="D11" s="7" t="str">
-        <f t="shared" si="4"/>
-        <v>03E000</v>
-      </c>
-      <c r="E11" s="7" t="str">
-        <f t="shared" si="5"/>
-        <v>03E7FF</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="H11" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
@@ -1225,101 +1332,105 @@
       </c>
       <c r="B12" s="7">
         <f t="shared" si="0"/>
+        <v>253952</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" ref="C12:C14" si="6">B12+A12-1</f>
+        <v>255999</v>
+      </c>
+      <c r="D12" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03E000</v>
+      </c>
+      <c r="E12" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03E7FF</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <f>2048</f>
+        <v>2048</v>
+      </c>
+      <c r="B13" s="7">
+        <f t="shared" si="0"/>
         <v>256000</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C13" s="7">
         <f t="shared" si="6"/>
         <v>258047</v>
       </c>
-      <c r="D12" s="7" t="str">
-        <f t="shared" si="4"/>
+      <c r="D13" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>03E800</v>
       </c>
-      <c r="E12" s="7" t="str">
-        <f t="shared" si="5"/>
+      <c r="E13" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>03EFFF</v>
       </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8" t="s">
+      <c r="F13" s="7"/>
+      <c r="G13" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="H13" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I12" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
+      <c r="I13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
         <v>2048</v>
       </c>
-      <c r="B13" s="7">
+      <c r="B14" s="7">
         <f t="shared" si="0"/>
         <v>258048</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C14" s="7">
         <f t="shared" si="6"/>
         <v>260095</v>
       </c>
-      <c r="D13" s="7" t="str">
-        <f t="shared" si="4"/>
+      <c r="D14" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>03F000</v>
       </c>
-      <c r="E13" s="7" t="str">
-        <f t="shared" si="5"/>
+      <c r="E14" s="7" t="str">
+        <f t="shared" si="1"/>
         <v>03F7FF</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8" t="s">
+      <c r="F14" s="7"/>
+      <c r="G14" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="H14" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I13" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-    </row>
-    <row r="15" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="14" t="s">
+      <c r="I14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="3"/>
+    </row>
+    <row r="16" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="H15" s="31"/>
-      <c r="I15"/>
-      <c r="J15"/>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15"/>
-    </row>
-    <row r="16" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D16" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="13"/>
-      <c r="G16" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="32"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="H16" s="31"/>
       <c r="I16"/>
       <c r="J16"/>
       <c r="K16"/>
@@ -1327,22 +1438,27 @@
       <c r="M16"/>
       <c r="N16"/>
     </row>
-    <row r="17" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="15"/>
+    <row r="17" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="13" t="s">
+        <v>6</v>
+      </c>
       <c r="B17" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F17" s="13"/>
-      <c r="H17" s="33"/>
+      <c r="G17" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="32"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1350,14 +1466,21 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="11"/>
+    <row r="18" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="15"/>
+      <c r="B18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" s="13"/>
       <c r="H18" s="33"/>
       <c r="I18"/>
       <c r="J18"/>
@@ -1366,97 +1489,82 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="7">
-        <v>4</v>
-      </c>
-      <c r="B19" s="7">
-        <f>C13+1</f>
-        <v>260096</v>
-      </c>
-      <c r="C19" s="7">
-        <f>B19+A19-1</f>
-        <v>260099</v>
-      </c>
-      <c r="D19" s="7" t="str">
-        <f t="shared" ref="D19:D38" si="7">DEC2HEX(B19,6)</f>
-        <v>03F800</v>
-      </c>
-      <c r="E19" s="7" t="str">
-        <f t="shared" ref="E19:E38" si="8">DEC2HEX(C19,6)</f>
-        <v>03F803</v>
-      </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H19" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I19" t="s">
-        <v>28</v>
-      </c>
+    <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="33"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>4</v>
       </c>
       <c r="B20" s="7">
-        <f>B19+4</f>
-        <v>260100</v>
+        <f>C14+1</f>
+        <v>260096</v>
       </c>
       <c r="C20" s="7">
-        <f t="shared" ref="C20" si="9">B20+A20-1</f>
-        <v>260103</v>
+        <f>B20+A20-1</f>
+        <v>260099</v>
       </c>
       <c r="D20" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F804</v>
+        <f t="shared" ref="D20:E39" si="7">DEC2HEX(B20,6)</f>
+        <v>03F800</v>
       </c>
       <c r="E20" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F807</v>
+        <f t="shared" si="7"/>
+        <v>03F803</v>
       </c>
       <c r="F20" s="7"/>
       <c r="G20" s="8" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H20" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B21" s="7">
-        <f t="shared" ref="B21:B37" si="10">B20+4</f>
-        <v>260104</v>
+        <f>B20+4</f>
+        <v>260100</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" ref="C21:C24" si="11">B21+A21-1</f>
-        <v>260104</v>
+        <f t="shared" ref="C21:C38" si="8">B21+A21-1</f>
+        <v>260103</v>
       </c>
       <c r="D21" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F808</v>
+        <v>03F804</v>
       </c>
       <c r="E21" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F808</v>
+        <f t="shared" si="7"/>
+        <v>03F807</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H21" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
@@ -1464,30 +1572,30 @@
         <v>1</v>
       </c>
       <c r="B22" s="7">
-        <f t="shared" si="10"/>
-        <v>260108</v>
+        <f t="shared" ref="B22:B38" si="9">B21+4</f>
+        <v>260104</v>
       </c>
       <c r="C22" s="7">
-        <f t="shared" si="11"/>
-        <v>260108</v>
+        <f t="shared" si="8"/>
+        <v>260104</v>
       </c>
       <c r="D22" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F80C</v>
+        <v>03F808</v>
       </c>
       <c r="E22" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F80C</v>
+        <f t="shared" si="7"/>
+        <v>03F808</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I22" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1495,30 +1603,30 @@
         <v>1</v>
       </c>
       <c r="B23" s="7">
-        <f t="shared" si="10"/>
-        <v>260112</v>
+        <f t="shared" si="9"/>
+        <v>260108</v>
       </c>
       <c r="C23" s="7">
-        <f t="shared" si="11"/>
-        <v>260112</v>
+        <f t="shared" si="8"/>
+        <v>260108</v>
       </c>
       <c r="D23" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F810</v>
+        <v>03F80C</v>
       </c>
       <c r="E23" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F810</v>
+        <f t="shared" si="7"/>
+        <v>03F80C</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I23" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1526,92 +1634,92 @@
         <v>1</v>
       </c>
       <c r="B24" s="7">
-        <f t="shared" si="10"/>
-        <v>260116</v>
+        <f t="shared" si="9"/>
+        <v>260112</v>
       </c>
       <c r="C24" s="7">
-        <f t="shared" si="11"/>
-        <v>260116</v>
+        <f t="shared" si="8"/>
+        <v>260112</v>
       </c>
       <c r="D24" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F814</v>
+        <v>03F810</v>
       </c>
       <c r="E24" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F814</v>
+        <f t="shared" si="7"/>
+        <v>03F810</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I24" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25" s="7">
-        <f t="shared" si="10"/>
-        <v>260120</v>
+        <f t="shared" si="9"/>
+        <v>260116</v>
       </c>
       <c r="C25" s="7">
-        <f t="shared" ref="C25:C27" si="12">B25+A25-1</f>
-        <v>260121</v>
+        <f t="shared" si="8"/>
+        <v>260116</v>
       </c>
       <c r="D25" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F818</v>
+        <v>03F814</v>
       </c>
       <c r="E25" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F819</v>
+        <f t="shared" si="7"/>
+        <v>03F814</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H25" s="30" t="s">
         <v>73</v>
       </c>
       <c r="I25" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B26" s="7">
-        <f t="shared" si="10"/>
-        <v>260124</v>
+        <f t="shared" si="9"/>
+        <v>260120</v>
       </c>
       <c r="C26" s="7">
-        <f>B26+A26-1</f>
-        <v>260124</v>
+        <f t="shared" si="8"/>
+        <v>260121</v>
       </c>
       <c r="D26" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F81C</v>
+        <v>03F818</v>
       </c>
       <c r="E26" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F81C</v>
+        <f t="shared" si="7"/>
+        <v>03F819</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -1619,61 +1727,61 @@
         <v>1</v>
       </c>
       <c r="B27" s="7">
-        <f t="shared" si="10"/>
-        <v>260128</v>
+        <f t="shared" si="9"/>
+        <v>260124</v>
       </c>
       <c r="C27" s="7">
-        <f t="shared" si="12"/>
-        <v>260128</v>
+        <f>B27+A27-1</f>
+        <v>260124</v>
       </c>
       <c r="D27" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F820</v>
+        <v>03F81C</v>
       </c>
       <c r="E27" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F820</v>
+        <f t="shared" si="7"/>
+        <v>03F81C</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8" t="s">
-        <v>36</v>
+        <v>20</v>
       </c>
       <c r="H27" s="30" t="s">
         <v>74</v>
       </c>
       <c r="I27" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B28" s="7">
-        <f t="shared" si="10"/>
-        <v>260132</v>
+        <f t="shared" si="9"/>
+        <v>260128</v>
       </c>
       <c r="C28" s="7">
-        <f t="shared" ref="C28" si="13">B28+A28-1</f>
-        <v>260135</v>
+        <f t="shared" si="8"/>
+        <v>260128</v>
       </c>
       <c r="D28" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F824</v>
+        <v>03F820</v>
       </c>
       <c r="E28" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F827</v>
+        <f t="shared" si="7"/>
+        <v>03F820</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H28" s="30" t="s">
         <v>74</v>
       </c>
       <c r="I28" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -1681,61 +1789,61 @@
         <v>4</v>
       </c>
       <c r="B29" s="7">
-        <f t="shared" si="10"/>
-        <v>260136</v>
+        <f t="shared" si="9"/>
+        <v>260132</v>
       </c>
       <c r="C29" s="7">
-        <f t="shared" ref="C29" si="14">B29+A29-1</f>
-        <v>260139</v>
+        <f t="shared" si="8"/>
+        <v>260135</v>
       </c>
       <c r="D29" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F828</v>
+        <v>03F824</v>
       </c>
       <c r="E29" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F82B</v>
+        <f t="shared" si="7"/>
+        <v>03F827</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H29" s="30" t="s">
         <v>74</v>
       </c>
       <c r="I29" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B30" s="7">
-        <f t="shared" si="10"/>
-        <v>260140</v>
+        <f t="shared" si="9"/>
+        <v>260136</v>
       </c>
       <c r="C30" s="7">
-        <f t="shared" ref="C30" si="15">B30+A30-1</f>
-        <v>260141</v>
+        <f t="shared" si="8"/>
+        <v>260139</v>
       </c>
       <c r="D30" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F82C</v>
+        <v>03F828</v>
       </c>
       <c r="E30" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F82D</v>
+        <f t="shared" si="7"/>
+        <v>03F82B</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I30" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
@@ -1743,61 +1851,61 @@
         <v>2</v>
       </c>
       <c r="B31" s="7">
-        <f t="shared" si="10"/>
-        <v>260144</v>
+        <f t="shared" si="9"/>
+        <v>260140</v>
       </c>
       <c r="C31" s="7">
-        <f t="shared" ref="C31:C32" si="16">B31+A31-1</f>
-        <v>260145</v>
+        <f t="shared" si="8"/>
+        <v>260141</v>
       </c>
       <c r="D31" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F830</v>
+        <v>03F82C</v>
       </c>
       <c r="E31" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F831</v>
+        <f t="shared" si="7"/>
+        <v>03F82D</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I31" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B32" s="7">
-        <f t="shared" si="10"/>
-        <v>260148</v>
+        <f t="shared" si="9"/>
+        <v>260144</v>
       </c>
       <c r="C32" s="7">
-        <f t="shared" si="16"/>
-        <v>260148</v>
+        <f t="shared" si="8"/>
+        <v>260145</v>
       </c>
       <c r="D32" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F834</v>
+        <v>03F830</v>
       </c>
       <c r="E32" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F834</v>
+        <f t="shared" si="7"/>
+        <v>03F831</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="8" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I32" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -1805,30 +1913,30 @@
         <v>1</v>
       </c>
       <c r="B33" s="7">
-        <f t="shared" si="10"/>
-        <v>260152</v>
+        <f t="shared" si="9"/>
+        <v>260148</v>
       </c>
       <c r="C33" s="7">
-        <f t="shared" ref="C33:C35" si="17">B33+A33-1</f>
-        <v>260152</v>
+        <f t="shared" si="8"/>
+        <v>260148</v>
       </c>
       <c r="D33" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F838</v>
+        <v>03F834</v>
       </c>
       <c r="E33" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F838</v>
+        <f t="shared" si="7"/>
+        <v>03F834</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I33" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -1836,30 +1944,30 @@
         <v>1</v>
       </c>
       <c r="B34" s="7">
-        <f t="shared" si="10"/>
-        <v>260156</v>
+        <f t="shared" si="9"/>
+        <v>260152</v>
       </c>
       <c r="C34" s="7">
-        <f t="shared" si="17"/>
-        <v>260156</v>
+        <f t="shared" si="8"/>
+        <v>260152</v>
       </c>
       <c r="D34" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F83C</v>
+        <v>03F838</v>
       </c>
       <c r="E34" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F83C</v>
+        <f t="shared" si="7"/>
+        <v>03F838</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H34" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I34" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -1867,27 +1975,27 @@
         <v>1</v>
       </c>
       <c r="B35" s="7">
-        <f t="shared" si="10"/>
-        <v>260160</v>
+        <f t="shared" si="9"/>
+        <v>260156</v>
       </c>
       <c r="C35" s="7">
-        <f t="shared" si="17"/>
-        <v>260160</v>
+        <f t="shared" si="8"/>
+        <v>260156</v>
       </c>
       <c r="D35" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F840</v>
+        <v>03F83C</v>
       </c>
       <c r="E35" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F840</v>
+        <f t="shared" si="7"/>
+        <v>03F83C</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I35" t="s">
         <v>33</v>
@@ -1898,30 +2006,30 @@
         <v>1</v>
       </c>
       <c r="B36" s="7">
-        <f t="shared" si="10"/>
-        <v>260164</v>
+        <f t="shared" si="9"/>
+        <v>260160</v>
       </c>
       <c r="C36" s="7">
-        <f t="shared" ref="C36" si="18">B36+A36-1</f>
-        <v>260164</v>
+        <f t="shared" si="8"/>
+        <v>260160</v>
       </c>
       <c r="D36" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F844</v>
+        <v>03F840</v>
       </c>
       <c r="E36" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F844</v>
+        <f t="shared" si="7"/>
+        <v>03F840</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="8" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I36" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -1929,421 +2037,615 @@
         <v>1</v>
       </c>
       <c r="B37" s="7">
-        <f t="shared" si="10"/>
-        <v>260168</v>
+        <f t="shared" si="9"/>
+        <v>260164</v>
       </c>
       <c r="C37" s="7">
-        <f t="shared" ref="C37" si="19">B37+A37-1</f>
-        <v>260168</v>
+        <f t="shared" si="8"/>
+        <v>260164</v>
       </c>
       <c r="D37" s="7" t="str">
         <f t="shared" si="7"/>
-        <v>03F848</v>
+        <v>03F844</v>
       </c>
       <c r="E37" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F848</v>
+        <f t="shared" si="7"/>
+        <v>03F844</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="8" t="s">
-        <v>93</v>
+        <v>25</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I37" t="s">
-        <v>94</v>
+        <v>53</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
-        <f>C38-B38</f>
-        <v>1971</v>
+        <v>1</v>
       </c>
       <c r="B38" s="7">
-        <f>B37+4</f>
+        <f t="shared" si="9"/>
+        <v>260168</v>
+      </c>
+      <c r="C38" s="7">
+        <f t="shared" si="8"/>
+        <v>260168</v>
+      </c>
+      <c r="D38" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F848</v>
+      </c>
+      <c r="E38" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F848</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H38" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I38" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <f>C39-B39</f>
+        <v>1827</v>
+      </c>
+      <c r="B39" s="7">
+        <f>B38+4</f>
         <v>260172</v>
       </c>
-      <c r="C38" s="7">
-        <f>A44-1</f>
+      <c r="C39" s="7">
+        <f>B40-1</f>
+        <v>261999</v>
+      </c>
+      <c r="D39" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F84C</v>
+      </c>
+      <c r="E39" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03FF6F</v>
+      </c>
+      <c r="F39" s="7"/>
+      <c r="G39" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <f>4*32</f>
+        <v>128</v>
+      </c>
+      <c r="B40" s="7">
+        <f>B41-A40</f>
+        <v>262000</v>
+      </c>
+      <c r="C40" s="7">
+        <f>B40+A40-1</f>
+        <v>262127</v>
+      </c>
+      <c r="D40" s="7" t="str">
+        <f t="shared" ref="D40:D41" si="10">DEC2HEX(B40,6)</f>
+        <v>03FF70</v>
+      </c>
+      <c r="E40" s="7" t="str">
+        <f t="shared" ref="E40:E41" si="11">DEC2HEX(C40,6)</f>
+        <v>03FFEF</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="H40" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I40" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>4</v>
+      </c>
+      <c r="B41" s="7">
+        <f t="shared" ref="B41" si="12">B42-A41</f>
+        <v>262128</v>
+      </c>
+      <c r="C41" s="7">
+        <f>B41+A41-1</f>
+        <v>262131</v>
+      </c>
+      <c r="D41" s="7" t="str">
+        <f t="shared" si="10"/>
+        <v>03FFF0</v>
+      </c>
+      <c r="E41" s="7" t="str">
+        <f t="shared" si="11"/>
+        <v>03FFF3</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I41" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>4</v>
+      </c>
+      <c r="B42" s="7">
+        <f t="shared" ref="B42:B43" si="13">B43-A42</f>
+        <v>262132</v>
+      </c>
+      <c r="C42" s="7">
+        <f>B42+A42-1</f>
+        <v>262135</v>
+      </c>
+      <c r="D42" s="7" t="str">
+        <f t="shared" ref="D42" si="14">DEC2HEX(B42,6)</f>
+        <v>03FFF4</v>
+      </c>
+      <c r="E42" s="7" t="str">
+        <f t="shared" ref="E42" si="15">DEC2HEX(C42,6)</f>
+        <v>03FFF7</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="H42" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>4</v>
+      </c>
+      <c r="B43" s="7">
+        <f t="shared" si="13"/>
+        <v>262136</v>
+      </c>
+      <c r="C43" s="7">
+        <f>B43+A43-1</f>
+        <v>262139</v>
+      </c>
+      <c r="D43" s="7" t="str">
+        <f t="shared" ref="D43" si="16">DEC2HEX(B43,6)</f>
+        <v>03FFF8</v>
+      </c>
+      <c r="E43" s="7" t="str">
+        <f t="shared" ref="E43" si="17">DEC2HEX(C43,6)</f>
+        <v>03FFFB</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H43" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I43" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A44" s="7">
+        <v>4</v>
+      </c>
+      <c r="B44" s="7">
+        <f>B51-A44</f>
+        <v>262140</v>
+      </c>
+      <c r="C44" s="7">
+        <f>B44+A44-1</f>
         <v>262143</v>
       </c>
-      <c r="D38" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F84C</v>
-      </c>
-      <c r="E38" s="7" t="str">
-        <f t="shared" si="8"/>
+      <c r="D44" s="7" t="str">
+        <f t="shared" ref="D44" si="18">DEC2HEX(B44,6)</f>
+        <v>03FFFC</v>
+      </c>
+      <c r="E44" s="7" t="str">
+        <f t="shared" ref="E44" si="19">DEC2HEX(C44,6)</f>
         <v>03FFFF</v>
       </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="H38" s="34"/>
-    </row>
-    <row r="40" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="10" t="s">
+      <c r="F44" s="7"/>
+      <c r="G44" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I44" t="s">
+        <v>111</v>
+      </c>
+      <c r="J44" s="37">
+        <f>B20+255</f>
+        <v>260351</v>
+      </c>
+      <c r="K44" s="37" t="str">
+        <f>DEC2HEX(J44,6)</f>
+        <v>03F8FF</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
-      <c r="F40" s="16"/>
-      <c r="H40" s="31"/>
-      <c r="I40"/>
-      <c r="J40"/>
-      <c r="K40"/>
-      <c r="L40"/>
-      <c r="M40"/>
-      <c r="N40"/>
-    </row>
-    <row r="41" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="D46" s="16"/>
+      <c r="E46" s="16"/>
+      <c r="F46" s="16"/>
+      <c r="H46" s="30"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+    </row>
+    <row r="47" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B47" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C47" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="D47" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E47" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F41" s="13"/>
-      <c r="G41" s="10" t="s">
+      <c r="F47" s="13"/>
+      <c r="G47" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H41" s="32"/>
-      <c r="I41"/>
-      <c r="J41"/>
-      <c r="K41"/>
-      <c r="L41"/>
-      <c r="M41"/>
-      <c r="N41"/>
-    </row>
-    <row r="42" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13" t="s">
+      <c r="H47" s="30"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+    </row>
+    <row r="48" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="13"/>
+      <c r="B48" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C48" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="D48" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E42" s="13" t="s">
+      <c r="E48" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F42" s="13"/>
-      <c r="H42" s="32"/>
-      <c r="I42"/>
-      <c r="J42"/>
-      <c r="K42"/>
-      <c r="L42"/>
-      <c r="M42"/>
-      <c r="N42"/>
-    </row>
-    <row r="43" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="6"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="6"/>
-      <c r="F43" s="6"/>
-      <c r="G43" s="10"/>
-      <c r="H43" s="32"/>
-      <c r="I43"/>
-      <c r="J43"/>
-      <c r="K43"/>
-      <c r="L43"/>
-      <c r="M43"/>
-      <c r="N43"/>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
+      <c r="F48" s="13"/>
+      <c r="H48" s="30"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+    </row>
+    <row r="49" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="30"/>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
         <f>256*1024</f>
         <v>262144</v>
       </c>
-      <c r="B44" s="7">
+      <c r="B50" s="7">
         <v>0</v>
       </c>
-      <c r="C44" s="7">
-        <f>A44-1</f>
+      <c r="C50" s="7">
+        <f>A50-1</f>
         <v>262143</v>
       </c>
-      <c r="D44" s="7" t="str">
-        <f>DEC2HEX(B44,6)</f>
+      <c r="D50" s="7" t="str">
+        <f>DEC2HEX(B50,6)</f>
         <v>000000</v>
       </c>
-      <c r="E44" s="7" t="str">
-        <f>DEC2HEX(C44,6)</f>
+      <c r="E50" s="7" t="str">
+        <f>DEC2HEX(C50,6)</f>
         <v>03FFFF</v>
       </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="12" t="s">
+      <c r="F50" s="7"/>
+      <c r="G50" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H44" s="34"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
+      <c r="H50" s="34"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
         <v>256</v>
       </c>
-      <c r="B45" s="7">
-        <f>C44+1</f>
+      <c r="B51" s="7">
+        <f>C50+1</f>
         <v>262144</v>
       </c>
-      <c r="C45" s="7">
-        <f t="shared" ref="C45" si="20">B45+A45-1</f>
+      <c r="C51" s="7">
+        <f t="shared" ref="C51:C58" si="20">B51+A51-1</f>
         <v>262399</v>
       </c>
-      <c r="D45" s="7" t="str">
-        <f t="shared" ref="D45:D46" si="21">DEC2HEX(B45,6)</f>
+      <c r="D51" s="7" t="str">
+        <f t="shared" ref="D51:E59" si="21">DEC2HEX(B51,6)</f>
         <v>040000</v>
       </c>
-      <c r="E45" s="7" t="str">
-        <f t="shared" ref="E45:E46" si="22">DEC2HEX(C45,6)</f>
+      <c r="E51" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>0400FF</v>
       </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="8" t="s">
+      <c r="F51" s="7"/>
+      <c r="G51" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="H45" s="30" t="s">
+      <c r="H51" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
         <v>256</v>
       </c>
-      <c r="B46" s="7">
-        <f>C45+1</f>
+      <c r="B52" s="7">
+        <f>C51+1</f>
         <v>262400</v>
       </c>
-      <c r="C46" s="7">
-        <f t="shared" ref="C46" si="23">B46+A46-1</f>
+      <c r="C52" s="7">
+        <f t="shared" si="20"/>
         <v>262655</v>
       </c>
-      <c r="D46" s="7" t="str">
+      <c r="D52" s="7" t="str">
         <f t="shared" si="21"/>
         <v>040100</v>
       </c>
-      <c r="E46" s="7" t="str">
+      <c r="E52" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>0401FF</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="G52" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H52" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>256</v>
+      </c>
+      <c r="B53" s="7">
+        <f>C52+1</f>
+        <v>262656</v>
+      </c>
+      <c r="C53" s="7">
+        <f t="shared" si="20"/>
+        <v>262911</v>
+      </c>
+      <c r="D53" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>040200</v>
+      </c>
+      <c r="E53" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>0402FF</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H53" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>256</v>
+      </c>
+      <c r="B54" s="7">
+        <f>C53+1</f>
+        <v>262912</v>
+      </c>
+      <c r="C54" s="7">
+        <f t="shared" si="20"/>
+        <v>263167</v>
+      </c>
+      <c r="D54" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>040300</v>
+      </c>
+      <c r="E54" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>0403FF</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H54" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>256</v>
+      </c>
+      <c r="B55" s="7">
+        <f t="shared" ref="B55:B56" si="22">C54+1</f>
+        <v>263168</v>
+      </c>
+      <c r="C55" s="7">
+        <f t="shared" si="20"/>
+        <v>263423</v>
+      </c>
+      <c r="D55" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>040400</v>
+      </c>
+      <c r="E55" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>0404FF</v>
+      </c>
+      <c r="F55" s="7"/>
+      <c r="G55" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H55" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>256</v>
+      </c>
+      <c r="B56" s="7">
         <f t="shared" si="22"/>
-        <v>0401FF</v>
-      </c>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="H46" s="30" t="s">
+        <v>263424</v>
+      </c>
+      <c r="C56" s="7">
+        <f t="shared" si="20"/>
+        <v>263679</v>
+      </c>
+      <c r="D56" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>040500</v>
+      </c>
+      <c r="E56" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>0405FF</v>
+      </c>
+      <c r="F56" s="7"/>
+      <c r="G56" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H56" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
-        <v>256</v>
-      </c>
-      <c r="B47" s="7">
-        <f>C46+1</f>
-        <v>262656</v>
-      </c>
-      <c r="C47" s="7">
-        <f t="shared" ref="C47:C51" si="24">B47+A47-1</f>
-        <v>262911</v>
-      </c>
-      <c r="D47" s="7" t="str">
-        <f t="shared" ref="D47:D53" si="25">DEC2HEX(B47,6)</f>
-        <v>040200</v>
-      </c>
-      <c r="E47" s="7" t="str">
-        <f t="shared" ref="E47:E53" si="26">DEC2HEX(C47,6)</f>
-        <v>0402FF</v>
-      </c>
-      <c r="F47" s="7"/>
-      <c r="G47" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="H47" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
-        <v>256</v>
-      </c>
-      <c r="B48" s="7">
-        <f>C47+1</f>
-        <v>262912</v>
-      </c>
-      <c r="C48" s="7">
-        <f t="shared" si="24"/>
-        <v>263167</v>
-      </c>
-      <c r="D48" s="7" t="str">
-        <f t="shared" si="25"/>
-        <v>040300</v>
-      </c>
-      <c r="E48" s="7" t="str">
-        <f t="shared" si="26"/>
-        <v>0403FF</v>
-      </c>
-      <c r="F48" s="7"/>
-      <c r="G48" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H48" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
-        <v>256</v>
-      </c>
-      <c r="B49" s="7">
-        <f t="shared" ref="B49" si="27">C48+1</f>
-        <v>263168</v>
-      </c>
-      <c r="C49" s="7">
-        <f t="shared" si="24"/>
-        <v>263423</v>
-      </c>
-      <c r="D49" s="7" t="str">
-        <f t="shared" si="25"/>
-        <v>040400</v>
-      </c>
-      <c r="E49" s="7" t="str">
-        <f t="shared" si="26"/>
-        <v>0404FF</v>
-      </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H49" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
-        <v>256</v>
-      </c>
-      <c r="B50" s="7">
-        <f t="shared" ref="B50" si="28">C49+1</f>
-        <v>263424</v>
-      </c>
-      <c r="C50" s="7">
-        <f t="shared" ref="C50" si="29">B50+A50-1</f>
-        <v>263679</v>
-      </c>
-      <c r="D50" s="7" t="str">
-        <f t="shared" ref="D50" si="30">DEC2HEX(B50,6)</f>
-        <v>040500</v>
-      </c>
-      <c r="E50" s="7" t="str">
-        <f t="shared" ref="E50" si="31">DEC2HEX(C50,6)</f>
-        <v>0405FF</v>
-      </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H50" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
         <f>2*(128*96*2)</f>
         <v>49152</v>
       </c>
-      <c r="B51" s="7">
-        <f>C50+1</f>
+      <c r="B57" s="7">
+        <f>C56+1</f>
         <v>263680</v>
       </c>
-      <c r="C51" s="7">
-        <f t="shared" si="24"/>
+      <c r="C57" s="7">
+        <f t="shared" si="20"/>
         <v>312831</v>
       </c>
-      <c r="D51" s="7" t="str">
-        <f t="shared" si="25"/>
+      <c r="D57" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>040600</v>
       </c>
-      <c r="E51" s="7" t="str">
-        <f t="shared" si="26"/>
+      <c r="E57" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>04C5FF</v>
       </c>
-      <c r="F51" s="7"/>
-      <c r="G51" s="8" t="s">
+      <c r="F57" s="7"/>
+      <c r="G57" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H51" s="30" t="s">
+      <c r="H57" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
         <v>1024</v>
       </c>
-      <c r="B52" s="7">
-        <f>C51+1</f>
+      <c r="B58" s="7">
+        <f>C57+1</f>
         <v>312832</v>
       </c>
-      <c r="C52" s="7">
-        <f t="shared" ref="C52" si="32">B52+A52-1</f>
+      <c r="C58" s="7">
+        <f t="shared" si="20"/>
         <v>313855</v>
       </c>
-      <c r="D52" s="7" t="str">
-        <f t="shared" ref="D52" si="33">DEC2HEX(B52,6)</f>
+      <c r="D58" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>04C600</v>
       </c>
-      <c r="E52" s="7" t="str">
-        <f t="shared" ref="E52" si="34">DEC2HEX(C52,6)</f>
+      <c r="E58" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>04C9FF</v>
       </c>
-      <c r="F52" s="7"/>
-      <c r="G52" s="8" t="s">
+      <c r="F58" s="7"/>
+      <c r="G58" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="H52" s="30" t="s">
+      <c r="H58" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
-        <f>C53-B53</f>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <f>C59-B59</f>
         <v>16463359</v>
       </c>
-      <c r="B53" s="7">
-        <f>C52+1</f>
+      <c r="B59" s="7">
+        <f>C58+1</f>
         <v>313856</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C59" s="7">
         <f>16*1024*1024-1</f>
         <v>16777215</v>
       </c>
-      <c r="D53" s="7" t="str">
-        <f t="shared" si="25"/>
+      <c r="D59" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>04CA00</v>
       </c>
-      <c r="E53" s="7" t="str">
-        <f t="shared" si="26"/>
+      <c r="E59" s="7" t="str">
+        <f t="shared" si="21"/>
         <v>FFFFFF</v>
       </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="8" t="s">
+      <c r="F59" s="7"/>
+      <c r="G59" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H53" s="30" t="s">
+      <c r="H59" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I59" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2354,6 +2656,552 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
+    <col min="7" max="7" width="51.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="38" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <f>B6+A6-1</f>
+        <v>3</v>
+      </c>
+      <c r="D6" s="7" t="str">
+        <f>DEC2HEX(B6,6)</f>
+        <v>000000</v>
+      </c>
+      <c r="E6" s="7" t="str">
+        <f>DEC2HEX(C6,6)</f>
+        <v>000003</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="H6" s="30">
+        <f>B6+'NEW Memory Map'!$B$9</f>
+        <v>245760</v>
+      </c>
+      <c r="I6" s="7" t="str">
+        <f>DEC2HEX(H6,6)</f>
+        <v>03C000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7">
+        <f>C6+1</f>
+        <v>4</v>
+      </c>
+      <c r="C7" s="7">
+        <f>B7+A7-1</f>
+        <v>7</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f>DEC2HEX(B7,6)</f>
+        <v>000004</v>
+      </c>
+      <c r="E7" s="7" t="str">
+        <f>DEC2HEX(C7,6)</f>
+        <v>000007</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="H7" s="30">
+        <f>B7+'NEW Memory Map'!$B$9</f>
+        <v>245764</v>
+      </c>
+      <c r="I7" s="7" t="str">
+        <f t="shared" ref="I7:I19" si="0">DEC2HEX(H7,6)</f>
+        <v>03C004</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7">
+        <f>C7+1</f>
+        <v>8</v>
+      </c>
+      <c r="C8" s="7">
+        <f>B8+A8-1</f>
+        <v>11</v>
+      </c>
+      <c r="D8" s="7" t="str">
+        <f>DEC2HEX(B8,6)</f>
+        <v>000008</v>
+      </c>
+      <c r="E8" s="7" t="str">
+        <f>DEC2HEX(C8,6)</f>
+        <v>00000B</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="H8" s="30">
+        <f>B8+'NEW Memory Map'!$B$9</f>
+        <v>245768</v>
+      </c>
+      <c r="I8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C008</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7">
+        <f t="shared" ref="B9:B15" si="1">C8+1</f>
+        <v>12</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" ref="C9:C15" si="2">B9+A9-1</f>
+        <v>15</v>
+      </c>
+      <c r="D9" s="7" t="str">
+        <f t="shared" ref="D9:D15" si="3">DEC2HEX(B9,6)</f>
+        <v>00000C</v>
+      </c>
+      <c r="E9" s="7" t="str">
+        <f t="shared" ref="E9:E15" si="4">DEC2HEX(C9,6)</f>
+        <v>00000F</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="H9" s="30">
+        <f>B9+'NEW Memory Map'!$B$9</f>
+        <v>245772</v>
+      </c>
+      <c r="I9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C00C</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="D10" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>000010</v>
+      </c>
+      <c r="E10" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>000013</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="H10" s="30">
+        <f>B10+'NEW Memory Map'!$B$9</f>
+        <v>245776</v>
+      </c>
+      <c r="I10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C010</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>4</v>
+      </c>
+      <c r="B11" s="7">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="D11" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>000014</v>
+      </c>
+      <c r="E11" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>000017</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H11" s="30">
+        <f>B11+'NEW Memory Map'!$B$9</f>
+        <v>245780</v>
+      </c>
+      <c r="I11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C014</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="D12" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>000018</v>
+      </c>
+      <c r="E12" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>00001B</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="H12" s="30">
+        <f>B12+'NEW Memory Map'!$B$9</f>
+        <v>245784</v>
+      </c>
+      <c r="I12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>1</v>
+      </c>
+      <c r="B13" s="7">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="D13" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>00001C</v>
+      </c>
+      <c r="E13" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>00001C</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="H13" s="30">
+        <f>B13+'NEW Memory Map'!$B$9</f>
+        <v>245788</v>
+      </c>
+      <c r="I13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C01C</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>1</v>
+      </c>
+      <c r="B14" s="7">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="C14" s="7">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="D14" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>00001D</v>
+      </c>
+      <c r="E14" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>00001D</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="H14" s="30">
+        <f>B14+'NEW Memory Map'!$B$9</f>
+        <v>245789</v>
+      </c>
+      <c r="I14" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C01D</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="D15" s="7" t="str">
+        <f t="shared" si="3"/>
+        <v>00001E</v>
+      </c>
+      <c r="E15" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>00002B</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="H15" s="30">
+        <f>B15+'NEW Memory Map'!$B$9</f>
+        <v>245790</v>
+      </c>
+      <c r="I15" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C01E</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <f>C16-B16+1</f>
+        <v>980</v>
+      </c>
+      <c r="B16" s="7">
+        <f>C15+1</f>
+        <v>44</v>
+      </c>
+      <c r="C16" s="7">
+        <f>B17-1</f>
+        <v>1023</v>
+      </c>
+      <c r="D16" s="7" t="str">
+        <f t="shared" ref="D16:D19" si="5">DEC2HEX(B16,6)</f>
+        <v>00002C</v>
+      </c>
+      <c r="E16" s="7" t="str">
+        <f t="shared" ref="E16:E19" si="6">DEC2HEX(C16,6)</f>
+        <v>0003FF</v>
+      </c>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H16" s="30">
+        <f>B16+'NEW Memory Map'!$B$9</f>
+        <v>245804</v>
+      </c>
+      <c r="I16" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C02C</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>512</v>
+      </c>
+      <c r="B17" s="7">
+        <f>C17-A17+1</f>
+        <v>1024</v>
+      </c>
+      <c r="C17" s="7">
+        <f>B18-1</f>
+        <v>1535</v>
+      </c>
+      <c r="D17" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>000400</v>
+      </c>
+      <c r="E17" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>0005FF</v>
+      </c>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="H17" s="30">
+        <f>B17+'NEW Memory Map'!$B$9</f>
+        <v>246784</v>
+      </c>
+      <c r="I17" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="7">
+        <v>256</v>
+      </c>
+      <c r="B18" s="7">
+        <f>C18-A18+1</f>
+        <v>1536</v>
+      </c>
+      <c r="C18" s="7">
+        <f>B19-1</f>
+        <v>1791</v>
+      </c>
+      <c r="D18" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>000600</v>
+      </c>
+      <c r="E18" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>0006FF</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="H18" s="30">
+        <f>B18+'NEW Memory Map'!$B$9</f>
+        <v>247296</v>
+      </c>
+      <c r="I18" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>256</v>
+      </c>
+      <c r="B19" s="7">
+        <f>C19-A19+1</f>
+        <v>1792</v>
+      </c>
+      <c r="C19" s="7">
+        <f>2048-1</f>
+        <v>2047</v>
+      </c>
+      <c r="D19" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>000700</v>
+      </c>
+      <c r="E19" s="7" t="str">
+        <f t="shared" si="6"/>
+        <v>0007FF</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="H19" s="30">
+        <f>B19+'NEW Memory Map'!$B$9</f>
+        <v>247552</v>
+      </c>
+      <c r="I19" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>03C700</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
@@ -2495,28 +3343,28 @@
     </row>
     <row r="6" spans="1:15" s="21" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22">
-        <f>'Memory Map'!A22</f>
+        <f>'OLD Memory Map'!A22</f>
         <v>1</v>
       </c>
       <c r="B6" s="22">
-        <f>'Memory Map'!B22</f>
+        <f>'OLD Memory Map'!B22</f>
         <v>260108</v>
       </c>
       <c r="C6" s="22">
-        <f>'Memory Map'!C22</f>
+        <f>'OLD Memory Map'!C22</f>
         <v>260108</v>
       </c>
       <c r="D6" s="22" t="str">
-        <f>'Memory Map'!D22</f>
+        <f>'OLD Memory Map'!D22</f>
         <v>03F80C</v>
       </c>
       <c r="E6" s="22" t="str">
-        <f>'Memory Map'!E22</f>
+        <f>'OLD Memory Map'!E22</f>
         <v>03F80C</v>
       </c>
       <c r="F6" s="23"/>
       <c r="G6" s="28" t="str">
-        <f>'Memory Map'!G22</f>
+        <f>'OLD Memory Map'!G22</f>
         <v>Graphics mode</v>
       </c>
       <c r="H6" s="24" t="s">
@@ -2576,28 +3424,28 @@
     </row>
     <row r="9" spans="1:15" s="21" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="22">
-        <f>'Memory Map'!A26</f>
+        <f>'OLD Memory Map'!A26</f>
         <v>1</v>
       </c>
       <c r="B9" s="22">
-        <f>'Memory Map'!B26</f>
+        <f>'OLD Memory Map'!B26</f>
         <v>260124</v>
       </c>
       <c r="C9" s="22">
-        <f>'Memory Map'!C26</f>
+        <f>'OLD Memory Map'!C26</f>
         <v>260124</v>
       </c>
       <c r="D9" s="22" t="str">
-        <f>'Memory Map'!D26</f>
+        <f>'OLD Memory Map'!D26</f>
         <v>03F81C</v>
       </c>
       <c r="E9" s="22" t="str">
-        <f>'Memory Map'!E26</f>
+        <f>'OLD Memory Map'!E26</f>
         <v>03F81C</v>
       </c>
       <c r="F9" s="23"/>
       <c r="G9" s="28" t="str">
-        <f>'Memory Map'!G26</f>
+        <f>'OLD Memory Map'!G26</f>
         <v>RS232 status signals</v>
       </c>
       <c r="H9" s="24" t="s">
@@ -2661,31 +3509,31 @@
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <f>'Memory Map'!A30-1</f>
+        <f>'OLD Memory Map'!A30-1</f>
         <v>1</v>
       </c>
       <c r="B12" s="1">
-        <f>'Memory Map'!B30</f>
+        <f>'OLD Memory Map'!B30</f>
         <v>260140</v>
       </c>
       <c r="C12" s="1">
-        <f>'Memory Map'!C30</f>
+        <f>'OLD Memory Map'!C30</f>
         <v>260141</v>
       </c>
       <c r="D12" s="1" t="str">
-        <f>'Memory Map'!D30</f>
+        <f>'OLD Memory Map'!D30</f>
         <v>03F82C</v>
       </c>
       <c r="E12" s="1" t="str">
-        <f>'Memory Map'!E30</f>
+        <f>'OLD Memory Map'!E30</f>
         <v>03F82D</v>
       </c>
       <c r="F12">
-        <f>'Memory Map'!F30</f>
+        <f>'OLD Memory Map'!F30</f>
         <v>0</v>
       </c>
       <c r="G12" s="2" t="str">
-        <f>'Memory Map'!G30</f>
+        <f>'OLD Memory Map'!G30</f>
         <v>IRQ mask</v>
       </c>
       <c r="H12" s="24" t="s">
@@ -2755,27 +3603,27 @@
     </row>
     <row r="17" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="22">
-        <f>'Memory Map'!A34</f>
+        <f>'OLD Memory Map'!A34</f>
         <v>1</v>
       </c>
       <c r="B17" s="22">
-        <f>'Memory Map'!B34</f>
+        <f>'OLD Memory Map'!B34</f>
         <v>260156</v>
       </c>
       <c r="C17" s="22">
-        <f>'Memory Map'!C34</f>
+        <f>'OLD Memory Map'!C34</f>
         <v>260156</v>
       </c>
       <c r="D17" s="22" t="str">
-        <f>'Memory Map'!D34</f>
+        <f>'OLD Memory Map'!D34</f>
         <v>03F83C</v>
       </c>
       <c r="E17" s="22" t="str">
-        <f>'Memory Map'!E34</f>
+        <f>'OLD Memory Map'!E34</f>
         <v>03F83C</v>
       </c>
       <c r="G17" s="29" t="str">
-        <f>'Memory Map'!G34</f>
+        <f>'OLD Memory Map'!G34</f>
         <v>SPI control</v>
       </c>
       <c r="H17" s="24" t="s">
@@ -2823,27 +3671,27 @@
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="22">
-        <f>'Memory Map'!A35</f>
+        <f>'OLD Memory Map'!A35</f>
         <v>1</v>
       </c>
       <c r="B20" s="22">
-        <f>'Memory Map'!B35</f>
+        <f>'OLD Memory Map'!B35</f>
         <v>260160</v>
       </c>
       <c r="C20" s="22">
-        <f>'Memory Map'!C35</f>
+        <f>'OLD Memory Map'!C35</f>
         <v>260160</v>
       </c>
       <c r="D20" s="22" t="str">
-        <f>'Memory Map'!D35</f>
+        <f>'OLD Memory Map'!D35</f>
         <v>03F840</v>
       </c>
       <c r="E20" s="22" t="str">
-        <f>'Memory Map'!E35</f>
+        <f>'OLD Memory Map'!E35</f>
         <v>03F840</v>
       </c>
       <c r="G20" s="2" t="str">
-        <f>'Memory Map'!G35</f>
+        <f>'OLD Memory Map'!G35</f>
         <v>SPI status</v>
       </c>
       <c r="H20" s="24" t="s">
@@ -2885,7 +3733,1404 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:N53"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="5" width="12.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="3.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="34.28515625" style="8" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="30" customWidth="1"/>
+    <col min="9" max="9" width="79.140625" customWidth="1"/>
+    <col min="10" max="12" width="19.140625" customWidth="1"/>
+    <col min="13" max="13" width="11.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+    </row>
+    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H4" s="32" t="s">
+        <v>72</v>
+      </c>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+    </row>
+    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="13"/>
+      <c r="B5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="13"/>
+      <c r="H5" s="32"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+    </row>
+    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="33"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <f>(128)*1024</f>
+        <v>131072</v>
+      </c>
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <f>B7+A7-1</f>
+        <v>131071</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f>DEC2HEX(B7,6)</f>
+        <v>000000</v>
+      </c>
+      <c r="E7" s="7" t="str">
+        <f>DEC2HEX(C7,6)</f>
+        <v>01FFFF</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I7" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <f>(128-12)*1024</f>
+        <v>118784</v>
+      </c>
+      <c r="B8" s="7">
+        <f t="shared" ref="B8:B13" si="0">C7+1</f>
+        <v>131072</v>
+      </c>
+      <c r="C8" s="7">
+        <f>B8+A8-1</f>
+        <v>249855</v>
+      </c>
+      <c r="D8" s="7" t="str">
+        <f t="shared" ref="D8:D9" si="1">DEC2HEX(B8,6)</f>
+        <v>020000</v>
+      </c>
+      <c r="E8" s="7" t="str">
+        <f t="shared" ref="E8:E9" si="2">DEC2HEX(C8,6)</f>
+        <v>03CFFF</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>2048</v>
+      </c>
+      <c r="B9" s="7">
+        <f t="shared" si="0"/>
+        <v>249856</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" ref="C9" si="3">B9+A9-1</f>
+        <v>251903</v>
+      </c>
+      <c r="D9" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03D000</v>
+      </c>
+      <c r="E9" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>03D7FF</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H9" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>2048</v>
+      </c>
+      <c r="B10" s="7">
+        <f t="shared" si="0"/>
+        <v>251904</v>
+      </c>
+      <c r="C10" s="7">
+        <f>B10+A10-1</f>
+        <v>253951</v>
+      </c>
+      <c r="D10" s="7" t="str">
+        <f t="shared" ref="D10:D13" si="4">DEC2HEX(B10,6)</f>
+        <v>03D800</v>
+      </c>
+      <c r="E10" s="7" t="str">
+        <f t="shared" ref="E10:E13" si="5">DEC2HEX(C10,6)</f>
+        <v>03DFFF</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="H10" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <f>2048</f>
+        <v>2048</v>
+      </c>
+      <c r="B11" s="7">
+        <f t="shared" si="0"/>
+        <v>253952</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" ref="C11:C13" si="6">B11+A11-1</f>
+        <v>255999</v>
+      </c>
+      <c r="D11" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>03E000</v>
+      </c>
+      <c r="E11" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>03E7FF</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <f>2048</f>
+        <v>2048</v>
+      </c>
+      <c r="B12" s="7">
+        <f t="shared" si="0"/>
+        <v>256000</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="6"/>
+        <v>258047</v>
+      </c>
+      <c r="D12" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>03E800</v>
+      </c>
+      <c r="E12" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>03EFFF</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>2048</v>
+      </c>
+      <c r="B13" s="7">
+        <f t="shared" si="0"/>
+        <v>258048</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="6"/>
+        <v>260095</v>
+      </c>
+      <c r="D13" s="7" t="str">
+        <f t="shared" si="4"/>
+        <v>03F000</v>
+      </c>
+      <c r="E13" s="7" t="str">
+        <f t="shared" si="5"/>
+        <v>03F7FF</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H13" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="H15" s="31"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+    </row>
+    <row r="16" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="32"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+    </row>
+    <row r="17" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="H17" s="33"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+    </row>
+    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="33"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>4</v>
+      </c>
+      <c r="B19" s="7">
+        <f>C13+1</f>
+        <v>260096</v>
+      </c>
+      <c r="C19" s="7">
+        <f>B19+A19-1</f>
+        <v>260099</v>
+      </c>
+      <c r="D19" s="7" t="str">
+        <f t="shared" ref="D19:D38" si="7">DEC2HEX(B19,6)</f>
+        <v>03F800</v>
+      </c>
+      <c r="E19" s="7" t="str">
+        <f t="shared" ref="E19:E38" si="8">DEC2HEX(C19,6)</f>
+        <v>03F803</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>4</v>
+      </c>
+      <c r="B20" s="7">
+        <f>B19+4</f>
+        <v>260100</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" ref="C20" si="9">B20+A20-1</f>
+        <v>260103</v>
+      </c>
+      <c r="D20" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F804</v>
+      </c>
+      <c r="E20" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F807</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="7">
+        <v>1</v>
+      </c>
+      <c r="B21" s="7">
+        <f t="shared" ref="B21:B37" si="10">B20+4</f>
+        <v>260104</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" ref="C21:C24" si="11">B21+A21-1</f>
+        <v>260104</v>
+      </c>
+      <c r="D21" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F808</v>
+      </c>
+      <c r="E21" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F808</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H21" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>1</v>
+      </c>
+      <c r="B22" s="7">
+        <f t="shared" si="10"/>
+        <v>260108</v>
+      </c>
+      <c r="C22" s="7">
+        <f t="shared" si="11"/>
+        <v>260108</v>
+      </c>
+      <c r="D22" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F80C</v>
+      </c>
+      <c r="E22" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F80C</v>
+      </c>
+      <c r="F22" s="7"/>
+      <c r="G22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="7">
+        <v>1</v>
+      </c>
+      <c r="B23" s="7">
+        <f t="shared" si="10"/>
+        <v>260112</v>
+      </c>
+      <c r="C23" s="7">
+        <f t="shared" si="11"/>
+        <v>260112</v>
+      </c>
+      <c r="D23" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F810</v>
+      </c>
+      <c r="E23" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F810</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H23" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I23" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>1</v>
+      </c>
+      <c r="B24" s="7">
+        <f t="shared" si="10"/>
+        <v>260116</v>
+      </c>
+      <c r="C24" s="7">
+        <f t="shared" si="11"/>
+        <v>260116</v>
+      </c>
+      <c r="D24" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F814</v>
+      </c>
+      <c r="E24" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F814</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
+        <v>2</v>
+      </c>
+      <c r="B25" s="7">
+        <f t="shared" si="10"/>
+        <v>260120</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" ref="C25:C27" si="12">B25+A25-1</f>
+        <v>260121</v>
+      </c>
+      <c r="D25" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F818</v>
+      </c>
+      <c r="E25" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F819</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>1</v>
+      </c>
+      <c r="B26" s="7">
+        <f t="shared" si="10"/>
+        <v>260124</v>
+      </c>
+      <c r="C26" s="7">
+        <f>B26+A26-1</f>
+        <v>260124</v>
+      </c>
+      <c r="D26" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F81C</v>
+      </c>
+      <c r="E26" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F81C</v>
+      </c>
+      <c r="F26" s="7"/>
+      <c r="G26" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
+        <v>1</v>
+      </c>
+      <c r="B27" s="7">
+        <f t="shared" si="10"/>
+        <v>260128</v>
+      </c>
+      <c r="C27" s="7">
+        <f t="shared" si="12"/>
+        <v>260128</v>
+      </c>
+      <c r="D27" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F820</v>
+      </c>
+      <c r="E27" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F820</v>
+      </c>
+      <c r="F27" s="7"/>
+      <c r="G27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I27" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>4</v>
+      </c>
+      <c r="B28" s="7">
+        <f t="shared" si="10"/>
+        <v>260132</v>
+      </c>
+      <c r="C28" s="7">
+        <f t="shared" ref="C28" si="13">B28+A28-1</f>
+        <v>260135</v>
+      </c>
+      <c r="D28" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F824</v>
+      </c>
+      <c r="E28" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F827</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>4</v>
+      </c>
+      <c r="B29" s="7">
+        <f t="shared" si="10"/>
+        <v>260136</v>
+      </c>
+      <c r="C29" s="7">
+        <f t="shared" ref="C29" si="14">B29+A29-1</f>
+        <v>260139</v>
+      </c>
+      <c r="D29" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F828</v>
+      </c>
+      <c r="E29" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F82B</v>
+      </c>
+      <c r="F29" s="7"/>
+      <c r="G29" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="H29" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I29" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="7">
+        <v>2</v>
+      </c>
+      <c r="B30" s="7">
+        <f t="shared" si="10"/>
+        <v>260140</v>
+      </c>
+      <c r="C30" s="7">
+        <f t="shared" ref="C30" si="15">B30+A30-1</f>
+        <v>260141</v>
+      </c>
+      <c r="D30" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F82C</v>
+      </c>
+      <c r="E30" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F82D</v>
+      </c>
+      <c r="F30" s="7"/>
+      <c r="G30" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="H30" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="7">
+        <v>2</v>
+      </c>
+      <c r="B31" s="7">
+        <f t="shared" si="10"/>
+        <v>260144</v>
+      </c>
+      <c r="C31" s="7">
+        <f t="shared" ref="C31:C32" si="16">B31+A31-1</f>
+        <v>260145</v>
+      </c>
+      <c r="D31" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F830</v>
+      </c>
+      <c r="E31" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F831</v>
+      </c>
+      <c r="F31" s="7"/>
+      <c r="G31" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I31" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
+        <v>1</v>
+      </c>
+      <c r="B32" s="7">
+        <f t="shared" si="10"/>
+        <v>260148</v>
+      </c>
+      <c r="C32" s="7">
+        <f t="shared" si="16"/>
+        <v>260148</v>
+      </c>
+      <c r="D32" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F834</v>
+      </c>
+      <c r="E32" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F834</v>
+      </c>
+      <c r="F32" s="7"/>
+      <c r="G32" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I32" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
+        <v>1</v>
+      </c>
+      <c r="B33" s="7">
+        <f t="shared" si="10"/>
+        <v>260152</v>
+      </c>
+      <c r="C33" s="7">
+        <f t="shared" ref="C33:C35" si="17">B33+A33-1</f>
+        <v>260152</v>
+      </c>
+      <c r="D33" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F838</v>
+      </c>
+      <c r="E33" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F838</v>
+      </c>
+      <c r="F33" s="7"/>
+      <c r="G33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="H33" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I33" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A34" s="7">
+        <v>1</v>
+      </c>
+      <c r="B34" s="7">
+        <f t="shared" si="10"/>
+        <v>260156</v>
+      </c>
+      <c r="C34" s="7">
+        <f t="shared" si="17"/>
+        <v>260156</v>
+      </c>
+      <c r="D34" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F83C</v>
+      </c>
+      <c r="E34" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F83C</v>
+      </c>
+      <c r="F34" s="7"/>
+      <c r="G34" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A35" s="7">
+        <v>1</v>
+      </c>
+      <c r="B35" s="7">
+        <f t="shared" si="10"/>
+        <v>260160</v>
+      </c>
+      <c r="C35" s="7">
+        <f t="shared" si="17"/>
+        <v>260160</v>
+      </c>
+      <c r="D35" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F840</v>
+      </c>
+      <c r="E35" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F840</v>
+      </c>
+      <c r="F35" s="7"/>
+      <c r="G35" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="H35" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I35" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36" s="7">
+        <v>1</v>
+      </c>
+      <c r="B36" s="7">
+        <f t="shared" si="10"/>
+        <v>260164</v>
+      </c>
+      <c r="C36" s="7">
+        <f t="shared" ref="C36" si="18">B36+A36-1</f>
+        <v>260164</v>
+      </c>
+      <c r="D36" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F844</v>
+      </c>
+      <c r="E36" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F844</v>
+      </c>
+      <c r="F36" s="7"/>
+      <c r="G36" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I36" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
+        <v>1</v>
+      </c>
+      <c r="B37" s="7">
+        <f t="shared" si="10"/>
+        <v>260168</v>
+      </c>
+      <c r="C37" s="7">
+        <f t="shared" ref="C37" si="19">B37+A37-1</f>
+        <v>260168</v>
+      </c>
+      <c r="D37" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F848</v>
+      </c>
+      <c r="E37" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F848</v>
+      </c>
+      <c r="F37" s="7"/>
+      <c r="G37" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="H37" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I37" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A38" s="7">
+        <f>C38-B38</f>
+        <v>1971</v>
+      </c>
+      <c r="B38" s="7">
+        <f>B37+4</f>
+        <v>260172</v>
+      </c>
+      <c r="C38" s="7">
+        <f>A44-1</f>
+        <v>262143</v>
+      </c>
+      <c r="D38" s="7" t="str">
+        <f t="shared" si="7"/>
+        <v>03F84C</v>
+      </c>
+      <c r="E38" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03FFFF</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H38" s="34"/>
+    </row>
+    <row r="40" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D40" s="16"/>
+      <c r="E40" s="16"/>
+      <c r="F40" s="16"/>
+      <c r="H40" s="31"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+    </row>
+    <row r="41" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" s="13"/>
+      <c r="G41" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H41" s="32"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+    </row>
+    <row r="42" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="13"/>
+      <c r="B42" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F42" s="13"/>
+      <c r="H42" s="32"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+    </row>
+    <row r="43" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="10"/>
+      <c r="H43" s="32"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <f>256*1024</f>
+        <v>262144</v>
+      </c>
+      <c r="B44" s="7">
+        <v>0</v>
+      </c>
+      <c r="C44" s="7">
+        <f>A44-1</f>
+        <v>262143</v>
+      </c>
+      <c r="D44" s="7" t="str">
+        <f>DEC2HEX(B44,6)</f>
+        <v>000000</v>
+      </c>
+      <c r="E44" s="7" t="str">
+        <f>DEC2HEX(C44,6)</f>
+        <v>03FFFF</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H44" s="34"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>256</v>
+      </c>
+      <c r="B45" s="7">
+        <f>C44+1</f>
+        <v>262144</v>
+      </c>
+      <c r="C45" s="7">
+        <f t="shared" ref="C45" si="20">B45+A45-1</f>
+        <v>262399</v>
+      </c>
+      <c r="D45" s="7" t="str">
+        <f t="shared" ref="D45:D46" si="21">DEC2HEX(B45,6)</f>
+        <v>040000</v>
+      </c>
+      <c r="E45" s="7" t="str">
+        <f t="shared" ref="E45:E46" si="22">DEC2HEX(C45,6)</f>
+        <v>0400FF</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>256</v>
+      </c>
+      <c r="B46" s="7">
+        <f>C45+1</f>
+        <v>262400</v>
+      </c>
+      <c r="C46" s="7">
+        <f t="shared" ref="C46" si="23">B46+A46-1</f>
+        <v>262655</v>
+      </c>
+      <c r="D46" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>040100</v>
+      </c>
+      <c r="E46" s="7" t="str">
+        <f t="shared" si="22"/>
+        <v>0401FF</v>
+      </c>
+      <c r="F46" s="7"/>
+      <c r="G46" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H46" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>256</v>
+      </c>
+      <c r="B47" s="7">
+        <f>C46+1</f>
+        <v>262656</v>
+      </c>
+      <c r="C47" s="7">
+        <f t="shared" ref="C47:C51" si="24">B47+A47-1</f>
+        <v>262911</v>
+      </c>
+      <c r="D47" s="7" t="str">
+        <f t="shared" ref="D47:D53" si="25">DEC2HEX(B47,6)</f>
+        <v>040200</v>
+      </c>
+      <c r="E47" s="7" t="str">
+        <f t="shared" ref="E47:E53" si="26">DEC2HEX(C47,6)</f>
+        <v>0402FF</v>
+      </c>
+      <c r="F47" s="7"/>
+      <c r="G47" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="H47" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>256</v>
+      </c>
+      <c r="B48" s="7">
+        <f>C47+1</f>
+        <v>262912</v>
+      </c>
+      <c r="C48" s="7">
+        <f t="shared" si="24"/>
+        <v>263167</v>
+      </c>
+      <c r="D48" s="7" t="str">
+        <f t="shared" si="25"/>
+        <v>040300</v>
+      </c>
+      <c r="E48" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v>0403FF</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>256</v>
+      </c>
+      <c r="B49" s="7">
+        <f t="shared" ref="B49" si="27">C48+1</f>
+        <v>263168</v>
+      </c>
+      <c r="C49" s="7">
+        <f t="shared" si="24"/>
+        <v>263423</v>
+      </c>
+      <c r="D49" s="7" t="str">
+        <f t="shared" si="25"/>
+        <v>040400</v>
+      </c>
+      <c r="E49" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v>0404FF</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>256</v>
+      </c>
+      <c r="B50" s="7">
+        <f t="shared" ref="B50" si="28">C49+1</f>
+        <v>263424</v>
+      </c>
+      <c r="C50" s="7">
+        <f t="shared" ref="C50" si="29">B50+A50-1</f>
+        <v>263679</v>
+      </c>
+      <c r="D50" s="7" t="str">
+        <f t="shared" ref="D50" si="30">DEC2HEX(B50,6)</f>
+        <v>040500</v>
+      </c>
+      <c r="E50" s="7" t="str">
+        <f t="shared" ref="E50" si="31">DEC2HEX(C50,6)</f>
+        <v>0405FF</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="H50" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <f>2*(128*96*2)</f>
+        <v>49152</v>
+      </c>
+      <c r="B51" s="7">
+        <f>C50+1</f>
+        <v>263680</v>
+      </c>
+      <c r="C51" s="7">
+        <f t="shared" si="24"/>
+        <v>312831</v>
+      </c>
+      <c r="D51" s="7" t="str">
+        <f t="shared" si="25"/>
+        <v>040600</v>
+      </c>
+      <c r="E51" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v>04C5FF</v>
+      </c>
+      <c r="F51" s="7"/>
+      <c r="G51" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="H51" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>1024</v>
+      </c>
+      <c r="B52" s="7">
+        <f>C51+1</f>
+        <v>312832</v>
+      </c>
+      <c r="C52" s="7">
+        <f t="shared" ref="C52" si="32">B52+A52-1</f>
+        <v>313855</v>
+      </c>
+      <c r="D52" s="7" t="str">
+        <f t="shared" ref="D52" si="33">DEC2HEX(B52,6)</f>
+        <v>04C600</v>
+      </c>
+      <c r="E52" s="7" t="str">
+        <f t="shared" ref="E52" si="34">DEC2HEX(C52,6)</f>
+        <v>04C9FF</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="G52" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="H52" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <f>C53-B53</f>
+        <v>16463359</v>
+      </c>
+      <c r="B53" s="7">
+        <f>C52+1</f>
+        <v>313856</v>
+      </c>
+      <c r="C53" s="7">
+        <f>16*1024*1024-1</f>
+        <v>16777215</v>
+      </c>
+      <c r="D53" s="7" t="str">
+        <f t="shared" si="25"/>
+        <v>04CA00</v>
+      </c>
+      <c r="E53" s="7" t="str">
+        <f t="shared" si="26"/>
+        <v>FFFFFF</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="H53" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="0.74803149606299202" header="0.31496062992126" footer="0.31496062992126"/>
+  <pageSetup paperSize="9" scale="63" orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Moved up buffers in PSDRAM into available space
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="NEW Memory Map" sheetId="4" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="135">
   <si>
     <t>Name</t>
   </si>
@@ -554,6 +554,12 @@
   </si>
   <si>
     <t>Absolute address</t>
+  </si>
+  <si>
+    <t>FAT buffers for FAT table</t>
+  </si>
+  <si>
+    <t>FAT buffer for sector R/W</t>
   </si>
 </sst>
 </file>
@@ -756,14 +762,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1069,10 +1075,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N59"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2275,11 +2281,11 @@
       <c r="I44" t="s">
         <v>111</v>
       </c>
-      <c r="J44" s="37">
+      <c r="J44" s="36">
         <f>B20+255</f>
         <v>260351</v>
       </c>
-      <c r="K44" s="37" t="str">
+      <c r="K44" s="36" t="str">
         <f>DEC2HEX(J44,6)</f>
         <v>03F8FF</v>
       </c>
@@ -2394,27 +2400,28 @@
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
-        <v>256</v>
+        <f>2*(128*96*2)</f>
+        <v>49152</v>
       </c>
       <c r="B51" s="7">
         <f>C50+1</f>
         <v>262144</v>
       </c>
       <c r="C51" s="7">
-        <f t="shared" ref="C51:C58" si="20">B51+A51-1</f>
-        <v>262399</v>
+        <f t="shared" ref="C51:C53" si="20">B51+A51-1</f>
+        <v>311295</v>
       </c>
       <c r="D51" s="7" t="str">
-        <f t="shared" ref="D51:E59" si="21">DEC2HEX(B51,6)</f>
+        <f t="shared" ref="D51:E54" si="21">DEC2HEX(B51,6)</f>
         <v>040000</v>
       </c>
       <c r="E51" s="7" t="str">
         <f t="shared" si="21"/>
-        <v>0400FF</v>
+        <v>04BFFF</v>
       </c>
       <c r="F51" s="7"/>
       <c r="G51" s="8" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="H51" s="30" t="s">
         <v>72</v>
@@ -2422,27 +2429,27 @@
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="B52" s="7">
         <f>C51+1</f>
-        <v>262400</v>
+        <v>311296</v>
       </c>
       <c r="C52" s="7">
-        <f t="shared" si="20"/>
-        <v>262655</v>
+        <f t="shared" ref="C52" si="22">B52+A52-1</f>
+        <v>311807</v>
       </c>
       <c r="D52" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>040100</v>
+        <f t="shared" ref="D52" si="23">DEC2HEX(B52,6)</f>
+        <v>04C000</v>
       </c>
       <c r="E52" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>0401FF</v>
+        <f t="shared" ref="E52" si="24">DEC2HEX(C52,6)</f>
+        <v>04C1FF</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="8" t="s">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="H52" s="30" t="s">
         <v>72</v>
@@ -2450,27 +2457,27 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
-        <v>256</v>
+        <v>512</v>
       </c>
       <c r="B53" s="7">
         <f>C52+1</f>
-        <v>262656</v>
+        <v>311808</v>
       </c>
       <c r="C53" s="7">
         <f t="shared" si="20"/>
-        <v>262911</v>
+        <v>312319</v>
       </c>
       <c r="D53" s="7" t="str">
         <f t="shared" si="21"/>
-        <v>040200</v>
+        <v>04C200</v>
       </c>
       <c r="E53" s="7" t="str">
         <f t="shared" si="21"/>
-        <v>0402FF</v>
+        <v>04C3FF</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="8" t="s">
-        <v>15</v>
+        <v>133</v>
       </c>
       <c r="H53" s="30" t="s">
         <v>72</v>
@@ -2478,174 +2485,33 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <v>256</v>
+        <f>C54-B54</f>
+        <v>16464895</v>
       </c>
       <c r="B54" s="7">
         <f>C53+1</f>
-        <v>262912</v>
+        <v>312320</v>
       </c>
       <c r="C54" s="7">
-        <f t="shared" si="20"/>
-        <v>263167</v>
+        <f>16*1024*1024-1</f>
+        <v>16777215</v>
       </c>
       <c r="D54" s="7" t="str">
         <f t="shared" si="21"/>
-        <v>040300</v>
+        <v>04C400</v>
       </c>
       <c r="E54" s="7" t="str">
         <f t="shared" si="21"/>
-        <v>0403FF</v>
+        <v>FFFFFF</v>
       </c>
       <c r="F54" s="7"/>
       <c r="G54" s="8" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="H54" s="30" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="7">
-        <v>256</v>
-      </c>
-      <c r="B55" s="7">
-        <f t="shared" ref="B55:B56" si="22">C54+1</f>
-        <v>263168</v>
-      </c>
-      <c r="C55" s="7">
-        <f t="shared" si="20"/>
-        <v>263423</v>
-      </c>
-      <c r="D55" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>040400</v>
-      </c>
-      <c r="E55" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>0404FF</v>
-      </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="H55" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="7">
-        <v>256</v>
-      </c>
-      <c r="B56" s="7">
-        <f t="shared" si="22"/>
-        <v>263424</v>
-      </c>
-      <c r="C56" s="7">
-        <f t="shared" si="20"/>
-        <v>263679</v>
-      </c>
-      <c r="D56" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>040500</v>
-      </c>
-      <c r="E56" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>0405FF</v>
-      </c>
-      <c r="F56" s="7"/>
-      <c r="G56" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="H56" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="7">
-        <f>2*(128*96*2)</f>
-        <v>49152</v>
-      </c>
-      <c r="B57" s="7">
-        <f>C56+1</f>
-        <v>263680</v>
-      </c>
-      <c r="C57" s="7">
-        <f t="shared" si="20"/>
-        <v>312831</v>
-      </c>
-      <c r="D57" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>040600</v>
-      </c>
-      <c r="E57" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>04C5FF</v>
-      </c>
-      <c r="F57" s="7"/>
-      <c r="G57" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="H57" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="7">
-        <v>1024</v>
-      </c>
-      <c r="B58" s="7">
-        <f>C57+1</f>
-        <v>312832</v>
-      </c>
-      <c r="C58" s="7">
-        <f t="shared" si="20"/>
-        <v>313855</v>
-      </c>
-      <c r="D58" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>04C600</v>
-      </c>
-      <c r="E58" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>04C9FF</v>
-      </c>
-      <c r="F58" s="7"/>
-      <c r="G58" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="H58" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="7">
-        <f>C59-B59</f>
-        <v>16463359</v>
-      </c>
-      <c r="B59" s="7">
-        <f>C58+1</f>
-        <v>313856</v>
-      </c>
-      <c r="C59" s="7">
-        <f>16*1024*1024-1</f>
-        <v>16777215</v>
-      </c>
-      <c r="D59" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>04CA00</v>
-      </c>
-      <c r="E59" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>FFFFFF</v>
-      </c>
-      <c r="F59" s="7"/>
-      <c r="G59" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H59" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I59" t="s">
+      <c r="I54" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2659,7 +2525,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -2697,7 +2563,7 @@
       <c r="G3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="37" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2746,11 +2612,11 @@
         <v>3</v>
       </c>
       <c r="D6" s="7" t="str">
-        <f>DEC2HEX(B6,6)</f>
+        <f t="shared" ref="D6:E8" si="0">DEC2HEX(B6,6)</f>
         <v>000000</v>
       </c>
       <c r="E6" s="7" t="str">
-        <f>DEC2HEX(C6,6)</f>
+        <f t="shared" si="0"/>
         <v>000003</v>
       </c>
       <c r="F6" s="7"/>
@@ -2779,11 +2645,11 @@
         <v>7</v>
       </c>
       <c r="D7" s="7" t="str">
-        <f>DEC2HEX(B7,6)</f>
+        <f t="shared" si="0"/>
         <v>000004</v>
       </c>
       <c r="E7" s="7" t="str">
-        <f>DEC2HEX(C7,6)</f>
+        <f t="shared" si="0"/>
         <v>000007</v>
       </c>
       <c r="F7" s="7"/>
@@ -2795,7 +2661,7 @@
         <v>245764</v>
       </c>
       <c r="I7" s="7" t="str">
-        <f t="shared" ref="I7:I19" si="0">DEC2HEX(H7,6)</f>
+        <f t="shared" ref="I7:I19" si="1">DEC2HEX(H7,6)</f>
         <v>03C004</v>
       </c>
     </row>
@@ -2812,11 +2678,11 @@
         <v>11</v>
       </c>
       <c r="D8" s="7" t="str">
-        <f>DEC2HEX(B8,6)</f>
+        <f t="shared" si="0"/>
         <v>000008</v>
       </c>
       <c r="E8" s="7" t="str">
-        <f>DEC2HEX(C8,6)</f>
+        <f t="shared" si="0"/>
         <v>00000B</v>
       </c>
       <c r="F8" s="7"/>
@@ -2828,7 +2694,7 @@
         <v>245768</v>
       </c>
       <c r="I8" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C008</v>
       </c>
     </row>
@@ -2837,19 +2703,19 @@
         <v>4</v>
       </c>
       <c r="B9" s="7">
-        <f t="shared" ref="B9:B15" si="1">C8+1</f>
+        <f t="shared" ref="B9:B15" si="2">C8+1</f>
         <v>12</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" ref="C9:C15" si="2">B9+A9-1</f>
+        <f t="shared" ref="C9:C15" si="3">B9+A9-1</f>
         <v>15</v>
       </c>
       <c r="D9" s="7" t="str">
-        <f t="shared" ref="D9:D15" si="3">DEC2HEX(B9,6)</f>
+        <f t="shared" ref="D9:D15" si="4">DEC2HEX(B9,6)</f>
         <v>00000C</v>
       </c>
       <c r="E9" s="7" t="str">
-        <f t="shared" ref="E9:E15" si="4">DEC2HEX(C9,6)</f>
+        <f t="shared" ref="E9:E15" si="5">DEC2HEX(C9,6)</f>
         <v>00000F</v>
       </c>
       <c r="F9" s="7"/>
@@ -2861,7 +2727,7 @@
         <v>245772</v>
       </c>
       <c r="I9" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C00C</v>
       </c>
     </row>
@@ -2870,19 +2736,19 @@
         <v>4</v>
       </c>
       <c r="B10" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="C10" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="D10" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>000010</v>
       </c>
       <c r="E10" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>000013</v>
       </c>
       <c r="F10" s="7"/>
@@ -2894,7 +2760,7 @@
         <v>245776</v>
       </c>
       <c r="I10" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C010</v>
       </c>
     </row>
@@ -2903,19 +2769,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="C11" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>23</v>
       </c>
       <c r="D11" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>000014</v>
       </c>
       <c r="E11" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>000017</v>
       </c>
       <c r="F11" s="7"/>
@@ -2927,7 +2793,7 @@
         <v>245780</v>
       </c>
       <c r="I11" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C014</v>
       </c>
     </row>
@@ -2936,19 +2802,19 @@
         <v>4</v>
       </c>
       <c r="B12" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="C12" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>27</v>
       </c>
       <c r="D12" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>000018</v>
       </c>
       <c r="E12" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00001B</v>
       </c>
       <c r="F12" s="7"/>
@@ -2960,7 +2826,7 @@
         <v>245784</v>
       </c>
       <c r="I12" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C018</v>
       </c>
     </row>
@@ -2969,19 +2835,19 @@
         <v>1</v>
       </c>
       <c r="B13" s="7">
-        <f t="shared" si="1"/>
-        <v>28</v>
-      </c>
-      <c r="C13" s="7">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
+      <c r="C13" s="7">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
       <c r="D13" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00001C</v>
       </c>
       <c r="E13" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00001C</v>
       </c>
       <c r="F13" s="7"/>
@@ -2993,7 +2859,7 @@
         <v>245788</v>
       </c>
       <c r="I13" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C01C</v>
       </c>
     </row>
@@ -3002,19 +2868,19 @@
         <v>1</v>
       </c>
       <c r="B14" s="7">
-        <f t="shared" si="1"/>
-        <v>29</v>
-      </c>
-      <c r="C14" s="7">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
+      <c r="C14" s="7">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
       <c r="D14" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00001D</v>
       </c>
       <c r="E14" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00001D</v>
       </c>
       <c r="F14" s="7"/>
@@ -3026,7 +2892,7 @@
         <v>245789</v>
       </c>
       <c r="I14" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C01D</v>
       </c>
     </row>
@@ -3035,19 +2901,19 @@
         <v>14</v>
       </c>
       <c r="B15" s="7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>30</v>
       </c>
       <c r="C15" s="7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
       <c r="D15" s="7" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>00001E</v>
       </c>
       <c r="E15" s="7" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>00002B</v>
       </c>
       <c r="F15" s="7"/>
@@ -3059,7 +2925,7 @@
         <v>245790</v>
       </c>
       <c r="I15" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C01E</v>
       </c>
     </row>
@@ -3077,11 +2943,11 @@
         <v>1023</v>
       </c>
       <c r="D16" s="7" t="str">
-        <f t="shared" ref="D16:D19" si="5">DEC2HEX(B16,6)</f>
+        <f t="shared" ref="D16:D19" si="6">DEC2HEX(B16,6)</f>
         <v>00002C</v>
       </c>
       <c r="E16" s="7" t="str">
-        <f t="shared" ref="E16:E19" si="6">DEC2HEX(C16,6)</f>
+        <f t="shared" ref="E16:E19" si="7">DEC2HEX(C16,6)</f>
         <v>0003FF</v>
       </c>
       <c r="F16" s="7"/>
@@ -3093,7 +2959,7 @@
         <v>245804</v>
       </c>
       <c r="I16" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C02C</v>
       </c>
     </row>
@@ -3110,11 +2976,11 @@
         <v>1535</v>
       </c>
       <c r="D17" s="7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>000400</v>
       </c>
       <c r="E17" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0005FF</v>
       </c>
       <c r="F17" s="7"/>
@@ -3126,7 +2992,7 @@
         <v>246784</v>
       </c>
       <c r="I17" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C400</v>
       </c>
     </row>
@@ -3143,11 +3009,11 @@
         <v>1791</v>
       </c>
       <c r="D18" s="7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>000600</v>
       </c>
       <c r="E18" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0006FF</v>
       </c>
       <c r="F18" s="7"/>
@@ -3159,7 +3025,7 @@
         <v>247296</v>
       </c>
       <c r="I18" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C600</v>
       </c>
     </row>
@@ -3176,11 +3042,11 @@
         <v>2047</v>
       </c>
       <c r="D19" s="7" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>000700</v>
       </c>
       <c r="E19" s="7" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0007FF</v>
       </c>
       <c r="F19" s="7"/>
@@ -3192,7 +3058,7 @@
         <v>247552</v>
       </c>
       <c r="I19" s="7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>03C700</v>
       </c>
     </row>
@@ -3382,11 +3248,11 @@
       <c r="L6" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="M6" s="36" t="s">
+      <c r="M6" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
     </row>
     <row r="7" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>

</xml_diff>

<commit_message>
Tested first stage of virtualization module (system memory interface) in hardware Updated distributed RAM to register outputs (i.e. synchronous read mode)
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -4,21 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425"/>
+    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NEW Memory Map" sheetId="4" r:id="rId1"/>
     <sheet name="USER" sheetId="5" r:id="rId2"/>
-    <sheet name="Hardware registers" sheetId="2" r:id="rId3"/>
-    <sheet name="OLD Memory Map" sheetId="1" r:id="rId4"/>
-    <sheet name="Copyright and license" sheetId="3" r:id="rId5"/>
+    <sheet name="Virtualization" sheetId="6" r:id="rId3"/>
+    <sheet name="Hardware registers" sheetId="2" r:id="rId4"/>
+    <sheet name="OLD Memory Map" sheetId="1" r:id="rId5"/>
+    <sheet name="Copyright and license" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="142">
   <si>
     <t>Name</t>
   </si>
@@ -560,6 +561,27 @@
   </si>
   <si>
     <t>FAT buffer for sector R/W</t>
+  </si>
+  <si>
+    <t>Virtualization control</t>
+  </si>
+  <si>
+    <t>Access to virtualization control registers</t>
+  </si>
+  <si>
+    <t>Virtualization registers</t>
+  </si>
+  <si>
+    <t>SingleMulti</t>
+  </si>
+  <si>
+    <t>Task Control</t>
+  </si>
+  <si>
+    <t>PC Override</t>
+  </si>
+  <si>
+    <t>Virtual interrupt</t>
   </si>
 </sst>
 </file>
@@ -1075,10 +1097,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1214,24 +1236,24 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <f>(128-16)*1024</f>
-        <v>114688</v>
+        <f>(128-18)*1024</f>
+        <v>112640</v>
       </c>
       <c r="B8" s="7">
-        <f t="shared" ref="B8:B14" si="0">C7+1</f>
+        <f t="shared" ref="B8:B15" si="0">C7+1</f>
         <v>131072</v>
       </c>
       <c r="C8" s="7">
         <f>B8+A8-1</f>
-        <v>245759</v>
+        <v>243711</v>
       </c>
       <c r="D8" s="7" t="str">
-        <f t="shared" ref="D8:E14" si="1">DEC2HEX(B8,6)</f>
+        <f t="shared" ref="D8:E15" si="1">DEC2HEX(B8,6)</f>
         <v>020000</v>
       </c>
       <c r="E8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03BFFF</v>
+        <v>03B7FF</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8" t="s">
@@ -1240,64 +1262,64 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <v>4096</v>
+        <v>2048</v>
       </c>
       <c r="B9" s="7">
         <f>C8+1</f>
-        <v>245760</v>
+        <v>243712</v>
       </c>
       <c r="C9" s="7">
         <f t="shared" ref="C9" si="2">B9+A9-1</f>
-        <v>249855</v>
+        <v>245759</v>
       </c>
       <c r="D9" s="7" t="str">
-        <f t="shared" ref="D9" si="3">DEC2HEX(B9,6)</f>
-        <v>03C000</v>
+        <f t="shared" si="1"/>
+        <v>03B800</v>
       </c>
       <c r="E9" s="7" t="str">
-        <f t="shared" ref="E9" si="4">DEC2HEX(C9,6)</f>
-        <v>03CFFF</v>
+        <f t="shared" si="1"/>
+        <v>03BFFF</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8" t="s">
-        <v>102</v>
+        <v>135</v>
       </c>
       <c r="H9" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>103</v>
+        <v>136</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="B10" s="7">
         <f>C9+1</f>
-        <v>249856</v>
+        <v>245760</v>
       </c>
       <c r="C10" s="7">
-        <f t="shared" ref="C10" si="5">B10+A10-1</f>
-        <v>251903</v>
+        <f t="shared" ref="C10" si="3">B10+A10-1</f>
+        <v>249855</v>
       </c>
       <c r="D10" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>03D000</v>
+        <f t="shared" ref="D10" si="4">DEC2HEX(B10,6)</f>
+        <v>03C000</v>
       </c>
       <c r="E10" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>03D7FF</v>
+        <f t="shared" ref="E10" si="5">DEC2HEX(C10,6)</f>
+        <v>03CFFF</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8" t="s">
-        <v>4</v>
+        <v>102</v>
       </c>
       <c r="H10" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I10" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1305,62 +1327,61 @@
         <v>2048</v>
       </c>
       <c r="B11" s="7">
+        <f>C10+1</f>
+        <v>249856</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" ref="C11" si="6">B11+A11-1</f>
+        <v>251903</v>
+      </c>
+      <c r="D11" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03D000</v>
+      </c>
+      <c r="E11" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03D7FF</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>2048</v>
+      </c>
+      <c r="B12" s="7">
         <f t="shared" si="0"/>
         <v>251904</v>
       </c>
-      <c r="C11" s="7">
-        <f>B11+A11-1</f>
+      <c r="C12" s="7">
+        <f>B12+A12-1</f>
         <v>253951</v>
       </c>
-      <c r="D11" s="7" t="str">
+      <c r="D12" s="7" t="str">
         <f t="shared" si="1"/>
         <v>03D800</v>
       </c>
-      <c r="E11" s="7" t="str">
+      <c r="E12" s="7" t="str">
         <f t="shared" si="1"/>
         <v>03DFFF</v>
       </c>
-      <c r="F11" s="7"/>
-      <c r="G11" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="H11" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <f>2048</f>
-        <v>2048</v>
-      </c>
-      <c r="B12" s="7">
-        <f t="shared" si="0"/>
-        <v>253952</v>
-      </c>
-      <c r="C12" s="7">
-        <f t="shared" ref="C12:C14" si="6">B12+A12-1</f>
-        <v>255999</v>
-      </c>
-      <c r="D12" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>03E000</v>
-      </c>
-      <c r="E12" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>03E7FF</v>
-      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="8" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="H12" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I12" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1370,101 +1391,105 @@
       </c>
       <c r="B13" s="7">
         <f t="shared" si="0"/>
-        <v>256000</v>
+        <v>253952</v>
       </c>
       <c r="C13" s="7">
-        <f t="shared" si="6"/>
-        <v>258047</v>
+        <f t="shared" ref="C13:C15" si="7">B13+A13-1</f>
+        <v>255999</v>
       </c>
       <c r="D13" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03E800</v>
+        <v>03E000</v>
       </c>
       <c r="E13" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03EFFF</v>
+        <v>03E7FF</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H13" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
+        <f>2048</f>
         <v>2048</v>
       </c>
       <c r="B14" s="7">
         <f t="shared" si="0"/>
-        <v>258048</v>
+        <v>256000</v>
       </c>
       <c r="C14" s="7">
-        <f t="shared" si="6"/>
-        <v>260095</v>
+        <f t="shared" si="7"/>
+        <v>258047</v>
       </c>
       <c r="D14" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03F000</v>
+        <v>03E800</v>
       </c>
       <c r="E14" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03F7FF</v>
+        <v>03EFFF</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8" t="s">
-        <v>101</v>
+        <v>3</v>
       </c>
       <c r="H14" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="7">
+        <v>2048</v>
+      </c>
+      <c r="B15" s="7">
+        <f t="shared" si="0"/>
+        <v>258048</v>
+      </c>
+      <c r="C15" s="7">
+        <f t="shared" si="7"/>
+        <v>260095</v>
+      </c>
+      <c r="D15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03F000</v>
+      </c>
+      <c r="E15" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03F7FF</v>
+      </c>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="H15" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I15" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="14" t="s">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="3"/>
+    </row>
+    <row r="17" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="H16" s="31"/>
-      <c r="I16"/>
-      <c r="J16"/>
-      <c r="K16"/>
-      <c r="L16"/>
-      <c r="M16"/>
-      <c r="N16"/>
-    </row>
-    <row r="17" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D17" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="13"/>
-      <c r="G17" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="32"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="16"/>
+      <c r="F17" s="16"/>
+      <c r="H17" s="31"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1472,22 +1497,27 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="15"/>
+    <row r="18" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="13" t="s">
+        <v>6</v>
+      </c>
       <c r="B18" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F18" s="13"/>
-      <c r="H18" s="33"/>
+      <c r="G18" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="32"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1495,14 +1525,21 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="11"/>
+    <row r="19" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" s="13"/>
       <c r="H19" s="33"/>
       <c r="I19"/>
       <c r="J19"/>
@@ -1511,97 +1548,82 @@
       <c r="M19"/>
       <c r="N19"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="7">
-        <v>4</v>
-      </c>
-      <c r="B20" s="7">
-        <f>C14+1</f>
-        <v>260096</v>
-      </c>
-      <c r="C20" s="7">
-        <f>B20+A20-1</f>
-        <v>260099</v>
-      </c>
-      <c r="D20" s="7" t="str">
-        <f t="shared" ref="D20:E39" si="7">DEC2HEX(B20,6)</f>
-        <v>03F800</v>
-      </c>
-      <c r="E20" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F803</v>
-      </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H20" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I20" t="s">
-        <v>28</v>
-      </c>
+    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+      <c r="B20" s="4"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="33"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>4</v>
       </c>
       <c r="B21" s="7">
-        <f>B20+4</f>
-        <v>260100</v>
+        <f>C15+1</f>
+        <v>260096</v>
       </c>
       <c r="C21" s="7">
-        <f t="shared" ref="C21:C38" si="8">B21+A21-1</f>
-        <v>260103</v>
+        <f>B21+A21-1</f>
+        <v>260099</v>
       </c>
       <c r="D21" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F804</v>
+        <f t="shared" ref="D21:E40" si="8">DEC2HEX(B21,6)</f>
+        <v>03F800</v>
       </c>
       <c r="E21" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F807</v>
+        <f t="shared" si="8"/>
+        <v>03F803</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="8" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
       <c r="H21" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B22" s="7">
-        <f t="shared" ref="B22:B38" si="9">B21+4</f>
-        <v>260104</v>
+        <f>B21+4</f>
+        <v>260100</v>
       </c>
       <c r="C22" s="7">
-        <f t="shared" si="8"/>
-        <v>260104</v>
+        <f t="shared" ref="C22:C39" si="9">B22+A22-1</f>
+        <v>260103</v>
       </c>
       <c r="D22" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F808</v>
+        <f t="shared" si="8"/>
+        <v>03F804</v>
       </c>
       <c r="E22" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F808</v>
+        <f t="shared" si="8"/>
+        <v>03F807</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1609,30 +1631,30 @@
         <v>1</v>
       </c>
       <c r="B23" s="7">
+        <f t="shared" ref="B23:B39" si="10">B22+4</f>
+        <v>260104</v>
+      </c>
+      <c r="C23" s="7">
         <f t="shared" si="9"/>
-        <v>260108</v>
-      </c>
-      <c r="C23" s="7">
-        <f t="shared" si="8"/>
-        <v>260108</v>
+        <v>260104</v>
       </c>
       <c r="D23" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F80C</v>
+        <f t="shared" si="8"/>
+        <v>03F808</v>
       </c>
       <c r="E23" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F80C</v>
+        <f t="shared" si="8"/>
+        <v>03F808</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1640,30 +1662,30 @@
         <v>1</v>
       </c>
       <c r="B24" s="7">
+        <f t="shared" si="10"/>
+        <v>260108</v>
+      </c>
+      <c r="C24" s="7">
         <f t="shared" si="9"/>
-        <v>260112</v>
-      </c>
-      <c r="C24" s="7">
-        <f t="shared" si="8"/>
-        <v>260112</v>
+        <v>260108</v>
       </c>
       <c r="D24" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F810</v>
+        <f t="shared" si="8"/>
+        <v>03F80C</v>
       </c>
       <c r="E24" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F810</v>
+        <f t="shared" si="8"/>
+        <v>03F80C</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I24" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
@@ -1671,92 +1693,92 @@
         <v>1</v>
       </c>
       <c r="B25" s="7">
+        <f t="shared" si="10"/>
+        <v>260112</v>
+      </c>
+      <c r="C25" s="7">
+        <f t="shared" si="9"/>
+        <v>260112</v>
+      </c>
+      <c r="D25" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F810</v>
+      </c>
+      <c r="E25" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F810</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H25" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I25" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="7">
+        <v>1</v>
+      </c>
+      <c r="B26" s="7">
+        <f t="shared" si="10"/>
+        <v>260116</v>
+      </c>
+      <c r="C26" s="7">
         <f t="shared" si="9"/>
         <v>260116</v>
       </c>
-      <c r="C25" s="7">
-        <f t="shared" si="8"/>
-        <v>260116</v>
-      </c>
-      <c r="D25" s="7" t="str">
-        <f t="shared" si="7"/>
+      <c r="D26" s="7" t="str">
+        <f t="shared" si="8"/>
         <v>03F814</v>
       </c>
-      <c r="E25" s="7" t="str">
-        <f t="shared" si="7"/>
+      <c r="E26" s="7" t="str">
+        <f t="shared" si="8"/>
         <v>03F814</v>
-      </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="I25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="7">
-        <v>2</v>
-      </c>
-      <c r="B26" s="7">
-        <f t="shared" si="9"/>
-        <v>260120</v>
-      </c>
-      <c r="C26" s="7">
-        <f t="shared" si="8"/>
-        <v>260121</v>
-      </c>
-      <c r="D26" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F818</v>
-      </c>
-      <c r="E26" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F819</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="H26" s="30" t="s">
         <v>73</v>
       </c>
       <c r="I26" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" s="7">
+        <f t="shared" si="10"/>
+        <v>260120</v>
+      </c>
+      <c r="C27" s="7">
         <f t="shared" si="9"/>
-        <v>260124</v>
-      </c>
-      <c r="C27" s="7">
-        <f>B27+A27-1</f>
-        <v>260124</v>
+        <v>260121</v>
       </c>
       <c r="D27" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F81C</v>
+        <f t="shared" si="8"/>
+        <v>03F818</v>
       </c>
       <c r="E27" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F81C</v>
+        <f t="shared" si="8"/>
+        <v>03F819</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I27" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -1764,61 +1786,61 @@
         <v>1</v>
       </c>
       <c r="B28" s="7">
+        <f t="shared" si="10"/>
+        <v>260124</v>
+      </c>
+      <c r="C28" s="7">
+        <f>B28+A28-1</f>
+        <v>260124</v>
+      </c>
+      <c r="D28" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F81C</v>
+      </c>
+      <c r="E28" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F81C</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="I28" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>1</v>
+      </c>
+      <c r="B29" s="7">
+        <f t="shared" si="10"/>
+        <v>260128</v>
+      </c>
+      <c r="C29" s="7">
         <f t="shared" si="9"/>
         <v>260128</v>
       </c>
-      <c r="C28" s="7">
-        <f t="shared" si="8"/>
-        <v>260128</v>
-      </c>
-      <c r="D28" s="7" t="str">
-        <f t="shared" si="7"/>
+      <c r="D29" s="7" t="str">
+        <f t="shared" si="8"/>
         <v>03F820</v>
       </c>
-      <c r="E28" s="7" t="str">
-        <f t="shared" si="7"/>
+      <c r="E29" s="7" t="str">
+        <f t="shared" si="8"/>
         <v>03F820</v>
-      </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="I28" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="7">
-        <v>4</v>
-      </c>
-      <c r="B29" s="7">
-        <f t="shared" si="9"/>
-        <v>260132</v>
-      </c>
-      <c r="C29" s="7">
-        <f t="shared" si="8"/>
-        <v>260135</v>
-      </c>
-      <c r="D29" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F824</v>
-      </c>
-      <c r="E29" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F827</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H29" s="30" t="s">
         <v>74</v>
       </c>
       <c r="I29" t="s">
-        <v>106</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -1826,61 +1848,61 @@
         <v>4</v>
       </c>
       <c r="B30" s="7">
+        <f t="shared" si="10"/>
+        <v>260132</v>
+      </c>
+      <c r="C30" s="7">
         <f t="shared" si="9"/>
-        <v>260136</v>
-      </c>
-      <c r="C30" s="7">
-        <f t="shared" si="8"/>
-        <v>260139</v>
+        <v>260135</v>
       </c>
       <c r="D30" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F828</v>
+        <f t="shared" si="8"/>
+        <v>03F824</v>
       </c>
       <c r="E30" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F82B</v>
+        <f t="shared" si="8"/>
+        <v>03F827</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H30" s="30" t="s">
         <v>74</v>
       </c>
       <c r="I30" t="s">
-        <v>41</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B31" s="7">
+        <f t="shared" si="10"/>
+        <v>260136</v>
+      </c>
+      <c r="C31" s="7">
         <f t="shared" si="9"/>
-        <v>260140</v>
-      </c>
-      <c r="C31" s="7">
-        <f t="shared" si="8"/>
-        <v>260141</v>
+        <v>260139</v>
       </c>
       <c r="D31" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F82C</v>
+        <f t="shared" si="8"/>
+        <v>03F828</v>
       </c>
       <c r="E31" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F82D</v>
+        <f t="shared" si="8"/>
+        <v>03F82B</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I31" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
@@ -1888,61 +1910,61 @@
         <v>2</v>
       </c>
       <c r="B32" s="7">
+        <f t="shared" si="10"/>
+        <v>260140</v>
+      </c>
+      <c r="C32" s="7">
         <f t="shared" si="9"/>
-        <v>260144</v>
-      </c>
-      <c r="C32" s="7">
-        <f t="shared" si="8"/>
-        <v>260145</v>
+        <v>260141</v>
       </c>
       <c r="D32" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F830</v>
+        <f t="shared" si="8"/>
+        <v>03F82C</v>
       </c>
       <c r="E32" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F831</v>
+        <f t="shared" si="8"/>
+        <v>03F82D</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="8" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I32" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" s="7">
+        <f t="shared" si="10"/>
+        <v>260144</v>
+      </c>
+      <c r="C33" s="7">
         <f t="shared" si="9"/>
-        <v>260148</v>
-      </c>
-      <c r="C33" s="7">
-        <f t="shared" si="8"/>
-        <v>260148</v>
+        <v>260145</v>
       </c>
       <c r="D33" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F834</v>
+        <f t="shared" si="8"/>
+        <v>03F830</v>
       </c>
       <c r="E33" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F834</v>
+        <f t="shared" si="8"/>
+        <v>03F831</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="8" t="s">
-        <v>17</v>
+        <v>44</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I33" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -1950,30 +1972,30 @@
         <v>1</v>
       </c>
       <c r="B34" s="7">
+        <f t="shared" si="10"/>
+        <v>260148</v>
+      </c>
+      <c r="C34" s="7">
         <f t="shared" si="9"/>
-        <v>260152</v>
-      </c>
-      <c r="C34" s="7">
-        <f t="shared" si="8"/>
-        <v>260152</v>
+        <v>260148</v>
       </c>
       <c r="D34" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F838</v>
+        <f t="shared" si="8"/>
+        <v>03F834</v>
       </c>
       <c r="E34" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F838</v>
+        <f t="shared" si="8"/>
+        <v>03F834</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I34" t="s">
-        <v>77</v>
+        <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -1981,30 +2003,30 @@
         <v>1</v>
       </c>
       <c r="B35" s="7">
+        <f t="shared" si="10"/>
+        <v>260152</v>
+      </c>
+      <c r="C35" s="7">
         <f t="shared" si="9"/>
-        <v>260156</v>
-      </c>
-      <c r="C35" s="7">
-        <f t="shared" si="8"/>
-        <v>260156</v>
+        <v>260152</v>
       </c>
       <c r="D35" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F83C</v>
+        <f t="shared" si="8"/>
+        <v>03F838</v>
       </c>
       <c r="E35" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F83C</v>
+        <f t="shared" si="8"/>
+        <v>03F838</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H35" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I35" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -2012,27 +2034,27 @@
         <v>1</v>
       </c>
       <c r="B36" s="7">
+        <f t="shared" si="10"/>
+        <v>260156</v>
+      </c>
+      <c r="C36" s="7">
         <f t="shared" si="9"/>
-        <v>260160</v>
-      </c>
-      <c r="C36" s="7">
-        <f t="shared" si="8"/>
-        <v>260160</v>
+        <v>260156</v>
       </c>
       <c r="D36" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F840</v>
+        <f t="shared" si="8"/>
+        <v>03F83C</v>
       </c>
       <c r="E36" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F840</v>
+        <f t="shared" si="8"/>
+        <v>03F83C</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="8" t="s">
-        <v>86</v>
+        <v>24</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I36" t="s">
         <v>33</v>
@@ -2043,30 +2065,30 @@
         <v>1</v>
       </c>
       <c r="B37" s="7">
+        <f t="shared" si="10"/>
+        <v>260160</v>
+      </c>
+      <c r="C37" s="7">
         <f t="shared" si="9"/>
-        <v>260164</v>
-      </c>
-      <c r="C37" s="7">
-        <f t="shared" si="8"/>
-        <v>260164</v>
+        <v>260160</v>
       </c>
       <c r="D37" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F844</v>
+        <f t="shared" si="8"/>
+        <v>03F840</v>
       </c>
       <c r="E37" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F844</v>
+        <f t="shared" si="8"/>
+        <v>03F840</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="8" t="s">
-        <v>25</v>
+        <v>86</v>
       </c>
       <c r="H37" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I37" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -2074,119 +2096,119 @@
         <v>1</v>
       </c>
       <c r="B38" s="7">
+        <f t="shared" si="10"/>
+        <v>260164</v>
+      </c>
+      <c r="C38" s="7">
+        <f t="shared" si="9"/>
+        <v>260164</v>
+      </c>
+      <c r="D38" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F844</v>
+      </c>
+      <c r="E38" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F844</v>
+      </c>
+      <c r="F38" s="7"/>
+      <c r="G38" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="H38" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="I38" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A39" s="7">
+        <v>1</v>
+      </c>
+      <c r="B39" s="7">
+        <f t="shared" si="10"/>
+        <v>260168</v>
+      </c>
+      <c r="C39" s="7">
         <f t="shared" si="9"/>
         <v>260168</v>
       </c>
-      <c r="C38" s="7">
-        <f t="shared" si="8"/>
-        <v>260168</v>
-      </c>
-      <c r="D38" s="7" t="str">
-        <f t="shared" si="7"/>
+      <c r="D39" s="7" t="str">
+        <f t="shared" si="8"/>
         <v>03F848</v>
       </c>
-      <c r="E38" s="7" t="str">
-        <f t="shared" si="7"/>
+      <c r="E39" s="7" t="str">
+        <f t="shared" si="8"/>
         <v>03F848</v>
       </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8" t="s">
+      <c r="F39" s="7"/>
+      <c r="G39" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H38" s="30" t="s">
+      <c r="H39" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I39" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="7">
-        <f>C39-B39</f>
-        <v>1827</v>
-      </c>
-      <c r="B39" s="7">
-        <f>B38+4</f>
-        <v>260172</v>
-      </c>
-      <c r="C39" s="7">
-        <f>B40-1</f>
-        <v>261999</v>
-      </c>
-      <c r="D39" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03F84C</v>
-      </c>
-      <c r="E39" s="7" t="str">
-        <f t="shared" si="7"/>
-        <v>03FF6F</v>
-      </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="12" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
+        <f>C40-B40</f>
+        <v>1827</v>
+      </c>
+      <c r="B40" s="7">
+        <f>B39+4</f>
+        <v>260172</v>
+      </c>
+      <c r="C40" s="7">
+        <f>B41-1</f>
+        <v>261999</v>
+      </c>
+      <c r="D40" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03F84C</v>
+      </c>
+      <c r="E40" s="7" t="str">
+        <f t="shared" si="8"/>
+        <v>03FF6F</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
         <f>4*32</f>
         <v>128</v>
       </c>
-      <c r="B40" s="7">
-        <f>B41-A40</f>
+      <c r="B41" s="7">
+        <f>B42-A41</f>
         <v>262000</v>
-      </c>
-      <c r="C40" s="7">
-        <f>B40+A40-1</f>
-        <v>262127</v>
-      </c>
-      <c r="D40" s="7" t="str">
-        <f t="shared" ref="D40:D41" si="10">DEC2HEX(B40,6)</f>
-        <v>03FF70</v>
-      </c>
-      <c r="E40" s="7" t="str">
-        <f t="shared" ref="E40:E41" si="11">DEC2HEX(C40,6)</f>
-        <v>03FFEF</v>
-      </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H40" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I40" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
-        <v>4</v>
-      </c>
-      <c r="B41" s="7">
-        <f t="shared" ref="B41" si="12">B42-A41</f>
-        <v>262128</v>
       </c>
       <c r="C41" s="7">
         <f>B41+A41-1</f>
-        <v>262131</v>
+        <v>262127</v>
       </c>
       <c r="D41" s="7" t="str">
-        <f t="shared" si="10"/>
-        <v>03FFF0</v>
+        <f t="shared" ref="D41:D42" si="11">DEC2HEX(B41,6)</f>
+        <v>03FF70</v>
       </c>
       <c r="E41" s="7" t="str">
-        <f t="shared" si="11"/>
-        <v>03FFF3</v>
+        <f t="shared" ref="E41:E42" si="12">DEC2HEX(C41,6)</f>
+        <v>03FFEF</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="8" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H41" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I41" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -2194,30 +2216,30 @@
         <v>4</v>
       </c>
       <c r="B42" s="7">
-        <f t="shared" ref="B42:B43" si="13">B43-A42</f>
-        <v>262132</v>
+        <f t="shared" ref="B42" si="13">B43-A42</f>
+        <v>262128</v>
       </c>
       <c r="C42" s="7">
         <f>B42+A42-1</f>
-        <v>262135</v>
+        <v>262131</v>
       </c>
       <c r="D42" s="7" t="str">
-        <f t="shared" ref="D42" si="14">DEC2HEX(B42,6)</f>
-        <v>03FFF4</v>
+        <f t="shared" si="11"/>
+        <v>03FFF0</v>
       </c>
       <c r="E42" s="7" t="str">
-        <f t="shared" ref="E42" si="15">DEC2HEX(C42,6)</f>
-        <v>03FFF7</v>
+        <f t="shared" si="12"/>
+        <v>03FFF3</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="8" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I42" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -2225,106 +2247,109 @@
         <v>4</v>
       </c>
       <c r="B43" s="7">
-        <f t="shared" si="13"/>
-        <v>262136</v>
+        <f t="shared" ref="B43:B44" si="14">B44-A43</f>
+        <v>262132</v>
       </c>
       <c r="C43" s="7">
         <f>B43+A43-1</f>
-        <v>262139</v>
+        <v>262135</v>
       </c>
       <c r="D43" s="7" t="str">
-        <f t="shared" ref="D43" si="16">DEC2HEX(B43,6)</f>
-        <v>03FFF8</v>
+        <f t="shared" ref="D43" si="15">DEC2HEX(B43,6)</f>
+        <v>03FFF4</v>
       </c>
       <c r="E43" s="7" t="str">
-        <f t="shared" ref="E43" si="17">DEC2HEX(C43,6)</f>
-        <v>03FFFB</v>
+        <f t="shared" ref="E43" si="16">DEC2HEX(C43,6)</f>
+        <v>03FFF7</v>
       </c>
       <c r="F43" s="7"/>
       <c r="G43" s="8" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H43" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I43" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>4</v>
       </c>
       <c r="B44" s="7">
-        <f>B51-A44</f>
-        <v>262140</v>
+        <f t="shared" si="14"/>
+        <v>262136</v>
       </c>
       <c r="C44" s="7">
         <f>B44+A44-1</f>
-        <v>262143</v>
+        <v>262139</v>
       </c>
       <c r="D44" s="7" t="str">
-        <f t="shared" ref="D44" si="18">DEC2HEX(B44,6)</f>
-        <v>03FFFC</v>
+        <f t="shared" ref="D44" si="17">DEC2HEX(B44,6)</f>
+        <v>03FFF8</v>
       </c>
       <c r="E44" s="7" t="str">
-        <f t="shared" ref="E44" si="19">DEC2HEX(C44,6)</f>
-        <v>03FFFF</v>
+        <f t="shared" ref="E44" si="18">DEC2HEX(C44,6)</f>
+        <v>03FFFB</v>
       </c>
       <c r="F44" s="7"/>
       <c r="G44" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A45" s="7">
+        <v>4</v>
+      </c>
+      <c r="B45" s="7">
+        <f>B52-A45</f>
+        <v>262140</v>
+      </c>
+      <c r="C45" s="7">
+        <f>B45+A45-1</f>
+        <v>262143</v>
+      </c>
+      <c r="D45" s="7" t="str">
+        <f t="shared" ref="D45" si="19">DEC2HEX(B45,6)</f>
+        <v>03FFFC</v>
+      </c>
+      <c r="E45" s="7" t="str">
+        <f t="shared" ref="E45" si="20">DEC2HEX(C45,6)</f>
+        <v>03FFFF</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="H44" s="30" t="s">
+      <c r="H45" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I45" t="s">
         <v>111</v>
       </c>
-      <c r="J44" s="36">
-        <f>B20+255</f>
+      <c r="J45" s="36">
+        <f>B21+255</f>
         <v>260351</v>
       </c>
-      <c r="K44" s="36" t="str">
-        <f>DEC2HEX(J44,6)</f>
+      <c r="K45" s="36" t="str">
+        <f>DEC2HEX(J45,6)</f>
         <v>03F8FF</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="10" t="s">
+    <row r="47" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D46" s="16"/>
-      <c r="E46" s="16"/>
-      <c r="F46" s="16"/>
-      <c r="H46" s="30"/>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46"/>
-      <c r="L46"/>
-      <c r="M46"/>
-      <c r="N46"/>
-    </row>
-    <row r="47" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B47" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C47" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D47" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F47" s="13"/>
-      <c r="G47" s="10" t="s">
-        <v>0</v>
-      </c>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
       <c r="H47" s="30"/>
       <c r="I47"/>
       <c r="J47"/>
@@ -2334,20 +2359,25 @@
       <c r="N47"/>
     </row>
     <row r="48" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
+      <c r="A48" s="13" t="s">
+        <v>6</v>
+      </c>
       <c r="B48" s="13" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C48" s="13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="D48" s="13" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F48" s="13"/>
+      <c r="G48" s="10" t="s">
+        <v>0</v>
+      </c>
       <c r="H48" s="30"/>
       <c r="I48"/>
       <c r="J48"/>
@@ -2356,14 +2386,21 @@
       <c r="M48"/>
       <c r="N48"/>
     </row>
-    <row r="49" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="F49" s="6"/>
-      <c r="G49" s="10"/>
+    <row r="49" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="13"/>
+      <c r="B49" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E49" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F49" s="13"/>
       <c r="H49" s="30"/>
       <c r="I49"/>
       <c r="J49"/>
@@ -2372,84 +2409,72 @@
       <c r="M49"/>
       <c r="N49"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
+    <row r="50" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="30"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
         <f>256*1024</f>
         <v>262144</v>
       </c>
-      <c r="B50" s="7">
+      <c r="B51" s="7">
         <v>0</v>
       </c>
-      <c r="C50" s="7">
-        <f>A50-1</f>
+      <c r="C51" s="7">
+        <f>A51-1</f>
         <v>262143</v>
       </c>
-      <c r="D50" s="7" t="str">
-        <f>DEC2HEX(B50,6)</f>
+      <c r="D51" s="7" t="str">
+        <f>DEC2HEX(B51,6)</f>
         <v>000000</v>
       </c>
-      <c r="E50" s="7" t="str">
-        <f>DEC2HEX(C50,6)</f>
+      <c r="E51" s="7" t="str">
+        <f>DEC2HEX(C51,6)</f>
         <v>03FFFF</v>
       </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="12" t="s">
+      <c r="F51" s="7"/>
+      <c r="G51" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H50" s="34"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+      <c r="H51" s="34"/>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
         <f>2*(128*96*2)</f>
         <v>49152</v>
       </c>
-      <c r="B51" s="7">
-        <f>C50+1</f>
-        <v>262144</v>
-      </c>
-      <c r="C51" s="7">
-        <f t="shared" ref="C51:C53" si="20">B51+A51-1</f>
-        <v>311295</v>
-      </c>
-      <c r="D51" s="7" t="str">
-        <f t="shared" ref="D51:E54" si="21">DEC2HEX(B51,6)</f>
-        <v>040000</v>
-      </c>
-      <c r="E51" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>04BFFF</v>
-      </c>
-      <c r="F51" s="7"/>
-      <c r="G51" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="H51" s="30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
-        <v>512</v>
-      </c>
       <c r="B52" s="7">
         <f>C51+1</f>
-        <v>311296</v>
+        <v>262144</v>
       </c>
       <c r="C52" s="7">
-        <f t="shared" ref="C52" si="22">B52+A52-1</f>
-        <v>311807</v>
+        <f t="shared" ref="C52:C54" si="21">B52+A52-1</f>
+        <v>311295</v>
       </c>
       <c r="D52" s="7" t="str">
-        <f t="shared" ref="D52" si="23">DEC2HEX(B52,6)</f>
-        <v>04C000</v>
+        <f t="shared" ref="D52:E55" si="22">DEC2HEX(B52,6)</f>
+        <v>040000</v>
       </c>
       <c r="E52" s="7" t="str">
-        <f t="shared" ref="E52" si="24">DEC2HEX(C52,6)</f>
-        <v>04C1FF</v>
+        <f t="shared" si="22"/>
+        <v>04BFFF</v>
       </c>
       <c r="F52" s="7"/>
       <c r="G52" s="8" t="s">
-        <v>134</v>
+        <v>98</v>
       </c>
       <c r="H52" s="30" t="s">
         <v>72</v>
@@ -2461,23 +2486,23 @@
       </c>
       <c r="B53" s="7">
         <f>C52+1</f>
-        <v>311808</v>
+        <v>311296</v>
       </c>
       <c r="C53" s="7">
-        <f t="shared" si="20"/>
-        <v>312319</v>
+        <f t="shared" ref="C53" si="23">B53+A53-1</f>
+        <v>311807</v>
       </c>
       <c r="D53" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>04C200</v>
+        <f t="shared" ref="D53" si="24">DEC2HEX(B53,6)</f>
+        <v>04C000</v>
       </c>
       <c r="E53" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>04C3FF</v>
+        <f t="shared" ref="E53" si="25">DEC2HEX(C53,6)</f>
+        <v>04C1FF</v>
       </c>
       <c r="F53" s="7"/>
       <c r="G53" s="8" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H53" s="30" t="s">
         <v>72</v>
@@ -2485,33 +2510,61 @@
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <f>C54-B54</f>
-        <v>16464895</v>
+        <v>512</v>
       </c>
       <c r="B54" s="7">
         <f>C53+1</f>
+        <v>311808</v>
+      </c>
+      <c r="C54" s="7">
+        <f t="shared" si="21"/>
+        <v>312319</v>
+      </c>
+      <c r="D54" s="7" t="str">
+        <f t="shared" si="22"/>
+        <v>04C200</v>
+      </c>
+      <c r="E54" s="7" t="str">
+        <f t="shared" si="22"/>
+        <v>04C3FF</v>
+      </c>
+      <c r="F54" s="7"/>
+      <c r="G54" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="H54" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <f>C55-B55</f>
+        <v>16464895</v>
+      </c>
+      <c r="B55" s="7">
+        <f>C54+1</f>
         <v>312320</v>
       </c>
-      <c r="C54" s="7">
+      <c r="C55" s="7">
         <f>16*1024*1024-1</f>
         <v>16777215</v>
       </c>
-      <c r="D54" s="7" t="str">
-        <f t="shared" si="21"/>
+      <c r="D55" s="7" t="str">
+        <f t="shared" si="22"/>
         <v>04C400</v>
       </c>
-      <c r="E54" s="7" t="str">
-        <f t="shared" si="21"/>
+      <c r="E55" s="7" t="str">
+        <f t="shared" si="22"/>
         <v>FFFFFF</v>
       </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="8" t="s">
+      <c r="F55" s="7"/>
+      <c r="G55" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H54" s="30" t="s">
+      <c r="H55" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I54" t="s">
+      <c r="I55" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2624,7 +2677,7 @@
         <v>124</v>
       </c>
       <c r="H6" s="30">
-        <f>B6+'NEW Memory Map'!$B$9</f>
+        <f>B6+'NEW Memory Map'!$B$10</f>
         <v>245760</v>
       </c>
       <c r="I6" s="7" t="str">
@@ -2657,7 +2710,7 @@
         <v>125</v>
       </c>
       <c r="H7" s="30">
-        <f>B7+'NEW Memory Map'!$B$9</f>
+        <f>B7+'NEW Memory Map'!$B$10</f>
         <v>245764</v>
       </c>
       <c r="I7" s="7" t="str">
@@ -2690,7 +2743,7 @@
         <v>126</v>
       </c>
       <c r="H8" s="30">
-        <f>B8+'NEW Memory Map'!$B$9</f>
+        <f>B8+'NEW Memory Map'!$B$10</f>
         <v>245768</v>
       </c>
       <c r="I8" s="7" t="str">
@@ -2723,7 +2776,7 @@
         <v>127</v>
       </c>
       <c r="H9" s="30">
-        <f>B9+'NEW Memory Map'!$B$9</f>
+        <f>B9+'NEW Memory Map'!$B$10</f>
         <v>245772</v>
       </c>
       <c r="I9" s="7" t="str">
@@ -2756,7 +2809,7 @@
         <v>131</v>
       </c>
       <c r="H10" s="30">
-        <f>B10+'NEW Memory Map'!$B$9</f>
+        <f>B10+'NEW Memory Map'!$B$10</f>
         <v>245776</v>
       </c>
       <c r="I10" s="7" t="str">
@@ -2789,7 +2842,7 @@
         <v>122</v>
       </c>
       <c r="H11" s="30">
-        <f>B11+'NEW Memory Map'!$B$9</f>
+        <f>B11+'NEW Memory Map'!$B$10</f>
         <v>245780</v>
       </c>
       <c r="I11" s="7" t="str">
@@ -2822,7 +2875,7 @@
         <v>123</v>
       </c>
       <c r="H12" s="30">
-        <f>B12+'NEW Memory Map'!$B$9</f>
+        <f>B12+'NEW Memory Map'!$B$10</f>
         <v>245784</v>
       </c>
       <c r="I12" s="7" t="str">
@@ -2855,7 +2908,7 @@
         <v>128</v>
       </c>
       <c r="H13" s="30">
-        <f>B13+'NEW Memory Map'!$B$9</f>
+        <f>B13+'NEW Memory Map'!$B$10</f>
         <v>245788</v>
       </c>
       <c r="I13" s="7" t="str">
@@ -2888,7 +2941,7 @@
         <v>129</v>
       </c>
       <c r="H14" s="30">
-        <f>B14+'NEW Memory Map'!$B$9</f>
+        <f>B14+'NEW Memory Map'!$B$10</f>
         <v>245789</v>
       </c>
       <c r="I14" s="7" t="str">
@@ -2921,7 +2974,7 @@
         <v>130</v>
       </c>
       <c r="H15" s="30">
-        <f>B15+'NEW Memory Map'!$B$9</f>
+        <f>B15+'NEW Memory Map'!$B$10</f>
         <v>245790</v>
       </c>
       <c r="I15" s="7" t="str">
@@ -2955,7 +3008,7 @@
         <v>121</v>
       </c>
       <c r="H16" s="30">
-        <f>B16+'NEW Memory Map'!$B$9</f>
+        <f>B16+'NEW Memory Map'!$B$10</f>
         <v>245804</v>
       </c>
       <c r="I16" s="7" t="str">
@@ -2988,7 +3041,7 @@
         <v>120</v>
       </c>
       <c r="H17" s="30">
-        <f>B17+'NEW Memory Map'!$B$9</f>
+        <f>B17+'NEW Memory Map'!$B$10</f>
         <v>246784</v>
       </c>
       <c r="I17" s="7" t="str">
@@ -3021,7 +3074,7 @@
         <v>119</v>
       </c>
       <c r="H18" s="30">
-        <f>B18+'NEW Memory Map'!$B$9</f>
+        <f>B18+'NEW Memory Map'!$B$10</f>
         <v>247296</v>
       </c>
       <c r="I18" s="7" t="str">
@@ -3054,7 +3107,7 @@
         <v>99</v>
       </c>
       <c r="H19" s="30">
-        <f>B19+'NEW Memory Map'!$B$9</f>
+        <f>B19+'NEW Memory Map'!$B$10</f>
         <v>247552</v>
       </c>
       <c r="I19" s="7" t="str">
@@ -3068,6 +3121,343 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" customWidth="1"/>
+    <col min="7" max="7" width="51.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="13"/>
+      <c r="G3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H3" s="37" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="13"/>
+      <c r="B4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F4" s="13"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="33"/>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <f>B6+A6-1</f>
+        <v>3</v>
+      </c>
+      <c r="D6" s="7" t="str">
+        <f t="shared" ref="D6:E13" si="0">DEC2HEX(B6,6)</f>
+        <v>000000</v>
+      </c>
+      <c r="E6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>000003</v>
+      </c>
+      <c r="F6" s="7"/>
+      <c r="G6" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="H6" s="30">
+        <f>B6+'NEW Memory Map'!$B$9</f>
+        <v>243712</v>
+      </c>
+      <c r="I6" s="7" t="str">
+        <f>DEC2HEX(H6,6)</f>
+        <v>03B800</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7">
+        <f>C6+1</f>
+        <v>4</v>
+      </c>
+      <c r="C7" s="7">
+        <f>B7+A7-1</f>
+        <v>7</v>
+      </c>
+      <c r="D7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>000004</v>
+      </c>
+      <c r="E7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>000007</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="30">
+        <f>B7+'NEW Memory Map'!$B$9</f>
+        <v>243716</v>
+      </c>
+      <c r="I7" s="7" t="str">
+        <f t="shared" ref="I7:I13" si="1">DEC2HEX(H7,6)</f>
+        <v>03B804</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7">
+        <f>C7+1</f>
+        <v>8</v>
+      </c>
+      <c r="C8" s="7">
+        <f>B8+A8-1</f>
+        <v>11</v>
+      </c>
+      <c r="D8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>000008</v>
+      </c>
+      <c r="E8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>00000B</v>
+      </c>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="30">
+        <f>B8+'NEW Memory Map'!$B$9</f>
+        <v>243720</v>
+      </c>
+      <c r="I8" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03B808</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7">
+        <f t="shared" ref="B9:B10" si="2">C8+1</f>
+        <v>12</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" ref="C9:C13" si="3">B9+A9-1</f>
+        <v>15</v>
+      </c>
+      <c r="D9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>00000C</v>
+      </c>
+      <c r="E9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>00000F</v>
+      </c>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="30">
+        <f>B9+'NEW Memory Map'!$B$9</f>
+        <v>243724</v>
+      </c>
+      <c r="I9" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03B80C</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="C10" s="7">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="D10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>000010</v>
+      </c>
+      <c r="E10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>000013</v>
+      </c>
+      <c r="F10" s="7"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="30">
+        <f>B10+'NEW Memory Map'!$B$9</f>
+        <v>243728</v>
+      </c>
+      <c r="I10" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03B810</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>128</v>
+      </c>
+      <c r="B11" s="7">
+        <v>512</v>
+      </c>
+      <c r="C11" s="7">
+        <f t="shared" si="3"/>
+        <v>639</v>
+      </c>
+      <c r="D11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>000200</v>
+      </c>
+      <c r="E11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>00027F</v>
+      </c>
+      <c r="F11" s="7"/>
+      <c r="G11" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="H11" s="30">
+        <f>B11+'NEW Memory Map'!$B$9</f>
+        <v>244224</v>
+      </c>
+      <c r="I11" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03BA00</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>128</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1024</v>
+      </c>
+      <c r="C12" s="7">
+        <f t="shared" si="3"/>
+        <v>1151</v>
+      </c>
+      <c r="D12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>000400</v>
+      </c>
+      <c r="E12" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>00047F</v>
+      </c>
+      <c r="F12" s="7"/>
+      <c r="G12" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="H12" s="30">
+        <f>B12+'NEW Memory Map'!$B$9</f>
+        <v>244736</v>
+      </c>
+      <c r="I12" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03BC00</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>128</v>
+      </c>
+      <c r="B13" s="7">
+        <f>1024+512</f>
+        <v>1536</v>
+      </c>
+      <c r="C13" s="7">
+        <f t="shared" si="3"/>
+        <v>1663</v>
+      </c>
+      <c r="D13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>000600</v>
+      </c>
+      <c r="E13" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>00067F</v>
+      </c>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8" t="s">
+        <v>141</v>
+      </c>
+      <c r="H13" s="30">
+        <f>B13+'NEW Memory Map'!$B$9</f>
+        <v>245248</v>
+      </c>
+      <c r="I13" s="7" t="str">
+        <f t="shared" si="1"/>
+        <v>03BE00</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O23"/>
   <sheetViews>
@@ -3599,7 +3989,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -4996,7 +5386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A10"/>
   <sheetViews>

</xml_diff>

<commit_message>
First draft of Virtual Machine Manager code, reviewed but not yet tested.
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="143">
   <si>
     <t>Name</t>
   </si>
@@ -582,6 +582,9 @@
   </si>
   <si>
     <t>Virtual interrupt</t>
+  </si>
+  <si>
+    <t>Current Virtual Machine</t>
   </si>
 </sst>
 </file>
@@ -3125,7 +3128,7 @@
   <dimension ref="A2:I13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3252,7 +3255,9 @@
         <v>000007</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="8"/>
+      <c r="G7" s="8" t="s">
+        <v>142</v>
+      </c>
       <c r="H7" s="30">
         <f>B7+'NEW Memory Map'!$B$9</f>
         <v>243716</v>

</xml_diff>

<commit_message>
Expanded number of virtual machines to 32 and updated stack depths
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="NEW Memory Map" sheetId="4" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="Hardware registers" sheetId="2" r:id="rId4"/>
     <sheet name="OLD Memory Map" sheetId="1" r:id="rId5"/>
     <sheet name="Copyright and license" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="160">
   <si>
     <t>Name</t>
   </si>
@@ -585,6 +586,57 @@
   </si>
   <si>
     <t>Current Virtual Machine</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vmp_w </t>
+  </si>
+  <si>
+    <t xml:space="preserve">psp_w </t>
+  </si>
+  <si>
+    <t xml:space="preserve">rsp_w </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ssp_w </t>
+  </si>
+  <si>
+    <t xml:space="preserve">esp_w </t>
+  </si>
+  <si>
+    <t>Parameter stack depth</t>
+  </si>
+  <si>
+    <t>Return stack depth</t>
+  </si>
+  <si>
+    <t>Subroutine stack depth</t>
+  </si>
+  <si>
+    <t>Exception stack depth</t>
+  </si>
+  <si>
+    <t>User data area</t>
+  </si>
+  <si>
+    <t>user_w</t>
+  </si>
+  <si>
+    <t>Number of virtual machines</t>
+  </si>
+  <si>
+    <t>cells</t>
+  </si>
+  <si>
+    <t>longwords</t>
+  </si>
+  <si>
+    <t>instances</t>
   </si>
 </sst>
 </file>
@@ -704,7 +756,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -795,6 +847,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3127,7 +3182,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
@@ -5453,4 +5508,177 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
+    <col min="5" max="6" width="15.5703125" customWidth="1"/>
+    <col min="9" max="10" width="10.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>156</v>
+      </c>
+      <c r="E2" s="39">
+        <f>2^B2</f>
+        <v>32</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" s="39">
+        <f t="shared" ref="E3:E6" si="0">2^B3</f>
+        <v>256</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="H3">
+        <v>32</v>
+      </c>
+      <c r="I3">
+        <f>2^($B$2+B3)</f>
+        <v>8192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4">
+        <v>7</v>
+      </c>
+      <c r="D4" t="s">
+        <v>151</v>
+      </c>
+      <c r="E4" s="39">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="H4">
+        <v>32</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I7" si="1">2^($B$2+B4)</f>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7</v>
+      </c>
+      <c r="D5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E5" s="39">
+        <f t="shared" si="0"/>
+        <v>128</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="H5">
+        <v>544</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>4096</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="D6" t="s">
+        <v>153</v>
+      </c>
+      <c r="E6" s="39">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="H6">
+        <v>304</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>154</v>
+      </c>
+      <c r="E7" s="39">
+        <f t="shared" ref="E7" si="2">2^B7</f>
+        <v>512</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="H7">
+        <v>32</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>16384</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added new registers to HW_Registers in anticipation of variable size font display
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="NEW Memory Map" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="170">
   <si>
     <t>Name</t>
   </si>
@@ -637,6 +637,36 @@
   </si>
   <si>
     <t>instances</t>
+  </si>
+  <si>
+    <t>Interlace - number of interlace scanlines between character rows</t>
+  </si>
+  <si>
+    <t>charHeight - height of each character in pixels</t>
+  </si>
+  <si>
+    <t>charWidth - width of each character in pixels</t>
+  </si>
+  <si>
+    <t>Interlace</t>
+  </si>
+  <si>
+    <t>charWidth</t>
+  </si>
+  <si>
+    <t>charHeight</t>
+  </si>
+  <si>
+    <t>VGArows</t>
+  </si>
+  <si>
+    <t>VGAcols</t>
+  </si>
+  <si>
+    <t>Number of complete rows on screen</t>
+  </si>
+  <si>
+    <t>Number of complete columns on screen</t>
   </si>
 </sst>
 </file>
@@ -846,10 +876,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="right" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" indent="1"/>
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1155,10 +1185,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1635,7 +1665,7 @@
         <v>260099</v>
       </c>
       <c r="D21" s="7" t="str">
-        <f t="shared" ref="D21:E40" si="8">DEC2HEX(B21,6)</f>
+        <f t="shared" ref="D21:E45" si="8">DEC2HEX(B21,6)</f>
         <v>03F800</v>
       </c>
       <c r="E21" s="7" t="str">
@@ -1689,7 +1719,7 @@
         <v>1</v>
       </c>
       <c r="B23" s="7">
-        <f t="shared" ref="B23:B39" si="10">B22+4</f>
+        <f t="shared" ref="B23:B44" si="10">B22+4</f>
         <v>260104</v>
       </c>
       <c r="C23" s="7">
@@ -1994,7 +2024,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>2</v>
       </c>
@@ -2025,7 +2055,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>1</v>
       </c>
@@ -2056,7 +2086,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>1</v>
       </c>
@@ -2087,7 +2117,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>1</v>
       </c>
@@ -2118,7 +2148,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>1</v>
       </c>
@@ -2149,7 +2179,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>1</v>
       </c>
@@ -2180,7 +2210,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>1</v>
       </c>
@@ -2211,418 +2241,573 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
-        <f>C40-B40</f>
-        <v>1827</v>
+        <v>1</v>
       </c>
       <c r="B40" s="7">
-        <f>B39+4</f>
+        <f t="shared" si="10"/>
         <v>260172</v>
       </c>
       <c r="C40" s="7">
-        <f>B41-1</f>
+        <f t="shared" ref="C40:C44" si="11">B40+A40-1</f>
+        <v>260172</v>
+      </c>
+      <c r="D40" s="7" t="str">
+        <f t="shared" ref="D40:D44" si="12">DEC2HEX(B40,6)</f>
+        <v>03F84C</v>
+      </c>
+      <c r="E40" s="7" t="str">
+        <f t="shared" ref="E40:E44" si="13">DEC2HEX(C40,6)</f>
+        <v>03F84C</v>
+      </c>
+      <c r="F40" s="7"/>
+      <c r="G40" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H40" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I40" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>1</v>
+      </c>
+      <c r="B41" s="7">
+        <f t="shared" si="10"/>
+        <v>260176</v>
+      </c>
+      <c r="C41" s="7">
+        <f t="shared" si="11"/>
+        <v>260176</v>
+      </c>
+      <c r="D41" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>03F850</v>
+      </c>
+      <c r="E41" s="7" t="str">
+        <f t="shared" si="13"/>
+        <v>03F850</v>
+      </c>
+      <c r="F41" s="7"/>
+      <c r="G41" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H41" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="7">
+        <v>1</v>
+      </c>
+      <c r="B42" s="7">
+        <f t="shared" si="10"/>
+        <v>260180</v>
+      </c>
+      <c r="C42" s="7">
+        <f t="shared" si="11"/>
+        <v>260180</v>
+      </c>
+      <c r="D42" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>03F854</v>
+      </c>
+      <c r="E42" s="7" t="str">
+        <f t="shared" si="13"/>
+        <v>03F854</v>
+      </c>
+      <c r="F42" s="7"/>
+      <c r="G42" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H42" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I42" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>1</v>
+      </c>
+      <c r="B43" s="7">
+        <f t="shared" si="10"/>
+        <v>260184</v>
+      </c>
+      <c r="C43" s="7">
+        <f t="shared" si="11"/>
+        <v>260184</v>
+      </c>
+      <c r="D43" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>03F858</v>
+      </c>
+      <c r="E43" s="7" t="str">
+        <f t="shared" si="13"/>
+        <v>03F858</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="H43" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>1</v>
+      </c>
+      <c r="B44" s="7">
+        <f t="shared" si="10"/>
+        <v>260188</v>
+      </c>
+      <c r="C44" s="7">
+        <f t="shared" si="11"/>
+        <v>260188</v>
+      </c>
+      <c r="D44" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>03F85C</v>
+      </c>
+      <c r="E44" s="7" t="str">
+        <f t="shared" si="13"/>
+        <v>03F85C</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I44" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <f>C45-B45</f>
+        <v>1807</v>
+      </c>
+      <c r="B45" s="7">
+        <f>B44+4</f>
+        <v>260192</v>
+      </c>
+      <c r="C45" s="7">
+        <f>B46-1</f>
         <v>261999</v>
       </c>
-      <c r="D40" s="7" t="str">
+      <c r="D45" s="7" t="str">
         <f t="shared" si="8"/>
-        <v>03F84C</v>
-      </c>
-      <c r="E40" s="7" t="str">
+        <v>03F860</v>
+      </c>
+      <c r="E45" s="7" t="str">
         <f t="shared" si="8"/>
         <v>03FF6F</v>
       </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="12" t="s">
+      <c r="F45" s="7"/>
+      <c r="G45" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="7">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
         <f>4*32</f>
         <v>128</v>
       </c>
-      <c r="B41" s="7">
-        <f>B42-A41</f>
+      <c r="B46" s="7">
+        <f>B47-A46</f>
         <v>262000</v>
       </c>
-      <c r="C41" s="7">
-        <f>B41+A41-1</f>
+      <c r="C46" s="7">
+        <f>B46+A46-1</f>
         <v>262127</v>
       </c>
-      <c r="D41" s="7" t="str">
-        <f t="shared" ref="D41:D42" si="11">DEC2HEX(B41,6)</f>
+      <c r="D46" s="7" t="str">
+        <f t="shared" ref="D46:D47" si="14">DEC2HEX(B46,6)</f>
         <v>03FF70</v>
       </c>
-      <c r="E41" s="7" t="str">
-        <f t="shared" ref="E41:E42" si="12">DEC2HEX(C41,6)</f>
+      <c r="E46" s="7" t="str">
+        <f t="shared" ref="E46:E47" si="15">DEC2HEX(C46,6)</f>
         <v>03FFEF</v>
       </c>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8" t="s">
+      <c r="F46" s="7"/>
+      <c r="G46" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="H41" s="30" t="s">
+      <c r="H46" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I46" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A42" s="7">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
         <v>4</v>
       </c>
-      <c r="B42" s="7">
-        <f t="shared" ref="B42" si="13">B43-A42</f>
+      <c r="B47" s="7">
+        <f t="shared" ref="B47" si="16">B48-A47</f>
         <v>262128</v>
       </c>
-      <c r="C42" s="7">
-        <f>B42+A42-1</f>
+      <c r="C47" s="7">
+        <f>B47+A47-1</f>
         <v>262131</v>
       </c>
-      <c r="D42" s="7" t="str">
-        <f t="shared" si="11"/>
+      <c r="D47" s="7" t="str">
+        <f t="shared" si="14"/>
         <v>03FFF0</v>
       </c>
-      <c r="E42" s="7" t="str">
-        <f t="shared" si="12"/>
+      <c r="E47" s="7" t="str">
+        <f t="shared" si="15"/>
         <v>03FFF3</v>
       </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8" t="s">
+      <c r="F47" s="7"/>
+      <c r="G47" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="H42" s="30" t="s">
+      <c r="H47" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I47" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A43" s="7">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
         <v>4</v>
       </c>
-      <c r="B43" s="7">
-        <f t="shared" ref="B43:B44" si="14">B44-A43</f>
+      <c r="B48" s="7">
+        <f t="shared" ref="B48:B49" si="17">B49-A48</f>
         <v>262132</v>
       </c>
-      <c r="C43" s="7">
-        <f>B43+A43-1</f>
+      <c r="C48" s="7">
+        <f>B48+A48-1</f>
         <v>262135</v>
       </c>
-      <c r="D43" s="7" t="str">
-        <f t="shared" ref="D43" si="15">DEC2HEX(B43,6)</f>
+      <c r="D48" s="7" t="str">
+        <f t="shared" ref="D48" si="18">DEC2HEX(B48,6)</f>
         <v>03FFF4</v>
       </c>
-      <c r="E43" s="7" t="str">
-        <f t="shared" ref="E43" si="16">DEC2HEX(C43,6)</f>
+      <c r="E48" s="7" t="str">
+        <f t="shared" ref="E48" si="19">DEC2HEX(C48,6)</f>
         <v>03FFF7</v>
       </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="8" t="s">
+      <c r="F48" s="7"/>
+      <c r="G48" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="H43" s="30" t="s">
+      <c r="H48" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I48" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
         <v>4</v>
       </c>
-      <c r="B44" s="7">
-        <f t="shared" si="14"/>
+      <c r="B49" s="7">
+        <f t="shared" si="17"/>
         <v>262136</v>
       </c>
-      <c r="C44" s="7">
-        <f>B44+A44-1</f>
+      <c r="C49" s="7">
+        <f>B49+A49-1</f>
         <v>262139</v>
       </c>
-      <c r="D44" s="7" t="str">
-        <f t="shared" ref="D44" si="17">DEC2HEX(B44,6)</f>
+      <c r="D49" s="7" t="str">
+        <f t="shared" ref="D49" si="20">DEC2HEX(B49,6)</f>
         <v>03FFF8</v>
       </c>
-      <c r="E44" s="7" t="str">
-        <f t="shared" ref="E44" si="18">DEC2HEX(C44,6)</f>
+      <c r="E49" s="7" t="str">
+        <f t="shared" ref="E49" si="21">DEC2HEX(C49,6)</f>
         <v>03FFFB</v>
       </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="8" t="s">
+      <c r="F49" s="7"/>
+      <c r="G49" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="H44" s="30" t="s">
+      <c r="H49" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I49" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A45" s="7">
+    <row r="50" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="A50" s="7">
         <v>4</v>
       </c>
-      <c r="B45" s="7">
-        <f>B52-A45</f>
+      <c r="B50" s="7">
+        <f>B57-A50</f>
         <v>262140</v>
       </c>
-      <c r="C45" s="7">
-        <f>B45+A45-1</f>
+      <c r="C50" s="7">
+        <f>B50+A50-1</f>
         <v>262143</v>
       </c>
-      <c r="D45" s="7" t="str">
-        <f t="shared" ref="D45" si="19">DEC2HEX(B45,6)</f>
+      <c r="D50" s="7" t="str">
+        <f t="shared" ref="D50" si="22">DEC2HEX(B50,6)</f>
         <v>03FFFC</v>
       </c>
-      <c r="E45" s="7" t="str">
-        <f t="shared" ref="E45" si="20">DEC2HEX(C45,6)</f>
+      <c r="E50" s="7" t="str">
+        <f t="shared" ref="E50" si="23">DEC2HEX(C50,6)</f>
         <v>03FFFF</v>
       </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="8" t="s">
+      <c r="F50" s="7"/>
+      <c r="G50" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="H45" s="30" t="s">
+      <c r="H50" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I50" t="s">
         <v>111</v>
       </c>
-      <c r="J45" s="36">
+      <c r="J50" s="36">
         <f>B21+255</f>
         <v>260351</v>
       </c>
-      <c r="K45" s="36" t="str">
-        <f>DEC2HEX(J45,6)</f>
+      <c r="K50" s="36" t="str">
+        <f>DEC2HEX(J50,6)</f>
         <v>03F8FF</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="10" t="s">
+    <row r="52" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D47" s="16"/>
-      <c r="E47" s="16"/>
-      <c r="F47" s="16"/>
-      <c r="H47" s="30"/>
-      <c r="I47"/>
-      <c r="J47"/>
-      <c r="K47"/>
-      <c r="L47"/>
-      <c r="M47"/>
-      <c r="N47"/>
-    </row>
-    <row r="48" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
+      <c r="D52" s="16"/>
+      <c r="E52" s="16"/>
+      <c r="F52" s="16"/>
+      <c r="H52" s="30"/>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+    </row>
+    <row r="53" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B48" s="13" t="s">
+      <c r="B53" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C53" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D53" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E53" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F48" s="13"/>
-      <c r="G48" s="10" t="s">
+      <c r="F53" s="13"/>
+      <c r="G53" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H48" s="30"/>
-      <c r="I48"/>
-      <c r="J48"/>
-      <c r="K48"/>
-      <c r="L48"/>
-      <c r="M48"/>
-      <c r="N48"/>
-    </row>
-    <row r="49" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
-      <c r="B49" s="13" t="s">
+      <c r="H53" s="30"/>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+    </row>
+    <row r="54" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="13"/>
+      <c r="B54" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C54" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="D54" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E54" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F49" s="13"/>
-      <c r="H49" s="30"/>
-      <c r="I49"/>
-      <c r="J49"/>
-      <c r="K49"/>
-      <c r="L49"/>
-      <c r="M49"/>
-      <c r="N49"/>
-    </row>
-    <row r="50" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="30"/>
-      <c r="I50"/>
-      <c r="J50"/>
-      <c r="K50"/>
-      <c r="L50"/>
-      <c r="M50"/>
-      <c r="N50"/>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+      <c r="F54" s="13"/>
+      <c r="H54" s="30"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+    </row>
+    <row r="55" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="6"/>
+      <c r="B55" s="6"/>
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="30"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
         <f>256*1024</f>
         <v>262144</v>
       </c>
-      <c r="B51" s="7">
+      <c r="B56" s="7">
         <v>0</v>
       </c>
-      <c r="C51" s="7">
-        <f>A51-1</f>
+      <c r="C56" s="7">
+        <f>A56-1</f>
         <v>262143</v>
       </c>
-      <c r="D51" s="7" t="str">
-        <f>DEC2HEX(B51,6)</f>
+      <c r="D56" s="7" t="str">
+        <f>DEC2HEX(B56,6)</f>
         <v>000000</v>
       </c>
-      <c r="E51" s="7" t="str">
-        <f>DEC2HEX(C51,6)</f>
+      <c r="E56" s="7" t="str">
+        <f>DEC2HEX(C56,6)</f>
         <v>03FFFF</v>
       </c>
-      <c r="F51" s="7"/>
-      <c r="G51" s="12" t="s">
+      <c r="F56" s="7"/>
+      <c r="G56" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H51" s="34"/>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+      <c r="H56" s="34"/>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
         <f>2*(128*96*2)</f>
         <v>49152</v>
       </c>
-      <c r="B52" s="7">
-        <f>C51+1</f>
+      <c r="B57" s="7">
+        <f>C56+1</f>
         <v>262144</v>
       </c>
-      <c r="C52" s="7">
-        <f t="shared" ref="C52:C54" si="21">B52+A52-1</f>
+      <c r="C57" s="7">
+        <f t="shared" ref="C57:C59" si="24">B57+A57-1</f>
         <v>311295</v>
       </c>
-      <c r="D52" s="7" t="str">
-        <f t="shared" ref="D52:E55" si="22">DEC2HEX(B52,6)</f>
+      <c r="D57" s="7" t="str">
+        <f t="shared" ref="D57:E60" si="25">DEC2HEX(B57,6)</f>
         <v>040000</v>
       </c>
-      <c r="E52" s="7" t="str">
-        <f t="shared" si="22"/>
+      <c r="E57" s="7" t="str">
+        <f t="shared" si="25"/>
         <v>04BFFF</v>
       </c>
-      <c r="F52" s="7"/>
-      <c r="G52" s="8" t="s">
+      <c r="F57" s="7"/>
+      <c r="G57" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H52" s="30" t="s">
+      <c r="H57" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
         <v>512</v>
       </c>
-      <c r="B53" s="7">
-        <f>C52+1</f>
+      <c r="B58" s="7">
+        <f>C57+1</f>
         <v>311296</v>
       </c>
-      <c r="C53" s="7">
-        <f t="shared" ref="C53" si="23">B53+A53-1</f>
+      <c r="C58" s="7">
+        <f t="shared" ref="C58" si="26">B58+A58-1</f>
         <v>311807</v>
       </c>
-      <c r="D53" s="7" t="str">
-        <f t="shared" ref="D53" si="24">DEC2HEX(B53,6)</f>
+      <c r="D58" s="7" t="str">
+        <f t="shared" ref="D58" si="27">DEC2HEX(B58,6)</f>
         <v>04C000</v>
       </c>
-      <c r="E53" s="7" t="str">
-        <f t="shared" ref="E53" si="25">DEC2HEX(C53,6)</f>
+      <c r="E58" s="7" t="str">
+        <f t="shared" ref="E58" si="28">DEC2HEX(C58,6)</f>
         <v>04C1FF</v>
       </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="8" t="s">
+      <c r="F58" s="7"/>
+      <c r="G58" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="H53" s="30" t="s">
+      <c r="H58" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A54" s="7">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
         <v>512</v>
       </c>
-      <c r="B54" s="7">
-        <f>C53+1</f>
+      <c r="B59" s="7">
+        <f>C58+1</f>
         <v>311808</v>
       </c>
-      <c r="C54" s="7">
-        <f t="shared" si="21"/>
+      <c r="C59" s="7">
+        <f t="shared" si="24"/>
         <v>312319</v>
       </c>
-      <c r="D54" s="7" t="str">
-        <f t="shared" si="22"/>
+      <c r="D59" s="7" t="str">
+        <f t="shared" si="25"/>
         <v>04C200</v>
       </c>
-      <c r="E54" s="7" t="str">
-        <f t="shared" si="22"/>
+      <c r="E59" s="7" t="str">
+        <f t="shared" si="25"/>
         <v>04C3FF</v>
       </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="8" t="s">
+      <c r="F59" s="7"/>
+      <c r="G59" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="H54" s="30" t="s">
+      <c r="H59" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="7">
-        <f>C55-B55</f>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <f>C60-B60</f>
         <v>16464895</v>
       </c>
-      <c r="B55" s="7">
-        <f>C54+1</f>
+      <c r="B60" s="7">
+        <f>C59+1</f>
         <v>312320</v>
       </c>
-      <c r="C55" s="7">
+      <c r="C60" s="7">
         <f>16*1024*1024-1</f>
         <v>16777215</v>
       </c>
-      <c r="D55" s="7" t="str">
-        <f t="shared" si="22"/>
+      <c r="D60" s="7" t="str">
+        <f t="shared" si="25"/>
         <v>04C400</v>
       </c>
-      <c r="E55" s="7" t="str">
-        <f t="shared" si="22"/>
+      <c r="E60" s="7" t="str">
+        <f t="shared" si="25"/>
         <v>FFFFFF</v>
       </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="8" t="s">
+      <c r="F60" s="7"/>
+      <c r="G60" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H55" s="30" t="s">
+      <c r="H60" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I55" t="s">
+      <c r="I60" t="s">
         <v>75</v>
       </c>
     </row>
@@ -3698,11 +3883,11 @@
       <c r="L6" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="M6" s="38" t="s">
+      <c r="M6" s="39" t="s">
         <v>97</v>
       </c>
-      <c r="N6" s="38"/>
-      <c r="O6" s="38"/>
+      <c r="N6" s="39"/>
+      <c r="O6" s="39"/>
     </row>
     <row r="7" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
@@ -5514,7 +5699,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
@@ -5545,7 +5730,7 @@
       <c r="D2" t="s">
         <v>156</v>
       </c>
-      <c r="E2" s="39">
+      <c r="E2" s="38">
         <f>2^B2</f>
         <v>32</v>
       </c>
@@ -5563,7 +5748,7 @@
       <c r="D3" t="s">
         <v>150</v>
       </c>
-      <c r="E3" s="39">
+      <c r="E3" s="38">
         <f t="shared" ref="E3:E6" si="0">2^B3</f>
         <v>256</v>
       </c>
@@ -5588,7 +5773,7 @@
       <c r="D4" t="s">
         <v>151</v>
       </c>
-      <c r="E4" s="39">
+      <c r="E4" s="38">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
@@ -5613,7 +5798,7 @@
       <c r="D5" t="s">
         <v>152</v>
       </c>
-      <c r="E5" s="39">
+      <c r="E5" s="38">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
@@ -5638,7 +5823,7 @@
       <c r="D6" t="s">
         <v>153</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="38">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
@@ -5663,7 +5848,7 @@
       <c r="D7" t="s">
         <v>154</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="38">
         <f t="shared" ref="E7" si="2">2^B7</f>
         <v>512</v>
       </c>

</xml_diff>

<commit_message>
Reorganized memory map and enabled 4k access to character RAM
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -4,10 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425"/>
+    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NEW Memory Map" sheetId="4" r:id="rId1"/>
+    <sheet name="Memory Map" sheetId="4" r:id="rId1"/>
     <sheet name="USER" sheetId="5" r:id="rId2"/>
     <sheet name="Virtualization" sheetId="6" r:id="rId3"/>
     <sheet name="Hardware registers" sheetId="2" r:id="rId4"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="161">
   <si>
     <t>Name</t>
   </si>
@@ -471,48 +471,12 @@
     <t>Access to each VM's local user data</t>
   </si>
   <si>
-    <t>VM#</t>
-  </si>
-  <si>
-    <t>Pre-emptive interval</t>
-  </si>
-  <si>
     <t>Unsigned 32-bit counter at 100MHz</t>
   </si>
   <si>
-    <t>Multi tasking on/off</t>
-  </si>
-  <si>
-    <t>When zero, PAUSE (pre-emptive or elective) becomes a NOP</t>
-  </si>
-  <si>
-    <t>VM schedule registers</t>
-  </si>
-  <si>
-    <t>32 registers, each of 16 bits.  Lowest 5 bits are interpreted as next task no.</t>
-  </si>
-  <si>
-    <t>Number of currently executing VM</t>
-  </si>
-  <si>
-    <t>PC of next-to-execute VM</t>
-  </si>
-  <si>
-    <t>Write through via next-task port of task table BLOCK RAM (need true dual port)</t>
-  </si>
-  <si>
-    <t>Access to the paramater stack in the CPU address space (current task)</t>
-  </si>
-  <si>
-    <t>Access to the return stack in the CPU address space (current task)</t>
-  </si>
-  <si>
     <t>Access to subroutine and exception stacks (current task)</t>
   </si>
   <si>
-    <t>Interval for pre-emptive multi-tasking (units: clock cycles).  Zero = pre-emptive off</t>
-  </si>
-  <si>
     <t>USER RAM</t>
   </si>
   <si>
@@ -564,12 +528,6 @@
     <t>FAT buffer for sector R/W</t>
   </si>
   <si>
-    <t>Virtualization control</t>
-  </si>
-  <si>
-    <t>Access to virtualization control registers</t>
-  </si>
-  <si>
     <t>Virtualization registers</t>
   </si>
   <si>
@@ -667,13 +625,28 @@
   </si>
   <si>
     <t>Number of complete columns on screen</t>
+  </si>
+  <si>
+    <t>MEMaddr(17 downto 11)</t>
+  </si>
+  <si>
+    <t>Multitasking control</t>
+  </si>
+  <si>
+    <t>Access to multitasking control registers</t>
+  </si>
+  <si>
+    <t>Local variables</t>
+  </si>
+  <si>
+    <t>Interval</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -749,13 +722,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -786,7 +752,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -868,9 +834,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1185,10 +1148,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1199,7 +1162,8 @@
     <col min="7" max="7" width="34.28515625" style="8" customWidth="1"/>
     <col min="8" max="8" width="10.140625" style="30" customWidth="1"/>
     <col min="9" max="9" width="79.140625" customWidth="1"/>
-    <col min="10" max="12" width="19.140625" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" customWidth="1"/>
+    <col min="11" max="12" width="19.140625" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="11.140625" customWidth="1"/>
   </cols>
@@ -1246,7 +1210,9 @@
         <v>72</v>
       </c>
       <c r="I4"/>
-      <c r="J4"/>
+      <c r="J4" s="32" t="s">
+        <v>156</v>
+      </c>
       <c r="K4"/>
       <c r="L4"/>
       <c r="M4"/>
@@ -1324,24 +1290,24 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <f>(128-18)*1024</f>
-        <v>112640</v>
+        <f>(128-16)*1024</f>
+        <v>114688</v>
       </c>
       <c r="B8" s="7">
-        <f t="shared" ref="B8:B15" si="0">C7+1</f>
+        <f t="shared" ref="B8:B12" si="0">C7+1</f>
         <v>131072</v>
       </c>
       <c r="C8" s="7">
         <f>B8+A8-1</f>
-        <v>243711</v>
+        <v>245759</v>
       </c>
       <c r="D8" s="7" t="str">
-        <f t="shared" ref="D8:E15" si="1">DEC2HEX(B8,6)</f>
+        <f t="shared" ref="D8:E13" si="1">DEC2HEX(B8,6)</f>
         <v>020000</v>
       </c>
       <c r="E8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03B7FF</v>
+        <v>03BFFF</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8" t="s">
@@ -1350,64 +1316,72 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="B9" s="7">
         <f>C8+1</f>
-        <v>243712</v>
+        <v>245760</v>
       </c>
       <c r="C9" s="7">
         <f t="shared" ref="C9" si="2">B9+A9-1</f>
-        <v>245759</v>
+        <v>249855</v>
       </c>
       <c r="D9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03B800</v>
+        <v>03C000</v>
       </c>
       <c r="E9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03BFFF</v>
+        <v>03CFFF</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8" t="s">
-        <v>135</v>
+        <v>4</v>
       </c>
       <c r="H9" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>136</v>
+        <v>51</v>
+      </c>
+      <c r="J9" t="str">
+        <f>DEC2BIN(B9/2^11,7)</f>
+        <v>1111000</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>4096</v>
+        <v>2048</v>
       </c>
       <c r="B10" s="7">
         <f>C9+1</f>
-        <v>245760</v>
+        <v>249856</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10" si="3">B10+A10-1</f>
-        <v>249855</v>
+        <v>251903</v>
       </c>
       <c r="D10" s="7" t="str">
         <f t="shared" ref="D10" si="4">DEC2HEX(B10,6)</f>
-        <v>03C000</v>
+        <v>03D000</v>
       </c>
       <c r="E10" s="7" t="str">
         <f t="shared" ref="E10" si="5">DEC2HEX(C10,6)</f>
-        <v>03CFFF</v>
+        <v>03D7FF</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="H10" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I10" t="s">
-        <v>103</v>
+        <v>96</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" ref="J10:J13" si="6">DEC2BIN(B10/2^11,7)</f>
+        <v>1111010</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
@@ -1416,168 +1390,165 @@
       </c>
       <c r="B11" s="7">
         <f>C10+1</f>
-        <v>249856</v>
+        <v>251904</v>
       </c>
       <c r="C11" s="7">
-        <f t="shared" ref="C11" si="6">B11+A11-1</f>
-        <v>251903</v>
+        <f t="shared" ref="C11" si="7">B11+A11-1</f>
+        <v>253951</v>
       </c>
       <c r="D11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D000</v>
+        <v>03D800</v>
       </c>
       <c r="E11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D7FF</v>
+        <v>03DFFF</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8" t="s">
-        <v>4</v>
+        <v>159</v>
       </c>
       <c r="H11" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I11" t="s">
-        <v>51</v>
+        <v>105</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="6"/>
+        <v>1111011</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
-        <v>2048</v>
+        <v>4096</v>
       </c>
       <c r="B12" s="7">
         <f t="shared" si="0"/>
-        <v>251904</v>
+        <v>253952</v>
       </c>
       <c r="C12" s="7">
         <f>B12+A12-1</f>
-        <v>253951</v>
+        <v>258047</v>
       </c>
       <c r="D12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D800</v>
+        <v>03E000</v>
       </c>
       <c r="E12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03DFFF</v>
+        <v>03EFFF</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="8" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="H12" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I12" t="s">
-        <v>96</v>
+        <v>103</v>
+      </c>
+      <c r="J12" t="str">
+        <f t="shared" si="6"/>
+        <v>1111100</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
-        <f>2048</f>
         <v>2048</v>
       </c>
       <c r="B13" s="7">
-        <f t="shared" si="0"/>
-        <v>253952</v>
+        <f>C12+1</f>
+        <v>258048</v>
       </c>
       <c r="C13" s="7">
-        <f t="shared" ref="C13:C15" si="7">B13+A13-1</f>
-        <v>255999</v>
+        <f t="shared" ref="C13" si="8">B13+A13-1</f>
+        <v>260095</v>
       </c>
       <c r="D13" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03E000</v>
+        <v>03F000</v>
       </c>
       <c r="E13" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03E7FF</v>
+        <v>03F7FF</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8" t="s">
-        <v>2</v>
+        <v>157</v>
       </c>
       <c r="H13" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I13" t="s">
-        <v>114</v>
+        <v>158</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" si="6"/>
+        <v>1111110</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14" s="7">
-        <f>2048</f>
-        <v>2048</v>
-      </c>
-      <c r="B14" s="7">
-        <f t="shared" si="0"/>
-        <v>256000</v>
-      </c>
-      <c r="C14" s="7">
-        <f t="shared" si="7"/>
-        <v>258047</v>
-      </c>
-      <c r="D14" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>03E800</v>
-      </c>
-      <c r="E14" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>03EFFF</v>
-      </c>
-      <c r="F14" s="7"/>
-      <c r="G14" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="H14" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I14" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A15" s="7">
-        <v>2048</v>
-      </c>
-      <c r="B15" s="7">
-        <f t="shared" si="0"/>
-        <v>258048</v>
-      </c>
-      <c r="C15" s="7">
-        <f t="shared" si="7"/>
-        <v>260095</v>
-      </c>
-      <c r="D15" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>03F000</v>
-      </c>
-      <c r="E15" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>03F7FF</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="H15" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A14" s="3"/>
+    </row>
+    <row r="15" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="D17" s="16"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="16"/>
-      <c r="H17" s="31"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+    </row>
+    <row r="16" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="13"/>
+      <c r="G16" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="32"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+    </row>
+    <row r="17" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="15"/>
+      <c r="B17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="13"/>
+      <c r="H17" s="33"/>
       <c r="I17"/>
       <c r="J17"/>
       <c r="K17"/>
@@ -1585,27 +1556,15 @@
       <c r="M17"/>
       <c r="N17"/>
     </row>
-    <row r="18" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" s="13"/>
-      <c r="G18" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" s="32"/>
+    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="33"/>
       <c r="I18"/>
       <c r="J18"/>
       <c r="K18"/>
@@ -1613,105 +1572,132 @@
       <c r="M18"/>
       <c r="N18"/>
     </row>
-    <row r="19" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="15"/>
-      <c r="B19" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F19" s="13"/>
-      <c r="H19" s="33"/>
-      <c r="I19"/>
-      <c r="J19"/>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-    </row>
-    <row r="20" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="33"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="7">
+        <v>4</v>
+      </c>
+      <c r="B19" s="7">
+        <f>C13+1</f>
+        <v>260096</v>
+      </c>
+      <c r="C19" s="7">
+        <f>B19+A19-1</f>
+        <v>260099</v>
+      </c>
+      <c r="D19" s="7" t="str">
+        <f t="shared" ref="D19:E43" si="9">DEC2HEX(B19,6)</f>
+        <v>03F800</v>
+      </c>
+      <c r="E19" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>03F803</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" t="str">
+        <f t="shared" ref="J19" si="10">DEC2BIN(B19/2^11,7)</f>
+        <v>1111111</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>4</v>
+      </c>
+      <c r="B20" s="7">
+        <f>B19+4</f>
+        <v>260100</v>
+      </c>
+      <c r="C20" s="7">
+        <f t="shared" ref="C20:C37" si="11">B20+A20-1</f>
+        <v>260103</v>
+      </c>
+      <c r="D20" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>03F804</v>
+      </c>
+      <c r="E20" s="7" t="str">
+        <f t="shared" si="9"/>
+        <v>03F807</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="H20" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I20" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B21" s="7">
-        <f>C15+1</f>
-        <v>260096</v>
+        <f t="shared" ref="B21:B42" si="12">B20+4</f>
+        <v>260104</v>
       </c>
       <c r="C21" s="7">
-        <f>B21+A21-1</f>
-        <v>260099</v>
+        <f t="shared" si="11"/>
+        <v>260104</v>
       </c>
       <c r="D21" s="7" t="str">
-        <f t="shared" ref="D21:E45" si="8">DEC2HEX(B21,6)</f>
-        <v>03F800</v>
+        <f t="shared" si="9"/>
+        <v>03F808</v>
       </c>
       <c r="E21" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F803</v>
+        <f t="shared" si="9"/>
+        <v>03F808</v>
       </c>
       <c r="F21" s="7"/>
       <c r="G21" s="8" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="H21" s="30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I21" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B22" s="7">
-        <f>B21+4</f>
-        <v>260100</v>
+        <f t="shared" si="12"/>
+        <v>260108</v>
       </c>
       <c r="C22" s="7">
-        <f t="shared" ref="C22:C39" si="9">B22+A22-1</f>
-        <v>260103</v>
+        <f t="shared" si="11"/>
+        <v>260108</v>
       </c>
       <c r="D22" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F804</v>
+        <f t="shared" si="9"/>
+        <v>03F80C</v>
       </c>
       <c r="E22" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F807</v>
+        <f t="shared" si="9"/>
+        <v>03F80C</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="8" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="H22" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I22" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1719,30 +1705,30 @@
         <v>1</v>
       </c>
       <c r="B23" s="7">
-        <f t="shared" ref="B23:B44" si="10">B22+4</f>
-        <v>260104</v>
+        <f t="shared" si="12"/>
+        <v>260112</v>
       </c>
       <c r="C23" s="7">
+        <f t="shared" si="11"/>
+        <v>260112</v>
+      </c>
+      <c r="D23" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260104</v>
-      </c>
-      <c r="D23" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F808</v>
+        <v>03F810</v>
       </c>
       <c r="E23" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F808</v>
+        <f t="shared" si="9"/>
+        <v>03F810</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="8" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="H23" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I23" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
@@ -1750,61 +1736,61 @@
         <v>1</v>
       </c>
       <c r="B24" s="7">
-        <f t="shared" si="10"/>
-        <v>260108</v>
+        <f t="shared" si="12"/>
+        <v>260116</v>
       </c>
       <c r="C24" s="7">
+        <f t="shared" si="11"/>
+        <v>260116</v>
+      </c>
+      <c r="D24" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260108</v>
-      </c>
-      <c r="D24" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F80C</v>
+        <v>03F814</v>
       </c>
       <c r="E24" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F80C</v>
+        <f t="shared" si="9"/>
+        <v>03F814</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="8" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>33</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B25" s="7">
-        <f t="shared" si="10"/>
-        <v>260112</v>
+        <f t="shared" si="12"/>
+        <v>260120</v>
       </c>
       <c r="C25" s="7">
+        <f t="shared" si="11"/>
+        <v>260121</v>
+      </c>
+      <c r="D25" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260112</v>
-      </c>
-      <c r="D25" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F810</v>
+        <v>03F818</v>
       </c>
       <c r="E25" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F810</v>
+        <f t="shared" si="9"/>
+        <v>03F819</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="8" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="H25" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I25" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -1812,1002 +1798,776 @@
         <v>1</v>
       </c>
       <c r="B26" s="7">
-        <f t="shared" si="10"/>
-        <v>260116</v>
+        <f t="shared" si="12"/>
+        <v>260124</v>
       </c>
       <c r="C26" s="7">
+        <f>B26+A26-1</f>
+        <v>260124</v>
+      </c>
+      <c r="D26" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260116</v>
-      </c>
-      <c r="D26" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F814</v>
+        <v>03F81C</v>
       </c>
       <c r="E26" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F814</v>
+        <f t="shared" si="9"/>
+        <v>03F81C</v>
       </c>
       <c r="F26" s="7"/>
       <c r="G26" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I26" t="s">
-        <v>76</v>
+        <v>33</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" s="7">
-        <f t="shared" si="10"/>
-        <v>260120</v>
+        <f t="shared" si="12"/>
+        <v>260128</v>
       </c>
       <c r="C27" s="7">
+        <f t="shared" si="11"/>
+        <v>260128</v>
+      </c>
+      <c r="D27" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260121</v>
-      </c>
-      <c r="D27" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F818</v>
+        <v>03F820</v>
       </c>
       <c r="E27" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F819</v>
+        <f t="shared" si="9"/>
+        <v>03F820</v>
       </c>
       <c r="F27" s="7"/>
       <c r="G27" s="8" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H27" s="30" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I27" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B28" s="7">
-        <f t="shared" si="10"/>
-        <v>260124</v>
+        <f t="shared" si="12"/>
+        <v>260132</v>
       </c>
       <c r="C28" s="7">
-        <f>B28+A28-1</f>
-        <v>260124</v>
+        <f t="shared" si="11"/>
+        <v>260135</v>
       </c>
       <c r="D28" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F81C</v>
+        <f t="shared" si="9"/>
+        <v>03F824</v>
       </c>
       <c r="E28" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F81C</v>
+        <f t="shared" si="9"/>
+        <v>03F827</v>
       </c>
       <c r="F28" s="7"/>
       <c r="G28" s="8" t="s">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="H28" s="30" t="s">
         <v>74</v>
       </c>
       <c r="I28" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B29" s="7">
-        <f t="shared" si="10"/>
-        <v>260128</v>
+        <f t="shared" si="12"/>
+        <v>260136</v>
       </c>
       <c r="C29" s="7">
+        <f t="shared" si="11"/>
+        <v>260139</v>
+      </c>
+      <c r="D29" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260128</v>
-      </c>
-      <c r="D29" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F820</v>
+        <v>03F828</v>
       </c>
       <c r="E29" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F820</v>
+        <f t="shared" si="9"/>
+        <v>03F82B</v>
       </c>
       <c r="F29" s="7"/>
       <c r="G29" s="8" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H29" s="30" t="s">
         <v>74</v>
       </c>
       <c r="I29" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B30" s="7">
-        <f t="shared" si="10"/>
-        <v>260132</v>
+        <f t="shared" si="12"/>
+        <v>260140</v>
       </c>
       <c r="C30" s="7">
+        <f t="shared" si="11"/>
+        <v>260141</v>
+      </c>
+      <c r="D30" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260135</v>
-      </c>
-      <c r="D30" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F824</v>
+        <v>03F82C</v>
       </c>
       <c r="E30" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F827</v>
+        <f t="shared" si="9"/>
+        <v>03F82D</v>
       </c>
       <c r="F30" s="7"/>
       <c r="G30" s="8" t="s">
-        <v>38</v>
+        <v>59</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I30" t="s">
-        <v>106</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B31" s="7">
-        <f t="shared" si="10"/>
-        <v>260136</v>
+        <f t="shared" si="12"/>
+        <v>260144</v>
       </c>
       <c r="C31" s="7">
+        <f t="shared" si="11"/>
+        <v>260145</v>
+      </c>
+      <c r="D31" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260139</v>
-      </c>
-      <c r="D31" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F828</v>
+        <v>03F830</v>
       </c>
       <c r="E31" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F82B</v>
+        <f t="shared" si="9"/>
+        <v>03F831</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="8" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H31" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I31" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="7">
-        <f t="shared" si="10"/>
-        <v>260140</v>
+        <f t="shared" si="12"/>
+        <v>260148</v>
       </c>
       <c r="C32" s="7">
+        <f t="shared" si="11"/>
+        <v>260148</v>
+      </c>
+      <c r="D32" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260141</v>
-      </c>
-      <c r="D32" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F82C</v>
+        <v>03F834</v>
       </c>
       <c r="E32" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F82D</v>
+        <f t="shared" si="9"/>
+        <v>03F834</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="8" t="s">
-        <v>59</v>
+        <v>17</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I32" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B33" s="7">
-        <f t="shared" si="10"/>
-        <v>260144</v>
+        <f t="shared" si="12"/>
+        <v>260152</v>
       </c>
       <c r="C33" s="7">
+        <f t="shared" si="11"/>
+        <v>260152</v>
+      </c>
+      <c r="D33" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260145</v>
-      </c>
-      <c r="D33" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F830</v>
+        <v>03F838</v>
       </c>
       <c r="E33" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F831</v>
+        <f t="shared" si="9"/>
+        <v>03F838</v>
       </c>
       <c r="F33" s="7"/>
       <c r="G33" s="8" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="H33" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I33" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>1</v>
       </c>
       <c r="B34" s="7">
-        <f t="shared" si="10"/>
-        <v>260148</v>
+        <f t="shared" si="12"/>
+        <v>260156</v>
       </c>
       <c r="C34" s="7">
+        <f t="shared" si="11"/>
+        <v>260156</v>
+      </c>
+      <c r="D34" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260148</v>
-      </c>
-      <c r="D34" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F834</v>
+        <v>03F83C</v>
       </c>
       <c r="E34" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F834</v>
+        <f t="shared" si="9"/>
+        <v>03F83C</v>
       </c>
       <c r="F34" s="7"/>
       <c r="G34" s="8" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I34" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>1</v>
       </c>
       <c r="B35" s="7">
-        <f t="shared" si="10"/>
-        <v>260152</v>
+        <f t="shared" si="12"/>
+        <v>260160</v>
       </c>
       <c r="C35" s="7">
+        <f t="shared" si="11"/>
+        <v>260160</v>
+      </c>
+      <c r="D35" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260152</v>
-      </c>
-      <c r="D35" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F838</v>
+        <v>03F840</v>
       </c>
       <c r="E35" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F838</v>
+        <f t="shared" si="9"/>
+        <v>03F840</v>
       </c>
       <c r="F35" s="7"/>
       <c r="G35" s="8" t="s">
-        <v>23</v>
+        <v>86</v>
       </c>
       <c r="H35" s="30" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>1</v>
       </c>
       <c r="B36" s="7">
-        <f t="shared" si="10"/>
-        <v>260156</v>
+        <f t="shared" si="12"/>
+        <v>260164</v>
       </c>
       <c r="C36" s="7">
+        <f t="shared" si="11"/>
+        <v>260164</v>
+      </c>
+      <c r="D36" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260156</v>
-      </c>
-      <c r="D36" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F83C</v>
+        <v>03F844</v>
       </c>
       <c r="E36" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F83C</v>
+        <f t="shared" si="9"/>
+        <v>03F844</v>
       </c>
       <c r="F36" s="7"/>
       <c r="G36" s="8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I36" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>1</v>
       </c>
       <c r="B37" s="7">
-        <f t="shared" si="10"/>
-        <v>260160</v>
+        <f t="shared" si="12"/>
+        <v>260168</v>
       </c>
       <c r="C37" s="7">
+        <f t="shared" si="11"/>
+        <v>260168</v>
+      </c>
+      <c r="D37" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>260160</v>
-      </c>
-      <c r="D37" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F840</v>
+        <v>03F848</v>
       </c>
       <c r="E37" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F840</v>
+        <f t="shared" si="9"/>
+        <v>03F848</v>
       </c>
       <c r="F37" s="7"/>
       <c r="G37" s="8" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="H37" s="30" t="s">
         <v>74</v>
       </c>
       <c r="I37" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>1</v>
       </c>
       <c r="B38" s="7">
-        <f t="shared" si="10"/>
-        <v>260164</v>
+        <f t="shared" si="12"/>
+        <v>260172</v>
       </c>
       <c r="C38" s="7">
-        <f t="shared" si="9"/>
-        <v>260164</v>
+        <f t="shared" ref="C38:C42" si="13">B38+A38-1</f>
+        <v>260172</v>
       </c>
       <c r="D38" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F844</v>
+        <f t="shared" ref="D38:D42" si="14">DEC2HEX(B38,6)</f>
+        <v>03F84C</v>
       </c>
       <c r="E38" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F844</v>
+        <f t="shared" ref="E38:E42" si="15">DEC2HEX(C38,6)</f>
+        <v>03F84C</v>
       </c>
       <c r="F38" s="7"/>
       <c r="G38" s="8" t="s">
-        <v>25</v>
+        <v>149</v>
       </c>
       <c r="H38" s="30" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I38" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>1</v>
       </c>
       <c r="B39" s="7">
-        <f t="shared" si="10"/>
-        <v>260168</v>
+        <f t="shared" si="12"/>
+        <v>260176</v>
       </c>
       <c r="C39" s="7">
-        <f t="shared" si="9"/>
-        <v>260168</v>
+        <f t="shared" si="13"/>
+        <v>260176</v>
       </c>
       <c r="D39" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F848</v>
+        <f t="shared" si="14"/>
+        <v>03F850</v>
       </c>
       <c r="E39" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F848</v>
+        <f t="shared" si="15"/>
+        <v>03F850</v>
       </c>
       <c r="F39" s="7"/>
       <c r="G39" s="8" t="s">
-        <v>93</v>
+        <v>150</v>
       </c>
       <c r="H39" s="30" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I39" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>1</v>
       </c>
       <c r="B40" s="7">
-        <f t="shared" si="10"/>
-        <v>260172</v>
+        <f t="shared" si="12"/>
+        <v>260180</v>
       </c>
       <c r="C40" s="7">
-        <f t="shared" ref="C40:C44" si="11">B40+A40-1</f>
-        <v>260172</v>
+        <f t="shared" si="13"/>
+        <v>260180</v>
       </c>
       <c r="D40" s="7" t="str">
-        <f t="shared" ref="D40:D44" si="12">DEC2HEX(B40,6)</f>
-        <v>03F84C</v>
+        <f t="shared" si="14"/>
+        <v>03F854</v>
       </c>
       <c r="E40" s="7" t="str">
-        <f t="shared" ref="E40:E44" si="13">DEC2HEX(C40,6)</f>
-        <v>03F84C</v>
+        <f t="shared" si="15"/>
+        <v>03F854</v>
       </c>
       <c r="F40" s="7"/>
       <c r="G40" s="8" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="H40" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I40" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>1</v>
       </c>
       <c r="B41" s="7">
-        <f t="shared" si="10"/>
-        <v>260176</v>
+        <f t="shared" si="12"/>
+        <v>260184</v>
       </c>
       <c r="C41" s="7">
-        <f t="shared" si="11"/>
-        <v>260176</v>
+        <f t="shared" si="13"/>
+        <v>260184</v>
       </c>
       <c r="D41" s="7" t="str">
-        <f t="shared" si="12"/>
-        <v>03F850</v>
+        <f t="shared" si="14"/>
+        <v>03F858</v>
       </c>
       <c r="E41" s="7" t="str">
-        <f t="shared" si="13"/>
-        <v>03F850</v>
+        <f t="shared" si="15"/>
+        <v>03F858</v>
       </c>
       <c r="F41" s="7"/>
       <c r="G41" s="8" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="H41" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I41" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>1</v>
       </c>
       <c r="B42" s="7">
-        <f t="shared" si="10"/>
-        <v>260180</v>
+        <f t="shared" si="12"/>
+        <v>260188</v>
       </c>
       <c r="C42" s="7">
-        <f t="shared" si="11"/>
-        <v>260180</v>
+        <f t="shared" si="13"/>
+        <v>260188</v>
       </c>
       <c r="D42" s="7" t="str">
-        <f t="shared" si="12"/>
-        <v>03F854</v>
+        <f t="shared" si="14"/>
+        <v>03F85C</v>
       </c>
       <c r="E42" s="7" t="str">
-        <f t="shared" si="13"/>
-        <v>03F854</v>
+        <f t="shared" si="15"/>
+        <v>03F85C</v>
       </c>
       <c r="F42" s="7"/>
       <c r="G42" s="8" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="H42" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I42" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
-        <v>1</v>
+        <f>C43-B43</f>
+        <v>1951</v>
       </c>
       <c r="B43" s="7">
-        <f t="shared" si="10"/>
-        <v>260184</v>
+        <f>B42+4</f>
+        <v>260192</v>
       </c>
       <c r="C43" s="7">
-        <f t="shared" si="11"/>
-        <v>260184</v>
+        <f>C49</f>
+        <v>262143</v>
       </c>
       <c r="D43" s="7" t="str">
-        <f t="shared" si="12"/>
-        <v>03F858</v>
+        <f t="shared" si="9"/>
+        <v>03F860</v>
       </c>
       <c r="E43" s="7" t="str">
-        <f t="shared" si="13"/>
-        <v>03F858</v>
+        <f t="shared" si="9"/>
+        <v>03FFFF</v>
       </c>
       <c r="F43" s="7"/>
-      <c r="G43" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="H43" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I43" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="7">
-        <v>1</v>
-      </c>
-      <c r="B44" s="7">
-        <f t="shared" si="10"/>
-        <v>260188</v>
-      </c>
-      <c r="C44" s="7">
-        <f t="shared" si="11"/>
-        <v>260188</v>
-      </c>
-      <c r="D44" s="7" t="str">
-        <f t="shared" si="12"/>
-        <v>03F85C</v>
-      </c>
-      <c r="E44" s="7" t="str">
-        <f t="shared" si="13"/>
-        <v>03F85C</v>
-      </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="H44" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I44" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="7">
-        <f>C45-B45</f>
-        <v>1807</v>
-      </c>
-      <c r="B45" s="7">
-        <f>B44+4</f>
-        <v>260192</v>
-      </c>
-      <c r="C45" s="7">
-        <f>B46-1</f>
-        <v>261999</v>
-      </c>
-      <c r="D45" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03F860</v>
-      </c>
-      <c r="E45" s="7" t="str">
-        <f t="shared" si="8"/>
-        <v>03FF6F</v>
-      </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="12" t="s">
+      <c r="G43" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A46" s="7">
-        <f>4*32</f>
-        <v>128</v>
-      </c>
-      <c r="B46" s="7">
-        <f>B47-A46</f>
-        <v>262000</v>
-      </c>
-      <c r="C46" s="7">
-        <f>B46+A46-1</f>
-        <v>262127</v>
-      </c>
-      <c r="D46" s="7" t="str">
-        <f t="shared" ref="D46:D47" si="14">DEC2HEX(B46,6)</f>
-        <v>03FF70</v>
-      </c>
-      <c r="E46" s="7" t="str">
-        <f t="shared" ref="E46:E47" si="15">DEC2HEX(C46,6)</f>
-        <v>03FFEF</v>
-      </c>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8" t="s">
-        <v>109</v>
-      </c>
-      <c r="H46" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I46" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="7">
-        <v>4</v>
-      </c>
-      <c r="B47" s="7">
-        <f t="shared" ref="B47" si="16">B48-A47</f>
-        <v>262128</v>
-      </c>
-      <c r="C47" s="7">
-        <f>B47+A47-1</f>
-        <v>262131</v>
-      </c>
-      <c r="D47" s="7" t="str">
-        <f t="shared" si="14"/>
-        <v>03FFF0</v>
-      </c>
-      <c r="E47" s="7" t="str">
-        <f t="shared" si="15"/>
-        <v>03FFF3</v>
-      </c>
-      <c r="F47" s="7"/>
-      <c r="G47" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="H47" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="I47" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A48" s="7">
-        <v>4</v>
-      </c>
-      <c r="B48" s="7">
-        <f t="shared" ref="B48:B49" si="17">B49-A48</f>
-        <v>262132</v>
-      </c>
-      <c r="C48" s="7">
-        <f>B48+A48-1</f>
-        <v>262135</v>
-      </c>
-      <c r="D48" s="7" t="str">
-        <f t="shared" ref="D48" si="18">DEC2HEX(B48,6)</f>
-        <v>03FFF4</v>
-      </c>
-      <c r="E48" s="7" t="str">
-        <f t="shared" ref="E48" si="19">DEC2HEX(C48,6)</f>
-        <v>03FFF7</v>
-      </c>
-      <c r="F48" s="7"/>
-      <c r="G48" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="H48" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I48" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D45" s="16"/>
+      <c r="E45" s="16"/>
+      <c r="F45" s="16"/>
+      <c r="H45" s="30"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+    </row>
+    <row r="46" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" s="13"/>
+      <c r="G46" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="H46" s="30"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+    </row>
+    <row r="47" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="13"/>
+      <c r="B47" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E47" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="F47" s="13"/>
+      <c r="H47" s="30"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+    </row>
+    <row r="48" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="10"/>
+      <c r="H48" s="30"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <v>4</v>
+        <f>256*1024</f>
+        <v>262144</v>
       </c>
       <c r="B49" s="7">
+        <v>0</v>
+      </c>
+      <c r="C49" s="7">
+        <f>A49-1</f>
+        <v>262143</v>
+      </c>
+      <c r="D49" s="7" t="str">
+        <f>DEC2HEX(B49,6)</f>
+        <v>000000</v>
+      </c>
+      <c r="E49" s="7" t="str">
+        <f>DEC2HEX(C49,6)</f>
+        <v>03FFFF</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H49" s="34"/>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <f>2*(128*96*2)</f>
+        <v>49152</v>
+      </c>
+      <c r="B50" s="7">
+        <f>C49+1</f>
+        <v>262144</v>
+      </c>
+      <c r="C50" s="7">
+        <f t="shared" ref="C50:C52" si="16">B50+A50-1</f>
+        <v>311295</v>
+      </c>
+      <c r="D50" s="7" t="str">
+        <f t="shared" ref="D50:E53" si="17">DEC2HEX(B50,6)</f>
+        <v>040000</v>
+      </c>
+      <c r="E50" s="7" t="str">
         <f t="shared" si="17"/>
-        <v>262136</v>
-      </c>
-      <c r="C49" s="7">
-        <f>B49+A49-1</f>
-        <v>262139</v>
-      </c>
-      <c r="D49" s="7" t="str">
-        <f t="shared" ref="D49" si="20">DEC2HEX(B49,6)</f>
-        <v>03FFF8</v>
-      </c>
-      <c r="E49" s="7" t="str">
-        <f t="shared" ref="E49" si="21">DEC2HEX(C49,6)</f>
-        <v>03FFFB</v>
-      </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="H49" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I49" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A50" s="7">
-        <v>4</v>
-      </c>
-      <c r="B50" s="7">
-        <f>B57-A50</f>
-        <v>262140</v>
-      </c>
-      <c r="C50" s="7">
-        <f>B50+A50-1</f>
-        <v>262143</v>
-      </c>
-      <c r="D50" s="7" t="str">
-        <f t="shared" ref="D50" si="22">DEC2HEX(B50,6)</f>
-        <v>03FFFC</v>
-      </c>
-      <c r="E50" s="7" t="str">
-        <f t="shared" ref="E50" si="23">DEC2HEX(C50,6)</f>
-        <v>03FFFF</v>
+        <v>04BFFF</v>
       </c>
       <c r="F50" s="7"/>
       <c r="G50" s="8" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>74</v>
-      </c>
-      <c r="I50" t="s">
-        <v>111</v>
-      </c>
-      <c r="J50" s="36">
-        <f>B21+255</f>
-        <v>260351</v>
-      </c>
-      <c r="K50" s="36" t="str">
-        <f>DEC2HEX(J50,6)</f>
-        <v>03F8FF</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D52" s="16"/>
-      <c r="E52" s="16"/>
-      <c r="F52" s="16"/>
-      <c r="H52" s="30"/>
-      <c r="I52"/>
-      <c r="J52"/>
-      <c r="K52"/>
-      <c r="L52"/>
-      <c r="M52"/>
-      <c r="N52"/>
-    </row>
-    <row r="53" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B53" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C53" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="D53" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F53" s="13"/>
-      <c r="G53" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H53" s="30"/>
-      <c r="I53"/>
-      <c r="J53"/>
-      <c r="K53"/>
-      <c r="L53"/>
-      <c r="M53"/>
-      <c r="N53"/>
-    </row>
-    <row r="54" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
-      <c r="B54" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="C54" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D54" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E54" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="F54" s="13"/>
-      <c r="H54" s="30"/>
-      <c r="I54"/>
-      <c r="J54"/>
-      <c r="K54"/>
-      <c r="L54"/>
-      <c r="M54"/>
-      <c r="N54"/>
-    </row>
-    <row r="55" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="6"/>
-      <c r="B55" s="6"/>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="6"/>
-      <c r="G55" s="10"/>
-      <c r="H55" s="30"/>
-      <c r="I55"/>
-      <c r="J55"/>
-      <c r="K55"/>
-      <c r="L55"/>
-      <c r="M55"/>
-      <c r="N55"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="7">
-        <f>256*1024</f>
-        <v>262144</v>
-      </c>
-      <c r="B56" s="7">
-        <v>0</v>
-      </c>
-      <c r="C56" s="7">
-        <f>A56-1</f>
-        <v>262143</v>
-      </c>
-      <c r="D56" s="7" t="str">
-        <f>DEC2HEX(B56,6)</f>
-        <v>000000</v>
-      </c>
-      <c r="E56" s="7" t="str">
-        <f>DEC2HEX(C56,6)</f>
-        <v>03FFFF</v>
-      </c>
-      <c r="F56" s="7"/>
-      <c r="G56" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="H56" s="34"/>
-    </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="7">
-        <f>2*(128*96*2)</f>
-        <v>49152</v>
-      </c>
-      <c r="B57" s="7">
-        <f>C56+1</f>
-        <v>262144</v>
-      </c>
-      <c r="C57" s="7">
-        <f t="shared" ref="C57:C59" si="24">B57+A57-1</f>
-        <v>311295</v>
-      </c>
-      <c r="D57" s="7" t="str">
-        <f t="shared" ref="D57:E60" si="25">DEC2HEX(B57,6)</f>
-        <v>040000</v>
-      </c>
-      <c r="E57" s="7" t="str">
-        <f t="shared" si="25"/>
-        <v>04BFFF</v>
-      </c>
-      <c r="F57" s="7"/>
-      <c r="G57" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="H57" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="7">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
         <v>512</v>
       </c>
-      <c r="B58" s="7">
-        <f>C57+1</f>
+      <c r="B51" s="7">
+        <f>C50+1</f>
         <v>311296</v>
       </c>
-      <c r="C58" s="7">
-        <f t="shared" ref="C58" si="26">B58+A58-1</f>
+      <c r="C51" s="7">
+        <f t="shared" ref="C51" si="18">B51+A51-1</f>
         <v>311807</v>
       </c>
-      <c r="D58" s="7" t="str">
-        <f t="shared" ref="D58" si="27">DEC2HEX(B58,6)</f>
+      <c r="D51" s="7" t="str">
+        <f t="shared" ref="D51" si="19">DEC2HEX(B51,6)</f>
         <v>04C000</v>
       </c>
-      <c r="E58" s="7" t="str">
-        <f t="shared" ref="E58" si="28">DEC2HEX(C58,6)</f>
+      <c r="E51" s="7" t="str">
+        <f t="shared" ref="E51" si="20">DEC2HEX(C51,6)</f>
         <v>04C1FF</v>
       </c>
-      <c r="F58" s="7"/>
-      <c r="G58" s="8" t="s">
-        <v>134</v>
-      </c>
-      <c r="H58" s="30" t="s">
+      <c r="F51" s="7"/>
+      <c r="G51" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="H51" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="7">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
         <v>512</v>
       </c>
-      <c r="B59" s="7">
-        <f>C58+1</f>
+      <c r="B52" s="7">
+        <f>C51+1</f>
         <v>311808</v>
       </c>
-      <c r="C59" s="7">
-        <f t="shared" si="24"/>
+      <c r="C52" s="7">
+        <f t="shared" si="16"/>
         <v>312319</v>
       </c>
-      <c r="D59" s="7" t="str">
-        <f t="shared" si="25"/>
+      <c r="D52" s="7" t="str">
+        <f t="shared" si="17"/>
         <v>04C200</v>
       </c>
-      <c r="E59" s="7" t="str">
-        <f t="shared" si="25"/>
+      <c r="E52" s="7" t="str">
+        <f t="shared" si="17"/>
         <v>04C3FF</v>
       </c>
-      <c r="F59" s="7"/>
-      <c r="G59" s="8" t="s">
-        <v>133</v>
-      </c>
-      <c r="H59" s="30" t="s">
+      <c r="F52" s="7"/>
+      <c r="G52" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="H52" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="7">
-        <f>C60-B60</f>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <f>C53-B53</f>
         <v>16464895</v>
       </c>
-      <c r="B60" s="7">
-        <f>C59+1</f>
+      <c r="B53" s="7">
+        <f>C52+1</f>
         <v>312320</v>
       </c>
-      <c r="C60" s="7">
+      <c r="C53" s="7">
         <f>16*1024*1024-1</f>
         <v>16777215</v>
       </c>
-      <c r="D60" s="7" t="str">
-        <f t="shared" si="25"/>
+      <c r="D53" s="7" t="str">
+        <f t="shared" si="17"/>
         <v>04C400</v>
       </c>
-      <c r="E60" s="7" t="str">
-        <f t="shared" si="25"/>
+      <c r="E53" s="7" t="str">
+        <f t="shared" si="17"/>
         <v>FFFFFF</v>
       </c>
-      <c r="F60" s="7"/>
-      <c r="G60" s="8" t="s">
+      <c r="F53" s="7"/>
+      <c r="G53" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H60" s="30" t="s">
+      <c r="H53" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I60" t="s">
+      <c r="I53" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2821,8 +2581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2836,7 +2596,7 @@
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2859,8 +2619,8 @@
       <c r="G3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="37" t="s">
-        <v>132</v>
+      <c r="H3" s="36" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2917,15 +2677,15 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="8" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="H6" s="30">
-        <f>B6+'NEW Memory Map'!$B$10</f>
-        <v>245760</v>
+        <f>B6+'Memory Map'!$B$10</f>
+        <v>249856</v>
       </c>
       <c r="I6" s="7" t="str">
         <f>DEC2HEX(H6,6)</f>
-        <v>03C000</v>
+        <v>03D000</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2950,15 +2710,15 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="H7" s="30">
-        <f>B7+'NEW Memory Map'!$B$10</f>
-        <v>245764</v>
+        <f>B7+'Memory Map'!$B$10</f>
+        <v>249860</v>
       </c>
       <c r="I7" s="7" t="str">
         <f t="shared" ref="I7:I19" si="1">DEC2HEX(H7,6)</f>
-        <v>03C004</v>
+        <v>03D004</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2983,15 +2743,15 @@
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="H8" s="30">
-        <f>B8+'NEW Memory Map'!$B$10</f>
-        <v>245768</v>
+        <f>B8+'Memory Map'!$B$10</f>
+        <v>249864</v>
       </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C008</v>
+        <v>03D008</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3016,15 +2776,15 @@
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="H9" s="30">
-        <f>B9+'NEW Memory Map'!$B$10</f>
-        <v>245772</v>
+        <f>B9+'Memory Map'!$B$10</f>
+        <v>249868</v>
       </c>
       <c r="I9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C00C</v>
+        <v>03D00C</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3049,15 +2809,15 @@
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="H10" s="30">
-        <f>B10+'NEW Memory Map'!$B$10</f>
-        <v>245776</v>
+        <f>B10+'Memory Map'!$B$10</f>
+        <v>249872</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C010</v>
+        <v>03D010</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3082,15 +2842,15 @@
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="H11" s="30">
-        <f>B11+'NEW Memory Map'!$B$10</f>
-        <v>245780</v>
+        <f>B11+'Memory Map'!$B$10</f>
+        <v>249876</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C014</v>
+        <v>03D014</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3115,15 +2875,15 @@
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="8" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="H12" s="30">
-        <f>B12+'NEW Memory Map'!$B$10</f>
-        <v>245784</v>
+        <f>B12+'Memory Map'!$B$10</f>
+        <v>249880</v>
       </c>
       <c r="I12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C018</v>
+        <v>03D018</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3148,15 +2908,15 @@
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="8" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="H13" s="30">
-        <f>B13+'NEW Memory Map'!$B$10</f>
-        <v>245788</v>
+        <f>B13+'Memory Map'!$B$10</f>
+        <v>249884</v>
       </c>
       <c r="I13" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C01C</v>
+        <v>03D01C</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3181,15 +2941,15 @@
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="8" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="H14" s="30">
-        <f>B14+'NEW Memory Map'!$B$10</f>
-        <v>245789</v>
+        <f>B14+'Memory Map'!$B$10</f>
+        <v>249885</v>
       </c>
       <c r="I14" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C01D</v>
+        <v>03D01D</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3214,15 +2974,15 @@
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
       <c r="H15" s="30">
-        <f>B15+'NEW Memory Map'!$B$10</f>
-        <v>245790</v>
+        <f>B15+'Memory Map'!$B$10</f>
+        <v>249886</v>
       </c>
       <c r="I15" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C01E</v>
+        <v>03D01E</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3248,15 +3008,15 @@
       </c>
       <c r="F16" s="7"/>
       <c r="G16" s="8" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
       <c r="H16" s="30">
-        <f>B16+'NEW Memory Map'!$B$10</f>
-        <v>245804</v>
+        <f>B16+'Memory Map'!$B$10</f>
+        <v>249900</v>
       </c>
       <c r="I16" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C02C</v>
+        <v>03D02C</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3281,15 +3041,15 @@
       </c>
       <c r="F17" s="7"/>
       <c r="G17" s="8" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
       <c r="H17" s="30">
-        <f>B17+'NEW Memory Map'!$B$10</f>
-        <v>246784</v>
+        <f>B17+'Memory Map'!$B$10</f>
+        <v>250880</v>
       </c>
       <c r="I17" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C400</v>
+        <v>03D400</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3314,15 +3074,15 @@
       </c>
       <c r="F18" s="7"/>
       <c r="G18" s="8" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
       <c r="H18" s="30">
-        <f>B18+'NEW Memory Map'!$B$10</f>
-        <v>247296</v>
+        <f>B18+'Memory Map'!$B$10</f>
+        <v>251392</v>
       </c>
       <c r="I18" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C600</v>
+        <v>03D600</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3350,12 +3110,12 @@
         <v>99</v>
       </c>
       <c r="H19" s="30">
-        <f>B19+'NEW Memory Map'!$B$10</f>
-        <v>247552</v>
+        <f>B19+'Memory Map'!$B$10</f>
+        <v>251648</v>
       </c>
       <c r="I19" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C700</v>
+        <v>03D700</v>
       </c>
     </row>
   </sheetData>
@@ -3365,10 +3125,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I13"/>
+  <dimension ref="A2:I11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3382,7 +3142,7 @@
   <sheetData>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3405,8 +3165,8 @@
       <c r="G3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="37" t="s">
-        <v>132</v>
+      <c r="H3" s="36" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3454,7 +3214,7 @@
         <v>3</v>
       </c>
       <c r="D6" s="7" t="str">
-        <f t="shared" ref="D6:E13" si="0">DEC2HEX(B6,6)</f>
+        <f t="shared" ref="D6:E11" si="0">DEC2HEX(B6,6)</f>
         <v>000000</v>
       </c>
       <c r="E6" s="7" t="str">
@@ -3463,15 +3223,15 @@
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="8" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="H6" s="30">
-        <f>B6+'NEW Memory Map'!$B$9</f>
-        <v>243712</v>
+        <f>B6+'Memory Map'!$B$13</f>
+        <v>258048</v>
       </c>
       <c r="I6" s="7" t="str">
         <f>DEC2HEX(H6,6)</f>
-        <v>03B800</v>
+        <v>03F000</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3496,15 +3256,15 @@
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="H7" s="30">
-        <f>B7+'NEW Memory Map'!$B$9</f>
-        <v>243716</v>
+        <f>B7+'Memory Map'!$B$13</f>
+        <v>258052</v>
       </c>
       <c r="I7" s="7" t="str">
-        <f t="shared" ref="I7:I13" si="1">DEC2HEX(H7,6)</f>
-        <v>03B804</v>
+        <f t="shared" ref="I7:I11" si="1">DEC2HEX(H7,6)</f>
+        <v>03F004</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3528,76 +3288,80 @@
         <v>00000B</v>
       </c>
       <c r="F8" s="7"/>
-      <c r="G8" s="8"/>
+      <c r="G8" s="8" t="s">
+        <v>160</v>
+      </c>
       <c r="H8" s="30">
-        <f>B8+'NEW Memory Map'!$B$9</f>
-        <v>243720</v>
+        <f>B8+'Memory Map'!$B$13</f>
+        <v>258056</v>
       </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03B808</v>
+        <v>03F008</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="B9" s="7">
-        <f t="shared" ref="B9:B10" si="2">C8+1</f>
-        <v>12</v>
+        <v>512</v>
       </c>
       <c r="C9" s="7">
-        <f t="shared" ref="C9:C13" si="3">B9+A9-1</f>
-        <v>15</v>
+        <f t="shared" ref="C9:C11" si="2">B9+A9-1</f>
+        <v>639</v>
       </c>
       <c r="D9" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>00000C</v>
+        <v>000200</v>
       </c>
       <c r="E9" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>00000F</v>
+        <v>00027F</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
+      <c r="G9" s="8" t="s">
+        <v>125</v>
+      </c>
       <c r="H9" s="30">
-        <f>B9+'NEW Memory Map'!$B$9</f>
-        <v>243724</v>
+        <f>B9+'Memory Map'!$B$13</f>
+        <v>258560</v>
       </c>
       <c r="I9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03B80C</v>
+        <v>03F200</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
-        <v>4</v>
+        <v>128</v>
       </c>
       <c r="B10" s="7">
+        <v>1024</v>
+      </c>
+      <c r="C10" s="7">
         <f t="shared" si="2"/>
-        <v>16</v>
-      </c>
-      <c r="C10" s="7">
-        <f t="shared" si="3"/>
-        <v>19</v>
+        <v>1151</v>
       </c>
       <c r="D10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>000010</v>
+        <v>000400</v>
       </c>
       <c r="E10" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>000013</v>
+        <v>00047F</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="8"/>
+      <c r="G10" s="8" t="s">
+        <v>126</v>
+      </c>
       <c r="H10" s="30">
-        <f>B10+'NEW Memory Map'!$B$9</f>
-        <v>243728</v>
+        <f>B10+'Memory Map'!$B$13</f>
+        <v>259072</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03B810</v>
+        <v>03F400</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3605,96 +3369,32 @@
         <v>128</v>
       </c>
       <c r="B11" s="7">
-        <v>512</v>
+        <f>1024+512</f>
+        <v>1536</v>
       </c>
       <c r="C11" s="7">
-        <f t="shared" si="3"/>
-        <v>639</v>
+        <f t="shared" si="2"/>
+        <v>1663</v>
       </c>
       <c r="D11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>000200</v>
+        <v>000600</v>
       </c>
       <c r="E11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>00027F</v>
+        <v>00067F</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="H11" s="30">
-        <f>B11+'NEW Memory Map'!$B$9</f>
-        <v>244224</v>
+        <f>B11+'Memory Map'!$B$13</f>
+        <v>259584</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03BA00</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="7">
-        <v>128</v>
-      </c>
-      <c r="B12" s="7">
-        <v>1024</v>
-      </c>
-      <c r="C12" s="7">
-        <f t="shared" si="3"/>
-        <v>1151</v>
-      </c>
-      <c r="D12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>000400</v>
-      </c>
-      <c r="E12" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>00047F</v>
-      </c>
-      <c r="F12" s="7"/>
-      <c r="G12" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="H12" s="30">
-        <f>B12+'NEW Memory Map'!$B$9</f>
-        <v>244736</v>
-      </c>
-      <c r="I12" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>03BC00</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="7">
-        <v>128</v>
-      </c>
-      <c r="B13" s="7">
-        <f>1024+512</f>
-        <v>1536</v>
-      </c>
-      <c r="C13" s="7">
-        <f t="shared" si="3"/>
-        <v>1663</v>
-      </c>
-      <c r="D13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>000600</v>
-      </c>
-      <c r="E13" s="7" t="str">
-        <f t="shared" si="0"/>
-        <v>00067F</v>
-      </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="8" t="s">
-        <v>141</v>
-      </c>
-      <c r="H13" s="30">
-        <f>B13+'NEW Memory Map'!$B$9</f>
-        <v>245248</v>
-      </c>
-      <c r="I13" s="7" t="str">
-        <f t="shared" si="1"/>
-        <v>03BE00</v>
+        <v>03F600</v>
       </c>
     </row>
   </sheetData>
@@ -3707,7 +3407,7 @@
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3883,11 +3583,11 @@
       <c r="L6" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="M6" s="39" t="s">
+      <c r="M6" s="38" t="s">
         <v>97</v>
       </c>
-      <c r="N6" s="39"/>
-      <c r="O6" s="39"/>
+      <c r="N6" s="38"/>
+      <c r="O6" s="38"/>
     </row>
     <row r="7" spans="1:15" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
@@ -5714,46 +5414,46 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="H1" s="1" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="B2">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>156</v>
-      </c>
-      <c r="E2" s="38">
+        <v>142</v>
+      </c>
+      <c r="E2" s="37">
         <f>2^B2</f>
         <v>32</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="B3">
         <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
-      </c>
-      <c r="E3" s="38">
+        <v>136</v>
+      </c>
+      <c r="E3" s="37">
         <f t="shared" ref="E3:E6" si="0">2^B3</f>
         <v>256</v>
       </c>
       <c r="F3" s="18" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="H3">
         <v>32</v>
@@ -5765,20 +5465,20 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="B4">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4" s="38">
+        <v>137</v>
+      </c>
+      <c r="E4" s="37">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="F4" s="18" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="H4">
         <v>32</v>
@@ -5790,20 +5490,20 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="B5" s="1">
         <v>7</v>
       </c>
       <c r="D5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E5" s="38">
+        <v>138</v>
+      </c>
+      <c r="E5" s="37">
         <f t="shared" si="0"/>
         <v>128</v>
       </c>
       <c r="F5" s="18" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="H5">
         <v>544</v>
@@ -5815,20 +5515,20 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>153</v>
-      </c>
-      <c r="E6" s="38">
+        <v>139</v>
+      </c>
+      <c r="E6" s="37">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="F6" s="18" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="H6">
         <v>304</v>
@@ -5840,20 +5540,20 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B7">
         <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
-      </c>
-      <c r="E7" s="38">
+        <v>140</v>
+      </c>
+      <c r="E7" s="37">
         <f t="shared" ref="E7" si="2">2^B7</f>
         <v>512</v>
       </c>
       <c r="F7" s="18" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="H7">
         <v>32</v>

</xml_diff>

<commit_message>
Fixed a bug in addressing character and color RAM Developed routines to write extracted Amiga fonts directly into character RAM
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Map" sheetId="4" r:id="rId1"/>
@@ -1150,8 +1150,8 @@
   </sheetPr>
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1290,8 +1290,8 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
-        <f>(128-16)*1024</f>
-        <v>114688</v>
+        <f>(128-20)*1024</f>
+        <v>110592</v>
       </c>
       <c r="B8" s="7">
         <f t="shared" ref="B8:B12" si="0">C7+1</f>
@@ -1299,7 +1299,7 @@
       </c>
       <c r="C8" s="7">
         <f>B8+A8-1</f>
-        <v>245759</v>
+        <v>241663</v>
       </c>
       <c r="D8" s="7" t="str">
         <f t="shared" ref="D8:E13" si="1">DEC2HEX(B8,6)</f>
@@ -1307,7 +1307,7 @@
       </c>
       <c r="E8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03BFFF</v>
+        <v>03AFFF</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="8" t="s">
@@ -1316,11 +1316,12 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <v>4096</v>
+        <f>2*4096</f>
+        <v>8192</v>
       </c>
       <c r="B9" s="7">
         <f>C8+1</f>
-        <v>245760</v>
+        <v>241664</v>
       </c>
       <c r="C9" s="7">
         <f t="shared" ref="C9" si="2">B9+A9-1</f>
@@ -1328,7 +1329,7 @@
       </c>
       <c r="D9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03C000</v>
+        <v>03B000</v>
       </c>
       <c r="E9" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1346,7 +1347,7 @@
       </c>
       <c r="J9" t="str">
         <f>DEC2BIN(B9/2^11,7)</f>
-        <v>1111000</v>
+        <v>1110110</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -2581,8 +2582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Working version of Amigafont
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -14,13 +14,14 @@
     <sheet name="OLD Memory Map" sheetId="1" r:id="rId5"/>
     <sheet name="Copyright and license" sheetId="3" r:id="rId6"/>
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="162">
   <si>
     <t>Name</t>
   </si>
@@ -640,6 +641,9 @@
   </si>
   <si>
     <t>Interval</t>
+  </si>
+  <si>
+    <t>03B000</t>
   </si>
 </sst>
 </file>
@@ -1151,7 +1155,7 @@
   <dimension ref="A1:N53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1159,9 +1163,9 @@
     <col min="1" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="5" width="12.42578125" style="1" customWidth="1"/>
     <col min="6" max="6" width="3.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="34.28515625" style="8" customWidth="1"/>
+    <col min="7" max="7" width="33.5703125" style="8" customWidth="1"/>
     <col min="8" max="8" width="10.140625" style="30" customWidth="1"/>
-    <col min="9" max="9" width="79.140625" customWidth="1"/>
+    <col min="9" max="9" width="79.140625" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="25.7109375" customWidth="1"/>
     <col min="11" max="12" width="19.140625" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" customWidth="1"/>
@@ -1316,8 +1320,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
-        <f>2*4096</f>
-        <v>8192</v>
+        <v>2048</v>
       </c>
       <c r="B9" s="7">
         <f>C8+1</f>
@@ -1325,7 +1328,7 @@
       </c>
       <c r="C9" s="7">
         <f t="shared" ref="C9" si="2">B9+A9-1</f>
-        <v>249855</v>
+        <v>243711</v>
       </c>
       <c r="D9" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1333,22 +1336,23 @@
       </c>
       <c r="E9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03CFFF</v>
+        <v>03B7FF</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="8" t="s">
-        <v>4</v>
+        <v>159</v>
       </c>
       <c r="H9" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>105</v>
       </c>
       <c r="J9" t="str">
         <f>DEC2BIN(B9/2^11,7)</f>
         <v>1110110</v>
       </c>
+      <c r="L9" s="8"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
@@ -1356,19 +1360,19 @@
       </c>
       <c r="B10" s="7">
         <f>C9+1</f>
-        <v>249856</v>
+        <v>243712</v>
       </c>
       <c r="C10" s="7">
         <f t="shared" ref="C10" si="3">B10+A10-1</f>
-        <v>251903</v>
+        <v>245759</v>
       </c>
       <c r="D10" s="7" t="str">
         <f t="shared" ref="D10" si="4">DEC2HEX(B10,6)</f>
-        <v>03D000</v>
+        <v>03B800</v>
       </c>
       <c r="E10" s="7" t="str">
         <f t="shared" ref="E10" si="5">DEC2HEX(C10,6)</f>
-        <v>03D7FF</v>
+        <v>03BFFF</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="8" t="s">
@@ -1381,25 +1385,26 @@
         <v>96</v>
       </c>
       <c r="J10" t="str">
-        <f t="shared" ref="J10:J13" si="6">DEC2BIN(B10/2^11,7)</f>
-        <v>1111010</v>
-      </c>
+        <f>DEC2BIN(B10/2^11,7)</f>
+        <v>1110111</v>
+      </c>
+      <c r="L10" s="8"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
-        <v>2048</v>
+        <v>8192</v>
       </c>
       <c r="B11" s="7">
         <f>C10+1</f>
-        <v>251904</v>
+        <v>245760</v>
       </c>
       <c r="C11" s="7">
-        <f t="shared" ref="C11" si="7">B11+A11-1</f>
+        <f t="shared" ref="C11" si="6">B11+A11-1</f>
         <v>253951</v>
       </c>
       <c r="D11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D800</v>
+        <v>03C000</v>
       </c>
       <c r="E11" s="7" t="str">
         <f t="shared" si="1"/>
@@ -1407,18 +1412,19 @@
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="8" t="s">
-        <v>159</v>
+        <v>4</v>
       </c>
       <c r="H11" s="30" t="s">
         <v>72</v>
       </c>
       <c r="I11" t="s">
-        <v>105</v>
+        <v>51</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" si="6"/>
-        <v>1111011</v>
-      </c>
+        <f t="shared" ref="J10:J13" si="7">DEC2BIN(B11/2^11,7)</f>
+        <v>1111000</v>
+      </c>
+      <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
@@ -1451,7 +1457,7 @@
         <v>103</v>
       </c>
       <c r="J12" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1111100</v>
       </c>
     </row>
@@ -1486,7 +1492,7 @@
         <v>158</v>
       </c>
       <c r="J13" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1111110</v>
       </c>
     </row>
@@ -2682,11 +2688,11 @@
       </c>
       <c r="H6" s="30">
         <f>B6+'Memory Map'!$B$10</f>
-        <v>249856</v>
+        <v>243712</v>
       </c>
       <c r="I6" s="7" t="str">
         <f>DEC2HEX(H6,6)</f>
-        <v>03D000</v>
+        <v>03B800</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2715,11 +2721,11 @@
       </c>
       <c r="H7" s="30">
         <f>B7+'Memory Map'!$B$10</f>
-        <v>249860</v>
+        <v>243716</v>
       </c>
       <c r="I7" s="7" t="str">
         <f t="shared" ref="I7:I19" si="1">DEC2HEX(H7,6)</f>
-        <v>03D004</v>
+        <v>03B804</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2748,11 +2754,11 @@
       </c>
       <c r="H8" s="30">
         <f>B8+'Memory Map'!$B$10</f>
-        <v>249864</v>
+        <v>243720</v>
       </c>
       <c r="I8" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D008</v>
+        <v>03B808</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2781,11 +2787,11 @@
       </c>
       <c r="H9" s="30">
         <f>B9+'Memory Map'!$B$10</f>
-        <v>249868</v>
+        <v>243724</v>
       </c>
       <c r="I9" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D00C</v>
+        <v>03B80C</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2814,11 +2820,11 @@
       </c>
       <c r="H10" s="30">
         <f>B10+'Memory Map'!$B$10</f>
-        <v>249872</v>
+        <v>243728</v>
       </c>
       <c r="I10" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D010</v>
+        <v>03B810</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2847,11 +2853,11 @@
       </c>
       <c r="H11" s="30">
         <f>B11+'Memory Map'!$B$10</f>
-        <v>249876</v>
+        <v>243732</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D014</v>
+        <v>03B814</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2880,11 +2886,11 @@
       </c>
       <c r="H12" s="30">
         <f>B12+'Memory Map'!$B$10</f>
-        <v>249880</v>
+        <v>243736</v>
       </c>
       <c r="I12" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D018</v>
+        <v>03B818</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2913,11 +2919,11 @@
       </c>
       <c r="H13" s="30">
         <f>B13+'Memory Map'!$B$10</f>
-        <v>249884</v>
+        <v>243740</v>
       </c>
       <c r="I13" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D01C</v>
+        <v>03B81C</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2946,11 +2952,11 @@
       </c>
       <c r="H14" s="30">
         <f>B14+'Memory Map'!$B$10</f>
-        <v>249885</v>
+        <v>243741</v>
       </c>
       <c r="I14" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D01D</v>
+        <v>03B81D</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -2979,11 +2985,11 @@
       </c>
       <c r="H15" s="30">
         <f>B15+'Memory Map'!$B$10</f>
-        <v>249886</v>
+        <v>243742</v>
       </c>
       <c r="I15" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D01E</v>
+        <v>03B81E</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3013,11 +3019,11 @@
       </c>
       <c r="H16" s="30">
         <f>B16+'Memory Map'!$B$10</f>
-        <v>249900</v>
+        <v>243756</v>
       </c>
       <c r="I16" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D02C</v>
+        <v>03B82C</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3046,11 +3052,11 @@
       </c>
       <c r="H17" s="30">
         <f>B17+'Memory Map'!$B$10</f>
-        <v>250880</v>
+        <v>244736</v>
       </c>
       <c r="I17" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D400</v>
+        <v>03BC00</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3079,11 +3085,11 @@
       </c>
       <c r="H18" s="30">
         <f>B18+'Memory Map'!$B$10</f>
-        <v>251392</v>
+        <v>245248</v>
       </c>
       <c r="I18" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D600</v>
+        <v>03BE00</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
@@ -3112,11 +3118,11 @@
       </c>
       <c r="H19" s="30">
         <f>B19+'Memory Map'!$B$10</f>
-        <v>251648</v>
+        <v>245504</v>
       </c>
       <c r="I19" s="7" t="str">
         <f t="shared" si="1"/>
-        <v>03D700</v>
+        <v>03BF00</v>
       </c>
     </row>
   </sheetData>
@@ -5567,4 +5573,31 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C2" t="e">
+        <f>HEX2BIN(B2/2^11,7)</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Incorporated new MAC controller into the N.I.G.E. Machine and completed loopback testing in simulator
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="168">
   <si>
     <t>Name</t>
   </si>
@@ -644,6 +644,24 @@
   </si>
   <si>
     <t>03B000</t>
+  </si>
+  <si>
+    <t>MACreadyRX</t>
+  </si>
+  <si>
+    <t>MACdataRX</t>
+  </si>
+  <si>
+    <t>MACchecksum_error</t>
+  </si>
+  <si>
+    <t>MACreadyTX</t>
+  </si>
+  <si>
+    <t>MACdataTX</t>
+  </si>
+  <si>
+    <t>MACtransmit_request</t>
   </si>
 </sst>
 </file>
@@ -1152,10 +1170,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1421,7 +1439,7 @@
         <v>51</v>
       </c>
       <c r="J11" t="str">
-        <f t="shared" ref="J10:J13" si="7">DEC2BIN(B11/2^11,7)</f>
+        <f t="shared" ref="J11:J13" si="7">DEC2BIN(B11/2^11,7)</f>
         <v>1111000</v>
       </c>
       <c r="L11" s="8"/>
@@ -1592,7 +1610,7 @@
         <v>260099</v>
       </c>
       <c r="D19" s="7" t="str">
-        <f t="shared" ref="D19:E43" si="9">DEC2HEX(B19,6)</f>
+        <f t="shared" ref="D19:E49" si="9">DEC2HEX(B19,6)</f>
         <v>03F800</v>
       </c>
       <c r="E19" s="7" t="str">
@@ -1650,7 +1668,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="7">
-        <f t="shared" ref="B21:B42" si="12">B20+4</f>
+        <f t="shared" ref="B21:B48" si="12">B20+4</f>
         <v>260104</v>
       </c>
       <c r="C21" s="7">
@@ -2017,7 +2035,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>1</v>
       </c>
@@ -2048,7 +2066,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>1</v>
       </c>
@@ -2079,7 +2097,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>1</v>
       </c>
@@ -2110,7 +2128,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>1</v>
       </c>
@@ -2141,7 +2159,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>1</v>
       </c>
@@ -2172,7 +2190,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>1</v>
       </c>
@@ -2203,7 +2221,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>1</v>
       </c>
@@ -2234,7 +2252,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>1</v>
       </c>
@@ -2265,7 +2283,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>1</v>
       </c>
@@ -2296,7 +2314,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>1</v>
       </c>
@@ -2327,254 +2345,440 @@
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
-        <f>C43-B43</f>
-        <v>1951</v>
+        <v>1</v>
       </c>
       <c r="B43" s="7">
-        <f>B42+4</f>
+        <f t="shared" si="12"/>
         <v>260192</v>
       </c>
       <c r="C43" s="7">
-        <f>C49</f>
+        <f t="shared" ref="C43:C48" si="16">B43+A43-1</f>
+        <v>260192</v>
+      </c>
+      <c r="D43" s="7" t="str">
+        <f t="shared" ref="D43:D48" si="17">DEC2HEX(B43,6)</f>
+        <v>03F860</v>
+      </c>
+      <c r="E43" s="7" t="str">
+        <f t="shared" ref="E43:E48" si="18">DEC2HEX(C43,6)</f>
+        <v>03F860</v>
+      </c>
+      <c r="F43" s="7"/>
+      <c r="G43" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="H43" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>1</v>
+      </c>
+      <c r="B44" s="7">
+        <f t="shared" si="12"/>
+        <v>260196</v>
+      </c>
+      <c r="C44" s="7">
+        <f t="shared" si="16"/>
+        <v>260196</v>
+      </c>
+      <c r="D44" s="7" t="str">
+        <f t="shared" si="17"/>
+        <v>03F864</v>
+      </c>
+      <c r="E44" s="7" t="str">
+        <f t="shared" si="18"/>
+        <v>03F864</v>
+      </c>
+      <c r="F44" s="7"/>
+      <c r="G44" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="H44" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I44" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="7">
+        <v>1</v>
+      </c>
+      <c r="B45" s="7">
+        <f t="shared" si="12"/>
+        <v>260200</v>
+      </c>
+      <c r="C45" s="7">
+        <f t="shared" si="16"/>
+        <v>260200</v>
+      </c>
+      <c r="D45" s="7" t="str">
+        <f t="shared" si="17"/>
+        <v>03F868</v>
+      </c>
+      <c r="E45" s="7" t="str">
+        <f t="shared" si="18"/>
+        <v>03F868</v>
+      </c>
+      <c r="F45" s="7"/>
+      <c r="G45" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="H45" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I45" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="7">
+        <v>1</v>
+      </c>
+      <c r="B46" s="7">
+        <f t="shared" si="12"/>
+        <v>260204</v>
+      </c>
+      <c r="C46" s="7">
+        <f t="shared" si="16"/>
+        <v>260204</v>
+      </c>
+      <c r="D46" s="7" t="str">
+        <f t="shared" si="17"/>
+        <v>03F86C</v>
+      </c>
+      <c r="E46" s="7" t="str">
+        <f t="shared" si="18"/>
+        <v>03F86C</v>
+      </c>
+      <c r="F46" s="7"/>
+      <c r="G46" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="H46" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I46" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="7">
+        <v>1</v>
+      </c>
+      <c r="B47" s="7">
+        <f t="shared" si="12"/>
+        <v>260208</v>
+      </c>
+      <c r="C47" s="7">
+        <f t="shared" si="16"/>
+        <v>260208</v>
+      </c>
+      <c r="D47" s="7" t="str">
+        <f t="shared" si="17"/>
+        <v>03F870</v>
+      </c>
+      <c r="E47" s="7" t="str">
+        <f t="shared" si="18"/>
+        <v>03F870</v>
+      </c>
+      <c r="F47" s="7"/>
+      <c r="G47" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="H47" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I47" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="7">
+        <v>1</v>
+      </c>
+      <c r="B48" s="7">
+        <f t="shared" si="12"/>
+        <v>260212</v>
+      </c>
+      <c r="C48" s="7">
+        <f t="shared" si="16"/>
+        <v>260212</v>
+      </c>
+      <c r="D48" s="7" t="str">
+        <f t="shared" si="17"/>
+        <v>03F874</v>
+      </c>
+      <c r="E48" s="7" t="str">
+        <f t="shared" si="18"/>
+        <v>03F874</v>
+      </c>
+      <c r="F48" s="7"/>
+      <c r="G48" s="8" t="s">
+        <v>167</v>
+      </c>
+      <c r="H48" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="I48" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <f>C49-B49</f>
+        <v>1927</v>
+      </c>
+      <c r="B49" s="7">
+        <f>B48+4</f>
+        <v>260216</v>
+      </c>
+      <c r="C49" s="7">
+        <f>C55</f>
         <v>262143</v>
       </c>
-      <c r="D43" s="7" t="str">
+      <c r="D49" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>03F860</v>
-      </c>
-      <c r="E43" s="7" t="str">
+        <v>03F878</v>
+      </c>
+      <c r="E49" s="7" t="str">
         <f t="shared" si="9"/>
         <v>03FFFF</v>
       </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="12" t="s">
+      <c r="F49" s="7"/>
+      <c r="G49" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="10" t="s">
+    <row r="51" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D45" s="16"/>
-      <c r="E45" s="16"/>
-      <c r="F45" s="16"/>
-      <c r="H45" s="30"/>
-      <c r="I45"/>
-      <c r="J45"/>
-      <c r="K45"/>
-      <c r="L45"/>
-      <c r="M45"/>
-      <c r="N45"/>
-    </row>
-    <row r="46" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="D51" s="16"/>
+      <c r="E51" s="16"/>
+      <c r="F51" s="16"/>
+      <c r="H51" s="30"/>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+    </row>
+    <row r="52" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B46" s="13" t="s">
+      <c r="B52" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C52" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="D52" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E46" s="13" t="s">
+      <c r="E52" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F46" s="13"/>
-      <c r="G46" s="10" t="s">
+      <c r="F52" s="13"/>
+      <c r="G52" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H46" s="30"/>
-      <c r="I46"/>
-      <c r="J46"/>
-      <c r="K46"/>
-      <c r="L46"/>
-      <c r="M46"/>
-      <c r="N46"/>
-    </row>
-    <row r="47" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13" t="s">
+      <c r="H52" s="30"/>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+    </row>
+    <row r="53" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="13"/>
+      <c r="B53" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C53" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="D53" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E53" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F47" s="13"/>
-      <c r="H47" s="30"/>
-      <c r="I47"/>
-      <c r="J47"/>
-      <c r="K47"/>
-      <c r="L47"/>
-      <c r="M47"/>
-      <c r="N47"/>
-    </row>
-    <row r="48" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="6"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="6"/>
-      <c r="F48" s="6"/>
-      <c r="G48" s="10"/>
-      <c r="H48" s="30"/>
-      <c r="I48"/>
-      <c r="J48"/>
-      <c r="K48"/>
-      <c r="L48"/>
-      <c r="M48"/>
-      <c r="N48"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A49" s="7">
+      <c r="F53" s="13"/>
+      <c r="H53" s="30"/>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+    </row>
+    <row r="54" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="6"/>
+      <c r="B54" s="6"/>
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="30"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
         <f>256*1024</f>
         <v>262144</v>
       </c>
-      <c r="B49" s="7">
+      <c r="B55" s="7">
         <v>0</v>
       </c>
-      <c r="C49" s="7">
-        <f>A49-1</f>
+      <c r="C55" s="7">
+        <f>A55-1</f>
         <v>262143</v>
       </c>
-      <c r="D49" s="7" t="str">
-        <f>DEC2HEX(B49,6)</f>
+      <c r="D55" s="7" t="str">
+        <f>DEC2HEX(B55,6)</f>
         <v>000000</v>
       </c>
-      <c r="E49" s="7" t="str">
-        <f>DEC2HEX(C49,6)</f>
+      <c r="E55" s="7" t="str">
+        <f>DEC2HEX(C55,6)</f>
         <v>03FFFF</v>
       </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="12" t="s">
+      <c r="F55" s="7"/>
+      <c r="G55" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H49" s="34"/>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A50" s="7">
+      <c r="H55" s="34"/>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
         <f>2*(128*96*2)</f>
         <v>49152</v>
       </c>
-      <c r="B50" s="7">
-        <f>C49+1</f>
+      <c r="B56" s="7">
+        <f>C55+1</f>
         <v>262144</v>
       </c>
-      <c r="C50" s="7">
-        <f t="shared" ref="C50:C52" si="16">B50+A50-1</f>
+      <c r="C56" s="7">
+        <f t="shared" ref="C56:C58" si="19">B56+A56-1</f>
         <v>311295</v>
       </c>
-      <c r="D50" s="7" t="str">
-        <f t="shared" ref="D50:E53" si="17">DEC2HEX(B50,6)</f>
+      <c r="D56" s="7" t="str">
+        <f t="shared" ref="D56:E59" si="20">DEC2HEX(B56,6)</f>
         <v>040000</v>
       </c>
-      <c r="E50" s="7" t="str">
-        <f t="shared" si="17"/>
+      <c r="E56" s="7" t="str">
+        <f t="shared" si="20"/>
         <v>04BFFF</v>
       </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="8" t="s">
+      <c r="F56" s="7"/>
+      <c r="G56" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H50" s="30" t="s">
+      <c r="H56" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="7">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
         <v>512</v>
       </c>
-      <c r="B51" s="7">
-        <f>C50+1</f>
+      <c r="B57" s="7">
+        <f>C56+1</f>
         <v>311296</v>
       </c>
-      <c r="C51" s="7">
-        <f t="shared" ref="C51" si="18">B51+A51-1</f>
+      <c r="C57" s="7">
+        <f t="shared" ref="C57" si="21">B57+A57-1</f>
         <v>311807</v>
       </c>
-      <c r="D51" s="7" t="str">
-        <f t="shared" ref="D51" si="19">DEC2HEX(B51,6)</f>
+      <c r="D57" s="7" t="str">
+        <f t="shared" ref="D57" si="22">DEC2HEX(B57,6)</f>
         <v>04C000</v>
       </c>
-      <c r="E51" s="7" t="str">
-        <f t="shared" ref="E51" si="20">DEC2HEX(C51,6)</f>
+      <c r="E57" s="7" t="str">
+        <f t="shared" ref="E57" si="23">DEC2HEX(C57,6)</f>
         <v>04C1FF</v>
       </c>
-      <c r="F51" s="7"/>
-      <c r="G51" s="8" t="s">
+      <c r="F57" s="7"/>
+      <c r="G57" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="H51" s="30" t="s">
+      <c r="H57" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A52" s="7">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
         <v>512</v>
       </c>
-      <c r="B52" s="7">
-        <f>C51+1</f>
+      <c r="B58" s="7">
+        <f>C57+1</f>
         <v>311808</v>
       </c>
-      <c r="C52" s="7">
-        <f t="shared" si="16"/>
+      <c r="C58" s="7">
+        <f t="shared" si="19"/>
         <v>312319</v>
       </c>
-      <c r="D52" s="7" t="str">
-        <f t="shared" si="17"/>
+      <c r="D58" s="7" t="str">
+        <f t="shared" si="20"/>
         <v>04C200</v>
       </c>
-      <c r="E52" s="7" t="str">
-        <f t="shared" si="17"/>
+      <c r="E58" s="7" t="str">
+        <f t="shared" si="20"/>
         <v>04C3FF</v>
       </c>
-      <c r="F52" s="7"/>
-      <c r="G52" s="8" t="s">
+      <c r="F58" s="7"/>
+      <c r="G58" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="H52" s="30" t="s">
+      <c r="H58" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A53" s="7">
-        <f>C53-B53</f>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <f>C59-B59</f>
         <v>16464895</v>
       </c>
-      <c r="B53" s="7">
-        <f>C52+1</f>
+      <c r="B59" s="7">
+        <f>C58+1</f>
         <v>312320</v>
       </c>
-      <c r="C53" s="7">
+      <c r="C59" s="7">
         <f>16*1024*1024-1</f>
         <v>16777215</v>
       </c>
-      <c r="D53" s="7" t="str">
-        <f t="shared" si="17"/>
+      <c r="D59" s="7" t="str">
+        <f t="shared" si="20"/>
         <v>04C400</v>
       </c>
-      <c r="E53" s="7" t="str">
-        <f t="shared" si="17"/>
+      <c r="E59" s="7" t="str">
+        <f t="shared" si="20"/>
         <v>FFFFFF</v>
       </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="8" t="s">
+      <c r="F59" s="7"/>
+      <c r="G59" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H53" s="30" t="s">
+      <c r="H59" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I53" t="s">
+      <c r="I59" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Incorporated Ethernet PHY serial management interface into the N.I.G.E. Machine and tested in simulator.  Next step hardware testing.
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="173">
   <si>
     <t>Name</t>
   </si>
@@ -662,6 +662,21 @@
   </si>
   <si>
     <t>MACtransmit_request</t>
+  </si>
+  <si>
+    <t>SMIread_request</t>
+  </si>
+  <si>
+    <t>SMIready</t>
+  </si>
+  <si>
+    <t>SMIaddr</t>
+  </si>
+  <si>
+    <t>SMIdataWrite</t>
+  </si>
+  <si>
+    <t>SMIdataRead</t>
   </si>
 </sst>
 </file>
@@ -1170,10 +1185,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N59"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1610,7 +1625,7 @@
         <v>260099</v>
       </c>
       <c r="D19" s="7" t="str">
-        <f t="shared" ref="D19:E49" si="9">DEC2HEX(B19,6)</f>
+        <f t="shared" ref="D19:E54" si="9">DEC2HEX(B19,6)</f>
         <v>03F800</v>
       </c>
       <c r="E19" s="7" t="str">
@@ -1668,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="B21" s="7">
-        <f t="shared" ref="B21:B48" si="12">B20+4</f>
+        <f t="shared" ref="B21:B53" si="12">B20+4</f>
         <v>260104</v>
       </c>
       <c r="C21" s="7">
@@ -2494,7 +2509,7 @@
         <v>166</v>
       </c>
       <c r="H47" s="30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I47" t="s">
         <v>155</v>
@@ -2525,7 +2540,7 @@
         <v>167</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I48" t="s">
         <v>155</v>
@@ -2533,252 +2548,392 @@
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
-        <f>C49-B49</f>
-        <v>1927</v>
+        <v>2</v>
       </c>
       <c r="B49" s="7">
-        <f>B48+4</f>
+        <f t="shared" si="12"/>
         <v>260216</v>
       </c>
       <c r="C49" s="7">
-        <f>C55</f>
+        <f t="shared" ref="C49:C53" si="19">B49+A49-1</f>
+        <v>260217</v>
+      </c>
+      <c r="D49" s="7" t="str">
+        <f t="shared" ref="D49:D53" si="20">DEC2HEX(B49,6)</f>
+        <v>03F878</v>
+      </c>
+      <c r="E49" s="7" t="str">
+        <f t="shared" ref="E49:E53" si="21">DEC2HEX(C49,6)</f>
+        <v>03F879</v>
+      </c>
+      <c r="F49" s="7"/>
+      <c r="G49" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="H49" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>2</v>
+      </c>
+      <c r="B50" s="7">
+        <f t="shared" si="12"/>
+        <v>260220</v>
+      </c>
+      <c r="C50" s="7">
+        <f t="shared" si="19"/>
+        <v>260221</v>
+      </c>
+      <c r="D50" s="7" t="str">
+        <f t="shared" si="20"/>
+        <v>03F87C</v>
+      </c>
+      <c r="E50" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>03F87D</v>
+      </c>
+      <c r="F50" s="7"/>
+      <c r="G50" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="H50" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>1</v>
+      </c>
+      <c r="B51" s="7">
+        <f t="shared" si="12"/>
+        <v>260224</v>
+      </c>
+      <c r="C51" s="7">
+        <f t="shared" si="19"/>
+        <v>260224</v>
+      </c>
+      <c r="D51" s="7" t="str">
+        <f t="shared" si="20"/>
+        <v>03F880</v>
+      </c>
+      <c r="E51" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>03F880</v>
+      </c>
+      <c r="F51" s="7"/>
+      <c r="G51" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="H51" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>1</v>
+      </c>
+      <c r="B52" s="7">
+        <f t="shared" si="12"/>
+        <v>260228</v>
+      </c>
+      <c r="C52" s="7">
+        <f t="shared" si="19"/>
+        <v>260228</v>
+      </c>
+      <c r="D52" s="7" t="str">
+        <f t="shared" si="20"/>
+        <v>03F884</v>
+      </c>
+      <c r="E52" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>03F884</v>
+      </c>
+      <c r="F52" s="7"/>
+      <c r="G52" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="H52" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>2</v>
+      </c>
+      <c r="B53" s="7">
+        <f t="shared" si="12"/>
+        <v>260232</v>
+      </c>
+      <c r="C53" s="7">
+        <f t="shared" si="19"/>
+        <v>260233</v>
+      </c>
+      <c r="D53" s="7" t="str">
+        <f t="shared" si="20"/>
+        <v>03F888</v>
+      </c>
+      <c r="E53" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>03F889</v>
+      </c>
+      <c r="F53" s="7"/>
+      <c r="G53" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="H53" s="30" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <f>C54-B54+1</f>
+        <v>1908</v>
+      </c>
+      <c r="B54" s="7">
+        <f>B53+4</f>
+        <v>260236</v>
+      </c>
+      <c r="C54" s="7">
+        <f>C60</f>
         <v>262143</v>
       </c>
-      <c r="D49" s="7" t="str">
+      <c r="D54" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>03F878</v>
-      </c>
-      <c r="E49" s="7" t="str">
+        <v>03F88C</v>
+      </c>
+      <c r="E54" s="7" t="str">
         <f t="shared" si="9"/>
         <v>03FFFF</v>
       </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="12" t="s">
+      <c r="F54" s="7"/>
+      <c r="G54" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="10" t="s">
+    <row r="56" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D51" s="16"/>
-      <c r="E51" s="16"/>
-      <c r="F51" s="16"/>
-      <c r="H51" s="30"/>
-      <c r="I51"/>
-      <c r="J51"/>
-      <c r="K51"/>
-      <c r="L51"/>
-      <c r="M51"/>
-      <c r="N51"/>
-    </row>
-    <row r="52" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+      <c r="D56" s="16"/>
+      <c r="E56" s="16"/>
+      <c r="F56" s="16"/>
+      <c r="H56" s="30"/>
+      <c r="I56"/>
+      <c r="J56"/>
+      <c r="K56"/>
+      <c r="L56"/>
+      <c r="M56"/>
+      <c r="N56"/>
+    </row>
+    <row r="57" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B52" s="13" t="s">
+      <c r="B57" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C57" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="13" t="s">
+      <c r="D57" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E57" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F52" s="13"/>
-      <c r="G52" s="10" t="s">
+      <c r="F57" s="13"/>
+      <c r="G57" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H52" s="30"/>
-      <c r="I52"/>
-      <c r="J52"/>
-      <c r="K52"/>
-      <c r="L52"/>
-      <c r="M52"/>
-      <c r="N52"/>
-    </row>
-    <row r="53" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13" t="s">
+      <c r="H57" s="30"/>
+      <c r="I57"/>
+      <c r="J57"/>
+      <c r="K57"/>
+      <c r="L57"/>
+      <c r="M57"/>
+      <c r="N57"/>
+    </row>
+    <row r="58" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="13"/>
+      <c r="B58" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C58" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D53" s="13" t="s">
+      <c r="D58" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E58" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F53" s="13"/>
-      <c r="H53" s="30"/>
-      <c r="I53"/>
-      <c r="J53"/>
-      <c r="K53"/>
-      <c r="L53"/>
-      <c r="M53"/>
-      <c r="N53"/>
-    </row>
-    <row r="54" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="6"/>
-      <c r="B54" s="6"/>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6"/>
-      <c r="F54" s="6"/>
-      <c r="G54" s="10"/>
-      <c r="H54" s="30"/>
-      <c r="I54"/>
-      <c r="J54"/>
-      <c r="K54"/>
-      <c r="L54"/>
-      <c r="M54"/>
-      <c r="N54"/>
-    </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A55" s="7">
+      <c r="F58" s="13"/>
+      <c r="H58" s="30"/>
+      <c r="I58"/>
+      <c r="J58"/>
+      <c r="K58"/>
+      <c r="L58"/>
+      <c r="M58"/>
+      <c r="N58"/>
+    </row>
+    <row r="59" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="6"/>
+      <c r="B59" s="6"/>
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="30"/>
+      <c r="I59"/>
+      <c r="J59"/>
+      <c r="K59"/>
+      <c r="L59"/>
+      <c r="M59"/>
+      <c r="N59"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
         <f>256*1024</f>
         <v>262144</v>
       </c>
-      <c r="B55" s="7">
+      <c r="B60" s="7">
         <v>0</v>
       </c>
-      <c r="C55" s="7">
-        <f>A55-1</f>
+      <c r="C60" s="7">
+        <f>A60-1</f>
         <v>262143</v>
       </c>
-      <c r="D55" s="7" t="str">
-        <f>DEC2HEX(B55,6)</f>
+      <c r="D60" s="7" t="str">
+        <f>DEC2HEX(B60,6)</f>
         <v>000000</v>
       </c>
-      <c r="E55" s="7" t="str">
-        <f>DEC2HEX(C55,6)</f>
+      <c r="E60" s="7" t="str">
+        <f>DEC2HEX(C60,6)</f>
         <v>03FFFF</v>
       </c>
-      <c r="F55" s="7"/>
-      <c r="G55" s="12" t="s">
+      <c r="F60" s="7"/>
+      <c r="G60" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H55" s="34"/>
-    </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A56" s="7">
+      <c r="H60" s="34"/>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
         <f>2*(128*96*2)</f>
         <v>49152</v>
       </c>
-      <c r="B56" s="7">
-        <f>C55+1</f>
+      <c r="B61" s="7">
+        <f>C60+1</f>
         <v>262144</v>
       </c>
-      <c r="C56" s="7">
-        <f t="shared" ref="C56:C58" si="19">B56+A56-1</f>
+      <c r="C61" s="7">
+        <f t="shared" ref="C61:C63" si="22">B61+A61-1</f>
         <v>311295</v>
       </c>
-      <c r="D56" s="7" t="str">
-        <f t="shared" ref="D56:E59" si="20">DEC2HEX(B56,6)</f>
+      <c r="D61" s="7" t="str">
+        <f t="shared" ref="D61:E64" si="23">DEC2HEX(B61,6)</f>
         <v>040000</v>
       </c>
-      <c r="E56" s="7" t="str">
-        <f t="shared" si="20"/>
+      <c r="E61" s="7" t="str">
+        <f t="shared" si="23"/>
         <v>04BFFF</v>
       </c>
-      <c r="F56" s="7"/>
-      <c r="G56" s="8" t="s">
+      <c r="F61" s="7"/>
+      <c r="G61" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H56" s="30" t="s">
+      <c r="H61" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A57" s="7">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
         <v>512</v>
       </c>
-      <c r="B57" s="7">
-        <f>C56+1</f>
+      <c r="B62" s="7">
+        <f>C61+1</f>
         <v>311296</v>
       </c>
-      <c r="C57" s="7">
-        <f t="shared" ref="C57" si="21">B57+A57-1</f>
+      <c r="C62" s="7">
+        <f t="shared" ref="C62" si="24">B62+A62-1</f>
         <v>311807</v>
       </c>
-      <c r="D57" s="7" t="str">
-        <f t="shared" ref="D57" si="22">DEC2HEX(B57,6)</f>
+      <c r="D62" s="7" t="str">
+        <f t="shared" ref="D62" si="25">DEC2HEX(B62,6)</f>
         <v>04C000</v>
       </c>
-      <c r="E57" s="7" t="str">
-        <f t="shared" ref="E57" si="23">DEC2HEX(C57,6)</f>
+      <c r="E62" s="7" t="str">
+        <f t="shared" ref="E62" si="26">DEC2HEX(C62,6)</f>
         <v>04C1FF</v>
       </c>
-      <c r="F57" s="7"/>
-      <c r="G57" s="8" t="s">
+      <c r="F62" s="7"/>
+      <c r="G62" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="H57" s="30" t="s">
+      <c r="H62" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A58" s="7">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63" s="7">
         <v>512</v>
       </c>
-      <c r="B58" s="7">
-        <f>C57+1</f>
+      <c r="B63" s="7">
+        <f>C62+1</f>
         <v>311808</v>
       </c>
-      <c r="C58" s="7">
-        <f t="shared" si="19"/>
+      <c r="C63" s="7">
+        <f t="shared" si="22"/>
         <v>312319</v>
       </c>
-      <c r="D58" s="7" t="str">
-        <f t="shared" si="20"/>
+      <c r="D63" s="7" t="str">
+        <f t="shared" si="23"/>
         <v>04C200</v>
       </c>
-      <c r="E58" s="7" t="str">
-        <f t="shared" si="20"/>
+      <c r="E63" s="7" t="str">
+        <f t="shared" si="23"/>
         <v>04C3FF</v>
       </c>
-      <c r="F58" s="7"/>
-      <c r="G58" s="8" t="s">
+      <c r="F63" s="7"/>
+      <c r="G63" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="H58" s="30" t="s">
+      <c r="H63" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A59" s="7">
-        <f>C59-B59</f>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64" s="7">
+        <f>C64-B64</f>
         <v>16464895</v>
       </c>
-      <c r="B59" s="7">
-        <f>C58+1</f>
+      <c r="B64" s="7">
+        <f>C63+1</f>
         <v>312320</v>
       </c>
-      <c r="C59" s="7">
+      <c r="C64" s="7">
         <f>16*1024*1024-1</f>
         <v>16777215</v>
       </c>
-      <c r="D59" s="7" t="str">
-        <f t="shared" si="20"/>
+      <c r="D64" s="7" t="str">
+        <f t="shared" si="23"/>
         <v>04C400</v>
       </c>
-      <c r="E59" s="7" t="str">
-        <f t="shared" si="20"/>
+      <c r="E64" s="7" t="str">
+        <f t="shared" si="23"/>
         <v>FFFFFF</v>
       </c>
-      <c r="F59" s="7"/>
-      <c r="G59" s="8" t="s">
+      <c r="F64" s="7"/>
+      <c r="G64" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H59" s="30" t="s">
+      <c r="H64" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I59" t="s">
+      <c r="I64" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ha, Hb, Hc, Hd, Va, Vb< Vc, Vd now moved to memory mapped registers VGATEST.F is a small application for setting these registers Currently the last text line on the screen is missing!
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\N.I.G.E.-Machine\Resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3974D07-E5E6-406A-A6B5-7FCEB29EC48A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425"/>
+    <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Memory Map" sheetId="4" r:id="rId1"/>
@@ -16,12 +22,12 @@
     <sheet name="Sheet1" sheetId="7" r:id="rId7"/>
     <sheet name="Sheet2" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="427" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="182">
   <si>
     <t>Name</t>
   </si>
@@ -678,11 +684,38 @@
   <si>
     <t>SMIdataRead</t>
   </si>
+  <si>
+    <t>VGA Ha</t>
+  </si>
+  <si>
+    <t>VGA Hb</t>
+  </si>
+  <si>
+    <t>VGA Hc</t>
+  </si>
+  <si>
+    <t>VGA Hd</t>
+  </si>
+  <si>
+    <t>VGA Va</t>
+  </si>
+  <si>
+    <t>VGA Vb</t>
+  </si>
+  <si>
+    <t>VGA Vc</t>
+  </si>
+  <si>
+    <t>VGA Vd</t>
+  </si>
+  <si>
+    <t>Local</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -891,6 +924,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -938,7 +974,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -971,9 +1007,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1006,6 +1059,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1181,49 +1251,51 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N64"/>
+  <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="5" width="12.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="3.85546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="33.5703125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" style="30" customWidth="1"/>
-    <col min="9" max="9" width="79.140625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" customWidth="1"/>
-    <col min="11" max="12" width="19.140625" customWidth="1"/>
-    <col min="13" max="13" width="11.42578125" customWidth="1"/>
-    <col min="14" max="14" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="2.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="33.5703125" style="8" customWidth="1"/>
+    <col min="9" max="9" width="10.140625" style="30" customWidth="1"/>
+    <col min="10" max="10" width="79.140625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" customWidth="1"/>
+    <col min="12" max="13" width="19.140625" customWidth="1"/>
+    <col min="14" max="14" width="11.42578125" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="16"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
-      <c r="J3"/>
+      <c r="G3" s="16"/>
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
       <c r="N3"/>
-    </row>
-    <row r="4" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O3"/>
+    </row>
+    <row r="4" spans="1:15" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>6</v>
       </c>
@@ -1239,23 +1311,26 @@
       <c r="E4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="13"/>
-      <c r="G4" s="10" t="s">
+      <c r="F4" s="13" t="s">
+        <v>181</v>
+      </c>
+      <c r="G4" s="13"/>
+      <c r="H4" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="I4" s="32" t="s">
         <v>72</v>
       </c>
-      <c r="I4"/>
-      <c r="J4" s="32" t="s">
+      <c r="J4"/>
+      <c r="K4" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="K4"/>
       <c r="L4"/>
       <c r="M4"/>
       <c r="N4"/>
-    </row>
-    <row r="5" spans="1:14" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O4"/>
+    </row>
+    <row r="5" spans="1:15" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="13"/>
       <c r="B5" s="13" t="s">
         <v>8</v>
@@ -1269,32 +1344,36 @@
       <c r="E5" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="13"/>
-      <c r="H5" s="32"/>
-      <c r="I5"/>
+      <c r="F5" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="13"/>
+      <c r="I5" s="32"/>
       <c r="J5"/>
       <c r="K5"/>
       <c r="L5"/>
       <c r="M5"/>
       <c r="N5"/>
-    </row>
-    <row r="6" spans="1:14" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O5"/>
+    </row>
+    <row r="6" spans="1:15" s="2" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="33"/>
-      <c r="I6"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="33"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
       <c r="N6"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O6"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="7">
         <f>(128)*1024</f>
         <v>131072</v>
@@ -1315,17 +1394,18 @@
         <v>01FFFF</v>
       </c>
       <c r="F7" s="7"/>
-      <c r="G7" s="8" t="s">
+      <c r="G7" s="7"/>
+      <c r="H7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="H7" s="30" t="s">
+      <c r="I7" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="7">
         <f>(128-20)*1024</f>
         <v>110592</v>
@@ -1347,11 +1427,12 @@
         <v>03AFFF</v>
       </c>
       <c r="F8" s="7"/>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7"/>
+      <c r="H8" s="8" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>2048</v>
       </c>
@@ -1372,22 +1453,23 @@
         <v>03B7FF</v>
       </c>
       <c r="F9" s="7"/>
-      <c r="G9" s="8" t="s">
+      <c r="G9" s="7"/>
+      <c r="H9" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="H9" s="30" t="s">
+      <c r="I9" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>105</v>
       </c>
-      <c r="J9" t="str">
+      <c r="K9" t="str">
         <f>DEC2BIN(B9/2^11,7)</f>
         <v>1110110</v>
       </c>
-      <c r="L9" s="8"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>2048</v>
       </c>
@@ -1408,22 +1490,23 @@
         <v>03BFFF</v>
       </c>
       <c r="F10" s="7"/>
-      <c r="G10" s="8" t="s">
+      <c r="G10" s="7"/>
+      <c r="H10" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="H10" s="30" t="s">
+      <c r="I10" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>96</v>
       </c>
-      <c r="J10" t="str">
+      <c r="K10" t="str">
         <f>DEC2BIN(B10/2^11,7)</f>
         <v>1110111</v>
       </c>
-      <c r="L10" s="8"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>8192</v>
       </c>
@@ -1444,22 +1527,23 @@
         <v>03DFFF</v>
       </c>
       <c r="F11" s="7"/>
-      <c r="G11" s="8" t="s">
+      <c r="G11" s="7"/>
+      <c r="H11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H11" s="30" t="s">
+      <c r="I11" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>51</v>
       </c>
-      <c r="J11" t="str">
-        <f t="shared" ref="J11:J13" si="7">DEC2BIN(B11/2^11,7)</f>
+      <c r="K11" t="str">
+        <f t="shared" ref="K11:K13" si="7">DEC2BIN(B11/2^11,7)</f>
         <v>1111000</v>
       </c>
-      <c r="L11" s="8"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>4096</v>
       </c>
@@ -1480,21 +1564,22 @@
         <v>03EFFF</v>
       </c>
       <c r="F12" s="7"/>
-      <c r="G12" s="8" t="s">
+      <c r="G12" s="7"/>
+      <c r="H12" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H12" s="30" t="s">
+      <c r="I12" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>103</v>
       </c>
-      <c r="J12" t="str">
+      <c r="K12" t="str">
         <f t="shared" si="7"/>
         <v>1111100</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>2048</v>
       </c>
@@ -1515,37 +1600,39 @@
         <v>03F7FF</v>
       </c>
       <c r="F13" s="7"/>
-      <c r="G13" s="8" t="s">
+      <c r="G13" s="7"/>
+      <c r="H13" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="H13" s="30" t="s">
+      <c r="I13" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>158</v>
       </c>
-      <c r="J13" t="str">
+      <c r="K13" t="str">
         <f t="shared" si="7"/>
         <v>1111110</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>50</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
-      <c r="J15"/>
+      <c r="G15" s="16"/>
       <c r="K15"/>
       <c r="L15"/>
       <c r="M15"/>
       <c r="N15"/>
-    </row>
-    <row r="16" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O15"/>
+    </row>
+    <row r="16" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="13" t="s">
         <v>6</v>
       </c>
@@ -1562,18 +1649,19 @@
         <v>12</v>
       </c>
       <c r="F16" s="13"/>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="13"/>
+      <c r="H16" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H16" s="32"/>
-      <c r="I16"/>
+      <c r="I16" s="32"/>
       <c r="J16"/>
       <c r="K16"/>
       <c r="L16"/>
       <c r="M16"/>
       <c r="N16"/>
-    </row>
-    <row r="17" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O16"/>
+    </row>
+    <row r="17" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="15"/>
       <c r="B17" s="13" t="s">
         <v>8</v>
@@ -1588,31 +1676,33 @@
         <v>9</v>
       </c>
       <c r="F17" s="13"/>
-      <c r="H17" s="33"/>
-      <c r="I17"/>
+      <c r="G17" s="13"/>
+      <c r="I17" s="33"/>
       <c r="J17"/>
       <c r="K17"/>
       <c r="L17"/>
       <c r="M17"/>
       <c r="N17"/>
-    </row>
-    <row r="18" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="O17"/>
+    </row>
+    <row r="18" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="33"/>
-      <c r="I18"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="33"/>
       <c r="J18"/>
       <c r="K18"/>
       <c r="L18"/>
       <c r="M18"/>
       <c r="N18"/>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O18"/>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>4</v>
       </c>
@@ -1625,29 +1715,33 @@
         <v>260099</v>
       </c>
       <c r="D19" s="7" t="str">
-        <f t="shared" ref="D19:E54" si="9">DEC2HEX(B19,6)</f>
+        <f t="shared" ref="D19:E62" si="9">DEC2HEX(B19,6)</f>
         <v>03F800</v>
       </c>
       <c r="E19" s="7" t="str">
         <f t="shared" si="9"/>
         <v>03F803</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8" t="s">
+      <c r="F19" s="7" t="str">
+        <f>DEC2HEX(B19-$B$19)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="7"/>
+      <c r="H19" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H19" s="30" t="s">
+      <c r="I19" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>28</v>
       </c>
-      <c r="J19" t="str">
-        <f t="shared" ref="J19" si="10">DEC2BIN(B19/2^11,7)</f>
+      <c r="K19" t="str">
+        <f t="shared" ref="K19" si="10">DEC2BIN(B19/2^11,7)</f>
         <v>1111111</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>4</v>
       </c>
@@ -1667,23 +1761,27 @@
         <f t="shared" si="9"/>
         <v>03F807</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="8" t="s">
+      <c r="F20" s="7" t="str">
+        <f t="shared" ref="F20:F61" si="12">DEC2HEX(B20-$B$19)</f>
+        <v>4</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="H20" s="30" t="s">
+      <c r="I20" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>1</v>
       </c>
       <c r="B21" s="7">
-        <f t="shared" ref="B21:B53" si="12">B20+4</f>
+        <f t="shared" ref="B21:B61" si="13">B20+4</f>
         <v>260104</v>
       </c>
       <c r="C21" s="7">
@@ -1698,23 +1796,27 @@
         <f t="shared" si="9"/>
         <v>03F808</v>
       </c>
-      <c r="F21" s="7"/>
-      <c r="G21" s="8" t="s">
+      <c r="F21" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>8</v>
+      </c>
+      <c r="G21" s="7"/>
+      <c r="H21" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="H21" s="30" t="s">
+      <c r="I21" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>1</v>
       </c>
       <c r="B22" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260108</v>
       </c>
       <c r="C22" s="7">
@@ -1729,23 +1831,27 @@
         <f t="shared" si="9"/>
         <v>03F80C</v>
       </c>
-      <c r="F22" s="7"/>
-      <c r="G22" s="8" t="s">
+      <c r="F22" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>C</v>
+      </c>
+      <c r="G22" s="7"/>
+      <c r="H22" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="H22" s="30" t="s">
+      <c r="I22" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>1</v>
       </c>
       <c r="B23" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260112</v>
       </c>
       <c r="C23" s="7">
@@ -1760,23 +1866,27 @@
         <f t="shared" si="9"/>
         <v>03F810</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="8" t="s">
+      <c r="F23" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>10</v>
+      </c>
+      <c r="G23" s="7"/>
+      <c r="H23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H23" s="30" t="s">
+      <c r="I23" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>1</v>
       </c>
       <c r="B24" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260116</v>
       </c>
       <c r="C24" s="7">
@@ -1791,23 +1901,27 @@
         <f t="shared" si="9"/>
         <v>03F814</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="8" t="s">
+      <c r="F24" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>14</v>
+      </c>
+      <c r="G24" s="7"/>
+      <c r="H24" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="H24" s="30" t="s">
+      <c r="I24" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>2</v>
       </c>
       <c r="B25" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260120</v>
       </c>
       <c r="C25" s="7">
@@ -1822,23 +1936,27 @@
         <f t="shared" si="9"/>
         <v>03F819</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="8" t="s">
+      <c r="F25" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>18</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="H25" s="30" t="s">
+      <c r="I25" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>1</v>
       </c>
       <c r="B26" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260124</v>
       </c>
       <c r="C26" s="7">
@@ -1853,23 +1971,27 @@
         <f t="shared" si="9"/>
         <v>03F81C</v>
       </c>
-      <c r="F26" s="7"/>
-      <c r="G26" s="8" t="s">
+      <c r="F26" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>1C</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="30" t="s">
+      <c r="I26" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="7">
         <v>1</v>
       </c>
       <c r="B27" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260128</v>
       </c>
       <c r="C27" s="7">
@@ -1884,23 +2006,27 @@
         <f t="shared" si="9"/>
         <v>03F820</v>
       </c>
-      <c r="F27" s="7"/>
-      <c r="G27" s="8" t="s">
+      <c r="F27" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>20</v>
+      </c>
+      <c r="G27" s="7"/>
+      <c r="H27" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="H27" s="30" t="s">
+      <c r="I27" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="7">
         <v>4</v>
       </c>
       <c r="B28" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260132</v>
       </c>
       <c r="C28" s="7">
@@ -1915,23 +2041,27 @@
         <f t="shared" si="9"/>
         <v>03F827</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="8" t="s">
+      <c r="F28" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>24</v>
+      </c>
+      <c r="G28" s="7"/>
+      <c r="H28" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H28" s="30" t="s">
+      <c r="I28" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>4</v>
       </c>
       <c r="B29" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260136</v>
       </c>
       <c r="C29" s="7">
@@ -1946,23 +2076,27 @@
         <f t="shared" si="9"/>
         <v>03F82B</v>
       </c>
-      <c r="F29" s="7"/>
-      <c r="G29" s="8" t="s">
+      <c r="F29" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>28</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="30" t="s">
+      <c r="I29" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>2</v>
       </c>
       <c r="B30" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260140</v>
       </c>
       <c r="C30" s="7">
@@ -1977,23 +2111,27 @@
         <f t="shared" si="9"/>
         <v>03F82D</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="8" t="s">
+      <c r="F30" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>2C</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H30" s="30" t="s">
+      <c r="I30" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>2</v>
       </c>
       <c r="B31" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260144</v>
       </c>
       <c r="C31" s="7">
@@ -2008,23 +2146,27 @@
         <f t="shared" si="9"/>
         <v>03F831</v>
       </c>
-      <c r="F31" s="7"/>
-      <c r="G31" s="8" t="s">
+      <c r="F31" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>30</v>
+      </c>
+      <c r="G31" s="7"/>
+      <c r="H31" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="H31" s="30" t="s">
+      <c r="I31" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>1</v>
       </c>
       <c r="B32" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260148</v>
       </c>
       <c r="C32" s="7">
@@ -2039,23 +2181,27 @@
         <f t="shared" si="9"/>
         <v>03F834</v>
       </c>
-      <c r="F32" s="7"/>
-      <c r="G32" s="8" t="s">
+      <c r="F32" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>34</v>
+      </c>
+      <c r="G32" s="7"/>
+      <c r="H32" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="30" t="s">
+      <c r="I32" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>1</v>
       </c>
       <c r="B33" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260152</v>
       </c>
       <c r="C33" s="7">
@@ -2070,23 +2216,27 @@
         <f t="shared" si="9"/>
         <v>03F838</v>
       </c>
-      <c r="F33" s="7"/>
-      <c r="G33" s="8" t="s">
+      <c r="F33" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>38</v>
+      </c>
+      <c r="G33" s="7"/>
+      <c r="H33" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="H33" s="30" t="s">
+      <c r="I33" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>1</v>
       </c>
       <c r="B34" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260156</v>
       </c>
       <c r="C34" s="7">
@@ -2101,23 +2251,27 @@
         <f t="shared" si="9"/>
         <v>03F83C</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="8" t="s">
+      <c r="F34" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>3C</v>
+      </c>
+      <c r="G34" s="7"/>
+      <c r="H34" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="H34" s="30" t="s">
+      <c r="I34" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>1</v>
       </c>
       <c r="B35" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260160</v>
       </c>
       <c r="C35" s="7">
@@ -2132,23 +2286,27 @@
         <f t="shared" si="9"/>
         <v>03F840</v>
       </c>
-      <c r="F35" s="7"/>
-      <c r="G35" s="8" t="s">
+      <c r="F35" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>40</v>
+      </c>
+      <c r="G35" s="7"/>
+      <c r="H35" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="H35" s="30" t="s">
+      <c r="I35" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>1</v>
       </c>
       <c r="B36" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260164</v>
       </c>
       <c r="C36" s="7">
@@ -2163,23 +2321,27 @@
         <f t="shared" si="9"/>
         <v>03F844</v>
       </c>
-      <c r="F36" s="7"/>
-      <c r="G36" s="8" t="s">
+      <c r="F36" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>44</v>
+      </c>
+      <c r="G36" s="7"/>
+      <c r="H36" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H36" s="30" t="s">
+      <c r="I36" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>1</v>
       </c>
       <c r="B37" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260168</v>
       </c>
       <c r="C37" s="7">
@@ -2194,746 +2356,1080 @@
         <f t="shared" si="9"/>
         <v>03F848</v>
       </c>
-      <c r="F37" s="7"/>
-      <c r="G37" s="8" t="s">
+      <c r="F37" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>48</v>
+      </c>
+      <c r="G37" s="7"/>
+      <c r="H37" s="8" t="s">
         <v>93</v>
       </c>
-      <c r="H37" s="30" t="s">
+      <c r="I37" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="7">
         <v>1</v>
       </c>
       <c r="B38" s="7">
+        <f t="shared" si="13"/>
+        <v>260172</v>
+      </c>
+      <c r="C38" s="7">
+        <f t="shared" ref="C38:C42" si="14">B38+A38-1</f>
+        <v>260172</v>
+      </c>
+      <c r="D38" s="7" t="str">
+        <f t="shared" ref="D38:D42" si="15">DEC2HEX(B38,6)</f>
+        <v>03F84C</v>
+      </c>
+      <c r="E38" s="7" t="str">
+        <f t="shared" ref="E38:E42" si="16">DEC2HEX(C38,6)</f>
+        <v>03F84C</v>
+      </c>
+      <c r="F38" s="7" t="str">
         <f t="shared" si="12"/>
-        <v>260172</v>
-      </c>
-      <c r="C38" s="7">
-        <f t="shared" ref="C38:C42" si="13">B38+A38-1</f>
-        <v>260172</v>
-      </c>
-      <c r="D38" s="7" t="str">
-        <f t="shared" ref="D38:D42" si="14">DEC2HEX(B38,6)</f>
-        <v>03F84C</v>
-      </c>
-      <c r="E38" s="7" t="str">
-        <f t="shared" ref="E38:E42" si="15">DEC2HEX(C38,6)</f>
-        <v>03F84C</v>
-      </c>
-      <c r="F38" s="7"/>
-      <c r="G38" s="8" t="s">
+        <v>4C</v>
+      </c>
+      <c r="G38" s="7"/>
+      <c r="H38" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="H38" s="30" t="s">
+      <c r="I38" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>1</v>
       </c>
       <c r="B39" s="7">
-        <f t="shared" si="12"/>
-        <v>260176</v>
-      </c>
-      <c r="C39" s="7">
         <f t="shared" si="13"/>
         <v>260176</v>
       </c>
+      <c r="C39" s="7">
+        <f t="shared" si="14"/>
+        <v>260176</v>
+      </c>
       <c r="D39" s="7" t="str">
-        <f t="shared" si="14"/>
-        <v>03F850</v>
-      </c>
-      <c r="E39" s="7" t="str">
         <f t="shared" si="15"/>
         <v>03F850</v>
       </c>
-      <c r="F39" s="7"/>
-      <c r="G39" s="8" t="s">
+      <c r="E39" s="7" t="str">
+        <f t="shared" si="16"/>
+        <v>03F850</v>
+      </c>
+      <c r="F39" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>50</v>
+      </c>
+      <c r="G39" s="7"/>
+      <c r="H39" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="H39" s="30" t="s">
+      <c r="I39" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>1</v>
       </c>
       <c r="B40" s="7">
-        <f t="shared" si="12"/>
-        <v>260180</v>
-      </c>
-      <c r="C40" s="7">
         <f t="shared" si="13"/>
         <v>260180</v>
       </c>
+      <c r="C40" s="7">
+        <f t="shared" si="14"/>
+        <v>260180</v>
+      </c>
       <c r="D40" s="7" t="str">
-        <f t="shared" si="14"/>
-        <v>03F854</v>
-      </c>
-      <c r="E40" s="7" t="str">
         <f t="shared" si="15"/>
         <v>03F854</v>
       </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="8" t="s">
+      <c r="E40" s="7" t="str">
+        <f t="shared" si="16"/>
+        <v>03F854</v>
+      </c>
+      <c r="F40" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>54</v>
+      </c>
+      <c r="G40" s="7"/>
+      <c r="H40" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="H40" s="30" t="s">
+      <c r="I40" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>1</v>
       </c>
       <c r="B41" s="7">
-        <f t="shared" si="12"/>
-        <v>260184</v>
-      </c>
-      <c r="C41" s="7">
         <f t="shared" si="13"/>
         <v>260184</v>
       </c>
+      <c r="C41" s="7">
+        <f t="shared" si="14"/>
+        <v>260184</v>
+      </c>
       <c r="D41" s="7" t="str">
-        <f t="shared" si="14"/>
-        <v>03F858</v>
-      </c>
-      <c r="E41" s="7" t="str">
         <f t="shared" si="15"/>
         <v>03F858</v>
       </c>
-      <c r="F41" s="7"/>
-      <c r="G41" s="8" t="s">
+      <c r="E41" s="7" t="str">
+        <f t="shared" si="16"/>
+        <v>03F858</v>
+      </c>
+      <c r="F41" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>58</v>
+      </c>
+      <c r="G41" s="7"/>
+      <c r="H41" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="H41" s="30" t="s">
+      <c r="I41" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>1</v>
       </c>
       <c r="B42" s="7">
-        <f t="shared" si="12"/>
-        <v>260188</v>
-      </c>
-      <c r="C42" s="7">
         <f t="shared" si="13"/>
         <v>260188</v>
       </c>
+      <c r="C42" s="7">
+        <f t="shared" si="14"/>
+        <v>260188</v>
+      </c>
       <c r="D42" s="7" t="str">
-        <f t="shared" si="14"/>
-        <v>03F85C</v>
-      </c>
-      <c r="E42" s="7" t="str">
         <f t="shared" si="15"/>
         <v>03F85C</v>
       </c>
-      <c r="F42" s="7"/>
-      <c r="G42" s="8" t="s">
+      <c r="E42" s="7" t="str">
+        <f t="shared" si="16"/>
+        <v>03F85C</v>
+      </c>
+      <c r="F42" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>5C</v>
+      </c>
+      <c r="G42" s="7"/>
+      <c r="H42" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="H42" s="30" t="s">
+      <c r="I42" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>1</v>
       </c>
       <c r="B43" s="7">
+        <f t="shared" si="13"/>
+        <v>260192</v>
+      </c>
+      <c r="C43" s="7">
+        <f t="shared" ref="C43:C48" si="17">B43+A43-1</f>
+        <v>260192</v>
+      </c>
+      <c r="D43" s="7" t="str">
+        <f t="shared" ref="D43:D48" si="18">DEC2HEX(B43,6)</f>
+        <v>03F860</v>
+      </c>
+      <c r="E43" s="7" t="str">
+        <f t="shared" ref="E43:E48" si="19">DEC2HEX(C43,6)</f>
+        <v>03F860</v>
+      </c>
+      <c r="F43" s="7" t="str">
         <f t="shared" si="12"/>
-        <v>260192</v>
-      </c>
-      <c r="C43" s="7">
-        <f t="shared" ref="C43:C48" si="16">B43+A43-1</f>
-        <v>260192</v>
-      </c>
-      <c r="D43" s="7" t="str">
-        <f t="shared" ref="D43:D48" si="17">DEC2HEX(B43,6)</f>
-        <v>03F860</v>
-      </c>
-      <c r="E43" s="7" t="str">
-        <f t="shared" ref="E43:E48" si="18">DEC2HEX(C43,6)</f>
-        <v>03F860</v>
-      </c>
-      <c r="F43" s="7"/>
-      <c r="G43" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="G43" s="7"/>
+      <c r="H43" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="H43" s="30" t="s">
+      <c r="I43" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>1</v>
       </c>
       <c r="B44" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260196</v>
       </c>
       <c r="C44" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>260196</v>
       </c>
       <c r="D44" s="7" t="str">
-        <f t="shared" si="17"/>
-        <v>03F864</v>
-      </c>
-      <c r="E44" s="7" t="str">
         <f t="shared" si="18"/>
         <v>03F864</v>
       </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="8" t="s">
+      <c r="E44" s="7" t="str">
+        <f t="shared" si="19"/>
+        <v>03F864</v>
+      </c>
+      <c r="F44" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>64</v>
+      </c>
+      <c r="G44" s="7"/>
+      <c r="H44" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="H44" s="30" t="s">
+      <c r="I44" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="7">
         <v>1</v>
       </c>
       <c r="B45" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260200</v>
       </c>
       <c r="C45" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>260200</v>
       </c>
       <c r="D45" s="7" t="str">
-        <f t="shared" si="17"/>
-        <v>03F868</v>
-      </c>
-      <c r="E45" s="7" t="str">
         <f t="shared" si="18"/>
         <v>03F868</v>
       </c>
-      <c r="F45" s="7"/>
-      <c r="G45" s="8" t="s">
+      <c r="E45" s="7" t="str">
+        <f t="shared" si="19"/>
+        <v>03F868</v>
+      </c>
+      <c r="F45" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>68</v>
+      </c>
+      <c r="G45" s="7"/>
+      <c r="H45" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="H45" s="30" t="s">
+      <c r="I45" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>1</v>
       </c>
       <c r="B46" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260204</v>
       </c>
       <c r="C46" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>260204</v>
       </c>
       <c r="D46" s="7" t="str">
-        <f t="shared" si="17"/>
-        <v>03F86C</v>
-      </c>
-      <c r="E46" s="7" t="str">
         <f t="shared" si="18"/>
         <v>03F86C</v>
       </c>
-      <c r="F46" s="7"/>
-      <c r="G46" s="8" t="s">
+      <c r="E46" s="7" t="str">
+        <f t="shared" si="19"/>
+        <v>03F86C</v>
+      </c>
+      <c r="F46" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>6C</v>
+      </c>
+      <c r="G46" s="7"/>
+      <c r="H46" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="H46" s="30" t="s">
+      <c r="I46" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="7">
         <v>1</v>
       </c>
       <c r="B47" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260208</v>
       </c>
       <c r="C47" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>260208</v>
       </c>
       <c r="D47" s="7" t="str">
-        <f t="shared" si="17"/>
-        <v>03F870</v>
-      </c>
-      <c r="E47" s="7" t="str">
         <f t="shared" si="18"/>
         <v>03F870</v>
       </c>
-      <c r="F47" s="7"/>
-      <c r="G47" s="8" t="s">
+      <c r="E47" s="7" t="str">
+        <f t="shared" si="19"/>
+        <v>03F870</v>
+      </c>
+      <c r="F47" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>70</v>
+      </c>
+      <c r="G47" s="7"/>
+      <c r="H47" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="H47" s="30" t="s">
+      <c r="I47" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>1</v>
       </c>
       <c r="B48" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260212</v>
       </c>
       <c r="C48" s="7">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>260212</v>
       </c>
       <c r="D48" s="7" t="str">
-        <f t="shared" si="17"/>
-        <v>03F874</v>
-      </c>
-      <c r="E48" s="7" t="str">
         <f t="shared" si="18"/>
         <v>03F874</v>
       </c>
-      <c r="F48" s="7"/>
-      <c r="G48" s="8" t="s">
+      <c r="E48" s="7" t="str">
+        <f t="shared" si="19"/>
+        <v>03F874</v>
+      </c>
+      <c r="F48" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>74</v>
+      </c>
+      <c r="G48" s="7"/>
+      <c r="H48" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="H48" s="30" t="s">
+      <c r="I48" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>2</v>
       </c>
       <c r="B49" s="7">
+        <f t="shared" si="13"/>
+        <v>260216</v>
+      </c>
+      <c r="C49" s="7">
+        <f t="shared" ref="C49:C53" si="20">B49+A49-1</f>
+        <v>260217</v>
+      </c>
+      <c r="D49" s="7" t="str">
+        <f t="shared" ref="D49:D53" si="21">DEC2HEX(B49,6)</f>
+        <v>03F878</v>
+      </c>
+      <c r="E49" s="7" t="str">
+        <f t="shared" ref="E49:E53" si="22">DEC2HEX(C49,6)</f>
+        <v>03F879</v>
+      </c>
+      <c r="F49" s="7" t="str">
         <f t="shared" si="12"/>
-        <v>260216</v>
-      </c>
-      <c r="C49" s="7">
-        <f t="shared" ref="C49:C53" si="19">B49+A49-1</f>
-        <v>260217</v>
-      </c>
-      <c r="D49" s="7" t="str">
-        <f t="shared" ref="D49:D53" si="20">DEC2HEX(B49,6)</f>
-        <v>03F878</v>
-      </c>
-      <c r="E49" s="7" t="str">
-        <f t="shared" ref="E49:E53" si="21">DEC2HEX(C49,6)</f>
-        <v>03F879</v>
-      </c>
-      <c r="F49" s="7"/>
-      <c r="G49" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G49" s="7"/>
+      <c r="H49" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="H49" s="30" t="s">
+      <c r="I49" s="30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>2</v>
       </c>
       <c r="B50" s="7">
+        <f t="shared" si="13"/>
+        <v>260220</v>
+      </c>
+      <c r="C50" s="7">
+        <f t="shared" si="20"/>
+        <v>260221</v>
+      </c>
+      <c r="D50" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>03F87C</v>
+      </c>
+      <c r="E50" s="7" t="str">
+        <f t="shared" si="22"/>
+        <v>03F87D</v>
+      </c>
+      <c r="F50" s="7" t="str">
         <f t="shared" si="12"/>
-        <v>260220</v>
-      </c>
-      <c r="C50" s="7">
-        <f t="shared" si="19"/>
-        <v>260221</v>
-      </c>
-      <c r="D50" s="7" t="str">
-        <f t="shared" si="20"/>
-        <v>03F87C</v>
-      </c>
-      <c r="E50" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>03F87D</v>
-      </c>
-      <c r="F50" s="7"/>
-      <c r="G50" s="8" t="s">
+        <v>7C</v>
+      </c>
+      <c r="G50" s="7"/>
+      <c r="H50" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="H50" s="30" t="s">
+      <c r="I50" s="30" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>1</v>
       </c>
       <c r="B51" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260224</v>
       </c>
       <c r="C51" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>260224</v>
       </c>
       <c r="D51" s="7" t="str">
-        <f t="shared" si="20"/>
-        <v>03F880</v>
-      </c>
-      <c r="E51" s="7" t="str">
         <f t="shared" si="21"/>
         <v>03F880</v>
       </c>
-      <c r="F51" s="7"/>
-      <c r="G51" s="8" t="s">
+      <c r="E51" s="7" t="str">
+        <f t="shared" si="22"/>
+        <v>03F880</v>
+      </c>
+      <c r="F51" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>80</v>
+      </c>
+      <c r="G51" s="7"/>
+      <c r="H51" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="H51" s="30" t="s">
+      <c r="I51" s="30" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>1</v>
       </c>
       <c r="B52" s="7">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>260228</v>
       </c>
       <c r="C52" s="7">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>260228</v>
       </c>
       <c r="D52" s="7" t="str">
-        <f t="shared" si="20"/>
-        <v>03F884</v>
-      </c>
-      <c r="E52" s="7" t="str">
         <f t="shared" si="21"/>
         <v>03F884</v>
       </c>
-      <c r="F52" s="7"/>
-      <c r="G52" s="8" t="s">
+      <c r="E52" s="7" t="str">
+        <f t="shared" si="22"/>
+        <v>03F884</v>
+      </c>
+      <c r="F52" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>84</v>
+      </c>
+      <c r="G52" s="7"/>
+      <c r="H52" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="H52" s="30" t="s">
+      <c r="I52" s="30" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>2</v>
       </c>
       <c r="B53" s="7">
+        <f t="shared" si="13"/>
+        <v>260232</v>
+      </c>
+      <c r="C53" s="7">
+        <f t="shared" si="20"/>
+        <v>260233</v>
+      </c>
+      <c r="D53" s="7" t="str">
+        <f t="shared" si="21"/>
+        <v>03F888</v>
+      </c>
+      <c r="E53" s="7" t="str">
+        <f t="shared" si="22"/>
+        <v>03F889</v>
+      </c>
+      <c r="F53" s="7" t="str">
         <f t="shared" si="12"/>
-        <v>260232</v>
-      </c>
-      <c r="C53" s="7">
-        <f t="shared" si="19"/>
-        <v>260233</v>
-      </c>
-      <c r="D53" s="7" t="str">
-        <f t="shared" si="20"/>
-        <v>03F888</v>
-      </c>
-      <c r="E53" s="7" t="str">
-        <f t="shared" si="21"/>
-        <v>03F889</v>
-      </c>
-      <c r="F53" s="7"/>
-      <c r="G53" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="G53" s="7"/>
+      <c r="H53" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="H53" s="30" t="s">
+      <c r="I53" s="30" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
-        <f>C54-B54+1</f>
-        <v>1908</v>
+        <v>2</v>
       </c>
       <c r="B54" s="7">
-        <f>B53+4</f>
+        <f t="shared" si="13"/>
         <v>260236</v>
       </c>
       <c r="C54" s="7">
-        <f>C60</f>
+        <f t="shared" ref="C54:C61" si="23">B54+A54-1</f>
+        <v>260237</v>
+      </c>
+      <c r="D54" s="7" t="str">
+        <f t="shared" ref="D54:D61" si="24">DEC2HEX(B54,6)</f>
+        <v>03F88C</v>
+      </c>
+      <c r="E54" s="7" t="str">
+        <f t="shared" ref="E54:E61" si="25">DEC2HEX(C54,6)</f>
+        <v>03F88D</v>
+      </c>
+      <c r="F54" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>8C</v>
+      </c>
+      <c r="G54" s="7"/>
+      <c r="H54" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="I54" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>2</v>
+      </c>
+      <c r="B55" s="7">
+        <f t="shared" si="13"/>
+        <v>260240</v>
+      </c>
+      <c r="C55" s="7">
+        <f t="shared" si="23"/>
+        <v>260241</v>
+      </c>
+      <c r="D55" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v>03F890</v>
+      </c>
+      <c r="E55" s="7" t="str">
+        <f t="shared" si="25"/>
+        <v>03F891</v>
+      </c>
+      <c r="F55" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>90</v>
+      </c>
+      <c r="G55" s="7"/>
+      <c r="H55" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I55" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>2</v>
+      </c>
+      <c r="B56" s="7">
+        <f t="shared" si="13"/>
+        <v>260244</v>
+      </c>
+      <c r="C56" s="7">
+        <f t="shared" si="23"/>
+        <v>260245</v>
+      </c>
+      <c r="D56" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v>03F894</v>
+      </c>
+      <c r="E56" s="7" t="str">
+        <f t="shared" si="25"/>
+        <v>03F895</v>
+      </c>
+      <c r="F56" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>94</v>
+      </c>
+      <c r="G56" s="7"/>
+      <c r="H56" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="I56" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
+        <v>2</v>
+      </c>
+      <c r="B57" s="7">
+        <f t="shared" si="13"/>
+        <v>260248</v>
+      </c>
+      <c r="C57" s="7">
+        <f t="shared" si="23"/>
+        <v>260249</v>
+      </c>
+      <c r="D57" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v>03F898</v>
+      </c>
+      <c r="E57" s="7" t="str">
+        <f t="shared" si="25"/>
+        <v>03F899</v>
+      </c>
+      <c r="F57" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>98</v>
+      </c>
+      <c r="G57" s="7"/>
+      <c r="H57" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="I57" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A58" s="7">
+        <v>2</v>
+      </c>
+      <c r="B58" s="7">
+        <f t="shared" si="13"/>
+        <v>260252</v>
+      </c>
+      <c r="C58" s="7">
+        <f t="shared" si="23"/>
+        <v>260253</v>
+      </c>
+      <c r="D58" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v>03F89C</v>
+      </c>
+      <c r="E58" s="7" t="str">
+        <f t="shared" si="25"/>
+        <v>03F89D</v>
+      </c>
+      <c r="F58" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>9C</v>
+      </c>
+      <c r="G58" s="7"/>
+      <c r="H58" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="I58" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A59" s="7">
+        <v>2</v>
+      </c>
+      <c r="B59" s="7">
+        <f t="shared" si="13"/>
+        <v>260256</v>
+      </c>
+      <c r="C59" s="7">
+        <f t="shared" si="23"/>
+        <v>260257</v>
+      </c>
+      <c r="D59" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v>03F8A0</v>
+      </c>
+      <c r="E59" s="7" t="str">
+        <f t="shared" si="25"/>
+        <v>03F8A1</v>
+      </c>
+      <c r="F59" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>A0</v>
+      </c>
+      <c r="G59" s="7"/>
+      <c r="H59" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="I59" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A60" s="7">
+        <v>2</v>
+      </c>
+      <c r="B60" s="7">
+        <f t="shared" si="13"/>
+        <v>260260</v>
+      </c>
+      <c r="C60" s="7">
+        <f t="shared" si="23"/>
+        <v>260261</v>
+      </c>
+      <c r="D60" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v>03F8A4</v>
+      </c>
+      <c r="E60" s="7" t="str">
+        <f t="shared" si="25"/>
+        <v>03F8A5</v>
+      </c>
+      <c r="F60" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>A4</v>
+      </c>
+      <c r="G60" s="7"/>
+      <c r="H60" s="8" t="s">
+        <v>179</v>
+      </c>
+      <c r="I60" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>2</v>
+      </c>
+      <c r="B61" s="7">
+        <f t="shared" si="13"/>
+        <v>260264</v>
+      </c>
+      <c r="C61" s="7">
+        <f t="shared" si="23"/>
+        <v>260265</v>
+      </c>
+      <c r="D61" s="7" t="str">
+        <f t="shared" si="24"/>
+        <v>03F8A8</v>
+      </c>
+      <c r="E61" s="7" t="str">
+        <f t="shared" si="25"/>
+        <v>03F8A9</v>
+      </c>
+      <c r="F61" s="7" t="str">
+        <f t="shared" si="12"/>
+        <v>A8</v>
+      </c>
+      <c r="G61" s="7"/>
+      <c r="H61" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="I61" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A62" s="7">
+        <f>C62-B62+1</f>
+        <v>1876</v>
+      </c>
+      <c r="B62" s="7">
+        <f>B61+4</f>
+        <v>260268</v>
+      </c>
+      <c r="C62" s="7">
+        <f>C68</f>
         <v>262143</v>
       </c>
-      <c r="D54" s="7" t="str">
+      <c r="D62" s="7" t="str">
         <f t="shared" si="9"/>
-        <v>03F88C</v>
-      </c>
-      <c r="E54" s="7" t="str">
+        <v>03F8AC</v>
+      </c>
+      <c r="E62" s="7" t="str">
         <f t="shared" si="9"/>
         <v>03FFFF</v>
       </c>
-      <c r="F54" s="7"/>
-      <c r="G54" s="12" t="s">
+      <c r="F62" s="7"/>
+      <c r="G62" s="7"/>
+      <c r="H62" s="12" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:14" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="10" t="s">
+    <row r="64" spans="1:15" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="D56" s="16"/>
-      <c r="E56" s="16"/>
-      <c r="F56" s="16"/>
-      <c r="H56" s="30"/>
-      <c r="I56"/>
-      <c r="J56"/>
-      <c r="K56"/>
-      <c r="L56"/>
-      <c r="M56"/>
-      <c r="N56"/>
-    </row>
-    <row r="57" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="D64" s="16"/>
+      <c r="E64" s="16"/>
+      <c r="F64" s="16"/>
+      <c r="G64" s="16"/>
+      <c r="I64" s="30"/>
+      <c r="J64"/>
+      <c r="K64"/>
+      <c r="L64"/>
+      <c r="M64"/>
+      <c r="N64"/>
+      <c r="O64"/>
+    </row>
+    <row r="65" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B65" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C65" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="13" t="s">
+      <c r="D65" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E57" s="13" t="s">
+      <c r="E65" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="F57" s="13"/>
-      <c r="G57" s="10" t="s">
+      <c r="F65" s="13"/>
+      <c r="G65" s="13"/>
+      <c r="H65" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H57" s="30"/>
-      <c r="I57"/>
-      <c r="J57"/>
-      <c r="K57"/>
-      <c r="L57"/>
-      <c r="M57"/>
-      <c r="N57"/>
-    </row>
-    <row r="58" spans="1:14" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13" t="s">
+      <c r="I65" s="30"/>
+      <c r="J65"/>
+      <c r="K65"/>
+      <c r="L65"/>
+      <c r="M65"/>
+      <c r="N65"/>
+      <c r="O65"/>
+    </row>
+    <row r="66" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="13"/>
+      <c r="B66" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C66" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D58" s="13" t="s">
+      <c r="D66" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E66" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="F58" s="13"/>
-      <c r="H58" s="30"/>
-      <c r="I58"/>
-      <c r="J58"/>
-      <c r="K58"/>
-      <c r="L58"/>
-      <c r="M58"/>
-      <c r="N58"/>
-    </row>
-    <row r="59" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="6"/>
-      <c r="B59" s="6"/>
-      <c r="C59" s="6"/>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6"/>
-      <c r="F59" s="6"/>
-      <c r="G59" s="10"/>
-      <c r="H59" s="30"/>
-      <c r="I59"/>
-      <c r="J59"/>
-      <c r="K59"/>
-      <c r="L59"/>
-      <c r="M59"/>
-      <c r="N59"/>
-    </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="7">
+      <c r="F66" s="13"/>
+      <c r="G66" s="13"/>
+      <c r="I66" s="30"/>
+      <c r="J66"/>
+      <c r="K66"/>
+      <c r="L66"/>
+      <c r="M66"/>
+      <c r="N66"/>
+      <c r="O66"/>
+    </row>
+    <row r="67" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="6"/>
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="10"/>
+      <c r="I67" s="30"/>
+      <c r="J67"/>
+      <c r="K67"/>
+      <c r="L67"/>
+      <c r="M67"/>
+      <c r="N67"/>
+      <c r="O67"/>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="7">
         <f>256*1024</f>
         <v>262144</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B68" s="7">
         <v>0</v>
       </c>
-      <c r="C60" s="7">
-        <f>A60-1</f>
+      <c r="C68" s="7">
+        <f>A68-1</f>
         <v>262143</v>
       </c>
-      <c r="D60" s="7" t="str">
-        <f>DEC2HEX(B60,6)</f>
+      <c r="D68" s="7" t="str">
+        <f>DEC2HEX(B68,6)</f>
         <v>000000</v>
       </c>
-      <c r="E60" s="7" t="str">
-        <f>DEC2HEX(C60,6)</f>
+      <c r="E68" s="7" t="str">
+        <f>DEC2HEX(C68,6)</f>
         <v>03FFFF</v>
       </c>
-      <c r="F60" s="7"/>
-      <c r="G60" s="12" t="s">
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="H60" s="34"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="7">
+      <c r="I68" s="34"/>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A69" s="7">
         <f>2*(128*96*2)</f>
         <v>49152</v>
       </c>
-      <c r="B61" s="7">
-        <f>C60+1</f>
+      <c r="B69" s="7">
+        <f>C68+1</f>
         <v>262144</v>
       </c>
-      <c r="C61" s="7">
-        <f t="shared" ref="C61:C63" si="22">B61+A61-1</f>
+      <c r="C69" s="7">
+        <f t="shared" ref="C69:C71" si="26">B69+A69-1</f>
         <v>311295</v>
       </c>
-      <c r="D61" s="7" t="str">
-        <f t="shared" ref="D61:E64" si="23">DEC2HEX(B61,6)</f>
+      <c r="D69" s="7" t="str">
+        <f t="shared" ref="D69:E72" si="27">DEC2HEX(B69,6)</f>
         <v>040000</v>
       </c>
-      <c r="E61" s="7" t="str">
-        <f t="shared" si="23"/>
+      <c r="E69" s="7" t="str">
+        <f t="shared" si="27"/>
         <v>04BFFF</v>
       </c>
-      <c r="F61" s="7"/>
-      <c r="G61" s="8" t="s">
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="H61" s="30" t="s">
+      <c r="I69" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="7">
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A70" s="7">
         <v>512</v>
       </c>
-      <c r="B62" s="7">
-        <f>C61+1</f>
+      <c r="B70" s="7">
+        <f>C69+1</f>
         <v>311296</v>
       </c>
-      <c r="C62" s="7">
-        <f t="shared" ref="C62" si="24">B62+A62-1</f>
+      <c r="C70" s="7">
+        <f t="shared" ref="C70" si="28">B70+A70-1</f>
         <v>311807</v>
       </c>
-      <c r="D62" s="7" t="str">
-        <f t="shared" ref="D62" si="25">DEC2HEX(B62,6)</f>
+      <c r="D70" s="7" t="str">
+        <f t="shared" ref="D70" si="29">DEC2HEX(B70,6)</f>
         <v>04C000</v>
       </c>
-      <c r="E62" s="7" t="str">
-        <f t="shared" ref="E62" si="26">DEC2HEX(C62,6)</f>
+      <c r="E70" s="7" t="str">
+        <f t="shared" ref="E70" si="30">DEC2HEX(C70,6)</f>
         <v>04C1FF</v>
       </c>
-      <c r="F62" s="7"/>
-      <c r="G62" s="8" t="s">
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="H62" s="30" t="s">
+      <c r="I70" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="7">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
         <v>512</v>
       </c>
-      <c r="B63" s="7">
-        <f>C62+1</f>
+      <c r="B71" s="7">
+        <f>C70+1</f>
         <v>311808</v>
       </c>
-      <c r="C63" s="7">
-        <f t="shared" si="22"/>
+      <c r="C71" s="7">
+        <f t="shared" si="26"/>
         <v>312319</v>
       </c>
-      <c r="D63" s="7" t="str">
-        <f t="shared" si="23"/>
+      <c r="D71" s="7" t="str">
+        <f t="shared" si="27"/>
         <v>04C200</v>
       </c>
-      <c r="E63" s="7" t="str">
-        <f t="shared" si="23"/>
+      <c r="E71" s="7" t="str">
+        <f t="shared" si="27"/>
         <v>04C3FF</v>
       </c>
-      <c r="F63" s="7"/>
-      <c r="G63" s="8" t="s">
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="H63" s="30" t="s">
+      <c r="I71" s="30" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="7">
-        <f>C64-B64</f>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
+        <f>C72-B72</f>
         <v>16464895</v>
       </c>
-      <c r="B64" s="7">
-        <f>C63+1</f>
+      <c r="B72" s="7">
+        <f>C71+1</f>
         <v>312320</v>
       </c>
-      <c r="C64" s="7">
+      <c r="C72" s="7">
         <f>16*1024*1024-1</f>
         <v>16777215</v>
       </c>
-      <c r="D64" s="7" t="str">
-        <f t="shared" si="23"/>
+      <c r="D72" s="7" t="str">
+        <f t="shared" si="27"/>
         <v>04C400</v>
       </c>
-      <c r="E64" s="7" t="str">
-        <f t="shared" si="23"/>
+      <c r="E72" s="7" t="str">
+        <f t="shared" si="27"/>
         <v>FFFFFF</v>
       </c>
-      <c r="F64" s="7"/>
-      <c r="G64" s="8" t="s">
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H64" s="30" t="s">
+      <c r="I72" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J72" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2944,7 +3440,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:I19"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -3490,7 +3986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:I11"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -3769,7 +4265,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:O23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -4301,7 +4797,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5698,7 +6194,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5762,7 +6258,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5935,7 +6431,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="B2:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Inserted a pipeline stage in the SRAM read databus, within the datapath.  Fetch instructions are now one cycle longer, but load literal instructions complete in one clock cycle.
</commit_message>
<xml_diff>
--- a/Resources/Memory map.xlsx
+++ b/Resources/Memory map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\N.I.G.E.-Machine\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3974D07-E5E6-406A-A6B5-7FCEB29EC48A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8BE5339-5A01-42F8-B433-D48958035DB4}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="195" windowWidth="22995" windowHeight="10425" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1257,8 +1257,8 @@
   </sheetPr>
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>